<commit_message>
message.xlsx change. SKIP_SCENARIO, SKIP_CASE
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F76CB9-9FF0-3C4E-9ECA-237D1223ECD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF4CA8F-C5FE-EF41-962F-A83B773FD213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35860" yWindow="2320" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -3964,18 +3964,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>case skipped.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>SKIP_SCENARIO</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>scenario skipped.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>elementNotFound</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4716,36 +4708,6 @@
   </si>
   <si>
     <t>テストが実装されていないか不完全です。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>case</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tsukushi A Round Gothic Bold"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>がスキップされました。</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>scenario</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tsukushi A Round Gothic Bold"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>がスキップされました。</t>
-    </r>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -9603,6 +9565,44 @@
         <charset val="128"/>
       </rPr>
       <t>であること</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skipping case</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skipping scenario</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>case</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>をスキップする</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>をスキップする</t>
     </r>
     <phoneticPr fontId="1"/>
   </si>
@@ -11251,16 +11251,16 @@
     </row>
     <row r="6" spans="1:9" ht="19" customHeight="1">
       <c r="A6" s="19" t="s">
+        <v>879</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>882</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>883</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>886</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>887</v>
-      </c>
       <c r="D6" s="20" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -11270,16 +11270,16 @@
     </row>
     <row r="7" spans="1:9" ht="19" customHeight="1">
       <c r="A7" s="19" t="s">
+        <v>880</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>881</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>884</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>885</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>888</v>
-      </c>
       <c r="D7" s="20" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -11292,7 +11292,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>21</v>
@@ -11311,7 +11311,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>23</v>
@@ -11330,7 +11330,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>25</v>
@@ -11349,7 +11349,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>27</v>
@@ -11368,7 +11368,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>29</v>
@@ -11387,7 +11387,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>31</v>
@@ -11406,7 +11406,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>33</v>
@@ -11425,7 +11425,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>35</v>
@@ -11444,7 +11444,7 @@
         <v>36</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>37</v>
@@ -11463,7 +11463,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>39</v>
@@ -11482,7 +11482,7 @@
         <v>40</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>41</v>
@@ -11501,7 +11501,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>43</v>
@@ -11520,7 +11520,7 @@
         <v>44</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>45</v>
@@ -11539,7 +11539,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>47</v>
@@ -11558,7 +11558,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>49</v>
@@ -11577,7 +11577,7 @@
         <v>50</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>51</v>
@@ -11596,7 +11596,7 @@
         <v>52</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>53</v>
@@ -11612,16 +11612,16 @@
     </row>
     <row r="25" spans="1:9" ht="19" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>922</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>924</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>926</v>
       </c>
-      <c r="B25" s="20" t="s">
-        <v>928</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>930</v>
-      </c>
       <c r="D25" s="20" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
@@ -11631,16 +11631,16 @@
     </row>
     <row r="26" spans="1:9" ht="19" customHeight="1">
       <c r="A26" s="19" t="s">
+        <v>923</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>925</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>927</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>929</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>931</v>
-      </c>
       <c r="D26" s="20" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
@@ -11650,16 +11650,16 @@
     </row>
     <row r="27" spans="1:9" ht="19" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
@@ -11672,7 +11672,7 @@
         <v>98</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>99</v>
@@ -11691,7 +11691,7 @@
         <v>54</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>55</v>
@@ -11710,10 +11710,10 @@
         <v>56</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>289</v>
@@ -11767,13 +11767,13 @@
         <v>100</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -11783,16 +11783,16 @@
     </row>
     <row r="34" spans="1:9" ht="19" customHeight="1">
       <c r="A34" s="19" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D34" s="20" t="s">
         <v>1112</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>1116</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -11802,16 +11802,16 @@
     </row>
     <row r="35" spans="1:9" ht="19" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
@@ -11821,16 +11821,16 @@
     </row>
     <row r="36" spans="1:9" ht="19" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
@@ -11843,7 +11843,7 @@
         <v>101</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>102</v>
@@ -11900,7 +11900,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>108</v>
@@ -11935,16 +11935,16 @@
     </row>
     <row r="42" spans="1:9" ht="19" customHeight="1">
       <c r="A42" s="19" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C42" s="20" t="s">
         <v>1077</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="D42" s="20" t="s">
         <v>1079</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>1081</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>1083</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
@@ -11954,16 +11954,16 @@
     </row>
     <row r="43" spans="1:9" ht="19" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>1078</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="D43" s="20" t="s">
         <v>1080</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>1084</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
@@ -11976,7 +11976,7 @@
         <v>111</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>112</v>
@@ -11995,7 +11995,7 @@
         <v>113</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>114</v>
@@ -12014,7 +12014,7 @@
         <v>115</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>116</v>
@@ -12087,16 +12087,16 @@
     </row>
     <row r="50" spans="1:9" ht="19" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C50" s="20" t="s">
         <v>1069</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="D50" s="20" t="s">
         <v>1071</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>1073</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>1075</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
@@ -12106,16 +12106,16 @@
     </row>
     <row r="51" spans="1:9" ht="19" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C51" s="20" t="s">
         <v>1070</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="D51" s="20" t="s">
         <v>1072</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>1074</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>1076</v>
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
@@ -12144,16 +12144,16 @@
     </row>
     <row r="53" spans="1:9" ht="19" customHeight="1">
       <c r="A53" s="19" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
@@ -12163,16 +12163,16 @@
     </row>
     <row r="54" spans="1:9" ht="19" customHeight="1">
       <c r="A54" s="19" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="E54" s="20"/>
       <c r="F54" s="20"/>
@@ -12182,16 +12182,16 @@
     </row>
     <row r="55" spans="1:9" ht="19" customHeight="1">
       <c r="A55" s="19" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -12201,16 +12201,16 @@
     </row>
     <row r="56" spans="1:9" ht="19" customHeight="1">
       <c r="A56" s="19" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="E56" s="20"/>
       <c r="F56" s="20"/>
@@ -12220,16 +12220,16 @@
     </row>
     <row r="57" spans="1:9" ht="19" customHeight="1">
       <c r="A57" s="19" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="E57" s="20"/>
       <c r="F57" s="20"/>
@@ -12242,7 +12242,7 @@
         <v>61</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>62</v>
@@ -12315,16 +12315,16 @@
     </row>
     <row r="62" spans="1:9" ht="19" customHeight="1">
       <c r="A62" s="19" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="20"/>
@@ -12334,16 +12334,16 @@
     </row>
     <row r="63" spans="1:9" ht="19" customHeight="1">
       <c r="A63" s="19" t="s">
+        <v>827</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>829</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>830</v>
+      </c>
+      <c r="D63" s="20" t="s">
         <v>831</v>
-      </c>
-      <c r="B63" s="20" t="s">
-        <v>833</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>834</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>835</v>
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
@@ -12353,16 +12353,16 @@
     </row>
     <row r="64" spans="1:9" ht="19" customHeight="1">
       <c r="A64" s="19" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="20"/>
@@ -12372,16 +12372,16 @@
     </row>
     <row r="65" spans="1:9" ht="19" customHeight="1">
       <c r="A65" s="19" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
@@ -12391,16 +12391,16 @@
     </row>
     <row r="66" spans="1:9" ht="19" customHeight="1">
       <c r="A66" s="19" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
@@ -12410,16 +12410,16 @@
     </row>
     <row r="67" spans="1:9" ht="19" customHeight="1">
       <c r="A67" s="19" t="s">
+        <v>840</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>843</v>
+      </c>
+      <c r="C67" s="20" t="s">
         <v>844</v>
       </c>
-      <c r="B67" s="20" t="s">
-        <v>847</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>848</v>
-      </c>
       <c r="D67" s="20" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
@@ -12429,16 +12429,16 @@
     </row>
     <row r="68" spans="1:9" ht="19" customHeight="1">
       <c r="A68" s="19" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="20"/>
@@ -12448,16 +12448,16 @@
     </row>
     <row r="69" spans="1:9" ht="19" customHeight="1">
       <c r="A69" s="19" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="20"/>
@@ -12467,16 +12467,16 @@
     </row>
     <row r="70" spans="1:9" ht="19" customHeight="1">
       <c r="A70" s="19" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
@@ -12495,7 +12495,7 @@
         <v>70</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
@@ -12533,7 +12533,7 @@
         <v>74</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="20"/>
@@ -12562,16 +12562,16 @@
     </row>
     <row r="75" spans="1:9" ht="19" customHeight="1">
       <c r="A75" s="19" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="E75" s="20"/>
       <c r="F75" s="20"/>
@@ -12600,16 +12600,16 @@
     </row>
     <row r="77" spans="1:9" ht="19" customHeight="1">
       <c r="A77" s="19" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="B77" s="20" t="s">
+        <v>908</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>909</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>912</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>913</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>916</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="20"/>
@@ -12771,16 +12771,16 @@
     </row>
     <row r="86" spans="1:9" ht="19" customHeight="1">
       <c r="A86" s="19" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="20"/>
@@ -12812,7 +12812,7 @@
         <v>96</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C88" s="20" t="s">
         <v>97</v>
@@ -12828,16 +12828,16 @@
     </row>
     <row r="89" spans="1:9" ht="19" customHeight="1">
       <c r="A89" s="19" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="B89" s="20" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="D89" s="20" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="20"/>
@@ -12847,16 +12847,16 @@
     </row>
     <row r="90" spans="1:9" ht="19" customHeight="1">
       <c r="A90" s="19" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B90" s="20" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="20"/>
@@ -12866,16 +12866,16 @@
     </row>
     <row r="91" spans="1:9" ht="19" customHeight="1">
       <c r="A91" s="19" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="E91" s="20"/>
       <c r="F91" s="20"/>
@@ -12885,16 +12885,16 @@
     </row>
     <row r="92" spans="1:9" ht="19" customHeight="1">
       <c r="A92" s="19" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="E92" s="20"/>
       <c r="F92" s="20"/>
@@ -12904,16 +12904,16 @@
     </row>
     <row r="93" spans="1:9" ht="19" customHeight="1">
       <c r="A93" s="19" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="E93" s="20"/>
       <c r="F93" s="20"/>
@@ -12923,16 +12923,16 @@
     </row>
     <row r="94" spans="1:9" ht="19" customHeight="1">
       <c r="A94" s="19" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="E94" s="20"/>
       <c r="F94" s="20"/>
@@ -12942,16 +12942,16 @@
     </row>
     <row r="95" spans="1:9" ht="19" customHeight="1">
       <c r="A95" s="19" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="D95" s="20" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="E95" s="20"/>
       <c r="F95" s="20"/>
@@ -12961,16 +12961,16 @@
     </row>
     <row r="96" spans="1:9" ht="19" customHeight="1">
       <c r="A96" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="B96" s="19" t="s">
+        <v>994</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>996</v>
+      </c>
+      <c r="D96" s="20" t="s">
         <v>997</v>
-      </c>
-      <c r="B96" s="19" t="s">
-        <v>998</v>
-      </c>
-      <c r="C96" s="20" t="s">
-        <v>1000</v>
-      </c>
-      <c r="D96" s="20" t="s">
-        <v>1001</v>
       </c>
       <c r="E96" s="20"/>
       <c r="F96" s="20"/>
@@ -12980,16 +12980,16 @@
     </row>
     <row r="97" spans="1:9" ht="19" customHeight="1">
       <c r="A97" s="19" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="E97" s="20"/>
       <c r="F97" s="20"/>
@@ -12999,16 +12999,16 @@
     </row>
     <row r="98" spans="1:9" ht="19" customHeight="1">
       <c r="A98" s="19" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="E98" s="20"/>
       <c r="F98" s="20"/>
@@ -13018,16 +13018,16 @@
     </row>
     <row r="99" spans="1:9" ht="19" customHeight="1">
       <c r="A99" s="19" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="E99" s="20"/>
       <c r="F99" s="20"/>
@@ -13037,16 +13037,16 @@
     </row>
     <row r="100" spans="1:9" ht="19" customHeight="1">
       <c r="A100" s="19" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E100" s="20"/>
       <c r="F100" s="20"/>
@@ -13056,16 +13056,16 @@
     </row>
     <row r="101" spans="1:9" ht="19" customHeight="1">
       <c r="A101" s="19" t="s">
+        <v>867</v>
+      </c>
+      <c r="B101" s="20" t="s">
         <v>871</v>
       </c>
-      <c r="B101" s="20" t="s">
-        <v>875</v>
-      </c>
       <c r="C101" s="20" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="20"/>
@@ -13075,16 +13075,16 @@
     </row>
     <row r="102" spans="1:9" ht="19" customHeight="1">
       <c r="A102" s="19" t="s">
+        <v>868</v>
+      </c>
+      <c r="B102" s="20" t="s">
         <v>872</v>
       </c>
-      <c r="B102" s="20" t="s">
-        <v>876</v>
-      </c>
       <c r="C102" s="20" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="D102" s="20" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="E102" s="20"/>
       <c r="F102" s="20"/>
@@ -13094,16 +13094,16 @@
     </row>
     <row r="103" spans="1:9" ht="19" customHeight="1">
       <c r="A103" s="19" t="s">
+        <v>869</v>
+      </c>
+      <c r="B103" s="20" t="s">
         <v>873</v>
       </c>
-      <c r="B103" s="20" t="s">
-        <v>877</v>
-      </c>
       <c r="C103" s="20" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="D103" s="20" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="20"/>
@@ -13113,16 +13113,16 @@
     </row>
     <row r="104" spans="1:9" ht="19" customHeight="1">
       <c r="A104" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="B104" s="19" t="s">
         <v>874</v>
       </c>
-      <c r="B104" s="19" t="s">
-        <v>878</v>
-      </c>
       <c r="C104" s="20" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="20"/>
@@ -13132,16 +13132,16 @@
     </row>
     <row r="105" spans="1:9" ht="19" customHeight="1">
       <c r="A105" s="19" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="20"/>
@@ -13151,16 +13151,16 @@
     </row>
     <row r="106" spans="1:9" ht="19" customHeight="1">
       <c r="A106" s="19" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="D106" s="20" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="20"/>
@@ -13173,7 +13173,7 @@
         <v>124</v>
       </c>
       <c r="B107" s="20" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C107" s="20" t="s">
         <v>125</v>
@@ -13189,16 +13189,16 @@
     </row>
     <row r="108" spans="1:9" ht="19" customHeight="1">
       <c r="A108" s="19" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="B108" s="20" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="D108" s="20" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="20"/>
@@ -13208,16 +13208,16 @@
     </row>
     <row r="109" spans="1:9" ht="19" customHeight="1">
       <c r="A109" s="19" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="B109" s="20" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="D109" s="20" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="20"/>
@@ -13227,16 +13227,16 @@
     </row>
     <row r="110" spans="1:9" ht="19" customHeight="1">
       <c r="A110" s="19" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="B110" s="20" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="D110" s="20" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="20"/>
@@ -13284,16 +13284,16 @@
     </row>
     <row r="113" spans="1:9" ht="19" customHeight="1">
       <c r="A113" s="19" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="C113" s="20" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="D113" s="20" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="E113" s="20"/>
       <c r="F113" s="20"/>
@@ -13303,16 +13303,16 @@
     </row>
     <row r="114" spans="1:9" ht="19" customHeight="1">
       <c r="A114" s="19" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="C114" s="20" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="D114" s="20" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E114" s="20"/>
       <c r="F114" s="20"/>
@@ -13325,7 +13325,7 @@
         <v>130</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="C115" s="20" t="s">
         <v>131</v>
@@ -13344,7 +13344,7 @@
         <v>132</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C116" s="20" t="s">
         <v>133</v>
@@ -13363,7 +13363,7 @@
         <v>134</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="C117" s="20" t="s">
         <v>135</v>
@@ -13382,7 +13382,7 @@
         <v>136</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C118" s="20" t="s">
         <v>137</v>
@@ -13401,7 +13401,7 @@
         <v>138</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C119" s="20" t="s">
         <v>139</v>
@@ -13420,7 +13420,7 @@
         <v>140</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="C120" s="20" t="s">
         <v>141</v>
@@ -13439,7 +13439,7 @@
         <v>142</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C121" s="20" t="s">
         <v>143</v>
@@ -13458,7 +13458,7 @@
         <v>144</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C122" s="20" t="s">
         <v>17</v>
@@ -13477,7 +13477,7 @@
         <v>145</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="C123" s="20" t="s">
         <v>146</v>
@@ -13496,7 +13496,7 @@
         <v>147</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="C124" s="20" t="s">
         <v>19</v>
@@ -13515,7 +13515,7 @@
         <v>148</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C125" s="20" t="s">
         <v>149</v>
@@ -13534,7 +13534,7 @@
         <v>150</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C126" s="20" t="s">
         <v>151</v>
@@ -13553,7 +13553,7 @@
         <v>152</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="C127" s="20" t="s">
         <v>153</v>
@@ -13572,7 +13572,7 @@
         <v>154</v>
       </c>
       <c r="B128" s="19" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C128" s="20" t="s">
         <v>155</v>
@@ -13591,7 +13591,7 @@
         <v>156</v>
       </c>
       <c r="B129" s="19" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C129" s="20" t="s">
         <v>157</v>
@@ -13610,7 +13610,7 @@
         <v>158</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C130" s="20" t="s">
         <v>159</v>
@@ -13629,7 +13629,7 @@
         <v>160</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C131" s="20" t="s">
         <v>161</v>
@@ -13648,7 +13648,7 @@
         <v>162</v>
       </c>
       <c r="B132" s="19" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C132" s="20" t="s">
         <v>163</v>
@@ -13667,7 +13667,7 @@
         <v>164</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C133" s="20" t="s">
         <v>165</v>
@@ -13686,7 +13686,7 @@
         <v>166</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C134" s="20" t="s">
         <v>167</v>
@@ -13705,7 +13705,7 @@
         <v>168</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="C135" s="20" t="s">
         <v>169</v>
@@ -13724,7 +13724,7 @@
         <v>170</v>
       </c>
       <c r="B136" s="19" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="C136" s="20" t="s">
         <v>171</v>
@@ -13743,7 +13743,7 @@
         <v>172</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C137" s="20" t="s">
         <v>173</v>
@@ -13762,7 +13762,7 @@
         <v>174</v>
       </c>
       <c r="B138" s="19" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C138" s="20" t="s">
         <v>175</v>
@@ -13781,7 +13781,7 @@
         <v>176</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C139" s="20" t="s">
         <v>177</v>
@@ -13800,7 +13800,7 @@
         <v>178</v>
       </c>
       <c r="B140" s="19" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="C140" s="20" t="s">
         <v>179</v>
@@ -13819,7 +13819,7 @@
         <v>180</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C141" s="20" t="s">
         <v>181</v>
@@ -14025,13 +14025,13 @@
     </row>
     <row r="152" spans="1:9" ht="19" customHeight="1">
       <c r="A152" s="19" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="B152" s="19" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="C152" s="20" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="D152" s="22" t="s">
         <v>359</v>
@@ -14044,13 +14044,13 @@
     </row>
     <row r="153" spans="1:9" ht="19" customHeight="1">
       <c r="A153" s="19" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="B153" s="19" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="D153" s="22" t="s">
         <v>360</v>
@@ -14164,7 +14164,7 @@
         <v>450</v>
       </c>
       <c r="C159" s="20" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="D159" s="22" t="s">
         <v>368</v>
@@ -14183,7 +14183,7 @@
         <v>457</v>
       </c>
       <c r="C160" s="20" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="D160" s="22" t="s">
         <v>375</v>
@@ -14202,7 +14202,7 @@
         <v>451</v>
       </c>
       <c r="C161" s="20" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="D161" s="22" t="s">
         <v>369</v>
@@ -14221,7 +14221,7 @@
         <v>452</v>
       </c>
       <c r="C162" s="20" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="D162" s="22" t="s">
         <v>370</v>
@@ -14240,7 +14240,7 @@
         <v>453</v>
       </c>
       <c r="C163" s="20" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="D163" s="22" t="s">
         <v>371</v>
@@ -14259,7 +14259,7 @@
         <v>454</v>
       </c>
       <c r="C164" s="20" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="D164" s="22" t="s">
         <v>372</v>
@@ -14278,7 +14278,7 @@
         <v>455</v>
       </c>
       <c r="C165" s="20" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="D165" s="22" t="s">
         <v>373</v>
@@ -14297,7 +14297,7 @@
         <v>456</v>
       </c>
       <c r="C166" s="20" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="D166" s="22" t="s">
         <v>374</v>
@@ -14386,16 +14386,16 @@
     </row>
     <row r="171" spans="1:9" ht="19" customHeight="1">
       <c r="A171" s="19" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="B171" s="19" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="C171" s="20" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="E171" s="20"/>
       <c r="F171" s="20"/>
@@ -14411,7 +14411,7 @@
         <v>462</v>
       </c>
       <c r="C172" s="20" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="D172" s="22" t="s">
         <v>378</v>
@@ -14430,10 +14430,10 @@
         <v>463</v>
       </c>
       <c r="C173" s="20" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="D173" s="22" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="E173" s="20"/>
       <c r="F173" s="20"/>
@@ -14449,7 +14449,7 @@
         <v>468</v>
       </c>
       <c r="C174" s="20" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="D174" s="22" t="s">
         <v>384</v>
@@ -14468,7 +14468,7 @@
         <v>469</v>
       </c>
       <c r="C175" s="20" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="D175" s="22" t="s">
         <v>385</v>
@@ -14487,7 +14487,7 @@
         <v>464</v>
       </c>
       <c r="C176" s="20" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="D176" s="22" t="s">
         <v>379</v>
@@ -14506,7 +14506,7 @@
         <v>465</v>
       </c>
       <c r="C177" s="20" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="D177" s="22" t="s">
         <v>380</v>
@@ -14525,7 +14525,7 @@
         <v>466</v>
       </c>
       <c r="C178" s="20" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="D178" s="22" t="s">
         <v>381</v>
@@ -14544,7 +14544,7 @@
         <v>467</v>
       </c>
       <c r="C179" s="20" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="D179" s="22" t="s">
         <v>382</v>
@@ -14712,7 +14712,7 @@
         <v>248</v>
       </c>
       <c r="B188" s="19" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="C188" s="20" t="s">
         <v>249</v>
@@ -14731,7 +14731,7 @@
         <v>250</v>
       </c>
       <c r="B189" s="19" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C189" s="20" t="s">
         <v>251</v>
@@ -14842,16 +14842,16 @@
     </row>
     <row r="195" spans="1:9" ht="19" customHeight="1">
       <c r="A195" s="19" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="B195" s="19" t="s">
         <v>438</v>
       </c>
       <c r="C195" s="20" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="D195" s="20" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="E195" s="20"/>
       <c r="F195" s="20"/>
@@ -14861,16 +14861,16 @@
     </row>
     <row r="196" spans="1:9" ht="19" customHeight="1">
       <c r="A196" s="19" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="B196" s="19" t="s">
         <v>438</v>
       </c>
       <c r="C196" s="20" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="D196" s="20" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="E196" s="20"/>
       <c r="F196" s="20"/>
@@ -14880,16 +14880,16 @@
     </row>
     <row r="197" spans="1:9" ht="19" customHeight="1">
       <c r="A197" s="19" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="B197" s="19" t="s">
         <v>438</v>
       </c>
       <c r="C197" s="20" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="D197" s="20" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="E197" s="20"/>
       <c r="F197" s="20"/>
@@ -14899,16 +14899,16 @@
     </row>
     <row r="198" spans="1:9" ht="19" customHeight="1">
       <c r="A198" s="19" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="B198" s="19" t="s">
         <v>438</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="D198" s="20" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="E198" s="20"/>
       <c r="F198" s="20"/>
@@ -15126,10 +15126,16 @@
       <c r="I209" s="18"/>
     </row>
     <row r="210" spans="1:9" ht="19" customHeight="1">
-      <c r="A210" s="19"/>
+      <c r="A210" s="19" t="s">
+        <v>492</v>
+      </c>
       <c r="B210" s="20"/>
-      <c r="C210" s="20"/>
-      <c r="D210" s="20"/>
+      <c r="C210" s="20" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D210" s="20" t="s">
+        <v>1116</v>
+      </c>
       <c r="E210" s="20"/>
       <c r="F210" s="20"/>
       <c r="G210" s="18"/>
@@ -15137,10 +15143,16 @@
       <c r="I210" s="18"/>
     </row>
     <row r="211" spans="1:9" ht="19" customHeight="1">
-      <c r="A211" s="19"/>
+      <c r="A211" s="19" t="s">
+        <v>493</v>
+      </c>
       <c r="B211" s="20"/>
-      <c r="C211" s="20"/>
-      <c r="D211" s="20"/>
+      <c r="C211" s="20" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D211" s="20" t="s">
+        <v>1117</v>
+      </c>
       <c r="E211" s="20"/>
       <c r="F211" s="20"/>
       <c r="G211" s="18"/>
@@ -15170,29 +15182,21 @@
       <c r="I213" s="18"/>
     </row>
     <row r="214" spans="1:9" ht="19" customHeight="1">
-      <c r="A214" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
-      <c r="D214" s="23"/>
-      <c r="E214" s="23"/>
-      <c r="F214" s="23"/>
-      <c r="G214" s="24"/>
-      <c r="H214" s="25"/>
-      <c r="I214" s="24"/>
+      <c r="A214" s="19"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
+      <c r="D214" s="20"/>
+      <c r="E214" s="20"/>
+      <c r="F214" s="20"/>
+      <c r="G214" s="18"/>
+      <c r="H214" s="17"/>
+      <c r="I214" s="18"/>
     </row>
     <row r="215" spans="1:9" ht="19" customHeight="1">
-      <c r="A215" s="19" t="s">
-        <v>487</v>
-      </c>
+      <c r="A215" s="19"/>
       <c r="B215" s="20"/>
-      <c r="C215" s="20" t="s">
-        <v>487</v>
-      </c>
-      <c r="D215" s="20" t="s">
-        <v>678</v>
-      </c>
+      <c r="C215" s="20"/>
+      <c r="D215" s="20"/>
       <c r="E215" s="20"/>
       <c r="F215" s="20"/>
       <c r="G215" s="18"/>
@@ -15200,32 +15204,28 @@
       <c r="I215" s="18"/>
     </row>
     <row r="216" spans="1:9" ht="19" customHeight="1">
-      <c r="A216" s="19" t="s">
-        <v>488</v>
-      </c>
-      <c r="B216" s="20"/>
-      <c r="C216" s="20" t="s">
-        <v>488</v>
-      </c>
-      <c r="D216" s="22" t="s">
-        <v>679</v>
-      </c>
-      <c r="E216" s="20"/>
-      <c r="F216" s="20"/>
-      <c r="G216" s="18"/>
-      <c r="H216" s="17"/>
-      <c r="I216" s="18"/>
+      <c r="A216" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="B216" s="23"/>
+      <c r="C216" s="23"/>
+      <c r="D216" s="23"/>
+      <c r="E216" s="23"/>
+      <c r="F216" s="23"/>
+      <c r="G216" s="24"/>
+      <c r="H216" s="25"/>
+      <c r="I216" s="24"/>
     </row>
     <row r="217" spans="1:9" ht="19" customHeight="1">
       <c r="A217" s="19" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B217" s="20"/>
       <c r="C217" s="20" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D217" s="20" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="E217" s="20"/>
       <c r="F217" s="20"/>
@@ -15235,14 +15235,14 @@
     </row>
     <row r="218" spans="1:9" ht="19" customHeight="1">
       <c r="A218" s="19" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B218" s="20"/>
       <c r="C218" s="20" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D218" s="22" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="E218" s="20"/>
       <c r="F218" s="20"/>
@@ -15252,14 +15252,14 @@
     </row>
     <row r="219" spans="1:9" ht="19" customHeight="1">
       <c r="A219" s="19" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B219" s="20"/>
       <c r="C219" s="20" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D219" s="20" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="E219" s="20"/>
       <c r="F219" s="20"/>
@@ -15269,14 +15269,14 @@
     </row>
     <row r="220" spans="1:9" ht="19" customHeight="1">
       <c r="A220" s="19" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B220" s="20"/>
       <c r="C220" s="20" t="s">
-        <v>495</v>
-      </c>
-      <c r="D220" s="20" t="s">
-        <v>683</v>
+        <v>491</v>
+      </c>
+      <c r="D220" s="22" t="s">
+        <v>679</v>
       </c>
       <c r="E220" s="20"/>
       <c r="F220" s="20"/>
@@ -15286,14 +15286,14 @@
     </row>
     <row r="221" spans="1:9" ht="19" customHeight="1">
       <c r="A221" s="19" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B221" s="20"/>
       <c r="C221" s="20" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D221" s="21" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="E221" s="20"/>
       <c r="F221" s="20"/>
@@ -15303,14 +15303,14 @@
     </row>
     <row r="222" spans="1:9" ht="19" customHeight="1">
       <c r="A222" s="19" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B222" s="20"/>
       <c r="C222" s="20" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D222" s="22" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="E222" s="20"/>
       <c r="F222" s="20"/>
@@ -15320,14 +15320,14 @@
     </row>
     <row r="223" spans="1:9" ht="19" customHeight="1">
       <c r="A223" s="19" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B223" s="20"/>
       <c r="C223" s="20" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D223" s="21" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="E223" s="20"/>
       <c r="F223" s="20"/>
@@ -15337,14 +15337,14 @@
     </row>
     <row r="224" spans="1:9" ht="19" customHeight="1">
       <c r="A224" s="19" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B224" s="20"/>
       <c r="C224" s="20" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D224" s="21" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="E224" s="20"/>
       <c r="F224" s="20"/>
@@ -15354,14 +15354,14 @@
     </row>
     <row r="225" spans="1:9" ht="19" customHeight="1">
       <c r="A225" s="19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B225" s="20"/>
       <c r="C225" s="20" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D225" s="21" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="E225" s="20"/>
       <c r="F225" s="20"/>
@@ -15371,14 +15371,14 @@
     </row>
     <row r="226" spans="1:9" ht="19" customHeight="1">
       <c r="A226" s="19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B226" s="20"/>
       <c r="C226" s="20" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="D226" s="21" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="E226" s="20"/>
       <c r="F226" s="20"/>
@@ -15388,14 +15388,14 @@
     </row>
     <row r="227" spans="1:9" ht="19" customHeight="1">
       <c r="A227" s="19" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B227" s="20"/>
       <c r="C227" s="20" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D227" s="21" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E227" s="20"/>
       <c r="F227" s="20"/>
@@ -15405,14 +15405,14 @@
     </row>
     <row r="228" spans="1:9" ht="19" customHeight="1">
       <c r="A228" s="19" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B228" s="20"/>
       <c r="C228" s="20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D228" s="21" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="E228" s="20"/>
       <c r="F228" s="20"/>
@@ -15422,14 +15422,14 @@
     </row>
     <row r="229" spans="1:9" ht="19" customHeight="1">
       <c r="A229" s="19" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B229" s="20"/>
       <c r="C229" s="20" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D229" s="21" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="E229" s="20"/>
       <c r="F229" s="20"/>
@@ -15439,14 +15439,14 @@
     </row>
     <row r="230" spans="1:9" ht="19" customHeight="1">
       <c r="A230" s="19" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B230" s="20"/>
       <c r="C230" s="20" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D230" s="21" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="E230" s="20"/>
       <c r="F230" s="20"/>
@@ -15456,14 +15456,14 @@
     </row>
     <row r="231" spans="1:9" ht="19" customHeight="1">
       <c r="A231" s="19" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B231" s="20"/>
       <c r="C231" s="20" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D231" s="21" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="E231" s="20"/>
       <c r="F231" s="20"/>
@@ -15473,14 +15473,14 @@
     </row>
     <row r="232" spans="1:9" ht="19" customHeight="1">
       <c r="A232" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B232" s="20"/>
       <c r="C232" s="20" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D232" s="21" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="E232" s="20"/>
       <c r="F232" s="20"/>
@@ -15490,14 +15490,14 @@
     </row>
     <row r="233" spans="1:9" ht="19" customHeight="1">
       <c r="A233" s="19" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B233" s="20"/>
       <c r="C233" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D233" s="21" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="E233" s="20"/>
       <c r="F233" s="20"/>
@@ -15507,14 +15507,14 @@
     </row>
     <row r="234" spans="1:9" ht="19" customHeight="1">
       <c r="A234" s="19" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B234" s="20"/>
       <c r="C234" s="20" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D234" s="20" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="E234" s="20"/>
       <c r="F234" s="20"/>
@@ -15524,14 +15524,14 @@
     </row>
     <row r="235" spans="1:9" ht="19" customHeight="1">
       <c r="A235" s="19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B235" s="20"/>
       <c r="C235" s="20" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D235" s="22" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="E235" s="20"/>
       <c r="F235" s="20"/>
@@ -15541,14 +15541,14 @@
     </row>
     <row r="236" spans="1:9" ht="19" customHeight="1">
       <c r="A236" s="19" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B236" s="20"/>
       <c r="C236" s="20" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D236" s="21" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="E236" s="20"/>
       <c r="F236" s="20"/>
@@ -15558,14 +15558,14 @@
     </row>
     <row r="237" spans="1:9" ht="19" customHeight="1">
       <c r="A237" s="19" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B237" s="20"/>
       <c r="C237" s="20" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D237" s="20" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E237" s="20"/>
       <c r="F237" s="20"/>
@@ -15575,14 +15575,14 @@
     </row>
     <row r="238" spans="1:9" ht="19" customHeight="1">
       <c r="A238" s="19" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B238" s="20"/>
       <c r="C238" s="20" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D238" s="20" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="E238" s="20"/>
       <c r="F238" s="20"/>
@@ -15592,14 +15592,14 @@
     </row>
     <row r="239" spans="1:9" ht="19" customHeight="1">
       <c r="A239" s="19" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B239" s="20"/>
       <c r="C239" s="20" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D239" s="20" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="E239" s="20"/>
       <c r="F239" s="20"/>
@@ -15609,14 +15609,14 @@
     </row>
     <row r="240" spans="1:9" ht="19" customHeight="1">
       <c r="A240" s="19" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B240" s="20"/>
       <c r="C240" s="20" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D240" s="20" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="E240" s="20"/>
       <c r="F240" s="20"/>
@@ -15626,14 +15626,14 @@
     </row>
     <row r="241" spans="1:9" ht="19" customHeight="1">
       <c r="A241" s="19" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B241" s="20"/>
       <c r="C241" s="20" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D241" s="20" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="E241" s="20"/>
       <c r="F241" s="20"/>
@@ -15643,14 +15643,14 @@
     </row>
     <row r="242" spans="1:9" ht="19" customHeight="1">
       <c r="A242" s="19" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B242" s="20"/>
       <c r="C242" s="20" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D242" s="20" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="E242" s="20"/>
       <c r="F242" s="20"/>
@@ -15660,14 +15660,14 @@
     </row>
     <row r="243" spans="1:9" ht="19" customHeight="1">
       <c r="A243" s="19" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B243" s="20"/>
       <c r="C243" s="20" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D243" s="20" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="E243" s="20"/>
       <c r="F243" s="20"/>
@@ -15677,14 +15677,14 @@
     </row>
     <row r="244" spans="1:9" ht="19" customHeight="1">
       <c r="A244" s="19" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B244" s="20"/>
       <c r="C244" s="20" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D244" s="21" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="E244" s="20"/>
       <c r="F244" s="20"/>
@@ -15694,14 +15694,14 @@
     </row>
     <row r="245" spans="1:9" ht="19" customHeight="1">
       <c r="A245" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B245" s="20"/>
       <c r="C245" s="20" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D245" s="20" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E245" s="20"/>
       <c r="F245" s="20"/>
@@ -15711,14 +15711,14 @@
     </row>
     <row r="246" spans="1:9" ht="19" customHeight="1">
       <c r="A246" s="19" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="B246" s="20"/>
       <c r="C246" s="20" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D246" s="20" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="E246" s="20"/>
       <c r="F246" s="20"/>
@@ -15728,14 +15728,14 @@
     </row>
     <row r="247" spans="1:9" ht="19" customHeight="1">
       <c r="A247" s="19" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="B247" s="20"/>
       <c r="C247" s="20" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D247" s="21" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="E247" s="20"/>
       <c r="F247" s="20"/>
@@ -15745,14 +15745,14 @@
     </row>
     <row r="248" spans="1:9" ht="19" customHeight="1">
       <c r="A248" s="19" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="B248" s="20"/>
       <c r="C248" s="20" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="D248" s="21" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="E248" s="20"/>
       <c r="F248" s="20"/>
@@ -15762,14 +15762,14 @@
     </row>
     <row r="249" spans="1:9" ht="19" customHeight="1">
       <c r="A249" s="19" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B249" s="20"/>
       <c r="C249" s="20" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D249" s="20" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="E249" s="20"/>
       <c r="F249" s="20"/>
@@ -15779,14 +15779,14 @@
     </row>
     <row r="250" spans="1:9" ht="19" customHeight="1">
       <c r="A250" s="19" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B250" s="20"/>
       <c r="C250" s="20" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D250" s="20" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="E250" s="20"/>
       <c r="F250" s="20"/>
@@ -15796,14 +15796,14 @@
     </row>
     <row r="251" spans="1:9" ht="19" customHeight="1">
       <c r="A251" s="19" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B251" s="20"/>
       <c r="C251" s="20" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D251" s="21" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="E251" s="20"/>
       <c r="F251" s="20"/>
@@ -15813,14 +15813,14 @@
     </row>
     <row r="252" spans="1:9" ht="19" customHeight="1">
       <c r="A252" s="19" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B252" s="20"/>
       <c r="C252" s="20" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D252" s="20" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="E252" s="20"/>
       <c r="F252" s="20"/>
@@ -15830,14 +15830,14 @@
     </row>
     <row r="253" spans="1:9" ht="19" customHeight="1">
       <c r="A253" s="19" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B253" s="20"/>
       <c r="C253" s="20" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D253" s="20" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="E253" s="20"/>
       <c r="F253" s="20"/>
@@ -15847,14 +15847,14 @@
     </row>
     <row r="254" spans="1:9" ht="19" customHeight="1">
       <c r="A254" s="19" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B254" s="20"/>
       <c r="C254" s="20" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D254" s="20" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="E254" s="20"/>
       <c r="F254" s="20"/>
@@ -15864,14 +15864,14 @@
     </row>
     <row r="255" spans="1:9" ht="19" customHeight="1">
       <c r="A255" s="19" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B255" s="20"/>
       <c r="C255" s="20" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D255" s="20" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="E255" s="20"/>
       <c r="F255" s="20"/>
@@ -15881,14 +15881,14 @@
     </row>
     <row r="256" spans="1:9" ht="19" customHeight="1">
       <c r="A256" s="19" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B256" s="20"/>
       <c r="C256" s="20" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D256" s="21" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="E256" s="20"/>
       <c r="F256" s="20"/>
@@ -15898,14 +15898,14 @@
     </row>
     <row r="257" spans="1:9" ht="19" customHeight="1">
       <c r="A257" s="19" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B257" s="20"/>
       <c r="C257" s="20" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D257" s="21" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="E257" s="20"/>
       <c r="F257" s="20"/>
@@ -15915,14 +15915,14 @@
     </row>
     <row r="258" spans="1:9" ht="19" customHeight="1">
       <c r="A258" s="19" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B258" s="20"/>
       <c r="C258" s="20" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D258" s="20" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="E258" s="20"/>
       <c r="F258" s="20"/>
@@ -15932,14 +15932,14 @@
     </row>
     <row r="259" spans="1:9" ht="19" customHeight="1">
       <c r="A259" s="19" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B259" s="20"/>
       <c r="C259" s="20" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D259" s="20" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="E259" s="20"/>
       <c r="F259" s="20"/>
@@ -15949,14 +15949,14 @@
     </row>
     <row r="260" spans="1:9" ht="19" customHeight="1">
       <c r="A260" s="19" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B260" s="20"/>
       <c r="C260" s="20" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D260" s="20" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="E260" s="20"/>
       <c r="F260" s="20"/>
@@ -15966,14 +15966,14 @@
     </row>
     <row r="261" spans="1:9" ht="19" customHeight="1">
       <c r="A261" s="19" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="B261" s="20"/>
       <c r="C261" s="20" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="D261" s="20" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="E261" s="20"/>
       <c r="F261" s="20"/>
@@ -15983,14 +15983,14 @@
     </row>
     <row r="262" spans="1:9" ht="19" customHeight="1">
       <c r="A262" s="19" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B262" s="20"/>
       <c r="C262" s="20" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D262" s="21" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="E262" s="20"/>
       <c r="F262" s="20"/>
@@ -16000,14 +16000,14 @@
     </row>
     <row r="263" spans="1:9" ht="19" customHeight="1">
       <c r="A263" s="19" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B263" s="20"/>
       <c r="C263" s="20" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D263" s="21" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="E263" s="20"/>
       <c r="F263" s="20"/>
@@ -16017,14 +16017,14 @@
     </row>
     <row r="264" spans="1:9" ht="19" customHeight="1">
       <c r="A264" s="19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B264" s="20"/>
       <c r="C264" s="20" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D264" s="20" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="E264" s="20"/>
       <c r="F264" s="20"/>
@@ -16034,14 +16034,14 @@
     </row>
     <row r="265" spans="1:9" ht="19" customHeight="1">
       <c r="A265" s="19" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B265" s="20"/>
       <c r="C265" s="20" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D265" s="20" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="E265" s="20"/>
       <c r="F265" s="20"/>
@@ -16051,14 +16051,14 @@
     </row>
     <row r="266" spans="1:9" ht="19" customHeight="1">
       <c r="A266" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B266" s="20"/>
       <c r="C266" s="20" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D266" s="20" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="E266" s="20"/>
       <c r="F266" s="20"/>
@@ -16068,14 +16068,14 @@
     </row>
     <row r="267" spans="1:9" ht="19" customHeight="1">
       <c r="A267" s="19" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="B267" s="20"/>
       <c r="C267" s="20" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="D267" s="20" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="E267" s="20"/>
       <c r="F267" s="20"/>
@@ -16085,14 +16085,14 @@
     </row>
     <row r="268" spans="1:9" ht="19" customHeight="1">
       <c r="A268" s="19" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B268" s="20"/>
       <c r="C268" s="20" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D268" s="20" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="E268" s="20"/>
       <c r="F268" s="20"/>
@@ -16102,14 +16102,14 @@
     </row>
     <row r="269" spans="1:9" ht="19" customHeight="1">
       <c r="A269" s="19" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B269" s="20"/>
       <c r="C269" s="20" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D269" s="20" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="E269" s="20"/>
       <c r="F269" s="20"/>
@@ -16119,14 +16119,14 @@
     </row>
     <row r="270" spans="1:9" ht="19" customHeight="1">
       <c r="A270" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B270" s="20"/>
       <c r="C270" s="20" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D270" s="21" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="E270" s="20"/>
       <c r="F270" s="20"/>
@@ -16136,14 +16136,14 @@
     </row>
     <row r="271" spans="1:9" ht="19" customHeight="1">
       <c r="A271" s="19" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B271" s="20"/>
       <c r="C271" s="20" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D271" s="21" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="E271" s="20"/>
       <c r="F271" s="20"/>
@@ -16153,14 +16153,14 @@
     </row>
     <row r="272" spans="1:9" ht="19" customHeight="1">
       <c r="A272" s="19" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B272" s="20"/>
       <c r="C272" s="20" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D272" s="20" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="E272" s="20"/>
       <c r="F272" s="20"/>
@@ -16170,14 +16170,14 @@
     </row>
     <row r="273" spans="1:9" ht="19" customHeight="1">
       <c r="A273" s="19" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B273" s="20"/>
       <c r="C273" s="20" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D273" s="21" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="E273" s="20"/>
       <c r="F273" s="20"/>
@@ -16187,14 +16187,14 @@
     </row>
     <row r="274" spans="1:9" ht="19" customHeight="1">
       <c r="A274" s="19" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B274" s="20"/>
       <c r="C274" s="20" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D274" s="21" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="E274" s="20"/>
       <c r="F274" s="20"/>
@@ -16204,14 +16204,14 @@
     </row>
     <row r="275" spans="1:9" ht="19" customHeight="1">
       <c r="A275" s="19" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B275" s="20"/>
       <c r="C275" s="20" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D275" s="21" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="E275" s="20"/>
       <c r="F275" s="20"/>
@@ -16221,14 +16221,14 @@
     </row>
     <row r="276" spans="1:9" ht="19" customHeight="1">
       <c r="A276" s="19" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B276" s="20"/>
       <c r="C276" s="20" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D276" s="21" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="E276" s="20"/>
       <c r="F276" s="20"/>
@@ -16238,14 +16238,14 @@
     </row>
     <row r="277" spans="1:9" ht="19" customHeight="1">
       <c r="A277" s="19" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B277" s="20"/>
       <c r="C277" s="20" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D277" s="21" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="E277" s="20"/>
       <c r="F277" s="20"/>
@@ -16255,14 +16255,14 @@
     </row>
     <row r="278" spans="1:9" ht="19" customHeight="1">
       <c r="A278" s="19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B278" s="20"/>
       <c r="C278" s="20" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D278" s="20" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="E278" s="20"/>
       <c r="F278" s="20"/>
@@ -16272,14 +16272,14 @@
     </row>
     <row r="279" spans="1:9" ht="19" customHeight="1">
       <c r="A279" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B279" s="20"/>
       <c r="C279" s="20" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D279" s="21" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="E279" s="20"/>
       <c r="F279" s="20"/>
@@ -16289,14 +16289,14 @@
     </row>
     <row r="280" spans="1:9" ht="19" customHeight="1">
       <c r="A280" s="19" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="B280" s="20"/>
       <c r="C280" s="20" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="D280" s="20" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="E280" s="20"/>
       <c r="F280" s="20"/>
@@ -16306,14 +16306,14 @@
     </row>
     <row r="281" spans="1:9" ht="19" customHeight="1">
       <c r="A281" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B281" s="20"/>
       <c r="C281" s="20" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D281" s="21" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E281" s="20"/>
       <c r="F281" s="20"/>
@@ -16323,14 +16323,14 @@
     </row>
     <row r="282" spans="1:9" ht="19" customHeight="1">
       <c r="A282" s="19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B282" s="20"/>
       <c r="C282" s="20" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D282" s="21" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="E282" s="20"/>
       <c r="F282" s="20"/>
@@ -16340,14 +16340,14 @@
     </row>
     <row r="283" spans="1:9" ht="19" customHeight="1">
       <c r="A283" s="19" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="B283" s="20"/>
       <c r="C283" s="20" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="D283" s="20" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="E283" s="20"/>
       <c r="F283" s="20"/>
@@ -16357,14 +16357,14 @@
     </row>
     <row r="284" spans="1:9" ht="19" customHeight="1">
       <c r="A284" s="19" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B284" s="20"/>
       <c r="C284" s="20" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D284" s="21" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="E284" s="20"/>
       <c r="F284" s="20"/>
@@ -16374,14 +16374,14 @@
     </row>
     <row r="285" spans="1:9" ht="19" customHeight="1">
       <c r="A285" s="19" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B285" s="20"/>
       <c r="C285" s="20" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D285" s="21" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="E285" s="20"/>
       <c r="F285" s="20"/>
@@ -16391,14 +16391,14 @@
     </row>
     <row r="286" spans="1:9" ht="19" customHeight="1">
       <c r="A286" s="19" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B286" s="20"/>
       <c r="C286" s="20" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D286" s="20" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="E286" s="20"/>
       <c r="F286" s="20"/>
@@ -16408,14 +16408,14 @@
     </row>
     <row r="287" spans="1:9" ht="19" customHeight="1">
       <c r="A287" s="19" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B287" s="20"/>
       <c r="C287" s="20" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D287" s="20" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E287" s="20"/>
       <c r="F287" s="20"/>
@@ -16425,14 +16425,14 @@
     </row>
     <row r="288" spans="1:9" ht="19" customHeight="1">
       <c r="A288" s="19" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B288" s="20"/>
       <c r="C288" s="20" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D288" s="21" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E288" s="20"/>
       <c r="F288" s="20"/>
@@ -16442,14 +16442,14 @@
     </row>
     <row r="289" spans="1:9" ht="19" customHeight="1">
       <c r="A289" s="19" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="B289" s="20"/>
       <c r="C289" s="20" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="D289" s="21" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="E289" s="20"/>
       <c r="F289" s="20"/>
@@ -16459,14 +16459,14 @@
     </row>
     <row r="290" spans="1:9" ht="19" customHeight="1">
       <c r="A290" s="19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B290" s="20"/>
       <c r="C290" s="20" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D290" s="22" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="E290" s="20"/>
       <c r="F290" s="20"/>
@@ -16476,14 +16476,14 @@
     </row>
     <row r="291" spans="1:9" ht="19" customHeight="1">
       <c r="A291" s="19" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B291" s="20"/>
       <c r="C291" s="20" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D291" s="21" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="E291" s="20"/>
       <c r="F291" s="20"/>
@@ -16493,14 +16493,14 @@
     </row>
     <row r="292" spans="1:9" ht="19" customHeight="1">
       <c r="A292" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B292" s="20"/>
       <c r="C292" s="20" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D292" s="21" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E292" s="20"/>
       <c r="F292" s="20"/>
@@ -16510,14 +16510,14 @@
     </row>
     <row r="293" spans="1:9" ht="19" customHeight="1">
       <c r="A293" s="19" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B293" s="20"/>
       <c r="C293" s="20" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D293" s="20" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="E293" s="20"/>
       <c r="F293" s="20"/>
@@ -16527,14 +16527,14 @@
     </row>
     <row r="294" spans="1:9" ht="19" customHeight="1">
       <c r="A294" s="19" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="B294" s="20"/>
       <c r="C294" s="20" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="E294" s="20"/>
       <c r="F294" s="20"/>
@@ -16544,14 +16544,14 @@
     </row>
     <row r="295" spans="1:9" ht="19" customHeight="1">
       <c r="A295" s="19" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B295" s="20"/>
       <c r="C295" s="20" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D295" s="21" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E295" s="20"/>
       <c r="F295" s="20"/>
@@ -16561,14 +16561,14 @@
     </row>
     <row r="296" spans="1:9" ht="19" customHeight="1">
       <c r="A296" s="19" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B296" s="20"/>
       <c r="C296" s="20" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D296" s="21" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="E296" s="20"/>
       <c r="F296" s="20"/>
@@ -16578,14 +16578,14 @@
     </row>
     <row r="297" spans="1:9" ht="19" customHeight="1">
       <c r="A297" s="19" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B297" s="20"/>
       <c r="C297" s="20" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="D297" s="21" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="E297" s="20"/>
       <c r="F297" s="20"/>
@@ -16595,14 +16595,14 @@
     </row>
     <row r="298" spans="1:9" ht="19" customHeight="1">
       <c r="A298" s="19" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B298" s="20"/>
       <c r="C298" s="20" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D298" s="21" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="E298" s="20"/>
       <c r="F298" s="20"/>
@@ -16612,14 +16612,14 @@
     </row>
     <row r="299" spans="1:9" ht="19" customHeight="1">
       <c r="A299" s="19" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="B299" s="20"/>
       <c r="C299" s="20" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
       <c r="D299" s="20" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="E299" s="20"/>
       <c r="F299" s="20"/>
@@ -16629,14 +16629,14 @@
     </row>
     <row r="300" spans="1:9" ht="19" customHeight="1">
       <c r="A300" s="19" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B300" s="20"/>
       <c r="C300" s="20" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D300" s="21" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="E300" s="20"/>
       <c r="F300" s="20"/>
@@ -16646,14 +16646,14 @@
     </row>
     <row r="301" spans="1:9" ht="19" customHeight="1">
       <c r="A301" s="19" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B301" s="20"/>
       <c r="C301" s="20" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D301" s="21" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="E301" s="20"/>
       <c r="F301" s="20"/>
@@ -16663,14 +16663,14 @@
     </row>
     <row r="302" spans="1:9" ht="19" customHeight="1">
       <c r="A302" s="19" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B302" s="20"/>
       <c r="C302" s="20" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D302" s="20" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="E302" s="20"/>
       <c r="F302" s="20"/>
@@ -16680,14 +16680,14 @@
     </row>
     <row r="303" spans="1:9" ht="19" customHeight="1">
       <c r="A303" s="19" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B303" s="20"/>
       <c r="C303" s="20" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D303" s="21" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="E303" s="20"/>
       <c r="F303" s="20"/>
@@ -16697,14 +16697,14 @@
     </row>
     <row r="304" spans="1:9" ht="19" customHeight="1">
       <c r="A304" s="19" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B304" s="20"/>
       <c r="C304" s="20" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D304" s="21" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="E304" s="20"/>
       <c r="F304" s="20"/>
@@ -16714,14 +16714,14 @@
     </row>
     <row r="305" spans="1:9" ht="19" customHeight="1">
       <c r="A305" s="19" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B305" s="20"/>
       <c r="C305" s="20" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D305" s="21" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="E305" s="20"/>
       <c r="F305" s="20"/>
@@ -16731,14 +16731,14 @@
     </row>
     <row r="306" spans="1:9" ht="19" customHeight="1">
       <c r="A306" s="19" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B306" s="20"/>
       <c r="C306" s="20" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D306" s="22" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="E306" s="20"/>
       <c r="F306" s="20"/>
@@ -16748,14 +16748,14 @@
     </row>
     <row r="307" spans="1:9" ht="19" customHeight="1">
       <c r="A307" s="19" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B307" s="20"/>
       <c r="C307" s="20" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D307" s="21" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="E307" s="20"/>
       <c r="F307" s="20"/>
@@ -16765,14 +16765,14 @@
     </row>
     <row r="308" spans="1:9" ht="19" customHeight="1">
       <c r="A308" s="19" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B308" s="20"/>
       <c r="C308" s="20" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D308" s="21" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="E308" s="20"/>
       <c r="F308" s="20"/>
@@ -16782,14 +16782,14 @@
     </row>
     <row r="309" spans="1:9" ht="19" customHeight="1">
       <c r="A309" s="19" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B309" s="20"/>
       <c r="C309" s="20" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D309" s="21" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="E309" s="20"/>
       <c r="F309" s="20"/>
@@ -16799,14 +16799,14 @@
     </row>
     <row r="310" spans="1:9" ht="19" customHeight="1">
       <c r="A310" s="19" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B310" s="20"/>
       <c r="C310" s="20" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D310" s="21" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="E310" s="20"/>
       <c r="F310" s="20"/>
@@ -16816,14 +16816,14 @@
     </row>
     <row r="311" spans="1:9" ht="19" customHeight="1">
       <c r="A311" s="19" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B311" s="20"/>
       <c r="C311" s="20" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D311" s="21" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E311" s="20"/>
       <c r="F311" s="20"/>
@@ -16833,14 +16833,14 @@
     </row>
     <row r="312" spans="1:9" ht="19" customHeight="1">
       <c r="A312" s="19" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B312" s="20"/>
       <c r="C312" s="20" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D312" s="20" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="E312" s="20"/>
       <c r="F312" s="20"/>
@@ -16850,14 +16850,14 @@
     </row>
     <row r="313" spans="1:9" ht="19" customHeight="1">
       <c r="A313" s="19" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B313" s="20"/>
       <c r="C313" s="27" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D313" s="27" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="E313" s="20"/>
       <c r="F313" s="20"/>
@@ -16867,14 +16867,14 @@
     </row>
     <row r="314" spans="1:9" ht="19" customHeight="1">
       <c r="A314" s="19" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B314" s="20"/>
       <c r="C314" s="20" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="E314" s="20"/>
       <c r="F314" s="20"/>
@@ -16884,14 +16884,14 @@
     </row>
     <row r="315" spans="1:9" ht="19" customHeight="1">
       <c r="A315" s="19" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B315" s="20"/>
       <c r="C315" s="20" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D315" s="21" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="E315" s="20"/>
       <c r="F315" s="20"/>
@@ -16901,14 +16901,14 @@
     </row>
     <row r="316" spans="1:9" ht="19" customHeight="1">
       <c r="A316" s="19" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B316" s="20"/>
       <c r="C316" s="20" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D316" s="21" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="E316" s="20"/>
       <c r="F316" s="20"/>
@@ -16918,14 +16918,14 @@
     </row>
     <row r="317" spans="1:9" ht="19" customHeight="1">
       <c r="A317" s="19" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B317" s="20"/>
       <c r="C317" s="20" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D317" s="21" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="E317" s="20"/>
       <c r="F317" s="20"/>
@@ -16935,14 +16935,14 @@
     </row>
     <row r="318" spans="1:9" ht="19" customHeight="1">
       <c r="A318" s="19" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B318" s="20"/>
       <c r="C318" s="20" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D318" s="20" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="E318" s="20"/>
       <c r="F318" s="20"/>
@@ -16952,14 +16952,14 @@
     </row>
     <row r="319" spans="1:9" ht="19" customHeight="1">
       <c r="A319" s="19" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B319" s="20"/>
       <c r="C319" s="20" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D319" s="22" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="E319" s="20"/>
       <c r="F319" s="20"/>
@@ -16969,14 +16969,14 @@
     </row>
     <row r="320" spans="1:9" ht="19" customHeight="1">
       <c r="A320" s="19" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B320" s="20"/>
       <c r="C320" s="20" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D320" s="20" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="E320" s="20"/>
       <c r="F320" s="20"/>
@@ -16986,14 +16986,14 @@
     </row>
     <row r="321" spans="1:9" ht="19" customHeight="1">
       <c r="A321" s="19" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B321" s="20"/>
       <c r="C321" s="20" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D321" s="20" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="E321" s="20"/>
       <c r="F321" s="20"/>
@@ -17003,14 +17003,14 @@
     </row>
     <row r="322" spans="1:9" ht="19" customHeight="1">
       <c r="A322" s="19" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="B322" s="20"/>
       <c r="C322" s="20" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="D322" s="20" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="E322" s="20"/>
       <c r="F322" s="20"/>
@@ -17020,14 +17020,14 @@
     </row>
     <row r="323" spans="1:9" ht="19" customHeight="1">
       <c r="A323" s="19" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="B323" s="20"/>
       <c r="C323" s="20" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="D323" s="20" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="E323" s="20"/>
       <c r="F323" s="20"/>
@@ -17731,12 +17731,12 @@
   </sheetData>
   <autoFilter ref="A4:J209" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A234:E235 E221:G221 A221:C233 A257:E258 A284:E285 A259:C283 E259:E283 A307:E308 E286:E306 A324:G386 A322:E323 A309:C321 E309:E321 E222:E233 B65:G65 D115:D133 A215:G220 I8:I28 A8:G28 A286:C306 A66:G114 A236:C256 E236:E256 G222:G323 I215:I386 F222:F271 A115:C141 E115:G141 D138:D141 A142:G213 I30:I213 A30:G64">
+  <conditionalFormatting sqref="A234:E235 E221:G221 A221:C233 A257:E258 A284:E285 A259:C283 E259:E283 A307:E308 E286:E306 A324:G386 A322:E323 A309:C321 E309:E321 E222:E233 B65:G65 D115:D133 I8:I28 A8:G28 A286:C306 A66:G114 A236:C256 E236:E256 G222:G323 F222:F271 A115:C141 E115:G141 D138:D141 A30:G64 A217:G220 I217:I386 A142:G215 I30:I215">
     <cfRule type="expression" dxfId="130" priority="260">
       <formula>$G8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H215:H386 H30:H85 H115:H213">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H217:H386 H115:H215">
     <cfRule type="cellIs" dxfId="129" priority="215" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
@@ -17750,7 +17750,7 @@
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H215:H386 H30:H85 H115:H213">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H217:H386 H115:H215">
     <cfRule type="cellIs" dxfId="125" priority="216" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -17767,7 +17767,7 @@
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H215:H386 H30:H85 H115:H213">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H217:H386 H115:H215">
     <cfRule type="cellIs" dxfId="120" priority="218" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
@@ -17828,26 +17828,26 @@
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C214:G214 I214 A214">
+  <conditionalFormatting sqref="C216:G216 I216 A216">
     <cfRule type="expression" dxfId="105" priority="120">
-      <formula>$G214&lt;&gt;""</formula>
+      <formula>$G216&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H214">
+  <conditionalFormatting sqref="H216">
     <cfRule type="cellIs" dxfId="104" priority="110" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="103" priority="117" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ERROR",H216)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="102" priority="118" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SKIP",H216)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="119" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H216)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H214">
+  <conditionalFormatting sqref="H216">
     <cfRule type="cellIs" dxfId="100" priority="111" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -17864,14 +17864,14 @@
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H214">
+  <conditionalFormatting sqref="H216">
     <cfRule type="cellIs" dxfId="95" priority="113" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B214">
+  <conditionalFormatting sqref="B216">
     <cfRule type="expression" dxfId="94" priority="109">
-      <formula>$G214&lt;&gt;""</formula>
+      <formula>$G216&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D295:D296 D300:D321 D221:D242 D245 D249:D258 D262:D264 D268:D277 D284:D286 D290:D291">

</xml_diff>

<commit_message>
Automatic emulator device detection.
Now you can specify AVD name as profileName, then platformVersion and udid are detected automatically.
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF4CA8F-C5FE-EF41-962F-A83B773FD213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45899F34-F1B3-A842-9766-D047B9982876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35860" yWindow="2320" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="1124">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -9604,6 +9604,52 @@
       </rPr>
       <t>をスキップする</t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>couldNotFindConnectedAndroidDeviceByUdid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Android</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>端末を検出できません。(udid=${subject})</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>couldNotFindConnectedAndroidDeviceByVersion</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not find a connected Android device. (platformVersion=${subject})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Android</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>端末を検出できません。(platformVersion=${subject})</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not find the connected Android device. (udid=${subject})</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -9948,7 +9994,7 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{C40AA10B-FA57-1748-8D8E-3E12991DC054}"/>
   </cellStyles>
-  <dxfs count="131">
+  <dxfs count="132">
     <dxf>
       <fill>
         <patternFill>
@@ -10156,6 +10202,13 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11182,7 +11235,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I386"/>
+  <dimension ref="A1:I388"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -15966,14 +16019,14 @@
     </row>
     <row r="261" spans="1:9" ht="19" customHeight="1">
       <c r="A261" s="19" t="s">
-        <v>919</v>
+        <v>1118</v>
       </c>
       <c r="B261" s="20"/>
       <c r="C261" s="20" t="s">
-        <v>921</v>
+        <v>1123</v>
       </c>
       <c r="D261" s="20" t="s">
-        <v>920</v>
+        <v>1119</v>
       </c>
       <c r="E261" s="20"/>
       <c r="F261" s="20"/>
@@ -15983,14 +16036,14 @@
     </row>
     <row r="262" spans="1:9" ht="19" customHeight="1">
       <c r="A262" s="19" t="s">
-        <v>569</v>
+        <v>1120</v>
       </c>
       <c r="B262" s="20"/>
       <c r="C262" s="20" t="s">
-        <v>570</v>
-      </c>
-      <c r="D262" s="21" t="s">
-        <v>718</v>
+        <v>1121</v>
+      </c>
+      <c r="D262" s="20" t="s">
+        <v>1122</v>
       </c>
       <c r="E262" s="20"/>
       <c r="F262" s="20"/>
@@ -16000,14 +16053,14 @@
     </row>
     <row r="263" spans="1:9" ht="19" customHeight="1">
       <c r="A263" s="19" t="s">
-        <v>571</v>
+        <v>919</v>
       </c>
       <c r="B263" s="20"/>
       <c r="C263" s="20" t="s">
-        <v>572</v>
-      </c>
-      <c r="D263" s="21" t="s">
-        <v>719</v>
+        <v>921</v>
+      </c>
+      <c r="D263" s="20" t="s">
+        <v>920</v>
       </c>
       <c r="E263" s="20"/>
       <c r="F263" s="20"/>
@@ -16017,14 +16070,14 @@
     </row>
     <row r="264" spans="1:9" ht="19" customHeight="1">
       <c r="A264" s="19" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B264" s="20"/>
       <c r="C264" s="20" t="s">
-        <v>574</v>
-      </c>
-      <c r="D264" s="20" t="s">
-        <v>720</v>
+        <v>570</v>
+      </c>
+      <c r="D264" s="21" t="s">
+        <v>718</v>
       </c>
       <c r="E264" s="20"/>
       <c r="F264" s="20"/>
@@ -16034,14 +16087,14 @@
     </row>
     <row r="265" spans="1:9" ht="19" customHeight="1">
       <c r="A265" s="19" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B265" s="20"/>
       <c r="C265" s="20" t="s">
-        <v>576</v>
-      </c>
-      <c r="D265" s="20" t="s">
-        <v>721</v>
+        <v>572</v>
+      </c>
+      <c r="D265" s="21" t="s">
+        <v>719</v>
       </c>
       <c r="E265" s="20"/>
       <c r="F265" s="20"/>
@@ -16051,14 +16104,14 @@
     </row>
     <row r="266" spans="1:9" ht="19" customHeight="1">
       <c r="A266" s="19" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B266" s="20"/>
       <c r="C266" s="20" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D266" s="20" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E266" s="20"/>
       <c r="F266" s="20"/>
@@ -16068,14 +16121,14 @@
     </row>
     <row r="267" spans="1:9" ht="19" customHeight="1">
       <c r="A267" s="19" t="s">
-        <v>1040</v>
+        <v>575</v>
       </c>
       <c r="B267" s="20"/>
       <c r="C267" s="20" t="s">
-        <v>1041</v>
+        <v>576</v>
       </c>
       <c r="D267" s="20" t="s">
-        <v>1042</v>
+        <v>721</v>
       </c>
       <c r="E267" s="20"/>
       <c r="F267" s="20"/>
@@ -16085,14 +16138,14 @@
     </row>
     <row r="268" spans="1:9" ht="19" customHeight="1">
       <c r="A268" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B268" s="20"/>
       <c r="C268" s="20" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D268" s="20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E268" s="20"/>
       <c r="F268" s="20"/>
@@ -16102,14 +16155,14 @@
     </row>
     <row r="269" spans="1:9" ht="19" customHeight="1">
       <c r="A269" s="19" t="s">
-        <v>581</v>
+        <v>1040</v>
       </c>
       <c r="B269" s="20"/>
       <c r="C269" s="20" t="s">
-        <v>582</v>
+        <v>1041</v>
       </c>
       <c r="D269" s="20" t="s">
-        <v>724</v>
+        <v>1042</v>
       </c>
       <c r="E269" s="20"/>
       <c r="F269" s="20"/>
@@ -16119,14 +16172,14 @@
     </row>
     <row r="270" spans="1:9" ht="19" customHeight="1">
       <c r="A270" s="19" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B270" s="20"/>
       <c r="C270" s="20" t="s">
-        <v>584</v>
-      </c>
-      <c r="D270" s="21" t="s">
-        <v>725</v>
+        <v>580</v>
+      </c>
+      <c r="D270" s="20" t="s">
+        <v>723</v>
       </c>
       <c r="E270" s="20"/>
       <c r="F270" s="20"/>
@@ -16136,14 +16189,14 @@
     </row>
     <row r="271" spans="1:9" ht="19" customHeight="1">
       <c r="A271" s="19" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B271" s="20"/>
       <c r="C271" s="20" t="s">
-        <v>586</v>
-      </c>
-      <c r="D271" s="21" t="s">
-        <v>726</v>
+        <v>582</v>
+      </c>
+      <c r="D271" s="20" t="s">
+        <v>724</v>
       </c>
       <c r="E271" s="20"/>
       <c r="F271" s="20"/>
@@ -16153,14 +16206,14 @@
     </row>
     <row r="272" spans="1:9" ht="19" customHeight="1">
       <c r="A272" s="19" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B272" s="20"/>
       <c r="C272" s="20" t="s">
-        <v>588</v>
-      </c>
-      <c r="D272" s="20" t="s">
-        <v>727</v>
+        <v>584</v>
+      </c>
+      <c r="D272" s="21" t="s">
+        <v>725</v>
       </c>
       <c r="E272" s="20"/>
       <c r="F272" s="20"/>
@@ -16170,14 +16223,14 @@
     </row>
     <row r="273" spans="1:9" ht="19" customHeight="1">
       <c r="A273" s="19" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B273" s="20"/>
       <c r="C273" s="20" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D273" s="21" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E273" s="20"/>
       <c r="F273" s="20"/>
@@ -16187,14 +16240,14 @@
     </row>
     <row r="274" spans="1:9" ht="19" customHeight="1">
       <c r="A274" s="19" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B274" s="20"/>
       <c r="C274" s="20" t="s">
-        <v>592</v>
-      </c>
-      <c r="D274" s="21" t="s">
-        <v>729</v>
+        <v>588</v>
+      </c>
+      <c r="D274" s="20" t="s">
+        <v>727</v>
       </c>
       <c r="E274" s="20"/>
       <c r="F274" s="20"/>
@@ -16204,14 +16257,14 @@
     </row>
     <row r="275" spans="1:9" ht="19" customHeight="1">
       <c r="A275" s="19" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B275" s="20"/>
       <c r="C275" s="20" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D275" s="21" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E275" s="20"/>
       <c r="F275" s="20"/>
@@ -16221,14 +16274,14 @@
     </row>
     <row r="276" spans="1:9" ht="19" customHeight="1">
       <c r="A276" s="19" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B276" s="20"/>
       <c r="C276" s="20" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D276" s="21" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E276" s="20"/>
       <c r="F276" s="20"/>
@@ -16238,14 +16291,14 @@
     </row>
     <row r="277" spans="1:9" ht="19" customHeight="1">
       <c r="A277" s="19" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B277" s="20"/>
       <c r="C277" s="20" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D277" s="21" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E277" s="20"/>
       <c r="F277" s="20"/>
@@ -16255,14 +16308,14 @@
     </row>
     <row r="278" spans="1:9" ht="19" customHeight="1">
       <c r="A278" s="19" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B278" s="20"/>
       <c r="C278" s="20" t="s">
-        <v>600</v>
-      </c>
-      <c r="D278" s="20" t="s">
-        <v>733</v>
+        <v>596</v>
+      </c>
+      <c r="D278" s="21" t="s">
+        <v>731</v>
       </c>
       <c r="E278" s="20"/>
       <c r="F278" s="20"/>
@@ -16272,14 +16325,14 @@
     </row>
     <row r="279" spans="1:9" ht="19" customHeight="1">
       <c r="A279" s="19" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B279" s="20"/>
       <c r="C279" s="20" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D279" s="21" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E279" s="20"/>
       <c r="F279" s="20"/>
@@ -16289,14 +16342,14 @@
     </row>
     <row r="280" spans="1:9" ht="19" customHeight="1">
       <c r="A280" s="19" t="s">
-        <v>960</v>
+        <v>599</v>
       </c>
       <c r="B280" s="20"/>
       <c r="C280" s="20" t="s">
-        <v>961</v>
+        <v>600</v>
       </c>
       <c r="D280" s="20" t="s">
-        <v>962</v>
+        <v>733</v>
       </c>
       <c r="E280" s="20"/>
       <c r="F280" s="20"/>
@@ -16306,14 +16359,14 @@
     </row>
     <row r="281" spans="1:9" ht="19" customHeight="1">
       <c r="A281" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B281" s="20"/>
       <c r="C281" s="20" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D281" s="21" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E281" s="20"/>
       <c r="F281" s="20"/>
@@ -16323,14 +16376,14 @@
     </row>
     <row r="282" spans="1:9" ht="19" customHeight="1">
       <c r="A282" s="19" t="s">
-        <v>605</v>
+        <v>960</v>
       </c>
       <c r="B282" s="20"/>
       <c r="C282" s="20" t="s">
-        <v>606</v>
-      </c>
-      <c r="D282" s="21" t="s">
-        <v>736</v>
+        <v>961</v>
+      </c>
+      <c r="D282" s="20" t="s">
+        <v>962</v>
       </c>
       <c r="E282" s="20"/>
       <c r="F282" s="20"/>
@@ -16340,14 +16393,14 @@
     </row>
     <row r="283" spans="1:9" ht="19" customHeight="1">
       <c r="A283" s="19" t="s">
-        <v>1032</v>
+        <v>603</v>
       </c>
       <c r="B283" s="20"/>
       <c r="C283" s="20" t="s">
-        <v>1033</v>
-      </c>
-      <c r="D283" s="20" t="s">
-        <v>1034</v>
+        <v>604</v>
+      </c>
+      <c r="D283" s="21" t="s">
+        <v>735</v>
       </c>
       <c r="E283" s="20"/>
       <c r="F283" s="20"/>
@@ -16357,14 +16410,14 @@
     </row>
     <row r="284" spans="1:9" ht="19" customHeight="1">
       <c r="A284" s="19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B284" s="20"/>
       <c r="C284" s="20" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D284" s="21" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E284" s="20"/>
       <c r="F284" s="20"/>
@@ -16374,14 +16427,14 @@
     </row>
     <row r="285" spans="1:9" ht="19" customHeight="1">
       <c r="A285" s="19" t="s">
-        <v>609</v>
+        <v>1032</v>
       </c>
       <c r="B285" s="20"/>
       <c r="C285" s="20" t="s">
-        <v>610</v>
-      </c>
-      <c r="D285" s="21" t="s">
-        <v>738</v>
+        <v>1033</v>
+      </c>
+      <c r="D285" s="20" t="s">
+        <v>1034</v>
       </c>
       <c r="E285" s="20"/>
       <c r="F285" s="20"/>
@@ -16391,14 +16444,14 @@
     </row>
     <row r="286" spans="1:9" ht="19" customHeight="1">
       <c r="A286" s="19" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B286" s="20"/>
       <c r="C286" s="20" t="s">
-        <v>612</v>
-      </c>
-      <c r="D286" s="20" t="s">
-        <v>739</v>
+        <v>608</v>
+      </c>
+      <c r="D286" s="21" t="s">
+        <v>737</v>
       </c>
       <c r="E286" s="20"/>
       <c r="F286" s="20"/>
@@ -16408,14 +16461,14 @@
     </row>
     <row r="287" spans="1:9" ht="19" customHeight="1">
       <c r="A287" s="19" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B287" s="20"/>
       <c r="C287" s="20" t="s">
-        <v>614</v>
-      </c>
-      <c r="D287" s="20" t="s">
-        <v>740</v>
+        <v>610</v>
+      </c>
+      <c r="D287" s="21" t="s">
+        <v>738</v>
       </c>
       <c r="E287" s="20"/>
       <c r="F287" s="20"/>
@@ -16425,14 +16478,14 @@
     </row>
     <row r="288" spans="1:9" ht="19" customHeight="1">
       <c r="A288" s="19" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B288" s="20"/>
       <c r="C288" s="20" t="s">
-        <v>616</v>
-      </c>
-      <c r="D288" s="21" t="s">
-        <v>741</v>
+        <v>612</v>
+      </c>
+      <c r="D288" s="20" t="s">
+        <v>739</v>
       </c>
       <c r="E288" s="20"/>
       <c r="F288" s="20"/>
@@ -16442,14 +16495,14 @@
     </row>
     <row r="289" spans="1:9" ht="19" customHeight="1">
       <c r="A289" s="19" t="s">
-        <v>1089</v>
+        <v>613</v>
       </c>
       <c r="B289" s="20"/>
       <c r="C289" s="20" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D289" s="21" t="s">
-        <v>1091</v>
+        <v>614</v>
+      </c>
+      <c r="D289" s="20" t="s">
+        <v>740</v>
       </c>
       <c r="E289" s="20"/>
       <c r="F289" s="20"/>
@@ -16459,14 +16512,14 @@
     </row>
     <row r="290" spans="1:9" ht="19" customHeight="1">
       <c r="A290" s="19" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B290" s="20"/>
       <c r="C290" s="20" t="s">
-        <v>618</v>
-      </c>
-      <c r="D290" s="22" t="s">
-        <v>742</v>
+        <v>616</v>
+      </c>
+      <c r="D290" s="21" t="s">
+        <v>741</v>
       </c>
       <c r="E290" s="20"/>
       <c r="F290" s="20"/>
@@ -16476,14 +16529,14 @@
     </row>
     <row r="291" spans="1:9" ht="19" customHeight="1">
       <c r="A291" s="19" t="s">
-        <v>619</v>
+        <v>1089</v>
       </c>
       <c r="B291" s="20"/>
       <c r="C291" s="20" t="s">
-        <v>620</v>
+        <v>1090</v>
       </c>
       <c r="D291" s="21" t="s">
-        <v>945</v>
+        <v>1091</v>
       </c>
       <c r="E291" s="20"/>
       <c r="F291" s="20"/>
@@ -16493,14 +16546,14 @@
     </row>
     <row r="292" spans="1:9" ht="19" customHeight="1">
       <c r="A292" s="19" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B292" s="20"/>
       <c r="C292" s="20" t="s">
-        <v>622</v>
-      </c>
-      <c r="D292" s="21" t="s">
-        <v>743</v>
+        <v>618</v>
+      </c>
+      <c r="D292" s="22" t="s">
+        <v>742</v>
       </c>
       <c r="E292" s="20"/>
       <c r="F292" s="20"/>
@@ -16510,14 +16563,14 @@
     </row>
     <row r="293" spans="1:9" ht="19" customHeight="1">
       <c r="A293" s="19" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B293" s="20"/>
       <c r="C293" s="20" t="s">
-        <v>624</v>
-      </c>
-      <c r="D293" s="20" t="s">
-        <v>744</v>
+        <v>620</v>
+      </c>
+      <c r="D293" s="21" t="s">
+        <v>945</v>
       </c>
       <c r="E293" s="20"/>
       <c r="F293" s="20"/>
@@ -16527,14 +16580,14 @@
     </row>
     <row r="294" spans="1:9" ht="19" customHeight="1">
       <c r="A294" s="19" t="s">
-        <v>957</v>
+        <v>621</v>
       </c>
       <c r="B294" s="20"/>
       <c r="C294" s="20" t="s">
-        <v>958</v>
-      </c>
-      <c r="D294" s="20" t="s">
-        <v>959</v>
+        <v>622</v>
+      </c>
+      <c r="D294" s="21" t="s">
+        <v>743</v>
       </c>
       <c r="E294" s="20"/>
       <c r="F294" s="20"/>
@@ -16544,14 +16597,14 @@
     </row>
     <row r="295" spans="1:9" ht="19" customHeight="1">
       <c r="A295" s="19" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B295" s="20"/>
       <c r="C295" s="20" t="s">
-        <v>626</v>
-      </c>
-      <c r="D295" s="21" t="s">
-        <v>745</v>
+        <v>624</v>
+      </c>
+      <c r="D295" s="20" t="s">
+        <v>744</v>
       </c>
       <c r="E295" s="20"/>
       <c r="F295" s="20"/>
@@ -16561,14 +16614,14 @@
     </row>
     <row r="296" spans="1:9" ht="19" customHeight="1">
       <c r="A296" s="19" t="s">
-        <v>627</v>
+        <v>957</v>
       </c>
       <c r="B296" s="20"/>
       <c r="C296" s="20" t="s">
-        <v>628</v>
-      </c>
-      <c r="D296" s="21" t="s">
-        <v>746</v>
+        <v>958</v>
+      </c>
+      <c r="D296" s="20" t="s">
+        <v>959</v>
       </c>
       <c r="E296" s="20"/>
       <c r="F296" s="20"/>
@@ -16578,14 +16631,14 @@
     </row>
     <row r="297" spans="1:9" ht="19" customHeight="1">
       <c r="A297" s="19" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B297" s="20"/>
       <c r="C297" s="20" t="s">
-        <v>963</v>
+        <v>626</v>
       </c>
       <c r="D297" s="21" t="s">
-        <v>964</v>
+        <v>745</v>
       </c>
       <c r="E297" s="20"/>
       <c r="F297" s="20"/>
@@ -16595,14 +16648,14 @@
     </row>
     <row r="298" spans="1:9" ht="19" customHeight="1">
       <c r="A298" s="19" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B298" s="20"/>
       <c r="C298" s="20" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D298" s="21" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E298" s="20"/>
       <c r="F298" s="20"/>
@@ -16612,14 +16665,14 @@
     </row>
     <row r="299" spans="1:9" ht="19" customHeight="1">
       <c r="A299" s="19" t="s">
-        <v>965</v>
+        <v>629</v>
       </c>
       <c r="B299" s="20"/>
       <c r="C299" s="20" t="s">
-        <v>966</v>
-      </c>
-      <c r="D299" s="20" t="s">
-        <v>967</v>
+        <v>963</v>
+      </c>
+      <c r="D299" s="21" t="s">
+        <v>964</v>
       </c>
       <c r="E299" s="20"/>
       <c r="F299" s="20"/>
@@ -16629,14 +16682,14 @@
     </row>
     <row r="300" spans="1:9" ht="19" customHeight="1">
       <c r="A300" s="19" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B300" s="20"/>
       <c r="C300" s="20" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D300" s="21" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E300" s="20"/>
       <c r="F300" s="20"/>
@@ -16646,14 +16699,14 @@
     </row>
     <row r="301" spans="1:9" ht="19" customHeight="1">
       <c r="A301" s="19" t="s">
-        <v>634</v>
+        <v>965</v>
       </c>
       <c r="B301" s="20"/>
       <c r="C301" s="20" t="s">
-        <v>635</v>
-      </c>
-      <c r="D301" s="21" t="s">
-        <v>749</v>
+        <v>966</v>
+      </c>
+      <c r="D301" s="20" t="s">
+        <v>967</v>
       </c>
       <c r="E301" s="20"/>
       <c r="F301" s="20"/>
@@ -16663,14 +16716,14 @@
     </row>
     <row r="302" spans="1:9" ht="19" customHeight="1">
       <c r="A302" s="19" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B302" s="20"/>
       <c r="C302" s="20" t="s">
-        <v>637</v>
-      </c>
-      <c r="D302" s="20" t="s">
-        <v>750</v>
+        <v>633</v>
+      </c>
+      <c r="D302" s="21" t="s">
+        <v>748</v>
       </c>
       <c r="E302" s="20"/>
       <c r="F302" s="20"/>
@@ -16680,14 +16733,14 @@
     </row>
     <row r="303" spans="1:9" ht="19" customHeight="1">
       <c r="A303" s="19" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B303" s="20"/>
       <c r="C303" s="20" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D303" s="21" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E303" s="20"/>
       <c r="F303" s="20"/>
@@ -16697,14 +16750,14 @@
     </row>
     <row r="304" spans="1:9" ht="19" customHeight="1">
       <c r="A304" s="19" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B304" s="20"/>
       <c r="C304" s="20" t="s">
-        <v>641</v>
-      </c>
-      <c r="D304" s="21" t="s">
-        <v>752</v>
+        <v>637</v>
+      </c>
+      <c r="D304" s="20" t="s">
+        <v>750</v>
       </c>
       <c r="E304" s="20"/>
       <c r="F304" s="20"/>
@@ -16714,14 +16767,14 @@
     </row>
     <row r="305" spans="1:9" ht="19" customHeight="1">
       <c r="A305" s="19" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B305" s="20"/>
       <c r="C305" s="20" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D305" s="21" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E305" s="20"/>
       <c r="F305" s="20"/>
@@ -16731,14 +16784,14 @@
     </row>
     <row r="306" spans="1:9" ht="19" customHeight="1">
       <c r="A306" s="19" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B306" s="20"/>
       <c r="C306" s="20" t="s">
-        <v>645</v>
-      </c>
-      <c r="D306" s="22" t="s">
-        <v>754</v>
+        <v>641</v>
+      </c>
+      <c r="D306" s="21" t="s">
+        <v>752</v>
       </c>
       <c r="E306" s="20"/>
       <c r="F306" s="20"/>
@@ -16748,14 +16801,14 @@
     </row>
     <row r="307" spans="1:9" ht="19" customHeight="1">
       <c r="A307" s="19" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B307" s="20"/>
       <c r="C307" s="20" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D307" s="21" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E307" s="20"/>
       <c r="F307" s="20"/>
@@ -16765,14 +16818,14 @@
     </row>
     <row r="308" spans="1:9" ht="19" customHeight="1">
       <c r="A308" s="19" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="B308" s="20"/>
       <c r="C308" s="20" t="s">
-        <v>648</v>
-      </c>
-      <c r="D308" s="21" t="s">
-        <v>756</v>
+        <v>645</v>
+      </c>
+      <c r="D308" s="22" t="s">
+        <v>754</v>
       </c>
       <c r="E308" s="20"/>
       <c r="F308" s="20"/>
@@ -16782,14 +16835,14 @@
     </row>
     <row r="309" spans="1:9" ht="19" customHeight="1">
       <c r="A309" s="19" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B309" s="20"/>
       <c r="C309" s="20" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D309" s="21" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E309" s="20"/>
       <c r="F309" s="20"/>
@@ -16799,14 +16852,14 @@
     </row>
     <row r="310" spans="1:9" ht="19" customHeight="1">
       <c r="A310" s="19" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B310" s="20"/>
       <c r="C310" s="20" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="D310" s="21" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E310" s="20"/>
       <c r="F310" s="20"/>
@@ -16816,14 +16869,14 @@
     </row>
     <row r="311" spans="1:9" ht="19" customHeight="1">
       <c r="A311" s="19" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B311" s="20"/>
       <c r="C311" s="20" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D311" s="21" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E311" s="20"/>
       <c r="F311" s="20"/>
@@ -16833,14 +16886,14 @@
     </row>
     <row r="312" spans="1:9" ht="19" customHeight="1">
       <c r="A312" s="19" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="B312" s="20"/>
       <c r="C312" s="20" t="s">
-        <v>657</v>
-      </c>
-      <c r="D312" s="20" t="s">
-        <v>760</v>
+        <v>653</v>
+      </c>
+      <c r="D312" s="21" t="s">
+        <v>758</v>
       </c>
       <c r="E312" s="20"/>
       <c r="F312" s="20"/>
@@ -16850,14 +16903,14 @@
     </row>
     <row r="313" spans="1:9" ht="19" customHeight="1">
       <c r="A313" s="19" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B313" s="20"/>
-      <c r="C313" s="27" t="s">
-        <v>659</v>
-      </c>
-      <c r="D313" s="27" t="s">
-        <v>761</v>
+      <c r="C313" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="D313" s="21" t="s">
+        <v>759</v>
       </c>
       <c r="E313" s="20"/>
       <c r="F313" s="20"/>
@@ -16867,14 +16920,14 @@
     </row>
     <row r="314" spans="1:9" ht="19" customHeight="1">
       <c r="A314" s="19" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="B314" s="20"/>
       <c r="C314" s="20" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E314" s="20"/>
       <c r="F314" s="20"/>
@@ -16884,14 +16937,14 @@
     </row>
     <row r="315" spans="1:9" ht="19" customHeight="1">
       <c r="A315" s="19" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B315" s="20"/>
-      <c r="C315" s="20" t="s">
-        <v>663</v>
-      </c>
-      <c r="D315" s="21" t="s">
-        <v>763</v>
+      <c r="C315" s="27" t="s">
+        <v>659</v>
+      </c>
+      <c r="D315" s="27" t="s">
+        <v>761</v>
       </c>
       <c r="E315" s="20"/>
       <c r="F315" s="20"/>
@@ -16901,14 +16954,14 @@
     </row>
     <row r="316" spans="1:9" ht="19" customHeight="1">
       <c r="A316" s="19" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B316" s="20"/>
       <c r="C316" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="D316" s="21" t="s">
-        <v>764</v>
+        <v>661</v>
+      </c>
+      <c r="D316" s="20" t="s">
+        <v>762</v>
       </c>
       <c r="E316" s="20"/>
       <c r="F316" s="20"/>
@@ -16918,14 +16971,14 @@
     </row>
     <row r="317" spans="1:9" ht="19" customHeight="1">
       <c r="A317" s="19" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B317" s="20"/>
       <c r="C317" s="20" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D317" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E317" s="20"/>
       <c r="F317" s="20"/>
@@ -16935,14 +16988,14 @@
     </row>
     <row r="318" spans="1:9" ht="19" customHeight="1">
       <c r="A318" s="19" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="B318" s="20"/>
       <c r="C318" s="20" t="s">
-        <v>669</v>
-      </c>
-      <c r="D318" s="20" t="s">
-        <v>766</v>
+        <v>665</v>
+      </c>
+      <c r="D318" s="21" t="s">
+        <v>764</v>
       </c>
       <c r="E318" s="20"/>
       <c r="F318" s="20"/>
@@ -16952,14 +17005,14 @@
     </row>
     <row r="319" spans="1:9" ht="19" customHeight="1">
       <c r="A319" s="19" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="B319" s="20"/>
       <c r="C319" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="D319" s="22" t="s">
-        <v>767</v>
+        <v>667</v>
+      </c>
+      <c r="D319" s="21" t="s">
+        <v>765</v>
       </c>
       <c r="E319" s="20"/>
       <c r="F319" s="20"/>
@@ -16969,14 +17022,14 @@
     </row>
     <row r="320" spans="1:9" ht="19" customHeight="1">
       <c r="A320" s="19" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="B320" s="20"/>
       <c r="C320" s="20" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D320" s="20" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E320" s="20"/>
       <c r="F320" s="20"/>
@@ -16986,14 +17039,14 @@
     </row>
     <row r="321" spans="1:9" ht="19" customHeight="1">
       <c r="A321" s="19" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="B321" s="20"/>
       <c r="C321" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="D321" s="20" t="s">
-        <v>769</v>
+        <v>671</v>
+      </c>
+      <c r="D321" s="22" t="s">
+        <v>767</v>
       </c>
       <c r="E321" s="20"/>
       <c r="F321" s="20"/>
@@ -17003,14 +17056,14 @@
     </row>
     <row r="322" spans="1:9" ht="19" customHeight="1">
       <c r="A322" s="19" t="s">
-        <v>954</v>
+        <v>672</v>
       </c>
       <c r="B322" s="20"/>
       <c r="C322" s="20" t="s">
-        <v>955</v>
+        <v>673</v>
       </c>
       <c r="D322" s="20" t="s">
-        <v>956</v>
+        <v>768</v>
       </c>
       <c r="E322" s="20"/>
       <c r="F322" s="20"/>
@@ -17020,14 +17073,14 @@
     </row>
     <row r="323" spans="1:9" ht="19" customHeight="1">
       <c r="A323" s="19" t="s">
-        <v>1081</v>
+        <v>674</v>
       </c>
       <c r="B323" s="20"/>
       <c r="C323" s="20" t="s">
-        <v>1082</v>
+        <v>675</v>
       </c>
       <c r="D323" s="20" t="s">
-        <v>1083</v>
+        <v>769</v>
       </c>
       <c r="E323" s="20"/>
       <c r="F323" s="20"/>
@@ -17036,10 +17089,16 @@
       <c r="I323" s="18"/>
     </row>
     <row r="324" spans="1:9" ht="19" customHeight="1">
-      <c r="A324" s="19"/>
+      <c r="A324" s="19" t="s">
+        <v>954</v>
+      </c>
       <c r="B324" s="20"/>
-      <c r="C324" s="20"/>
-      <c r="D324" s="20"/>
+      <c r="C324" s="20" t="s">
+        <v>955</v>
+      </c>
+      <c r="D324" s="20" t="s">
+        <v>956</v>
+      </c>
       <c r="E324" s="20"/>
       <c r="F324" s="20"/>
       <c r="G324" s="18"/>
@@ -17047,10 +17106,16 @@
       <c r="I324" s="18"/>
     </row>
     <row r="325" spans="1:9" ht="19" customHeight="1">
-      <c r="A325" s="19"/>
+      <c r="A325" s="19" t="s">
+        <v>1081</v>
+      </c>
       <c r="B325" s="20"/>
-      <c r="C325" s="20"/>
-      <c r="D325" s="20"/>
+      <c r="C325" s="20" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D325" s="20" t="s">
+        <v>1083</v>
+      </c>
       <c r="E325" s="20"/>
       <c r="F325" s="20"/>
       <c r="G325" s="18"/>
@@ -17728,400 +17793,427 @@
       <c r="H386" s="17"/>
       <c r="I386" s="18"/>
     </row>
+    <row r="387" spans="1:9" ht="19" customHeight="1">
+      <c r="A387" s="19"/>
+      <c r="B387" s="20"/>
+      <c r="C387" s="20"/>
+      <c r="D387" s="20"/>
+      <c r="E387" s="20"/>
+      <c r="F387" s="20"/>
+      <c r="G387" s="18"/>
+      <c r="H387" s="17"/>
+      <c r="I387" s="18"/>
+    </row>
+    <row r="388" spans="1:9" ht="19" customHeight="1">
+      <c r="A388" s="19"/>
+      <c r="B388" s="20"/>
+      <c r="C388" s="20"/>
+      <c r="D388" s="20"/>
+      <c r="E388" s="20"/>
+      <c r="F388" s="20"/>
+      <c r="G388" s="18"/>
+      <c r="H388" s="17"/>
+      <c r="I388" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J209" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A234:E235 E221:G221 A221:C233 A257:E258 A284:E285 A259:C283 E259:E283 A307:E308 E286:E306 A324:G386 A322:E323 A309:C321 E309:E321 E222:E233 B65:G65 D115:D133 I8:I28 A8:G28 A286:C306 A66:G114 A236:C256 E236:E256 G222:G323 F222:F271 A115:C141 E115:G141 D138:D141 A30:G64 A217:G220 I217:I386 A142:G215 I30:I215">
-    <cfRule type="expression" dxfId="130" priority="260">
+  <conditionalFormatting sqref="A234:E235 E221:G221 A221:C233 A257:E258 A286:E287 A309:E310 E288:E308 A326:G388 A324:E325 A311:C323 E311:E323 E222:E233 B65:G65 D115:D133 I8:I28 A8:G28 A288:C308 A66:G114 A236:C256 E236:E256 A115:C141 E115:G141 D138:D141 A30:G64 A217:G220 A142:G215 I30:I215 E259 F222:G259 F263:F273 G263:G325 E263:E285 E260:G262 A259:C285 I217:I388">
+    <cfRule type="expression" dxfId="131" priority="260">
       <formula>$G8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H217:H386 H115:H215">
-    <cfRule type="cellIs" dxfId="129" priority="215" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H388">
+    <cfRule type="cellIs" dxfId="130" priority="215" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="222" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="129" priority="222" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="223" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="128" priority="223" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="224" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="127" priority="224" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H217:H386 H115:H215">
-    <cfRule type="cellIs" dxfId="125" priority="216" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H388">
+    <cfRule type="cellIs" dxfId="126" priority="216" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="217" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="217" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="219" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="219" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="220" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="220" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="221" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="221" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H217:H386 H115:H215">
-    <cfRule type="cellIs" dxfId="120" priority="218" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H388">
+    <cfRule type="cellIs" dxfId="121" priority="218" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D134:D135">
-    <cfRule type="expression" dxfId="119" priority="139">
+    <cfRule type="expression" dxfId="120" priority="139">
       <formula>$G134&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136:D137">
-    <cfRule type="expression" dxfId="118" priority="138">
+    <cfRule type="expression" dxfId="119" priority="138">
       <formula>$G136&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:G5 I5 A5">
-    <cfRule type="expression" dxfId="117" priority="132">
+    <cfRule type="expression" dxfId="118" priority="132">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="116" priority="122" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="122" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="129" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="116" priority="129" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="130" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="115" priority="130" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="131" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="114" priority="131" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="112" priority="123" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="123" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="124" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="124" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="126" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="126" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="127" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="127" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="128" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="128" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="107" priority="125" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="125" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="106" priority="121">
+    <cfRule type="expression" dxfId="107" priority="121">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C216:G216 I216 A216">
-    <cfRule type="expression" dxfId="105" priority="120">
+    <cfRule type="expression" dxfId="106" priority="120">
       <formula>$G216&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H216">
-    <cfRule type="cellIs" dxfId="104" priority="110" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="110" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="117" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="104" priority="117" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="118" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="103" priority="118" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="119" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="102" priority="119" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H216">
-    <cfRule type="cellIs" dxfId="100" priority="111" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="111" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="112" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="112" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="114" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="114" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="115" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="115" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="116" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="116" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H216">
-    <cfRule type="cellIs" dxfId="95" priority="113" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="113" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B216">
-    <cfRule type="expression" dxfId="94" priority="109">
+    <cfRule type="expression" dxfId="95" priority="109">
       <formula>$G216&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D295:D296 D300:D321 D221:D242 D245 D249:D258 D262:D264 D268:D277 D284:D286 D290:D291">
-    <cfRule type="expression" dxfId="93" priority="262">
+  <conditionalFormatting sqref="D297:D298 D302:D323 D221:D242 D245 D264:D266 D270:D279 D286:D288 D292:D293 D249:D258">
+    <cfRule type="expression" dxfId="94" priority="262">
       <formula>$G223&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F272:F323">
-    <cfRule type="expression" dxfId="92" priority="108">
-      <formula>$G272&lt;&gt;""</formula>
+  <conditionalFormatting sqref="F274:F325">
+    <cfRule type="expression" dxfId="93" priority="108">
+      <formula>$G274&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6 I6 C6:G6">
-    <cfRule type="expression" dxfId="91" priority="93">
+    <cfRule type="expression" dxfId="92" priority="93">
       <formula>$G6&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="90" priority="83" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="83" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="90" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="90" priority="90" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="91" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="89" priority="91" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="92" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="88" priority="92" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="86" priority="84" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="84" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="85" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="85" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="87" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="87" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="88" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="88" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="89" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="89" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="81" priority="86" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="86" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B7 I7 E7:G7">
-    <cfRule type="expression" dxfId="80" priority="82">
+    <cfRule type="expression" dxfId="81" priority="82">
       <formula>$G7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="79" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="72" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="79" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="79" priority="79" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="80" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="78" priority="80" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="81" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="77" priority="81" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="75" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="73" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="74" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="74" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="76" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="77" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="78" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="70" priority="75" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="75" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="69" priority="71">
+    <cfRule type="expression" dxfId="70" priority="71">
       <formula>$G6&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="68" priority="70">
+    <cfRule type="expression" dxfId="69" priority="70">
       <formula>$G7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="67" priority="69">
+    <cfRule type="expression" dxfId="68" priority="69">
       <formula>$G7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="expression" dxfId="66" priority="57">
+    <cfRule type="expression" dxfId="67" priority="57">
       <formula>$G65&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113:H114">
-    <cfRule type="cellIs" dxfId="65" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="46" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="53" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="65" priority="53" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="54" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="64" priority="54" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="55" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="63" priority="55" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113:H114">
-    <cfRule type="cellIs" dxfId="61" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="47" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="48" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="50" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="51" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="52" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113:H114">
-    <cfRule type="cellIs" dxfId="56" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="49" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:G29 I29">
-    <cfRule type="expression" dxfId="55" priority="23">
+    <cfRule type="expression" dxfId="56" priority="23">
       <formula>$G29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="54" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="13" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="20" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="54" priority="20" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="21" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="53" priority="21" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="22" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="52" priority="22" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="50" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="14" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="15" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="17" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="18" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="19" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="45" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="16" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D259:D261 D292:D294 D297:D299 D281:D283 D278:D279 D246:D248 D265:D266 D287:D289">
-    <cfRule type="expression" dxfId="44" priority="265">
+  <conditionalFormatting sqref="D294:D296 D299:D301 D283:D285 D280:D281 D246:D248 D267:D268 D289:D291 D261:D263">
+    <cfRule type="expression" dxfId="45" priority="265">
       <formula>$G249&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="cellIs" dxfId="43" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="2" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="43" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="42" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="41" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="6" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="7" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="8" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="cellIs" dxfId="34" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D280">
-    <cfRule type="expression" dxfId="33" priority="269">
-      <formula>$G284&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D282">
+    <cfRule type="expression" dxfId="34" priority="269">
+      <formula>$G286&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D244">
-    <cfRule type="expression" dxfId="32" priority="300">
+    <cfRule type="expression" dxfId="33" priority="300">
       <formula>$G245&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D243">
-    <cfRule type="expression" dxfId="31" priority="301">
+    <cfRule type="expression" dxfId="32" priority="301">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D267">
-    <cfRule type="expression" dxfId="30" priority="1">
-      <formula>$G267&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D269">
+    <cfRule type="expression" dxfId="31" priority="1">
+      <formula>$G269&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D259:D260">
+    <cfRule type="expression" dxfId="30" priority="303">
+      <formula>$G264&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Automatic simulator device detection.
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45899F34-F1B3-A842-9766-D047B9982876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B794484-2A38-354C-A27E-2D0B77B2C0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35860" yWindow="2320" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">message!$A$4:$J$209</definedName>
     <definedName name="実施結果">List!$A$3:$A$12</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="1133">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -9650,6 +9650,65 @@
   </si>
   <si>
     <t>Could not find the connected Android device. (udid=${subject})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>couldNotFindIosDevice</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>searchingDeviceForProfile</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Searching device for (profileName=${subject})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>端末を検索しています。 (profileName=${subject})</t>
+    <rPh sb="0" eb="2">
+      <t>タンマテゥ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ケンサク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deviceFound</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Device found. (${subject})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>端末が見つかりました。(${subject})</t>
+    <rPh sb="0" eb="2">
+      <t>タンマテゥ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ミツカリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not find iOS device. (${subject})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>iOS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>端末を検出できません。(${subject})</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -9994,7 +10053,7 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{C40AA10B-FA57-1748-8D8E-3E12991DC054}"/>
   </cellStyles>
-  <dxfs count="132">
+  <dxfs count="135">
     <dxf>
       <fill>
         <patternFill>
@@ -10202,6 +10261,27 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11235,7 +11315,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I388"/>
+  <dimension ref="A1:I391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -16053,14 +16133,14 @@
     </row>
     <row r="263" spans="1:9" ht="19" customHeight="1">
       <c r="A263" s="19" t="s">
-        <v>919</v>
+        <v>1124</v>
       </c>
       <c r="B263" s="20"/>
       <c r="C263" s="20" t="s">
-        <v>921</v>
+        <v>1131</v>
       </c>
       <c r="D263" s="20" t="s">
-        <v>920</v>
+        <v>1132</v>
       </c>
       <c r="E263" s="20"/>
       <c r="F263" s="20"/>
@@ -16070,14 +16150,14 @@
     </row>
     <row r="264" spans="1:9" ht="19" customHeight="1">
       <c r="A264" s="19" t="s">
-        <v>569</v>
+        <v>919</v>
       </c>
       <c r="B264" s="20"/>
       <c r="C264" s="20" t="s">
-        <v>570</v>
-      </c>
-      <c r="D264" s="21" t="s">
-        <v>718</v>
+        <v>921</v>
+      </c>
+      <c r="D264" s="20" t="s">
+        <v>920</v>
       </c>
       <c r="E264" s="20"/>
       <c r="F264" s="20"/>
@@ -16087,14 +16167,14 @@
     </row>
     <row r="265" spans="1:9" ht="19" customHeight="1">
       <c r="A265" s="19" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B265" s="20"/>
       <c r="C265" s="20" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D265" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E265" s="20"/>
       <c r="F265" s="20"/>
@@ -16104,14 +16184,14 @@
     </row>
     <row r="266" spans="1:9" ht="19" customHeight="1">
       <c r="A266" s="19" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B266" s="20"/>
       <c r="C266" s="20" t="s">
-        <v>574</v>
-      </c>
-      <c r="D266" s="20" t="s">
-        <v>720</v>
+        <v>572</v>
+      </c>
+      <c r="D266" s="21" t="s">
+        <v>719</v>
       </c>
       <c r="E266" s="20"/>
       <c r="F266" s="20"/>
@@ -16121,14 +16201,14 @@
     </row>
     <row r="267" spans="1:9" ht="19" customHeight="1">
       <c r="A267" s="19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B267" s="20"/>
       <c r="C267" s="20" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D267" s="20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E267" s="20"/>
       <c r="F267" s="20"/>
@@ -16138,14 +16218,14 @@
     </row>
     <row r="268" spans="1:9" ht="19" customHeight="1">
       <c r="A268" s="19" t="s">
-        <v>577</v>
+        <v>1125</v>
       </c>
       <c r="B268" s="20"/>
       <c r="C268" s="20" t="s">
-        <v>578</v>
+        <v>1126</v>
       </c>
       <c r="D268" s="20" t="s">
-        <v>722</v>
+        <v>1127</v>
       </c>
       <c r="E268" s="20"/>
       <c r="F268" s="20"/>
@@ -16155,14 +16235,14 @@
     </row>
     <row r="269" spans="1:9" ht="19" customHeight="1">
       <c r="A269" s="19" t="s">
-        <v>1040</v>
+        <v>1128</v>
       </c>
       <c r="B269" s="20"/>
       <c r="C269" s="20" t="s">
-        <v>1041</v>
+        <v>1129</v>
       </c>
       <c r="D269" s="20" t="s">
-        <v>1042</v>
+        <v>1130</v>
       </c>
       <c r="E269" s="20"/>
       <c r="F269" s="20"/>
@@ -16172,14 +16252,14 @@
     </row>
     <row r="270" spans="1:9" ht="19" customHeight="1">
       <c r="A270" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B270" s="20"/>
       <c r="C270" s="20" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D270" s="20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E270" s="20"/>
       <c r="F270" s="20"/>
@@ -16189,14 +16269,14 @@
     </row>
     <row r="271" spans="1:9" ht="19" customHeight="1">
       <c r="A271" s="19" t="s">
-        <v>581</v>
+        <v>1040</v>
       </c>
       <c r="B271" s="20"/>
       <c r="C271" s="20" t="s">
-        <v>582</v>
+        <v>1041</v>
       </c>
       <c r="D271" s="20" t="s">
-        <v>724</v>
+        <v>1042</v>
       </c>
       <c r="E271" s="20"/>
       <c r="F271" s="20"/>
@@ -16206,14 +16286,14 @@
     </row>
     <row r="272" spans="1:9" ht="19" customHeight="1">
       <c r="A272" s="19" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="B272" s="20"/>
       <c r="C272" s="20" t="s">
-        <v>584</v>
-      </c>
-      <c r="D272" s="21" t="s">
-        <v>725</v>
+        <v>576</v>
+      </c>
+      <c r="D272" s="20" t="s">
+        <v>721</v>
       </c>
       <c r="E272" s="20"/>
       <c r="F272" s="20"/>
@@ -16223,14 +16303,14 @@
     </row>
     <row r="273" spans="1:9" ht="19" customHeight="1">
       <c r="A273" s="19" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B273" s="20"/>
       <c r="C273" s="20" t="s">
-        <v>586</v>
-      </c>
-      <c r="D273" s="21" t="s">
-        <v>726</v>
+        <v>580</v>
+      </c>
+      <c r="D273" s="20" t="s">
+        <v>723</v>
       </c>
       <c r="E273" s="20"/>
       <c r="F273" s="20"/>
@@ -16240,14 +16320,14 @@
     </row>
     <row r="274" spans="1:9" ht="19" customHeight="1">
       <c r="A274" s="19" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="B274" s="20"/>
       <c r="C274" s="20" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="D274" s="20" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E274" s="20"/>
       <c r="F274" s="20"/>
@@ -16257,14 +16337,14 @@
     </row>
     <row r="275" spans="1:9" ht="19" customHeight="1">
       <c r="A275" s="19" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="B275" s="20"/>
       <c r="C275" s="20" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="D275" s="21" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="E275" s="20"/>
       <c r="F275" s="20"/>
@@ -16274,14 +16354,14 @@
     </row>
     <row r="276" spans="1:9" ht="19" customHeight="1">
       <c r="A276" s="19" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="B276" s="20"/>
       <c r="C276" s="20" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="D276" s="21" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="E276" s="20"/>
       <c r="F276" s="20"/>
@@ -16291,14 +16371,14 @@
     </row>
     <row r="277" spans="1:9" ht="19" customHeight="1">
       <c r="A277" s="19" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B277" s="20"/>
       <c r="C277" s="20" t="s">
-        <v>594</v>
-      </c>
-      <c r="D277" s="21" t="s">
-        <v>730</v>
+        <v>588</v>
+      </c>
+      <c r="D277" s="20" t="s">
+        <v>727</v>
       </c>
       <c r="E277" s="20"/>
       <c r="F277" s="20"/>
@@ -16308,14 +16388,14 @@
     </row>
     <row r="278" spans="1:9" ht="19" customHeight="1">
       <c r="A278" s="19" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="B278" s="20"/>
       <c r="C278" s="20" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="D278" s="21" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="E278" s="20"/>
       <c r="F278" s="20"/>
@@ -16325,14 +16405,14 @@
     </row>
     <row r="279" spans="1:9" ht="19" customHeight="1">
       <c r="A279" s="19" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="B279" s="20"/>
       <c r="C279" s="20" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="D279" s="21" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="E279" s="20"/>
       <c r="F279" s="20"/>
@@ -16342,14 +16422,14 @@
     </row>
     <row r="280" spans="1:9" ht="19" customHeight="1">
       <c r="A280" s="19" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B280" s="20"/>
       <c r="C280" s="20" t="s">
-        <v>600</v>
-      </c>
-      <c r="D280" s="20" t="s">
-        <v>733</v>
+        <v>594</v>
+      </c>
+      <c r="D280" s="21" t="s">
+        <v>730</v>
       </c>
       <c r="E280" s="20"/>
       <c r="F280" s="20"/>
@@ -16359,14 +16439,14 @@
     </row>
     <row r="281" spans="1:9" ht="19" customHeight="1">
       <c r="A281" s="19" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B281" s="20"/>
       <c r="C281" s="20" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="D281" s="21" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E281" s="20"/>
       <c r="F281" s="20"/>
@@ -16376,14 +16456,14 @@
     </row>
     <row r="282" spans="1:9" ht="19" customHeight="1">
       <c r="A282" s="19" t="s">
-        <v>960</v>
+        <v>597</v>
       </c>
       <c r="B282" s="20"/>
       <c r="C282" s="20" t="s">
-        <v>961</v>
-      </c>
-      <c r="D282" s="20" t="s">
-        <v>962</v>
+        <v>598</v>
+      </c>
+      <c r="D282" s="21" t="s">
+        <v>732</v>
       </c>
       <c r="E282" s="20"/>
       <c r="F282" s="20"/>
@@ -16393,14 +16473,14 @@
     </row>
     <row r="283" spans="1:9" ht="19" customHeight="1">
       <c r="A283" s="19" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B283" s="20"/>
       <c r="C283" s="20" t="s">
-        <v>604</v>
-      </c>
-      <c r="D283" s="21" t="s">
-        <v>735</v>
+        <v>600</v>
+      </c>
+      <c r="D283" s="20" t="s">
+        <v>733</v>
       </c>
       <c r="E283" s="20"/>
       <c r="F283" s="20"/>
@@ -16410,14 +16490,14 @@
     </row>
     <row r="284" spans="1:9" ht="19" customHeight="1">
       <c r="A284" s="19" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B284" s="20"/>
       <c r="C284" s="20" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D284" s="21" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E284" s="20"/>
       <c r="F284" s="20"/>
@@ -16427,14 +16507,14 @@
     </row>
     <row r="285" spans="1:9" ht="19" customHeight="1">
       <c r="A285" s="19" t="s">
-        <v>1032</v>
+        <v>960</v>
       </c>
       <c r="B285" s="20"/>
       <c r="C285" s="20" t="s">
-        <v>1033</v>
+        <v>961</v>
       </c>
       <c r="D285" s="20" t="s">
-        <v>1034</v>
+        <v>962</v>
       </c>
       <c r="E285" s="20"/>
       <c r="F285" s="20"/>
@@ -16444,14 +16524,14 @@
     </row>
     <row r="286" spans="1:9" ht="19" customHeight="1">
       <c r="A286" s="19" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B286" s="20"/>
       <c r="C286" s="20" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D286" s="21" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E286" s="20"/>
       <c r="F286" s="20"/>
@@ -16461,14 +16541,14 @@
     </row>
     <row r="287" spans="1:9" ht="19" customHeight="1">
       <c r="A287" s="19" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B287" s="20"/>
       <c r="C287" s="20" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D287" s="21" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E287" s="20"/>
       <c r="F287" s="20"/>
@@ -16478,14 +16558,14 @@
     </row>
     <row r="288" spans="1:9" ht="19" customHeight="1">
       <c r="A288" s="19" t="s">
-        <v>611</v>
+        <v>1032</v>
       </c>
       <c r="B288" s="20"/>
       <c r="C288" s="20" t="s">
-        <v>612</v>
+        <v>1033</v>
       </c>
       <c r="D288" s="20" t="s">
-        <v>739</v>
+        <v>1034</v>
       </c>
       <c r="E288" s="20"/>
       <c r="F288" s="20"/>
@@ -16495,14 +16575,14 @@
     </row>
     <row r="289" spans="1:9" ht="19" customHeight="1">
       <c r="A289" s="19" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B289" s="20"/>
       <c r="C289" s="20" t="s">
-        <v>614</v>
-      </c>
-      <c r="D289" s="20" t="s">
-        <v>740</v>
+        <v>608</v>
+      </c>
+      <c r="D289" s="21" t="s">
+        <v>737</v>
       </c>
       <c r="E289" s="20"/>
       <c r="F289" s="20"/>
@@ -16512,14 +16592,14 @@
     </row>
     <row r="290" spans="1:9" ht="19" customHeight="1">
       <c r="A290" s="19" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="B290" s="20"/>
       <c r="C290" s="20" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="D290" s="21" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E290" s="20"/>
       <c r="F290" s="20"/>
@@ -16529,14 +16609,14 @@
     </row>
     <row r="291" spans="1:9" ht="19" customHeight="1">
       <c r="A291" s="19" t="s">
-        <v>1089</v>
+        <v>611</v>
       </c>
       <c r="B291" s="20"/>
       <c r="C291" s="20" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D291" s="21" t="s">
-        <v>1091</v>
+        <v>612</v>
+      </c>
+      <c r="D291" s="20" t="s">
+        <v>739</v>
       </c>
       <c r="E291" s="20"/>
       <c r="F291" s="20"/>
@@ -16546,14 +16626,14 @@
     </row>
     <row r="292" spans="1:9" ht="19" customHeight="1">
       <c r="A292" s="19" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B292" s="20"/>
       <c r="C292" s="20" t="s">
-        <v>618</v>
-      </c>
-      <c r="D292" s="22" t="s">
-        <v>742</v>
+        <v>614</v>
+      </c>
+      <c r="D292" s="20" t="s">
+        <v>740</v>
       </c>
       <c r="E292" s="20"/>
       <c r="F292" s="20"/>
@@ -16563,14 +16643,14 @@
     </row>
     <row r="293" spans="1:9" ht="19" customHeight="1">
       <c r="A293" s="19" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B293" s="20"/>
       <c r="C293" s="20" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="D293" s="21" t="s">
-        <v>945</v>
+        <v>741</v>
       </c>
       <c r="E293" s="20"/>
       <c r="F293" s="20"/>
@@ -16580,14 +16660,14 @@
     </row>
     <row r="294" spans="1:9" ht="19" customHeight="1">
       <c r="A294" s="19" t="s">
-        <v>621</v>
+        <v>1089</v>
       </c>
       <c r="B294" s="20"/>
       <c r="C294" s="20" t="s">
-        <v>622</v>
+        <v>1090</v>
       </c>
       <c r="D294" s="21" t="s">
-        <v>743</v>
+        <v>1091</v>
       </c>
       <c r="E294" s="20"/>
       <c r="F294" s="20"/>
@@ -16597,14 +16677,14 @@
     </row>
     <row r="295" spans="1:9" ht="19" customHeight="1">
       <c r="A295" s="19" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B295" s="20"/>
       <c r="C295" s="20" t="s">
-        <v>624</v>
-      </c>
-      <c r="D295" s="20" t="s">
-        <v>744</v>
+        <v>618</v>
+      </c>
+      <c r="D295" s="22" t="s">
+        <v>742</v>
       </c>
       <c r="E295" s="20"/>
       <c r="F295" s="20"/>
@@ -16614,14 +16694,14 @@
     </row>
     <row r="296" spans="1:9" ht="19" customHeight="1">
       <c r="A296" s="19" t="s">
-        <v>957</v>
+        <v>619</v>
       </c>
       <c r="B296" s="20"/>
       <c r="C296" s="20" t="s">
-        <v>958</v>
-      </c>
-      <c r="D296" s="20" t="s">
-        <v>959</v>
+        <v>620</v>
+      </c>
+      <c r="D296" s="21" t="s">
+        <v>945</v>
       </c>
       <c r="E296" s="20"/>
       <c r="F296" s="20"/>
@@ -16631,14 +16711,14 @@
     </row>
     <row r="297" spans="1:9" ht="19" customHeight="1">
       <c r="A297" s="19" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="B297" s="20"/>
       <c r="C297" s="20" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D297" s="21" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E297" s="20"/>
       <c r="F297" s="20"/>
@@ -16648,14 +16728,14 @@
     </row>
     <row r="298" spans="1:9" ht="19" customHeight="1">
       <c r="A298" s="19" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B298" s="20"/>
       <c r="C298" s="20" t="s">
-        <v>628</v>
-      </c>
-      <c r="D298" s="21" t="s">
-        <v>746</v>
+        <v>624</v>
+      </c>
+      <c r="D298" s="20" t="s">
+        <v>744</v>
       </c>
       <c r="E298" s="20"/>
       <c r="F298" s="20"/>
@@ -16665,14 +16745,14 @@
     </row>
     <row r="299" spans="1:9" ht="19" customHeight="1">
       <c r="A299" s="19" t="s">
-        <v>629</v>
+        <v>957</v>
       </c>
       <c r="B299" s="20"/>
       <c r="C299" s="20" t="s">
-        <v>963</v>
-      </c>
-      <c r="D299" s="21" t="s">
-        <v>964</v>
+        <v>958</v>
+      </c>
+      <c r="D299" s="20" t="s">
+        <v>959</v>
       </c>
       <c r="E299" s="20"/>
       <c r="F299" s="20"/>
@@ -16682,14 +16762,14 @@
     </row>
     <row r="300" spans="1:9" ht="19" customHeight="1">
       <c r="A300" s="19" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="B300" s="20"/>
       <c r="C300" s="20" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="D300" s="21" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E300" s="20"/>
       <c r="F300" s="20"/>
@@ -16699,14 +16779,14 @@
     </row>
     <row r="301" spans="1:9" ht="19" customHeight="1">
       <c r="A301" s="19" t="s">
-        <v>965</v>
+        <v>627</v>
       </c>
       <c r="B301" s="20"/>
       <c r="C301" s="20" t="s">
-        <v>966</v>
-      </c>
-      <c r="D301" s="20" t="s">
-        <v>967</v>
+        <v>628</v>
+      </c>
+      <c r="D301" s="21" t="s">
+        <v>746</v>
       </c>
       <c r="E301" s="20"/>
       <c r="F301" s="20"/>
@@ -16716,14 +16796,14 @@
     </row>
     <row r="302" spans="1:9" ht="19" customHeight="1">
       <c r="A302" s="19" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B302" s="20"/>
       <c r="C302" s="20" t="s">
-        <v>633</v>
+        <v>963</v>
       </c>
       <c r="D302" s="21" t="s">
-        <v>748</v>
+        <v>964</v>
       </c>
       <c r="E302" s="20"/>
       <c r="F302" s="20"/>
@@ -16733,14 +16813,14 @@
     </row>
     <row r="303" spans="1:9" ht="19" customHeight="1">
       <c r="A303" s="19" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B303" s="20"/>
       <c r="C303" s="20" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D303" s="21" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E303" s="20"/>
       <c r="F303" s="20"/>
@@ -16750,14 +16830,14 @@
     </row>
     <row r="304" spans="1:9" ht="19" customHeight="1">
       <c r="A304" s="19" t="s">
-        <v>636</v>
+        <v>965</v>
       </c>
       <c r="B304" s="20"/>
       <c r="C304" s="20" t="s">
-        <v>637</v>
+        <v>966</v>
       </c>
       <c r="D304" s="20" t="s">
-        <v>750</v>
+        <v>967</v>
       </c>
       <c r="E304" s="20"/>
       <c r="F304" s="20"/>
@@ -16767,14 +16847,14 @@
     </row>
     <row r="305" spans="1:9" ht="19" customHeight="1">
       <c r="A305" s="19" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="B305" s="20"/>
       <c r="C305" s="20" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D305" s="21" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="E305" s="20"/>
       <c r="F305" s="20"/>
@@ -16784,14 +16864,14 @@
     </row>
     <row r="306" spans="1:9" ht="19" customHeight="1">
       <c r="A306" s="19" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="B306" s="20"/>
       <c r="C306" s="20" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="D306" s="21" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="E306" s="20"/>
       <c r="F306" s="20"/>
@@ -16801,14 +16881,14 @@
     </row>
     <row r="307" spans="1:9" ht="19" customHeight="1">
       <c r="A307" s="19" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B307" s="20"/>
       <c r="C307" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="D307" s="21" t="s">
-        <v>753</v>
+        <v>637</v>
+      </c>
+      <c r="D307" s="20" t="s">
+        <v>750</v>
       </c>
       <c r="E307" s="20"/>
       <c r="F307" s="20"/>
@@ -16818,14 +16898,14 @@
     </row>
     <row r="308" spans="1:9" ht="19" customHeight="1">
       <c r="A308" s="19" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="B308" s="20"/>
       <c r="C308" s="20" t="s">
-        <v>645</v>
-      </c>
-      <c r="D308" s="22" t="s">
-        <v>754</v>
+        <v>639</v>
+      </c>
+      <c r="D308" s="21" t="s">
+        <v>751</v>
       </c>
       <c r="E308" s="20"/>
       <c r="F308" s="20"/>
@@ -16835,14 +16915,14 @@
     </row>
     <row r="309" spans="1:9" ht="19" customHeight="1">
       <c r="A309" s="19" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="B309" s="20"/>
       <c r="C309" s="20" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="D309" s="21" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="E309" s="20"/>
       <c r="F309" s="20"/>
@@ -16852,14 +16932,14 @@
     </row>
     <row r="310" spans="1:9" ht="19" customHeight="1">
       <c r="A310" s="19" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="B310" s="20"/>
       <c r="C310" s="20" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="D310" s="21" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="E310" s="20"/>
       <c r="F310" s="20"/>
@@ -16869,14 +16949,14 @@
     </row>
     <row r="311" spans="1:9" ht="19" customHeight="1">
       <c r="A311" s="19" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="B311" s="20"/>
       <c r="C311" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="D311" s="21" t="s">
-        <v>757</v>
+        <v>645</v>
+      </c>
+      <c r="D311" s="22" t="s">
+        <v>754</v>
       </c>
       <c r="E311" s="20"/>
       <c r="F311" s="20"/>
@@ -16886,14 +16966,14 @@
     </row>
     <row r="312" spans="1:9" ht="19" customHeight="1">
       <c r="A312" s="19" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="B312" s="20"/>
       <c r="C312" s="20" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="D312" s="21" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="E312" s="20"/>
       <c r="F312" s="20"/>
@@ -16903,14 +16983,14 @@
     </row>
     <row r="313" spans="1:9" ht="19" customHeight="1">
       <c r="A313" s="19" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="B313" s="20"/>
       <c r="C313" s="20" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="D313" s="21" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E313" s="20"/>
       <c r="F313" s="20"/>
@@ -16920,14 +17000,14 @@
     </row>
     <row r="314" spans="1:9" ht="19" customHeight="1">
       <c r="A314" s="19" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="B314" s="20"/>
       <c r="C314" s="20" t="s">
-        <v>657</v>
-      </c>
-      <c r="D314" s="20" t="s">
-        <v>760</v>
+        <v>651</v>
+      </c>
+      <c r="D314" s="21" t="s">
+        <v>757</v>
       </c>
       <c r="E314" s="20"/>
       <c r="F314" s="20"/>
@@ -16937,14 +17017,14 @@
     </row>
     <row r="315" spans="1:9" ht="19" customHeight="1">
       <c r="A315" s="19" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="B315" s="20"/>
-      <c r="C315" s="27" t="s">
-        <v>659</v>
-      </c>
-      <c r="D315" s="27" t="s">
-        <v>761</v>
+      <c r="C315" s="20" t="s">
+        <v>653</v>
+      </c>
+      <c r="D315" s="21" t="s">
+        <v>758</v>
       </c>
       <c r="E315" s="20"/>
       <c r="F315" s="20"/>
@@ -16954,14 +17034,14 @@
     </row>
     <row r="316" spans="1:9" ht="19" customHeight="1">
       <c r="A316" s="19" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B316" s="20"/>
       <c r="C316" s="20" t="s">
-        <v>661</v>
-      </c>
-      <c r="D316" s="20" t="s">
-        <v>762</v>
+        <v>655</v>
+      </c>
+      <c r="D316" s="21" t="s">
+        <v>759</v>
       </c>
       <c r="E316" s="20"/>
       <c r="F316" s="20"/>
@@ -16971,14 +17051,14 @@
     </row>
     <row r="317" spans="1:9" ht="19" customHeight="1">
       <c r="A317" s="19" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="B317" s="20"/>
       <c r="C317" s="20" t="s">
-        <v>663</v>
-      </c>
-      <c r="D317" s="21" t="s">
-        <v>763</v>
+        <v>657</v>
+      </c>
+      <c r="D317" s="20" t="s">
+        <v>760</v>
       </c>
       <c r="E317" s="20"/>
       <c r="F317" s="20"/>
@@ -16988,14 +17068,14 @@
     </row>
     <row r="318" spans="1:9" ht="19" customHeight="1">
       <c r="A318" s="19" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="B318" s="20"/>
-      <c r="C318" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="D318" s="21" t="s">
-        <v>764</v>
+      <c r="C318" s="27" t="s">
+        <v>659</v>
+      </c>
+      <c r="D318" s="27" t="s">
+        <v>761</v>
       </c>
       <c r="E318" s="20"/>
       <c r="F318" s="20"/>
@@ -17005,14 +17085,14 @@
     </row>
     <row r="319" spans="1:9" ht="19" customHeight="1">
       <c r="A319" s="19" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="B319" s="20"/>
       <c r="C319" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="D319" s="21" t="s">
-        <v>765</v>
+        <v>661</v>
+      </c>
+      <c r="D319" s="20" t="s">
+        <v>762</v>
       </c>
       <c r="E319" s="20"/>
       <c r="F319" s="20"/>
@@ -17022,14 +17102,14 @@
     </row>
     <row r="320" spans="1:9" ht="19" customHeight="1">
       <c r="A320" s="19" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="B320" s="20"/>
       <c r="C320" s="20" t="s">
-        <v>669</v>
-      </c>
-      <c r="D320" s="20" t="s">
-        <v>766</v>
+        <v>663</v>
+      </c>
+      <c r="D320" s="21" t="s">
+        <v>763</v>
       </c>
       <c r="E320" s="20"/>
       <c r="F320" s="20"/>
@@ -17039,14 +17119,14 @@
     </row>
     <row r="321" spans="1:9" ht="19" customHeight="1">
       <c r="A321" s="19" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="B321" s="20"/>
       <c r="C321" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="D321" s="22" t="s">
-        <v>767</v>
+        <v>665</v>
+      </c>
+      <c r="D321" s="21" t="s">
+        <v>764</v>
       </c>
       <c r="E321" s="20"/>
       <c r="F321" s="20"/>
@@ -17056,14 +17136,14 @@
     </row>
     <row r="322" spans="1:9" ht="19" customHeight="1">
       <c r="A322" s="19" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="B322" s="20"/>
       <c r="C322" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="D322" s="20" t="s">
-        <v>768</v>
+        <v>667</v>
+      </c>
+      <c r="D322" s="21" t="s">
+        <v>765</v>
       </c>
       <c r="E322" s="20"/>
       <c r="F322" s="20"/>
@@ -17073,14 +17153,14 @@
     </row>
     <row r="323" spans="1:9" ht="19" customHeight="1">
       <c r="A323" s="19" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="B323" s="20"/>
       <c r="C323" s="20" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="D323" s="20" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="E323" s="20"/>
       <c r="F323" s="20"/>
@@ -17090,14 +17170,14 @@
     </row>
     <row r="324" spans="1:9" ht="19" customHeight="1">
       <c r="A324" s="19" t="s">
-        <v>954</v>
+        <v>670</v>
       </c>
       <c r="B324" s="20"/>
       <c r="C324" s="20" t="s">
-        <v>955</v>
-      </c>
-      <c r="D324" s="20" t="s">
-        <v>956</v>
+        <v>671</v>
+      </c>
+      <c r="D324" s="22" t="s">
+        <v>767</v>
       </c>
       <c r="E324" s="20"/>
       <c r="F324" s="20"/>
@@ -17107,14 +17187,14 @@
     </row>
     <row r="325" spans="1:9" ht="19" customHeight="1">
       <c r="A325" s="19" t="s">
-        <v>1081</v>
+        <v>672</v>
       </c>
       <c r="B325" s="20"/>
       <c r="C325" s="20" t="s">
-        <v>1082</v>
+        <v>673</v>
       </c>
       <c r="D325" s="20" t="s">
-        <v>1083</v>
+        <v>768</v>
       </c>
       <c r="E325" s="20"/>
       <c r="F325" s="20"/>
@@ -17123,10 +17203,16 @@
       <c r="I325" s="18"/>
     </row>
     <row r="326" spans="1:9" ht="19" customHeight="1">
-      <c r="A326" s="19"/>
+      <c r="A326" s="19" t="s">
+        <v>674</v>
+      </c>
       <c r="B326" s="20"/>
-      <c r="C326" s="20"/>
-      <c r="D326" s="20"/>
+      <c r="C326" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="D326" s="20" t="s">
+        <v>769</v>
+      </c>
       <c r="E326" s="20"/>
       <c r="F326" s="20"/>
       <c r="G326" s="18"/>
@@ -17134,10 +17220,16 @@
       <c r="I326" s="18"/>
     </row>
     <row r="327" spans="1:9" ht="19" customHeight="1">
-      <c r="A327" s="19"/>
+      <c r="A327" s="19" t="s">
+        <v>954</v>
+      </c>
       <c r="B327" s="20"/>
-      <c r="C327" s="20"/>
-      <c r="D327" s="20"/>
+      <c r="C327" s="20" t="s">
+        <v>955</v>
+      </c>
+      <c r="D327" s="20" t="s">
+        <v>956</v>
+      </c>
       <c r="E327" s="20"/>
       <c r="F327" s="20"/>
       <c r="G327" s="18"/>
@@ -17145,10 +17237,16 @@
       <c r="I327" s="18"/>
     </row>
     <row r="328" spans="1:9" ht="19" customHeight="1">
-      <c r="A328" s="19"/>
+      <c r="A328" s="19" t="s">
+        <v>1081</v>
+      </c>
       <c r="B328" s="20"/>
-      <c r="C328" s="20"/>
-      <c r="D328" s="20"/>
+      <c r="C328" s="20" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D328" s="20" t="s">
+        <v>1083</v>
+      </c>
       <c r="E328" s="20"/>
       <c r="F328" s="20"/>
       <c r="G328" s="18"/>
@@ -17815,405 +17913,453 @@
       <c r="H388" s="17"/>
       <c r="I388" s="18"/>
     </row>
+    <row r="389" spans="1:9" ht="19" customHeight="1">
+      <c r="A389" s="19"/>
+      <c r="B389" s="20"/>
+      <c r="C389" s="20"/>
+      <c r="D389" s="20"/>
+      <c r="E389" s="20"/>
+      <c r="F389" s="20"/>
+      <c r="G389" s="18"/>
+      <c r="H389" s="17"/>
+      <c r="I389" s="18"/>
+    </row>
+    <row r="390" spans="1:9" ht="19" customHeight="1">
+      <c r="A390" s="19"/>
+      <c r="B390" s="20"/>
+      <c r="C390" s="20"/>
+      <c r="D390" s="20"/>
+      <c r="E390" s="20"/>
+      <c r="F390" s="20"/>
+      <c r="G390" s="18"/>
+      <c r="H390" s="17"/>
+      <c r="I390" s="18"/>
+    </row>
+    <row r="391" spans="1:9" ht="19" customHeight="1">
+      <c r="A391" s="19"/>
+      <c r="B391" s="20"/>
+      <c r="C391" s="20"/>
+      <c r="D391" s="20"/>
+      <c r="E391" s="20"/>
+      <c r="F391" s="20"/>
+      <c r="G391" s="18"/>
+      <c r="H391" s="17"/>
+      <c r="I391" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J209" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A234:E235 E221:G221 A221:C233 A257:E258 A286:E287 A309:E310 E288:E308 A326:G388 A324:E325 A311:C323 E311:E323 E222:E233 B65:G65 D115:D133 I8:I28 A8:G28 A288:C308 A66:G114 A236:C256 E236:E256 A115:C141 E115:G141 D138:D141 A30:G64 A217:G220 A142:G215 I30:I215 E259 F222:G259 F263:F273 G263:G325 E263:E285 E260:G262 A259:C285 I217:I388">
-    <cfRule type="expression" dxfId="131" priority="260">
+  <conditionalFormatting sqref="A234:E235 E221:G221 A221:C233 A257:E258 A289:E290 A312:E313 E291:E311 A329:G391 A327:E328 A314:C326 E314:E326 E222:E233 B65:G65 D115:D133 I8:I28 A8:G28 A291:C311 A66:G114 A236:C256 E236:E256 A115:C141 E115:G141 D138:D141 A30:G64 A217:G220 A142:G215 I30:I215 E259 F222:G259 F270:F276 G270:G328 E270:E288 D271 E260:G269 I217:I391 A259:C288">
+    <cfRule type="expression" dxfId="134" priority="262">
       <formula>$G8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H388">
-    <cfRule type="cellIs" dxfId="130" priority="215" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H391">
+    <cfRule type="cellIs" dxfId="133" priority="217" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="222" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="132" priority="224" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="223" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="131" priority="225" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="224" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="130" priority="226" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H388">
-    <cfRule type="cellIs" dxfId="126" priority="216" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H391">
+    <cfRule type="cellIs" dxfId="129" priority="218" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="217" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="219" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="219" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="221" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="220" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="222" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="221" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="223" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H388">
-    <cfRule type="cellIs" dxfId="121" priority="218" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H8:H28 H87:H112 H30:H85 H115:H215 H217:H391">
+    <cfRule type="cellIs" dxfId="124" priority="220" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D134:D135">
-    <cfRule type="expression" dxfId="120" priority="139">
+    <cfRule type="expression" dxfId="123" priority="141">
       <formula>$G134&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136:D137">
-    <cfRule type="expression" dxfId="119" priority="138">
+    <cfRule type="expression" dxfId="122" priority="140">
       <formula>$G136&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:G5 I5 A5">
-    <cfRule type="expression" dxfId="118" priority="132">
+    <cfRule type="expression" dxfId="121" priority="134">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="117" priority="122" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="124" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="129" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="119" priority="131" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="130" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="118" priority="132" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="131" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="117" priority="133" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="113" priority="123" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="125" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="124" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="126" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="126" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="128" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="127" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="129" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="128" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="130" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="108" priority="125" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="127" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="107" priority="121">
+    <cfRule type="expression" dxfId="110" priority="123">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C216:G216 I216 A216">
-    <cfRule type="expression" dxfId="106" priority="120">
+    <cfRule type="expression" dxfId="109" priority="122">
       <formula>$G216&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H216">
-    <cfRule type="cellIs" dxfId="105" priority="110" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="112" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="117" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="107" priority="119" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="118" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="106" priority="120" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="119" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="105" priority="121" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H216">
-    <cfRule type="cellIs" dxfId="101" priority="111" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="113" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="112" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="114" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="114" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="116" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="115" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="117" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="116" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="118" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H216">
-    <cfRule type="cellIs" dxfId="96" priority="113" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="115" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B216">
-    <cfRule type="expression" dxfId="95" priority="109">
+    <cfRule type="expression" dxfId="98" priority="111">
       <formula>$G216&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D297:D298 D302:D323 D221:D242 D245 D264:D266 D270:D279 D286:D288 D292:D293 D249:D258">
-    <cfRule type="expression" dxfId="94" priority="262">
+  <conditionalFormatting sqref="D300:D301 D305:D326 D221:D242 D245 D273:D282 D289:D291 D295:D296 D249:D258 D265">
+    <cfRule type="expression" dxfId="97" priority="264">
       <formula>$G223&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F274:F325">
-    <cfRule type="expression" dxfId="93" priority="108">
-      <formula>$G274&lt;&gt;""</formula>
+  <conditionalFormatting sqref="F277:F328">
+    <cfRule type="expression" dxfId="96" priority="110">
+      <formula>$G277&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6 I6 C6:G6">
-    <cfRule type="expression" dxfId="92" priority="93">
+    <cfRule type="expression" dxfId="95" priority="95">
       <formula>$G6&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="91" priority="83" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="85" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="90" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="93" priority="92" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="91" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="92" priority="93" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="92" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="91" priority="94" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="87" priority="84" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="86" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="85" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="87" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="87" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="89" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="88" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="90" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="89" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="91" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="82" priority="86" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="88" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B7 I7 E7:G7">
-    <cfRule type="expression" dxfId="81" priority="82">
+    <cfRule type="expression" dxfId="84" priority="84">
       <formula>$G7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="80" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="74" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="79" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="82" priority="81" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="80" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="81" priority="82" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="81" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="80" priority="83" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="76" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="75" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="74" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="76" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="78" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="79" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="80" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="71" priority="75" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="77" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="70" priority="71">
+    <cfRule type="expression" dxfId="73" priority="73">
       <formula>$G6&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="69" priority="70">
+    <cfRule type="expression" dxfId="72" priority="72">
       <formula>$G7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="68" priority="69">
+    <cfRule type="expression" dxfId="71" priority="71">
       <formula>$G7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="expression" dxfId="67" priority="57">
+    <cfRule type="expression" dxfId="70" priority="59">
       <formula>$G65&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113:H114">
-    <cfRule type="cellIs" dxfId="66" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="48" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="53" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="68" priority="55" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="54" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="67" priority="56" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="55" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="66" priority="57" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113:H114">
-    <cfRule type="cellIs" dxfId="62" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="49" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="50" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="52" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="53" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="54" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H113:H114">
-    <cfRule type="cellIs" dxfId="57" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="51" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:G29 I29">
-    <cfRule type="expression" dxfId="56" priority="23">
+    <cfRule type="expression" dxfId="59" priority="25">
       <formula>$G29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="55" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="15" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="20" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="57" priority="22" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="21" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="56" priority="23" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="22" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="55" priority="24" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="51" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="16" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="17" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="19" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="20" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="21" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="46" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="18" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D294:D296 D299:D301 D283:D285 D280:D281 D246:D248 D267:D268 D289:D291 D261:D263">
-    <cfRule type="expression" dxfId="45" priority="265">
+  <conditionalFormatting sqref="D297:D299 D302:D304 D286:D288 D283:D284 D246:D248 D292:D294 D264 D267">
+    <cfRule type="expression" dxfId="48" priority="267">
       <formula>$G249&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="cellIs" dxfId="44" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="46" priority="11" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="45" priority="12" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="44" priority="13" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="5" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="6" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="8" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="9" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="10" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D282">
-    <cfRule type="expression" dxfId="34" priority="269">
-      <formula>$G286&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D285 D270">
+    <cfRule type="expression" dxfId="37" priority="271">
+      <formula>$G274&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D244">
-    <cfRule type="expression" dxfId="33" priority="300">
+  <conditionalFormatting sqref="D244 D272">
+    <cfRule type="expression" dxfId="36" priority="302">
       <formula>$G245&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D243">
-    <cfRule type="expression" dxfId="32" priority="301">
+    <cfRule type="expression" dxfId="35" priority="303">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D269">
-    <cfRule type="expression" dxfId="31" priority="1">
-      <formula>$G269&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D259:D260">
+    <cfRule type="expression" dxfId="34" priority="305">
+      <formula>$G265&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D259:D260">
-    <cfRule type="expression" dxfId="30" priority="303">
-      <formula>$G264&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D261:D263">
+    <cfRule type="expression" dxfId="33" priority="307">
+      <formula>$G265&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D266">
+    <cfRule type="expression" dxfId="32" priority="339">
+      <formula>$G272&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D268">
+    <cfRule type="expression" dxfId="31" priority="2">
+      <formula>$G268&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D269">
+    <cfRule type="expression" dxfId="30" priority="1">
+      <formula>$G269&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve stability, HTML-Report, Test Report Index
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99A5E63-3C0D-ED48-9097-EE3C64CCFCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3634821C-AB41-6B40-B798-8209EF8E0A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35860" yWindow="2320" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="1167">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -9898,6 +9898,21 @@
   </si>
   <si>
     <t>アプリを起動できませんでした。(${arg1}) ${submessage}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reusingAppiumDriverSession</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Reusing AppiumDriver session. (configFile=${arg1}, profileName=${arg2})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AppiumDriverセッションを再利用します。(configFile=${arg1}, profileName=${arg2})</t>
+    <rPh sb="18" eb="21">
+      <t>サイリヨウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -11521,8 +11536,8 @@
   <dimension ref="A1:I396"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A338" sqref="A338"/>
+      <pane ySplit="4" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A340" sqref="A340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -17629,10 +17644,16 @@
       <c r="I338" s="18"/>
     </row>
     <row r="339" spans="1:9" ht="19" customHeight="1">
-      <c r="A339" s="19"/>
+      <c r="A339" s="19" t="s">
+        <v>1164</v>
+      </c>
       <c r="B339" s="20"/>
-      <c r="C339" s="20"/>
-      <c r="D339" s="20"/>
+      <c r="C339" s="20" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D339" s="20" t="s">
+        <v>1166</v>
+      </c>
       <c r="E339" s="20"/>
       <c r="F339" s="20"/>
       <c r="G339" s="18"/>

</xml_diff>

<commit_message>
Bug fix Getting device from profile name
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8967826-31C0-C949-815F-99EFAA545A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95158D38-ACD9-9945-9C05-356549A0814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35740" yWindow="1980" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -9595,10 +9595,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Could not find connected Android device. Connect a device or start an emulator. Enable USB debug option on Android device.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>端末が見つかりました。(${subject})</t>
     <rPh sb="6" eb="8">
       <t>タンマテゥ</t>
@@ -9643,14 +9639,6 @@
   </si>
   <si>
     <t>couldNotFindConnectedDeviceByProfile</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Could not find connected device. (profile=${subject})</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>端末を検出できません。(profile=${subject})</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -10008,6 +9996,18 @@
     <rPh sb="15" eb="17">
       <t>キドウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not find connected device(profile=${subject}). Falling back to ${arg1}.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>端末を検出できません(profile=${subject})。${arg1}へフォールバックします。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not find connected Android device. Connect a device or start an emulator. Enable USB debug option on Android device. (profileName=${arg1})</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -11631,8 +11631,8 @@
   <dimension ref="A1:I398"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -13258,13 +13258,13 @@
         <v>96</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="20"/>
@@ -13274,16 +13274,16 @@
     </row>
     <row r="89" spans="1:9" ht="19" customHeight="1">
       <c r="A89" s="19" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D89" s="21" t="s">
         <v>1151</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>1152</v>
-      </c>
-      <c r="C89" s="20" t="s">
-        <v>1153</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>1154</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="20"/>
@@ -13293,16 +13293,16 @@
     </row>
     <row r="90" spans="1:9" ht="19" customHeight="1">
       <c r="A90" s="19" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B90" s="19" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D90" s="21" t="s">
         <v>1173</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C90" s="20" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>1176</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="20"/>
@@ -16046,10 +16046,10 @@
       </c>
       <c r="B239" s="20"/>
       <c r="C239" s="20" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="D239" s="20" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="E239" s="20"/>
       <c r="F239" s="20"/>
@@ -16331,14 +16331,14 @@
     </row>
     <row r="256" spans="1:9" ht="19" customHeight="1">
       <c r="A256" s="19" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="B256" s="20"/>
       <c r="C256" s="20" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="D256" s="20" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="E256" s="20"/>
       <c r="F256" s="20"/>
@@ -16454,7 +16454,7 @@
       </c>
       <c r="B263" s="20"/>
       <c r="C263" s="20" t="s">
-        <v>1118</v>
+        <v>1176</v>
       </c>
       <c r="D263" s="20" t="s">
         <v>710</v>
@@ -16484,14 +16484,14 @@
     </row>
     <row r="265" spans="1:9" ht="19" customHeight="1">
       <c r="A265" s="19" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B265" s="20"/>
       <c r="C265" s="20" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="D265" s="22" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="E265" s="20"/>
       <c r="F265" s="20"/>
@@ -16501,14 +16501,14 @@
     </row>
     <row r="266" spans="1:9" ht="19" customHeight="1">
       <c r="A266" s="19" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B266" s="20"/>
       <c r="C266" s="20" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="D266" s="22" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="E266" s="20"/>
       <c r="F266" s="20"/>
@@ -16518,14 +16518,14 @@
     </row>
     <row r="267" spans="1:9" ht="19" customHeight="1">
       <c r="A267" s="19" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B267" s="20"/>
       <c r="C267" s="20" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="D267" s="22" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="E267" s="20"/>
       <c r="F267" s="20"/>
@@ -16535,14 +16535,14 @@
     </row>
     <row r="268" spans="1:9" ht="19" customHeight="1">
       <c r="A268" s="19" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B268" s="20"/>
       <c r="C268" s="20" t="s">
-        <v>1127</v>
+        <v>1174</v>
       </c>
       <c r="D268" s="22" t="s">
-        <v>1128</v>
+        <v>1175</v>
       </c>
       <c r="E268" s="20"/>
       <c r="F268" s="20"/>
@@ -16624,10 +16624,10 @@
       </c>
       <c r="B273" s="20"/>
       <c r="C273" s="20" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="D273" s="20" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="E273" s="20"/>
       <c r="F273" s="20"/>
@@ -16644,7 +16644,7 @@
         <v>1112</v>
       </c>
       <c r="D274" s="20" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E274" s="20"/>
       <c r="F274" s="20"/>
@@ -16654,14 +16654,14 @@
     </row>
     <row r="275" spans="1:9" ht="19" customHeight="1">
       <c r="A275" s="19" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B275" s="20"/>
       <c r="C275" s="20" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D275" s="20" t="s">
         <v>1121</v>
-      </c>
-      <c r="D275" s="20" t="s">
-        <v>1122</v>
       </c>
       <c r="E275" s="20"/>
       <c r="F275" s="20"/>
@@ -17674,14 +17674,14 @@
     </row>
     <row r="335" spans="1:9" ht="19" customHeight="1">
       <c r="A335" s="19" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="B335" s="20"/>
       <c r="C335" s="20" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="D335" s="20" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="E335" s="20"/>
       <c r="F335" s="20"/>
@@ -17691,14 +17691,14 @@
     </row>
     <row r="336" spans="1:9" ht="19" customHeight="1">
       <c r="A336" s="19" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="B336" s="20"/>
       <c r="C336" s="20" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="D336" s="20" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="E336" s="20"/>
       <c r="F336" s="20"/>
@@ -17708,14 +17708,14 @@
     </row>
     <row r="337" spans="1:9" ht="19" customHeight="1">
       <c r="A337" s="19" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="B337" s="20"/>
       <c r="C337" s="20" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="D337" s="20" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="E337" s="20"/>
       <c r="F337" s="20"/>
@@ -17725,14 +17725,14 @@
     </row>
     <row r="338" spans="1:9" ht="19" customHeight="1">
       <c r="A338" s="19" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="B338" s="20"/>
       <c r="C338" s="20" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="D338" s="20" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="E338" s="20"/>
       <c r="F338" s="20"/>
@@ -17742,14 +17742,14 @@
     </row>
     <row r="339" spans="1:9" ht="19" customHeight="1">
       <c r="A339" s="19" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="B339" s="20"/>
       <c r="C339" s="20" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="D339" s="20" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="E339" s="20"/>
       <c r="F339" s="20"/>
@@ -17759,14 +17759,14 @@
     </row>
     <row r="340" spans="1:9" ht="19" customHeight="1">
       <c r="A340" s="19" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="B340" s="20"/>
       <c r="C340" s="20" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="D340" s="20" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="E340" s="20"/>
       <c r="F340" s="20"/>
@@ -17776,14 +17776,14 @@
     </row>
     <row r="341" spans="1:9" ht="19" customHeight="1">
       <c r="A341" s="19" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="B341" s="20"/>
       <c r="C341" s="20" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="D341" s="20" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="E341" s="20"/>
       <c r="F341" s="20"/>
@@ -17793,14 +17793,14 @@
     </row>
     <row r="342" spans="1:9" ht="19" customHeight="1">
       <c r="A342" s="19" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="B342" s="20"/>
       <c r="C342" s="20" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="D342" s="20" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="E342" s="20"/>
       <c r="F342" s="20"/>

</xml_diff>

<commit_message>
Improve Direct access mode
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24645733-C574-C549-9865-25CFDFBC2328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1E91BF-76D6-E34E-A72E-C899FB078191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35740" yWindow="1980" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="1196">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -10128,6 +10128,24 @@
   </si>
   <si>
     <t>${subject} is greater than or equal to ${expected}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>invalidScreenWeight</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Invalid weight(weight=${subject}). Check screen file. (file=${file})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>weightが不正です。screenファイルを確認してください。(file=${file})</t>
+    <rPh sb="7" eb="9">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>カクニn</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -11751,8 +11769,8 @@
   <dimension ref="A1:I402"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
+      <pane ySplit="4" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A347" sqref="A347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -18005,10 +18023,16 @@
       <c r="I346" s="18"/>
     </row>
     <row r="347" spans="1:9" ht="19" customHeight="1">
-      <c r="A347" s="19"/>
+      <c r="A347" s="19" t="s">
+        <v>1193</v>
+      </c>
       <c r="B347" s="20"/>
-      <c r="C347" s="20"/>
-      <c r="D347" s="20"/>
+      <c r="C347" s="20" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D347" s="20" t="s">
+        <v>1195</v>
+      </c>
       <c r="E347" s="20"/>
       <c r="F347" s="20"/>
       <c r="G347" s="18"/>
@@ -18623,7 +18647,7 @@
   </sheetData>
   <autoFilter ref="A4:J215" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A240:E241 E227:G227 A227:C239 A264:E265 A300:E301 A322:E323 A324:C336 E324:E336 E228:E239 B65:G65 D121:D139 I8:I28 A8:G28 E242:E263 A121:C147 E121:G147 D144:D147 A30:G64 A223:G226 E266 F228:G266 E280:E299 D281 E302:E321 A302:C321 F280:G339 A337:E339 E267:G279 I223:I402 A266:C299 A242:C263 A340:G402 A148:G221 I30:I221 A66:G120">
+  <conditionalFormatting sqref="A240:E241 E227:G227 A227:C239 A264:E265 A300:E301 A322:E323 A324:C336 E324:E336 E228:E239 B65:G65 D121:D139 I8:I28 A8:G28 E242:E263 A121:C147 E121:G147 D144:D147 A30:G64 A223:G226 E266 F228:G266 E280:E299 D281 E302:E321 A302:C321 F280:G339 A337:E339 E267:G279 I223:I402 A266:C299 A242:C263 A148:G221 I30:I221 A66:G120 A340:G402">
     <cfRule type="expression" dxfId="136" priority="262">
       <formula>$G8&lt;&gt;""</formula>
     </cfRule>

</xml_diff>

<commit_message>
New Parameter - enableRelativeCommandTranslation
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9616E9B2-8EA1-8749-88E4-CD89B32B253C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEBF878-97DC-2B47-96E9-498E0BE4C6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="500" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="1436">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -10193,180 +10193,6 @@
     <t>:aboveSwitch</t>
   </si>
   <si>
-    <t>:右のアイテム</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:右のラベル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:右の入力項目</t>
-    <rPh sb="3" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:右の画像</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:右のボタン</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:右のスイッチ</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:下のアイテム</t>
-    <rPh sb="1" eb="2">
-      <t>シタノ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:下の入力項目</t>
-    <rPh sb="3" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:下のラベル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:下の画像</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:下のボタン</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:下のスイッチ</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:左のアイテム</t>
-    <rPh sb="1" eb="2">
-      <t>ヒダリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:左の入力項目</t>
-    <rPh sb="1" eb="2">
-      <t>ヒダリ</t>
-    </rPh>
-    <rPh sb="3" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:左のラベル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:左の画像</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:左のボタン</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:左のスイッチ</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:上のアイテム</t>
-    <rPh sb="1" eb="2">
-      <t>ウエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:上の入力項目</t>
-    <rPh sb="1" eb="2">
-      <t>ヒダリ</t>
-    </rPh>
-    <rPh sb="3" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:上のラベル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:上の画像</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:上のボタン</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:上のスイッチ</t>
-    <rPh sb="1" eb="2">
-      <t>ミギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>:flow</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -10535,349 +10361,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>:フロー要素</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:垂直フロー要素</t>
-    <rPh sb="1" eb="3">
-      <t>スイチョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:フローラベル</t>
-    <rPh sb="1" eb="3">
-      <t>フロー</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:ラベル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:フロー入力項目</t>
-    <rPh sb="4" eb="8">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:入力項目</t>
-    <rPh sb="0" eb="5">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:フロー画像</t>
-    <rPh sb="4" eb="6">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:画像</t>
-    <rPh sb="0" eb="3">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:フローボタン</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:ボタン</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:フロースイッチ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:スイッチ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部要素</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブヨウソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部ラベル</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部入力項目</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部画像</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部スイッチ</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部ボタン</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部垂直フロー要素</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイチョク</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヨウソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部垂直フローラベル</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイチョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部垂直フロー要素</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイチョクヨウソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部垂直フロー入力項目</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイチョク</t>
-    </rPh>
-    <rPh sb="8" eb="12">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部垂直フロー画像</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイチョク</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部垂直フローボタン</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイチョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部垂直フロースイッチ</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイチョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:子要素</t>
-    <rPh sb="1" eb="4">
-      <t>コヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:兄弟要素</t>
-    <rPh sb="1" eb="5">
-      <t>キョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:親要素</t>
-    <rPh sb="1" eb="2">
-      <t xml:space="preserve">オヤ </t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ヨウソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:子孫要素</t>
-    <rPh sb="1" eb="2">
-      <t>シソn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:祖先要素</t>
-    <rPh sb="1" eb="3">
-      <t>ソセn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:次の要素</t>
-    <rPh sb="1" eb="2">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ヨウソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:前の要素</t>
-    <rPh sb="1" eb="2">
-      <t>マエノ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ヨウソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:次の入力項目</t>
-    <rPh sb="1" eb="3">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="3" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:前の入力項目</t>
-    <rPh sb="1" eb="2">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="3" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:次のラベル</t>
-    <rPh sb="1" eb="2">
-      <t>ツギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:前のラベル</t>
-    <rPh sb="1" eb="2">
-      <t>マエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:次の画像</t>
-    <rPh sb="1" eb="2">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:前の画像</t>
-    <rPh sb="1" eb="2">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:次のボタン</t>
-    <rPh sb="1" eb="2">
-      <t>ツギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:前のボタン</t>
-    <rPh sb="1" eb="2">
-      <t>マエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:次のスイッチ</t>
-    <rPh sb="1" eb="2">
-      <t>ツギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:前のスイッチ</t>
-    <rPh sb="1" eb="2">
-      <t>マエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:否定</t>
-    <rPh sb="1" eb="3">
-      <t>ヒテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>:cellWidget</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -10902,65 +10385,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>:セル内要素</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">ナイ </t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ヨウソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:セル内ラベル</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">ナイ </t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:セル内入力項目</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">ナイ </t>
-    </rPh>
-    <rPh sb="4" eb="8">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:セル内画像</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">ナイ </t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:セル内ボタン</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">ナイ </t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:セル内スイッチ</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">ナイ </t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>:innerWidget</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>:内部要素</t>
-    <rPh sb="1" eb="3">
-      <t>ナイブヨウソ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -11078,6 +10503,870 @@
   </si>
   <si>
     <t>existImage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:right]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:rightInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:右のアイテム]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:右の入力項目]</t>
+    <rPh sb="4" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:右のスイッチ]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:rightSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:rightLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:rightImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:rightButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:below]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:belowInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:belowLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:belowImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:belowButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:belowSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:left]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:leftInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:leftLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:leftImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:leftButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:leftSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:above]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:aboveInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:aboveLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:aboveImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:aboveButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:aboveSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:flow]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:vflow]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:flowLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:label]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:flowInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:input]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:flowImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:image]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:flowButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:button]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:flowSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:switch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerWidget]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:inner]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:not]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerVWidget]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerV]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerVlabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerVinput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerVimage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerVbutton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:innerVswitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:cellWidget]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:cellLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:cellInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:cellImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:cellButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:cellSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:child]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:sibling]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:parent]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:ancestor]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:descendant]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:next]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:previous]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:nextInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:preInput]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:nextLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:preLabel]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:nextImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:preImage]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:nextButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:preButton]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:nextSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:preSwitch]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:右のラベル]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:右の画像]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:右のボタン]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:下のアイテム]</t>
+    <rPh sb="2" eb="3">
+      <t>シタノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:下の入力項目]</t>
+    <rPh sb="4" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:下のラベル]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:下の画像]</t>
+    <rPh sb="1" eb="2">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:下のボタン]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:下のスイッチ]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:左のアイテム]</t>
+    <rPh sb="2" eb="3">
+      <t>ヒダリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:左の入力項目]</t>
+    <rPh sb="2" eb="3">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="4" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:左のラベル]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:左の画像]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:左のボタン]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:左のスイッチ]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:上のアイテム]</t>
+    <rPh sb="2" eb="3">
+      <t>ウエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:上の入力項目]</t>
+    <rPh sb="2" eb="3">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="4" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:上のラベル]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:上の画像]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:上のボタン]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:上のスイッチ]</t>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:フロー要素]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:垂直フロー要素]</t>
+    <rPh sb="2" eb="4">
+      <t>スイチョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:フローラベル]</t>
+    <rPh sb="2" eb="4">
+      <t>フロー</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:ラベル]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:フロー入力項目]</t>
+    <rPh sb="5" eb="9">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:入力項目]</t>
+    <rPh sb="1" eb="6">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:フロー画像]</t>
+    <rPh sb="5" eb="7">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:画像]</t>
+    <rPh sb="1" eb="4">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:フローボタン]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:ボタン]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:フロースイッチ]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:スイッチ]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部要素]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部ラベル]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部入力項目]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部画像]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部ボタン]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部スイッチ]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部垂直フロー要素]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スイチョク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部垂直フロー要素]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スイチョクヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部垂直フローラベル]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スイチョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部垂直フロー入力項目]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スイチョク</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部垂直フロー画像]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スイチョク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部垂直フローボタン]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スイチョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:内部垂直フロースイッチ]</t>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スイチョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:セル内要素]</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ナイ </t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:セル内ラベル]</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ナイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:セル内入力項目]</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ナイ </t>
+    </rPh>
+    <rPh sb="5" eb="9">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:セル内画像]</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ナイ </t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:セル内ボタン]</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ナイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:セル内スイッチ]</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">ナイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:子要素]</t>
+    <rPh sb="2" eb="5">
+      <t>コヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:兄弟要素]</t>
+    <rPh sb="2" eb="6">
+      <t>キョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:親要素]</t>
+    <rPh sb="2" eb="3">
+      <t xml:space="preserve">オヤ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:祖先要素]</t>
+    <rPh sb="2" eb="4">
+      <t>ソセn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:子孫要素]</t>
+    <rPh sb="2" eb="3">
+      <t>シソn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:次の要素]</t>
+    <rPh sb="2" eb="3">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:前の要素]</t>
+    <rPh sb="2" eb="3">
+      <t>マエノ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:次の入力項目]</t>
+    <rPh sb="2" eb="4">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="4" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:前の入力項目]</t>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="4" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:次のラベル]</t>
+    <rPh sb="2" eb="3">
+      <t>ツギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:前のラベル]</t>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:次の画像]</t>
+    <rPh sb="2" eb="3">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:前の画像]</t>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:次のボタン]</t>
+    <rPh sb="2" eb="3">
+      <t>ツギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:前のボタン]</t>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:次のスイッチ]</t>
+    <rPh sb="2" eb="3">
+      <t>ツギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:前のスイッチ]</t>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[:否定]</t>
+    <rPh sb="2" eb="4">
+      <t>ヒテイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12771,8 +13060,8 @@
   <dimension ref="A1:I493"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="4" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A359" sqref="A359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -13217,16 +13506,16 @@
     </row>
     <row r="26" spans="1:9" ht="19" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>1350</v>
+        <v>1276</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>1351</v>
+        <v>1277</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>1348</v>
+        <v>1274</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>1349</v>
+        <v>1275</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
@@ -13483,16 +13772,16 @@
     </row>
     <row r="40" spans="1:9" ht="19" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>1357</v>
+        <v>1283</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>1358</v>
+        <v>1284</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>1345</v>
+        <v>1271</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>1347</v>
+        <v>1273</v>
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="20"/>
@@ -13673,16 +13962,16 @@
     </row>
     <row r="50" spans="1:9" ht="19" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>1362</v>
+        <v>1288</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>1359</v>
+        <v>1285</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>1361</v>
+        <v>1287</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>1360</v>
+        <v>1286</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
@@ -13768,16 +14057,16 @@
     </row>
     <row r="55" spans="1:9" ht="19" customHeight="1">
       <c r="A55" s="19" t="s">
-        <v>1342</v>
+        <v>1268</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>1343</v>
+        <v>1269</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>1344</v>
+        <v>1270</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>1346</v>
+        <v>1272</v>
       </c>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -13806,16 +14095,16 @@
     </row>
     <row r="57" spans="1:9" ht="19" customHeight="1">
       <c r="A57" s="19" t="s">
-        <v>1355</v>
+        <v>1281</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>1356</v>
+        <v>1282</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>1345</v>
+        <v>1271</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>1347</v>
+        <v>1273</v>
       </c>
       <c r="E57" s="20"/>
       <c r="F57" s="20"/>
@@ -19154,14 +19443,14 @@
     </row>
     <row r="355" spans="1:9" ht="19" customHeight="1">
       <c r="A355" s="19" t="s">
-        <v>1352</v>
+        <v>1278</v>
       </c>
       <c r="B355" s="20"/>
       <c r="C355" s="20" t="s">
-        <v>1353</v>
+        <v>1279</v>
       </c>
       <c r="D355" s="20" t="s">
-        <v>1354</v>
+        <v>1280</v>
       </c>
       <c r="E355" s="20"/>
       <c r="F355" s="20"/>
@@ -19232,10 +19521,10 @@
       </c>
       <c r="B361" s="20"/>
       <c r="C361" s="20" t="s">
-        <v>1194</v>
+        <v>1289</v>
       </c>
       <c r="D361" s="20" t="s">
-        <v>1218</v>
+        <v>1291</v>
       </c>
       <c r="E361" s="20"/>
       <c r="F361" s="20"/>
@@ -19249,10 +19538,10 @@
       </c>
       <c r="B362" s="20"/>
       <c r="C362" s="20" t="s">
-        <v>1195</v>
+        <v>1290</v>
       </c>
       <c r="D362" s="20" t="s">
-        <v>1220</v>
+        <v>1292</v>
       </c>
       <c r="E362" s="20"/>
       <c r="F362" s="20"/>
@@ -19266,10 +19555,10 @@
       </c>
       <c r="B363" s="20"/>
       <c r="C363" s="20" t="s">
-        <v>1196</v>
+        <v>1295</v>
       </c>
       <c r="D363" s="20" t="s">
-        <v>1219</v>
+        <v>1366</v>
       </c>
       <c r="E363" s="20"/>
       <c r="F363" s="20"/>
@@ -19283,10 +19572,10 @@
       </c>
       <c r="B364" s="20"/>
       <c r="C364" s="20" t="s">
-        <v>1197</v>
+        <v>1296</v>
       </c>
       <c r="D364" s="20" t="s">
-        <v>1221</v>
+        <v>1367</v>
       </c>
       <c r="E364" s="20"/>
       <c r="F364" s="20"/>
@@ -19300,10 +19589,10 @@
       </c>
       <c r="B365" s="20"/>
       <c r="C365" s="20" t="s">
-        <v>1198</v>
+        <v>1297</v>
       </c>
       <c r="D365" s="20" t="s">
-        <v>1222</v>
+        <v>1368</v>
       </c>
       <c r="E365" s="20"/>
       <c r="F365" s="20"/>
@@ -19317,10 +19606,10 @@
       </c>
       <c r="B366" s="20"/>
       <c r="C366" s="20" t="s">
-        <v>1199</v>
+        <v>1294</v>
       </c>
       <c r="D366" s="20" t="s">
-        <v>1223</v>
+        <v>1293</v>
       </c>
       <c r="E366" s="20"/>
       <c r="F366" s="20"/>
@@ -19334,10 +19623,10 @@
       </c>
       <c r="B367" s="20"/>
       <c r="C367" s="20" t="s">
-        <v>1200</v>
+        <v>1298</v>
       </c>
       <c r="D367" s="20" t="s">
-        <v>1224</v>
+        <v>1369</v>
       </c>
       <c r="E367" s="20"/>
       <c r="F367" s="20"/>
@@ -19351,10 +19640,10 @@
       </c>
       <c r="B368" s="20"/>
       <c r="C368" s="20" t="s">
-        <v>1201</v>
+        <v>1299</v>
       </c>
       <c r="D368" s="20" t="s">
-        <v>1225</v>
+        <v>1370</v>
       </c>
       <c r="E368" s="20"/>
       <c r="F368" s="20"/>
@@ -19368,10 +19657,10 @@
       </c>
       <c r="B369" s="20"/>
       <c r="C369" s="20" t="s">
-        <v>1202</v>
+        <v>1300</v>
       </c>
       <c r="D369" s="20" t="s">
-        <v>1226</v>
+        <v>1371</v>
       </c>
       <c r="E369" s="20"/>
       <c r="F369" s="20"/>
@@ -19385,10 +19674,10 @@
       </c>
       <c r="B370" s="20"/>
       <c r="C370" s="20" t="s">
-        <v>1203</v>
+        <v>1301</v>
       </c>
       <c r="D370" s="20" t="s">
-        <v>1227</v>
+        <v>1372</v>
       </c>
       <c r="E370" s="20"/>
       <c r="F370" s="20"/>
@@ -19402,10 +19691,10 @@
       </c>
       <c r="B371" s="20"/>
       <c r="C371" s="20" t="s">
-        <v>1204</v>
+        <v>1302</v>
       </c>
       <c r="D371" s="20" t="s">
-        <v>1228</v>
+        <v>1373</v>
       </c>
       <c r="E371" s="20"/>
       <c r="F371" s="20"/>
@@ -19419,10 +19708,10 @@
       </c>
       <c r="B372" s="20"/>
       <c r="C372" s="20" t="s">
-        <v>1205</v>
+        <v>1303</v>
       </c>
       <c r="D372" s="20" t="s">
-        <v>1229</v>
+        <v>1374</v>
       </c>
       <c r="E372" s="20"/>
       <c r="F372" s="20"/>
@@ -19436,10 +19725,10 @@
       </c>
       <c r="B373" s="20"/>
       <c r="C373" s="20" t="s">
-        <v>1206</v>
+        <v>1304</v>
       </c>
       <c r="D373" s="20" t="s">
-        <v>1230</v>
+        <v>1375</v>
       </c>
       <c r="E373" s="20"/>
       <c r="F373" s="20"/>
@@ -19453,10 +19742,10 @@
       </c>
       <c r="B374" s="20"/>
       <c r="C374" s="20" t="s">
-        <v>1207</v>
+        <v>1305</v>
       </c>
       <c r="D374" s="20" t="s">
-        <v>1231</v>
+        <v>1376</v>
       </c>
       <c r="E374" s="20"/>
       <c r="F374" s="20"/>
@@ -19470,10 +19759,10 @@
       </c>
       <c r="B375" s="20"/>
       <c r="C375" s="20" t="s">
-        <v>1208</v>
+        <v>1306</v>
       </c>
       <c r="D375" s="20" t="s">
-        <v>1232</v>
+        <v>1377</v>
       </c>
       <c r="E375" s="20"/>
       <c r="F375" s="20"/>
@@ -19487,10 +19776,10 @@
       </c>
       <c r="B376" s="20"/>
       <c r="C376" s="20" t="s">
-        <v>1209</v>
+        <v>1307</v>
       </c>
       <c r="D376" s="20" t="s">
-        <v>1233</v>
+        <v>1378</v>
       </c>
       <c r="E376" s="20"/>
       <c r="F376" s="20"/>
@@ -19504,10 +19793,10 @@
       </c>
       <c r="B377" s="20"/>
       <c r="C377" s="20" t="s">
-        <v>1210</v>
+        <v>1308</v>
       </c>
       <c r="D377" s="20" t="s">
-        <v>1234</v>
+        <v>1379</v>
       </c>
       <c r="E377" s="20"/>
       <c r="F377" s="20"/>
@@ -19521,10 +19810,10 @@
       </c>
       <c r="B378" s="20"/>
       <c r="C378" s="20" t="s">
-        <v>1211</v>
+        <v>1309</v>
       </c>
       <c r="D378" s="20" t="s">
-        <v>1235</v>
+        <v>1380</v>
       </c>
       <c r="E378" s="20"/>
       <c r="F378" s="20"/>
@@ -19538,10 +19827,10 @@
       </c>
       <c r="B379" s="20"/>
       <c r="C379" s="20" t="s">
-        <v>1212</v>
+        <v>1310</v>
       </c>
       <c r="D379" s="20" t="s">
-        <v>1236</v>
+        <v>1381</v>
       </c>
       <c r="E379" s="20"/>
       <c r="F379" s="20"/>
@@ -19555,10 +19844,10 @@
       </c>
       <c r="B380" s="20"/>
       <c r="C380" s="20" t="s">
-        <v>1213</v>
+        <v>1311</v>
       </c>
       <c r="D380" s="20" t="s">
-        <v>1237</v>
+        <v>1382</v>
       </c>
       <c r="E380" s="20"/>
       <c r="F380" s="20"/>
@@ -19572,10 +19861,10 @@
       </c>
       <c r="B381" s="20"/>
       <c r="C381" s="20" t="s">
-        <v>1214</v>
+        <v>1312</v>
       </c>
       <c r="D381" s="20" t="s">
-        <v>1238</v>
+        <v>1383</v>
       </c>
       <c r="E381" s="20"/>
       <c r="F381" s="20"/>
@@ -19589,10 +19878,10 @@
       </c>
       <c r="B382" s="20"/>
       <c r="C382" s="20" t="s">
-        <v>1215</v>
+        <v>1313</v>
       </c>
       <c r="D382" s="20" t="s">
-        <v>1239</v>
+        <v>1384</v>
       </c>
       <c r="E382" s="20"/>
       <c r="F382" s="20"/>
@@ -19606,10 +19895,10 @@
       </c>
       <c r="B383" s="20"/>
       <c r="C383" s="20" t="s">
-        <v>1216</v>
+        <v>1314</v>
       </c>
       <c r="D383" s="20" t="s">
-        <v>1240</v>
+        <v>1385</v>
       </c>
       <c r="E383" s="20"/>
       <c r="F383" s="20"/>
@@ -19623,10 +19912,10 @@
       </c>
       <c r="B384" s="20"/>
       <c r="C384" s="20" t="s">
-        <v>1217</v>
+        <v>1315</v>
       </c>
       <c r="D384" s="20" t="s">
-        <v>1241</v>
+        <v>1386</v>
       </c>
       <c r="E384" s="20"/>
       <c r="F384" s="20"/>
@@ -19636,14 +19925,14 @@
     </row>
     <row r="385" spans="1:9" ht="19" customHeight="1">
       <c r="A385" s="19" t="s">
-        <v>1242</v>
+        <v>1218</v>
       </c>
       <c r="B385" s="20"/>
       <c r="C385" s="19" t="s">
-        <v>1242</v>
+        <v>1316</v>
       </c>
       <c r="D385" s="20" t="s">
-        <v>1284</v>
+        <v>1387</v>
       </c>
       <c r="E385" s="20"/>
       <c r="F385" s="20"/>
@@ -19653,14 +19942,14 @@
     </row>
     <row r="386" spans="1:9" ht="19" customHeight="1">
       <c r="A386" s="19" t="s">
-        <v>1243</v>
+        <v>1219</v>
       </c>
       <c r="B386" s="20"/>
       <c r="C386" s="19" t="s">
-        <v>1243</v>
+        <v>1317</v>
       </c>
       <c r="D386" s="20" t="s">
-        <v>1285</v>
+        <v>1388</v>
       </c>
       <c r="E386" s="20"/>
       <c r="F386" s="20"/>
@@ -19670,14 +19959,14 @@
     </row>
     <row r="387" spans="1:9" ht="19" customHeight="1">
       <c r="A387" s="19" t="s">
-        <v>1244</v>
+        <v>1220</v>
       </c>
       <c r="B387" s="20"/>
       <c r="C387" s="19" t="s">
-        <v>1244</v>
+        <v>1318</v>
       </c>
       <c r="D387" s="20" t="s">
-        <v>1286</v>
+        <v>1389</v>
       </c>
       <c r="E387" s="20"/>
       <c r="F387" s="20"/>
@@ -19687,14 +19976,14 @@
     </row>
     <row r="388" spans="1:9" ht="19" customHeight="1">
       <c r="A388" s="19" t="s">
-        <v>1245</v>
+        <v>1221</v>
       </c>
       <c r="B388" s="20"/>
       <c r="C388" s="19" t="s">
-        <v>1245</v>
+        <v>1319</v>
       </c>
       <c r="D388" s="20" t="s">
-        <v>1287</v>
+        <v>1390</v>
       </c>
       <c r="E388" s="20"/>
       <c r="F388" s="20"/>
@@ -19704,14 +19993,14 @@
     </row>
     <row r="389" spans="1:9" ht="19" customHeight="1">
       <c r="A389" s="19" t="s">
-        <v>1246</v>
+        <v>1222</v>
       </c>
       <c r="B389" s="20"/>
       <c r="C389" s="19" t="s">
-        <v>1246</v>
+        <v>1320</v>
       </c>
       <c r="D389" s="20" t="s">
-        <v>1288</v>
+        <v>1391</v>
       </c>
       <c r="E389" s="20"/>
       <c r="F389" s="20"/>
@@ -19721,14 +20010,14 @@
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
       <c r="A390" s="19" t="s">
-        <v>1247</v>
+        <v>1223</v>
       </c>
       <c r="B390" s="20"/>
       <c r="C390" s="19" t="s">
-        <v>1247</v>
+        <v>1321</v>
       </c>
       <c r="D390" s="20" t="s">
-        <v>1289</v>
+        <v>1392</v>
       </c>
       <c r="E390" s="20"/>
       <c r="F390" s="20"/>
@@ -19738,14 +20027,14 @@
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
       <c r="A391" s="19" t="s">
-        <v>1248</v>
+        <v>1224</v>
       </c>
       <c r="B391" s="20"/>
       <c r="C391" s="19" t="s">
-        <v>1248</v>
+        <v>1322</v>
       </c>
       <c r="D391" s="20" t="s">
-        <v>1290</v>
+        <v>1393</v>
       </c>
       <c r="E391" s="20"/>
       <c r="F391" s="20"/>
@@ -19755,14 +20044,14 @@
     </row>
     <row r="392" spans="1:9" ht="19" customHeight="1">
       <c r="A392" s="19" t="s">
-        <v>1249</v>
+        <v>1225</v>
       </c>
       <c r="B392" s="20"/>
       <c r="C392" s="19" t="s">
-        <v>1249</v>
+        <v>1323</v>
       </c>
       <c r="D392" s="20" t="s">
-        <v>1291</v>
+        <v>1394</v>
       </c>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
@@ -19772,14 +20061,14 @@
     </row>
     <row r="393" spans="1:9" ht="19" customHeight="1">
       <c r="A393" s="19" t="s">
-        <v>1250</v>
+        <v>1226</v>
       </c>
       <c r="B393" s="20"/>
       <c r="C393" s="19" t="s">
-        <v>1250</v>
+        <v>1324</v>
       </c>
       <c r="D393" s="20" t="s">
-        <v>1292</v>
+        <v>1395</v>
       </c>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
@@ -19789,14 +20078,14 @@
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
       <c r="A394" s="19" t="s">
-        <v>1251</v>
+        <v>1227</v>
       </c>
       <c r="B394" s="20"/>
       <c r="C394" s="19" t="s">
-        <v>1251</v>
+        <v>1325</v>
       </c>
       <c r="D394" s="20" t="s">
-        <v>1293</v>
+        <v>1396</v>
       </c>
       <c r="E394" s="20"/>
       <c r="F394" s="20"/>
@@ -19806,14 +20095,14 @@
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
       <c r="A395" s="19" t="s">
-        <v>1252</v>
+        <v>1228</v>
       </c>
       <c r="B395" s="20"/>
       <c r="C395" s="19" t="s">
-        <v>1252</v>
+        <v>1326</v>
       </c>
       <c r="D395" s="20" t="s">
-        <v>1294</v>
+        <v>1397</v>
       </c>
       <c r="E395" s="20"/>
       <c r="F395" s="20"/>
@@ -19823,14 +20112,14 @@
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
       <c r="A396" s="19" t="s">
-        <v>1253</v>
+        <v>1229</v>
       </c>
       <c r="B396" s="20"/>
       <c r="C396" s="19" t="s">
-        <v>1253</v>
+        <v>1327</v>
       </c>
       <c r="D396" s="20" t="s">
-        <v>1295</v>
+        <v>1398</v>
       </c>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
@@ -19840,14 +20129,14 @@
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
       <c r="A397" s="19" t="s">
-        <v>1339</v>
+        <v>1266</v>
       </c>
       <c r="B397" s="20"/>
       <c r="C397" s="19" t="s">
-        <v>1339</v>
+        <v>1328</v>
       </c>
       <c r="D397" s="20" t="s">
-        <v>1340</v>
+        <v>1399</v>
       </c>
       <c r="E397" s="20"/>
       <c r="F397" s="20"/>
@@ -19857,14 +20146,14 @@
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1254</v>
+        <v>1230</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="19" t="s">
-        <v>1254</v>
+        <v>1329</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1296</v>
+        <v>1399</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -19874,14 +20163,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1255</v>
+        <v>1231</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="19" t="s">
-        <v>1255</v>
+        <v>1330</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1297</v>
+        <v>1400</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -19891,14 +20180,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1256</v>
+        <v>1232</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="19" t="s">
-        <v>1256</v>
+        <v>1331</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1298</v>
+        <v>1401</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -19908,14 +20197,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1257</v>
+        <v>1233</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="19" t="s">
-        <v>1257</v>
+        <v>1333</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1299</v>
+        <v>1402</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -19925,14 +20214,14 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1258</v>
+        <v>1234</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="19" t="s">
-        <v>1258</v>
+        <v>1334</v>
       </c>
       <c r="D402" s="20" t="s">
-        <v>1301</v>
+        <v>1403</v>
       </c>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
@@ -19942,14 +20231,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1259</v>
+        <v>1235</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="19" t="s">
-        <v>1259</v>
+        <v>1335</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1300</v>
+        <v>1404</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -19959,14 +20248,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1341</v>
+        <v>1267</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="19" t="s">
-        <v>1341</v>
+        <v>1336</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1302</v>
+        <v>1405</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -19976,14 +20265,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1260</v>
+        <v>1236</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="19" t="s">
-        <v>1260</v>
+        <v>1337</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1304</v>
+        <v>1406</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -19993,14 +20282,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1261</v>
+        <v>1237</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="19" t="s">
-        <v>1261</v>
+        <v>1338</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1303</v>
+        <v>1407</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -20010,14 +20299,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1262</v>
+        <v>1238</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="19" t="s">
-        <v>1262</v>
+        <v>1339</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1305</v>
+        <v>1408</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -20027,14 +20316,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1263</v>
+        <v>1239</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="19" t="s">
-        <v>1263</v>
+        <v>1340</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1306</v>
+        <v>1409</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -20044,14 +20333,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1264</v>
+        <v>1240</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="19" t="s">
-        <v>1264</v>
+        <v>1341</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1307</v>
+        <v>1410</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -20061,14 +20350,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1265</v>
+        <v>1241</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="19" t="s">
-        <v>1265</v>
+        <v>1342</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1308</v>
+        <v>1411</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -20078,14 +20367,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1327</v>
+        <v>1260</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="19" t="s">
-        <v>1327</v>
+        <v>1343</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1333</v>
+        <v>1412</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -20095,14 +20384,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1328</v>
+        <v>1261</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="19" t="s">
-        <v>1328</v>
+        <v>1344</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1334</v>
+        <v>1413</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -20112,14 +20401,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1329</v>
+        <v>1262</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="19" t="s">
-        <v>1329</v>
+        <v>1345</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1335</v>
+        <v>1414</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -20129,14 +20418,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1330</v>
+        <v>1263</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="19" t="s">
-        <v>1330</v>
+        <v>1346</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1336</v>
+        <v>1415</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -20146,14 +20435,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1331</v>
+        <v>1264</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="19" t="s">
-        <v>1331</v>
+        <v>1347</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1337</v>
+        <v>1416</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -20163,14 +20452,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1332</v>
+        <v>1265</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="19" t="s">
-        <v>1332</v>
+        <v>1348</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1338</v>
+        <v>1417</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -20180,14 +20469,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1266</v>
+        <v>1242</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="19" t="s">
-        <v>1266</v>
+        <v>1349</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1309</v>
+        <v>1418</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -20197,14 +20486,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1267</v>
+        <v>1243</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="19" t="s">
-        <v>1267</v>
+        <v>1350</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1310</v>
+        <v>1419</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -20214,14 +20503,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1268</v>
+        <v>1244</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="19" t="s">
-        <v>1268</v>
+        <v>1351</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1311</v>
+        <v>1420</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -20231,14 +20520,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1269</v>
+        <v>1245</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="19" t="s">
-        <v>1269</v>
+        <v>1352</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1313</v>
+        <v>1421</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -20248,14 +20537,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1270</v>
+        <v>1246</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="19" t="s">
-        <v>1270</v>
+        <v>1353</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1312</v>
+        <v>1422</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -20265,14 +20554,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1271</v>
+        <v>1247</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="19" t="s">
-        <v>1271</v>
+        <v>1354</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1314</v>
+        <v>1423</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -20282,14 +20571,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1272</v>
+        <v>1248</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="19" t="s">
-        <v>1272</v>
+        <v>1355</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1315</v>
+        <v>1424</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -20299,14 +20588,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1273</v>
+        <v>1249</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="19" t="s">
-        <v>1273</v>
+        <v>1356</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1316</v>
+        <v>1425</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -20316,14 +20605,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1274</v>
+        <v>1250</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="19" t="s">
-        <v>1274</v>
+        <v>1357</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1317</v>
+        <v>1426</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -20333,14 +20622,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1275</v>
+        <v>1251</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="19" t="s">
-        <v>1275</v>
+        <v>1358</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1318</v>
+        <v>1427</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -20350,14 +20639,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1276</v>
+        <v>1252</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="19" t="s">
-        <v>1276</v>
+        <v>1359</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1319</v>
+        <v>1428</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -20367,14 +20656,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1277</v>
+        <v>1253</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="19" t="s">
-        <v>1277</v>
+        <v>1360</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1320</v>
+        <v>1429</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -20384,14 +20673,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1278</v>
+        <v>1254</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1278</v>
+        <v>1361</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1321</v>
+        <v>1430</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -20401,14 +20690,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1279</v>
+        <v>1255</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1279</v>
+        <v>1362</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1322</v>
+        <v>1431</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -20418,14 +20707,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1280</v>
+        <v>1256</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1280</v>
+        <v>1363</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1323</v>
+        <v>1432</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -20435,14 +20724,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1281</v>
+        <v>1257</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1281</v>
+        <v>1364</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1324</v>
+        <v>1433</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -20452,14 +20741,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1282</v>
+        <v>1258</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1282</v>
+        <v>1365</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1325</v>
+        <v>1434</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -20469,14 +20758,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1283</v>
+        <v>1259</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1283</v>
+        <v>1332</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1326</v>
+        <v>1435</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>

</xml_diff>

<commit_message>
Improve - logging if* function - existInCell - comparing space
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D742DA-8EB7-0545-8CCE-400CD1550026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75D5E1B-DA27-8241-8EBD-536818D3234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27340" yWindow="500" windowWidth="40900" windowHeight="37920" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
+    <workbookView xWindow="30220" yWindow="3120" windowWidth="37140" windowHeight="33260" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
   <sheets>
     <sheet name="message" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="1422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="1434">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11287,6 +11287,84 @@
     <rPh sb="20" eb="22">
       <t>トウカ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>notMatch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ではない場合</t>
+    <rPh sb="4" eb="6">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>not match</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ifScreenIs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ifScreenIsNot</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画面が${subject}の場合</t>
+    <rPh sb="0" eb="2">
+      <t>ガメn</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ガメn</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画面が${subject}ではない場合</t>
+    <rPh sb="0" eb="2">
+      <t>ガメn</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ガメn</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ifElse</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if else</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>それ以外の場合</t>
+    <rPh sb="5" eb="7">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if screen is ${subject}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if screen is not ${subject}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12228,11 +12306,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I497"/>
+  <dimension ref="A1:I498"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="4" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -16403,7 +16481,9 @@
       <c r="A222" s="19" t="s">
         <v>490</v>
       </c>
-      <c r="B222" s="20"/>
+      <c r="B222" s="20" t="s">
+        <v>436</v>
+      </c>
       <c r="C222" s="20" t="s">
         <v>1095</v>
       </c>
@@ -16420,7 +16500,9 @@
       <c r="A223" s="19" t="s">
         <v>491</v>
       </c>
-      <c r="B223" s="20"/>
+      <c r="B223" s="20" t="s">
+        <v>436</v>
+      </c>
       <c r="C223" s="20" t="s">
         <v>1096</v>
       </c>
@@ -16434,10 +16516,18 @@
       <c r="I223" s="18"/>
     </row>
     <row r="224" spans="1:9" ht="19" customHeight="1">
-      <c r="A224" s="19"/>
-      <c r="B224" s="20"/>
-      <c r="C224" s="20"/>
-      <c r="D224" s="20"/>
+      <c r="A224" s="19" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B224" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C224" s="20" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D224" s="20" t="s">
+        <v>1427</v>
+      </c>
       <c r="E224" s="20"/>
       <c r="F224" s="20"/>
       <c r="G224" s="18"/>
@@ -16445,10 +16535,18 @@
       <c r="I224" s="18"/>
     </row>
     <row r="225" spans="1:9" ht="19" customHeight="1">
-      <c r="A225" s="19"/>
-      <c r="B225" s="20"/>
-      <c r="C225" s="20"/>
-      <c r="D225" s="20"/>
+      <c r="A225" s="19" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B225" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C225" s="20" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D225" s="20" t="s">
+        <v>1428</v>
+      </c>
       <c r="E225" s="20"/>
       <c r="F225" s="20"/>
       <c r="G225" s="18"/>
@@ -16456,10 +16554,18 @@
       <c r="I225" s="18"/>
     </row>
     <row r="226" spans="1:9" ht="19" customHeight="1">
-      <c r="A226" s="19"/>
-      <c r="B226" s="20"/>
-      <c r="C226" s="20"/>
-      <c r="D226" s="20"/>
+      <c r="A226" s="19" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B226" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C226" s="20" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D226" s="20" t="s">
+        <v>1431</v>
+      </c>
       <c r="E226" s="20"/>
       <c r="F226" s="20"/>
       <c r="G226" s="18"/>
@@ -16576,14 +16682,14 @@
     </row>
     <row r="235" spans="1:9" ht="19" customHeight="1">
       <c r="A235" s="19" t="s">
-        <v>488</v>
+        <v>1422</v>
       </c>
       <c r="B235" s="20"/>
       <c r="C235" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="D235" s="22" t="s">
-        <v>673</v>
+        <v>1424</v>
+      </c>
+      <c r="D235" s="20" t="s">
+        <v>1423</v>
       </c>
       <c r="E235" s="20"/>
       <c r="F235" s="20"/>
@@ -16593,14 +16699,14 @@
     </row>
     <row r="236" spans="1:9" ht="19" customHeight="1">
       <c r="A236" s="19" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B236" s="20"/>
       <c r="C236" s="20" t="s">
-        <v>493</v>
-      </c>
-      <c r="D236" s="21" t="s">
-        <v>674</v>
+        <v>489</v>
+      </c>
+      <c r="D236" s="22" t="s">
+        <v>673</v>
       </c>
       <c r="E236" s="20"/>
       <c r="F236" s="20"/>
@@ -16610,14 +16716,14 @@
     </row>
     <row r="237" spans="1:9" ht="19" customHeight="1">
       <c r="A237" s="19" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B237" s="20"/>
       <c r="C237" s="20" t="s">
-        <v>495</v>
-      </c>
-      <c r="D237" s="22" t="s">
-        <v>675</v>
+        <v>493</v>
+      </c>
+      <c r="D237" s="21" t="s">
+        <v>674</v>
       </c>
       <c r="E237" s="20"/>
       <c r="F237" s="20"/>
@@ -16627,14 +16733,14 @@
     </row>
     <row r="238" spans="1:9" ht="19" customHeight="1">
       <c r="A238" s="19" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B238" s="20"/>
       <c r="C238" s="20" t="s">
-        <v>497</v>
-      </c>
-      <c r="D238" s="21" t="s">
-        <v>676</v>
+        <v>495</v>
+      </c>
+      <c r="D238" s="22" t="s">
+        <v>675</v>
       </c>
       <c r="E238" s="20"/>
       <c r="F238" s="20"/>
@@ -16644,14 +16750,14 @@
     </row>
     <row r="239" spans="1:9" ht="19" customHeight="1">
       <c r="A239" s="19" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B239" s="20"/>
       <c r="C239" s="20" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D239" s="21" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E239" s="20"/>
       <c r="F239" s="20"/>
@@ -16661,14 +16767,14 @@
     </row>
     <row r="240" spans="1:9" ht="19" customHeight="1">
       <c r="A240" s="19" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B240" s="20"/>
       <c r="C240" s="20" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D240" s="21" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E240" s="20"/>
       <c r="F240" s="20"/>
@@ -16678,14 +16784,14 @@
     </row>
     <row r="241" spans="1:9" ht="19" customHeight="1">
       <c r="A241" s="19" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B241" s="20"/>
       <c r="C241" s="20" t="s">
-        <v>928</v>
+        <v>501</v>
       </c>
       <c r="D241" s="21" t="s">
-        <v>929</v>
+        <v>678</v>
       </c>
       <c r="E241" s="20"/>
       <c r="F241" s="20"/>
@@ -16695,14 +16801,14 @@
     </row>
     <row r="242" spans="1:9" ht="19" customHeight="1">
       <c r="A242" s="19" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B242" s="20"/>
       <c r="C242" s="20" t="s">
-        <v>504</v>
+        <v>928</v>
       </c>
       <c r="D242" s="21" t="s">
-        <v>679</v>
+        <v>929</v>
       </c>
       <c r="E242" s="20"/>
       <c r="F242" s="20"/>
@@ -16712,14 +16818,14 @@
     </row>
     <row r="243" spans="1:9" ht="19" customHeight="1">
       <c r="A243" s="19" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B243" s="20"/>
       <c r="C243" s="20" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D243" s="21" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E243" s="20"/>
       <c r="F243" s="20"/>
@@ -16729,14 +16835,14 @@
     </row>
     <row r="244" spans="1:9" ht="19" customHeight="1">
       <c r="A244" s="19" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B244" s="20"/>
       <c r="C244" s="20" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D244" s="21" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E244" s="20"/>
       <c r="F244" s="20"/>
@@ -16746,14 +16852,14 @@
     </row>
     <row r="245" spans="1:9" ht="19" customHeight="1">
       <c r="A245" s="19" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B245" s="20"/>
       <c r="C245" s="20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D245" s="21" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E245" s="20"/>
       <c r="F245" s="20"/>
@@ -16763,14 +16869,14 @@
     </row>
     <row r="246" spans="1:9" ht="19" customHeight="1">
       <c r="A246" s="19" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B246" s="20"/>
       <c r="C246" s="20" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D246" s="21" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E246" s="20"/>
       <c r="F246" s="20"/>
@@ -16780,14 +16886,14 @@
     </row>
     <row r="247" spans="1:9" ht="19" customHeight="1">
       <c r="A247" s="19" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B247" s="20"/>
       <c r="C247" s="20" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D247" s="21" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E247" s="20"/>
       <c r="F247" s="20"/>
@@ -16797,14 +16903,14 @@
     </row>
     <row r="248" spans="1:9" ht="19" customHeight="1">
       <c r="A248" s="19" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B248" s="20"/>
       <c r="C248" s="20" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D248" s="21" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E248" s="20"/>
       <c r="F248" s="20"/>
@@ -16814,14 +16920,14 @@
     </row>
     <row r="249" spans="1:9" ht="19" customHeight="1">
       <c r="A249" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B249" s="20"/>
       <c r="C249" s="20" t="s">
-        <v>518</v>
-      </c>
-      <c r="D249" s="20" t="s">
-        <v>686</v>
+        <v>516</v>
+      </c>
+      <c r="D249" s="21" t="s">
+        <v>685</v>
       </c>
       <c r="E249" s="20"/>
       <c r="F249" s="20"/>
@@ -16831,14 +16937,14 @@
     </row>
     <row r="250" spans="1:9" ht="19" customHeight="1">
       <c r="A250" s="19" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B250" s="20"/>
       <c r="C250" s="20" t="s">
-        <v>520</v>
-      </c>
-      <c r="D250" s="22" t="s">
-        <v>687</v>
+        <v>518</v>
+      </c>
+      <c r="D250" s="20" t="s">
+        <v>686</v>
       </c>
       <c r="E250" s="20"/>
       <c r="F250" s="20"/>
@@ -16848,14 +16954,14 @@
     </row>
     <row r="251" spans="1:9" ht="19" customHeight="1">
       <c r="A251" s="19" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B251" s="20"/>
       <c r="C251" s="20" t="s">
-        <v>522</v>
-      </c>
-      <c r="D251" s="21" t="s">
-        <v>688</v>
+        <v>520</v>
+      </c>
+      <c r="D251" s="22" t="s">
+        <v>687</v>
       </c>
       <c r="E251" s="20"/>
       <c r="F251" s="20"/>
@@ -16865,14 +16971,14 @@
     </row>
     <row r="252" spans="1:9" ht="19" customHeight="1">
       <c r="A252" s="19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B252" s="20"/>
       <c r="C252" s="20" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D252" s="20" t="s">
-        <v>1137</v>
+        <v>522</v>
+      </c>
+      <c r="D252" s="21" t="s">
+        <v>688</v>
       </c>
       <c r="E252" s="20"/>
       <c r="F252" s="20"/>
@@ -16882,14 +16988,14 @@
     </row>
     <row r="253" spans="1:9" ht="19" customHeight="1">
       <c r="A253" s="19" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B253" s="20"/>
       <c r="C253" s="20" t="s">
-        <v>525</v>
+        <v>1136</v>
       </c>
       <c r="D253" s="20" t="s">
-        <v>689</v>
+        <v>1137</v>
       </c>
       <c r="E253" s="20"/>
       <c r="F253" s="20"/>
@@ -16899,14 +17005,14 @@
     </row>
     <row r="254" spans="1:9" ht="19" customHeight="1">
       <c r="A254" s="19" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B254" s="20"/>
       <c r="C254" s="20" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D254" s="20" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E254" s="20"/>
       <c r="F254" s="20"/>
@@ -16916,14 +17022,14 @@
     </row>
     <row r="255" spans="1:9" ht="19" customHeight="1">
       <c r="A255" s="19" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B255" s="20"/>
       <c r="C255" s="20" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D255" s="20" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E255" s="20"/>
       <c r="F255" s="20"/>
@@ -16933,14 +17039,14 @@
     </row>
     <row r="256" spans="1:9" ht="19" customHeight="1">
       <c r="A256" s="19" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B256" s="20"/>
       <c r="C256" s="20" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D256" s="20" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E256" s="20"/>
       <c r="F256" s="20"/>
@@ -16950,14 +17056,14 @@
     </row>
     <row r="257" spans="1:9" ht="19" customHeight="1">
       <c r="A257" s="19" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B257" s="20"/>
       <c r="C257" s="20" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D257" s="20" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E257" s="20"/>
       <c r="F257" s="20"/>
@@ -16967,14 +17073,14 @@
     </row>
     <row r="258" spans="1:9" ht="19" customHeight="1">
       <c r="A258" s="19" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B258" s="20"/>
       <c r="C258" s="20" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D258" s="20" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E258" s="20"/>
       <c r="F258" s="20"/>
@@ -16984,14 +17090,14 @@
     </row>
     <row r="259" spans="1:9" ht="19" customHeight="1">
       <c r="A259" s="19" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B259" s="20"/>
       <c r="C259" s="20" t="s">
-        <v>537</v>
-      </c>
-      <c r="D259" s="21" t="s">
-        <v>695</v>
+        <v>535</v>
+      </c>
+      <c r="D259" s="20" t="s">
+        <v>694</v>
       </c>
       <c r="E259" s="20"/>
       <c r="F259" s="20"/>
@@ -17001,14 +17107,14 @@
     </row>
     <row r="260" spans="1:9" ht="19" customHeight="1">
       <c r="A260" s="19" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B260" s="20"/>
       <c r="C260" s="20" t="s">
-        <v>539</v>
-      </c>
-      <c r="D260" s="20" t="s">
-        <v>696</v>
+        <v>537</v>
+      </c>
+      <c r="D260" s="21" t="s">
+        <v>695</v>
       </c>
       <c r="E260" s="20"/>
       <c r="F260" s="20"/>
@@ -17018,14 +17124,14 @@
     </row>
     <row r="261" spans="1:9" ht="19" customHeight="1">
       <c r="A261" s="19" t="s">
-        <v>1017</v>
+        <v>538</v>
       </c>
       <c r="B261" s="20"/>
       <c r="C261" s="20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D261" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E261" s="20"/>
       <c r="F261" s="20"/>
@@ -17035,14 +17141,14 @@
     </row>
     <row r="262" spans="1:9" ht="19" customHeight="1">
       <c r="A262" s="19" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B262" s="20"/>
       <c r="C262" s="20" t="s">
-        <v>541</v>
-      </c>
-      <c r="D262" s="21" t="s">
-        <v>698</v>
+        <v>540</v>
+      </c>
+      <c r="D262" s="20" t="s">
+        <v>697</v>
       </c>
       <c r="E262" s="20"/>
       <c r="F262" s="20"/>
@@ -17052,14 +17158,14 @@
     </row>
     <row r="263" spans="1:9" ht="19" customHeight="1">
       <c r="A263" s="19" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B263" s="20"/>
       <c r="C263" s="20" t="s">
-        <v>1020</v>
+        <v>541</v>
       </c>
       <c r="D263" s="21" t="s">
-        <v>1021</v>
+        <v>698</v>
       </c>
       <c r="E263" s="20"/>
       <c r="F263" s="20"/>
@@ -17069,14 +17175,14 @@
     </row>
     <row r="264" spans="1:9" ht="19" customHeight="1">
       <c r="A264" s="19" t="s">
-        <v>542</v>
+        <v>1019</v>
       </c>
       <c r="B264" s="20"/>
       <c r="C264" s="20" t="s">
-        <v>543</v>
-      </c>
-      <c r="D264" s="20" t="s">
-        <v>699</v>
+        <v>1020</v>
+      </c>
+      <c r="D264" s="21" t="s">
+        <v>1021</v>
       </c>
       <c r="E264" s="20"/>
       <c r="F264" s="20"/>
@@ -17086,14 +17192,14 @@
     </row>
     <row r="265" spans="1:9" ht="19" customHeight="1">
       <c r="A265" s="19" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B265" s="20"/>
       <c r="C265" s="20" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D265" s="20" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E265" s="20"/>
       <c r="F265" s="20"/>
@@ -17103,14 +17209,14 @@
     </row>
     <row r="266" spans="1:9" ht="19" customHeight="1">
       <c r="A266" s="19" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B266" s="20"/>
       <c r="C266" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="D266" s="21" t="s">
-        <v>701</v>
+        <v>545</v>
+      </c>
+      <c r="D266" s="20" t="s">
+        <v>700</v>
       </c>
       <c r="E266" s="20"/>
       <c r="F266" s="20"/>
@@ -17120,14 +17226,14 @@
     </row>
     <row r="267" spans="1:9" ht="19" customHeight="1">
       <c r="A267" s="19" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B267" s="20"/>
       <c r="C267" s="20" t="s">
-        <v>549</v>
-      </c>
-      <c r="D267" s="20" t="s">
-        <v>702</v>
+        <v>547</v>
+      </c>
+      <c r="D267" s="21" t="s">
+        <v>701</v>
       </c>
       <c r="E267" s="20"/>
       <c r="F267" s="20"/>
@@ -17137,14 +17243,14 @@
     </row>
     <row r="268" spans="1:9" ht="19" customHeight="1">
       <c r="A268" s="19" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B268" s="20"/>
       <c r="C268" s="20" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D268" s="20" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E268" s="20"/>
       <c r="F268" s="20"/>
@@ -17154,14 +17260,14 @@
     </row>
     <row r="269" spans="1:9" ht="19" customHeight="1">
       <c r="A269" s="19" t="s">
-        <v>1156</v>
+        <v>550</v>
       </c>
       <c r="B269" s="20"/>
       <c r="C269" s="20" t="s">
-        <v>1155</v>
+        <v>551</v>
       </c>
       <c r="D269" s="20" t="s">
-        <v>1154</v>
+        <v>703</v>
       </c>
       <c r="E269" s="20"/>
       <c r="F269" s="20"/>
@@ -17171,14 +17277,14 @@
     </row>
     <row r="270" spans="1:9" ht="19" customHeight="1">
       <c r="A270" s="19" t="s">
-        <v>552</v>
+        <v>1156</v>
       </c>
       <c r="B270" s="20"/>
       <c r="C270" s="20" t="s">
-        <v>553</v>
+        <v>1155</v>
       </c>
       <c r="D270" s="20" t="s">
-        <v>704</v>
+        <v>1154</v>
       </c>
       <c r="E270" s="20"/>
       <c r="F270" s="20"/>
@@ -17188,14 +17294,14 @@
     </row>
     <row r="271" spans="1:9" ht="19" customHeight="1">
       <c r="A271" s="19" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B271" s="20"/>
       <c r="C271" s="20" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D271" s="20" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E271" s="20"/>
       <c r="F271" s="20"/>
@@ -17205,14 +17311,14 @@
     </row>
     <row r="272" spans="1:9" ht="19" customHeight="1">
       <c r="A272" s="19" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B272" s="20"/>
       <c r="C272" s="20" t="s">
-        <v>557</v>
-      </c>
-      <c r="D272" s="21" t="s">
-        <v>706</v>
+        <v>555</v>
+      </c>
+      <c r="D272" s="20" t="s">
+        <v>705</v>
       </c>
       <c r="E272" s="20"/>
       <c r="F272" s="20"/>
@@ -17222,14 +17328,14 @@
     </row>
     <row r="273" spans="1:9" ht="19" customHeight="1">
       <c r="A273" s="19" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B273" s="20"/>
       <c r="C273" s="20" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D273" s="21" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E273" s="20"/>
       <c r="F273" s="20"/>
@@ -17239,14 +17345,14 @@
     </row>
     <row r="274" spans="1:9" ht="19" customHeight="1">
       <c r="A274" s="19" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B274" s="20"/>
       <c r="C274" s="20" t="s">
-        <v>561</v>
-      </c>
-      <c r="D274" s="20" t="s">
-        <v>708</v>
+        <v>559</v>
+      </c>
+      <c r="D274" s="21" t="s">
+        <v>707</v>
       </c>
       <c r="E274" s="20"/>
       <c r="F274" s="20"/>
@@ -17256,14 +17362,14 @@
     </row>
     <row r="275" spans="1:9" ht="19" customHeight="1">
       <c r="A275" s="19" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B275" s="20"/>
       <c r="C275" s="20" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D275" s="20" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E275" s="20"/>
       <c r="F275" s="20"/>
@@ -17273,14 +17379,14 @@
     </row>
     <row r="276" spans="1:9" ht="19" customHeight="1">
       <c r="A276" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B276" s="20"/>
       <c r="C276" s="20" t="s">
-        <v>1163</v>
+        <v>563</v>
       </c>
       <c r="D276" s="20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E276" s="20"/>
       <c r="F276" s="20"/>
@@ -17290,14 +17396,14 @@
     </row>
     <row r="277" spans="1:9" ht="19" customHeight="1">
       <c r="A277" s="19" t="s">
-        <v>1099</v>
+        <v>564</v>
       </c>
       <c r="B277" s="20"/>
       <c r="C277" s="20" t="s">
-        <v>1103</v>
+        <v>1163</v>
       </c>
       <c r="D277" s="20" t="s">
-        <v>1104</v>
+        <v>710</v>
       </c>
       <c r="E277" s="20"/>
       <c r="F277" s="20"/>
@@ -17307,14 +17413,14 @@
     </row>
     <row r="278" spans="1:9" ht="19" customHeight="1">
       <c r="A278" s="19" t="s">
-        <v>1112</v>
+        <v>1099</v>
       </c>
       <c r="B278" s="20"/>
       <c r="C278" s="20" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D278" s="22" t="s">
-        <v>1121</v>
+        <v>1103</v>
+      </c>
+      <c r="D278" s="20" t="s">
+        <v>1104</v>
       </c>
       <c r="E278" s="20"/>
       <c r="F278" s="20"/>
@@ -17324,14 +17430,14 @@
     </row>
     <row r="279" spans="1:9" ht="19" customHeight="1">
       <c r="A279" s="19" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B279" s="20"/>
       <c r="C279" s="20" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="D279" s="22" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="E279" s="20"/>
       <c r="F279" s="20"/>
@@ -17341,14 +17447,14 @@
     </row>
     <row r="280" spans="1:9" ht="19" customHeight="1">
       <c r="A280" s="19" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B280" s="20"/>
       <c r="C280" s="20" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D280" s="22" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="E280" s="20"/>
       <c r="F280" s="20"/>
@@ -17358,14 +17464,14 @@
     </row>
     <row r="281" spans="1:9" ht="19" customHeight="1">
       <c r="A281" s="19" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B281" s="20"/>
       <c r="C281" s="20" t="s">
-        <v>1161</v>
+        <v>1116</v>
       </c>
       <c r="D281" s="22" t="s">
-        <v>1162</v>
+        <v>1117</v>
       </c>
       <c r="E281" s="20"/>
       <c r="F281" s="20"/>
@@ -17375,14 +17481,14 @@
     </row>
     <row r="282" spans="1:9" ht="19" customHeight="1">
       <c r="A282" s="19" t="s">
-        <v>904</v>
+        <v>1115</v>
       </c>
       <c r="B282" s="20"/>
       <c r="C282" s="20" t="s">
-        <v>906</v>
-      </c>
-      <c r="D282" s="20" t="s">
-        <v>905</v>
+        <v>1161</v>
+      </c>
+      <c r="D282" s="22" t="s">
+        <v>1162</v>
       </c>
       <c r="E282" s="20"/>
       <c r="F282" s="20"/>
@@ -17392,14 +17498,14 @@
     </row>
     <row r="283" spans="1:9" ht="19" customHeight="1">
       <c r="A283" s="19" t="s">
-        <v>565</v>
+        <v>904</v>
       </c>
       <c r="B283" s="20"/>
       <c r="C283" s="20" t="s">
-        <v>566</v>
-      </c>
-      <c r="D283" s="21" t="s">
-        <v>711</v>
+        <v>906</v>
+      </c>
+      <c r="D283" s="20" t="s">
+        <v>905</v>
       </c>
       <c r="E283" s="20"/>
       <c r="F283" s="20"/>
@@ -17409,14 +17515,14 @@
     </row>
     <row r="284" spans="1:9" ht="19" customHeight="1">
       <c r="A284" s="19" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B284" s="20"/>
       <c r="C284" s="20" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D284" s="21" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E284" s="20"/>
       <c r="F284" s="20"/>
@@ -17426,14 +17532,14 @@
     </row>
     <row r="285" spans="1:9" ht="19" customHeight="1">
       <c r="A285" s="19" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B285" s="20"/>
       <c r="C285" s="20" t="s">
-        <v>570</v>
-      </c>
-      <c r="D285" s="20" t="s">
-        <v>713</v>
+        <v>568</v>
+      </c>
+      <c r="D285" s="21" t="s">
+        <v>712</v>
       </c>
       <c r="E285" s="20"/>
       <c r="F285" s="20"/>
@@ -17443,14 +17549,14 @@
     </row>
     <row r="286" spans="1:9" ht="19" customHeight="1">
       <c r="A286" s="19" t="s">
-        <v>1100</v>
+        <v>569</v>
       </c>
       <c r="B286" s="20"/>
       <c r="C286" s="20" t="s">
-        <v>1122</v>
+        <v>570</v>
       </c>
       <c r="D286" s="20" t="s">
-        <v>1123</v>
+        <v>713</v>
       </c>
       <c r="E286" s="20"/>
       <c r="F286" s="20"/>
@@ -17460,14 +17566,14 @@
     </row>
     <row r="287" spans="1:9" ht="19" customHeight="1">
       <c r="A287" s="19" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B287" s="20"/>
       <c r="C287" s="20" t="s">
-        <v>1102</v>
+        <v>1122</v>
       </c>
       <c r="D287" s="20" t="s">
-        <v>1108</v>
+        <v>1123</v>
       </c>
       <c r="E287" s="20"/>
       <c r="F287" s="20"/>
@@ -17477,14 +17583,14 @@
     </row>
     <row r="288" spans="1:9" ht="19" customHeight="1">
       <c r="A288" s="19" t="s">
-        <v>1109</v>
+        <v>1101</v>
       </c>
       <c r="B288" s="20"/>
       <c r="C288" s="20" t="s">
-        <v>1110</v>
+        <v>1102</v>
       </c>
       <c r="D288" s="20" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="E288" s="20"/>
       <c r="F288" s="20"/>
@@ -17494,14 +17600,14 @@
     </row>
     <row r="289" spans="1:9" ht="19" customHeight="1">
       <c r="A289" s="19" t="s">
-        <v>573</v>
+        <v>1109</v>
       </c>
       <c r="B289" s="20"/>
       <c r="C289" s="20" t="s">
-        <v>574</v>
+        <v>1110</v>
       </c>
       <c r="D289" s="20" t="s">
-        <v>715</v>
+        <v>1111</v>
       </c>
       <c r="E289" s="20"/>
       <c r="F289" s="20"/>
@@ -17511,14 +17617,14 @@
     </row>
     <row r="290" spans="1:9" ht="19" customHeight="1">
       <c r="A290" s="19" t="s">
-        <v>1022</v>
+        <v>573</v>
       </c>
       <c r="B290" s="20"/>
       <c r="C290" s="20" t="s">
-        <v>1023</v>
+        <v>574</v>
       </c>
       <c r="D290" s="20" t="s">
-        <v>1164</v>
+        <v>715</v>
       </c>
       <c r="E290" s="20"/>
       <c r="F290" s="20"/>
@@ -17528,14 +17634,14 @@
     </row>
     <row r="291" spans="1:9" ht="19" customHeight="1">
       <c r="A291" s="19" t="s">
-        <v>571</v>
+        <v>1022</v>
       </c>
       <c r="B291" s="20"/>
       <c r="C291" s="20" t="s">
-        <v>572</v>
+        <v>1023</v>
       </c>
       <c r="D291" s="20" t="s">
-        <v>714</v>
+        <v>1164</v>
       </c>
       <c r="E291" s="20"/>
       <c r="F291" s="20"/>
@@ -17545,14 +17651,14 @@
     </row>
     <row r="292" spans="1:9" ht="19" customHeight="1">
       <c r="A292" s="19" t="s">
-        <v>1105</v>
+        <v>571</v>
       </c>
       <c r="B292" s="20"/>
       <c r="C292" s="20" t="s">
-        <v>1107</v>
+        <v>572</v>
       </c>
       <c r="D292" s="20" t="s">
-        <v>1106</v>
+        <v>714</v>
       </c>
       <c r="E292" s="20"/>
       <c r="F292" s="20"/>
@@ -17562,14 +17668,14 @@
     </row>
     <row r="293" spans="1:9" ht="19" customHeight="1">
       <c r="A293" s="19" t="s">
-        <v>575</v>
+        <v>1105</v>
       </c>
       <c r="B293" s="20"/>
       <c r="C293" s="20" t="s">
-        <v>576</v>
+        <v>1107</v>
       </c>
       <c r="D293" s="20" t="s">
-        <v>716</v>
+        <v>1106</v>
       </c>
       <c r="E293" s="20"/>
       <c r="F293" s="20"/>
@@ -17579,14 +17685,14 @@
     </row>
     <row r="294" spans="1:9" ht="19" customHeight="1">
       <c r="A294" s="19" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B294" s="20"/>
       <c r="C294" s="20" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E294" s="20"/>
       <c r="F294" s="20"/>
@@ -17596,14 +17702,14 @@
     </row>
     <row r="295" spans="1:9" ht="19" customHeight="1">
       <c r="A295" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B295" s="20"/>
       <c r="C295" s="20" t="s">
-        <v>580</v>
-      </c>
-      <c r="D295" s="21" t="s">
-        <v>718</v>
+        <v>578</v>
+      </c>
+      <c r="D295" s="20" t="s">
+        <v>717</v>
       </c>
       <c r="E295" s="20"/>
       <c r="F295" s="20"/>
@@ -17613,14 +17719,14 @@
     </row>
     <row r="296" spans="1:9" ht="19" customHeight="1">
       <c r="A296" s="19" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B296" s="20"/>
       <c r="C296" s="20" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D296" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E296" s="20"/>
       <c r="F296" s="20"/>
@@ -17630,14 +17736,14 @@
     </row>
     <row r="297" spans="1:9" ht="19" customHeight="1">
       <c r="A297" s="19" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B297" s="20"/>
       <c r="C297" s="20" t="s">
-        <v>584</v>
-      </c>
-      <c r="D297" s="20" t="s">
-        <v>720</v>
+        <v>582</v>
+      </c>
+      <c r="D297" s="21" t="s">
+        <v>719</v>
       </c>
       <c r="E297" s="20"/>
       <c r="F297" s="20"/>
@@ -17647,14 +17753,14 @@
     </row>
     <row r="298" spans="1:9" ht="19" customHeight="1">
       <c r="A298" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B298" s="20"/>
       <c r="C298" s="20" t="s">
-        <v>586</v>
-      </c>
-      <c r="D298" s="21" t="s">
-        <v>721</v>
+        <v>584</v>
+      </c>
+      <c r="D298" s="20" t="s">
+        <v>720</v>
       </c>
       <c r="E298" s="20"/>
       <c r="F298" s="20"/>
@@ -17664,14 +17770,14 @@
     </row>
     <row r="299" spans="1:9" ht="19" customHeight="1">
       <c r="A299" s="19" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B299" s="20"/>
       <c r="C299" s="20" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D299" s="21" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E299" s="20"/>
       <c r="F299" s="20"/>
@@ -17681,14 +17787,14 @@
     </row>
     <row r="300" spans="1:9" ht="19" customHeight="1">
       <c r="A300" s="19" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B300" s="20"/>
       <c r="C300" s="20" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D300" s="21" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E300" s="20"/>
       <c r="F300" s="20"/>
@@ -17698,14 +17804,14 @@
     </row>
     <row r="301" spans="1:9" ht="19" customHeight="1">
       <c r="A301" s="19" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B301" s="20"/>
       <c r="C301" s="20" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D301" s="21" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E301" s="20"/>
       <c r="F301" s="20"/>
@@ -17715,14 +17821,14 @@
     </row>
     <row r="302" spans="1:9" ht="19" customHeight="1">
       <c r="A302" s="19" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B302" s="20"/>
       <c r="C302" s="20" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D302" s="21" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E302" s="20"/>
       <c r="F302" s="20"/>
@@ -17732,14 +17838,14 @@
     </row>
     <row r="303" spans="1:9" ht="19" customHeight="1">
       <c r="A303" s="19" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B303" s="20"/>
       <c r="C303" s="20" t="s">
-        <v>596</v>
-      </c>
-      <c r="D303" s="20" t="s">
-        <v>726</v>
+        <v>594</v>
+      </c>
+      <c r="D303" s="21" t="s">
+        <v>725</v>
       </c>
       <c r="E303" s="20"/>
       <c r="F303" s="20"/>
@@ -17749,14 +17855,14 @@
     </row>
     <row r="304" spans="1:9" ht="19" customHeight="1">
       <c r="A304" s="19" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B304" s="20"/>
       <c r="C304" s="20" t="s">
-        <v>598</v>
-      </c>
-      <c r="D304" s="21" t="s">
-        <v>727</v>
+        <v>596</v>
+      </c>
+      <c r="D304" s="20" t="s">
+        <v>726</v>
       </c>
       <c r="E304" s="20"/>
       <c r="F304" s="20"/>
@@ -17766,14 +17872,14 @@
     </row>
     <row r="305" spans="1:9" ht="19" customHeight="1">
       <c r="A305" s="19" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B305" s="20"/>
       <c r="C305" s="20" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D305" s="21" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E305" s="20"/>
       <c r="F305" s="20"/>
@@ -17783,14 +17889,14 @@
     </row>
     <row r="306" spans="1:9" ht="19" customHeight="1">
       <c r="A306" s="19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B306" s="20"/>
       <c r="C306" s="20" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D306" s="21" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E306" s="20"/>
       <c r="F306" s="20"/>
@@ -17800,14 +17906,14 @@
     </row>
     <row r="307" spans="1:9" ht="19" customHeight="1">
       <c r="A307" s="19" t="s">
-        <v>1014</v>
+        <v>601</v>
       </c>
       <c r="B307" s="20"/>
       <c r="C307" s="20" t="s">
-        <v>1015</v>
-      </c>
-      <c r="D307" s="20" t="s">
-        <v>1016</v>
+        <v>602</v>
+      </c>
+      <c r="D307" s="21" t="s">
+        <v>729</v>
       </c>
       <c r="E307" s="20"/>
       <c r="F307" s="20"/>
@@ -17817,14 +17923,14 @@
     </row>
     <row r="308" spans="1:9" ht="19" customHeight="1">
       <c r="A308" s="19" t="s">
-        <v>603</v>
+        <v>1014</v>
       </c>
       <c r="B308" s="20"/>
       <c r="C308" s="20" t="s">
-        <v>604</v>
-      </c>
-      <c r="D308" s="21" t="s">
-        <v>730</v>
+        <v>1015</v>
+      </c>
+      <c r="D308" s="20" t="s">
+        <v>1016</v>
       </c>
       <c r="E308" s="20"/>
       <c r="F308" s="20"/>
@@ -17834,14 +17940,14 @@
     </row>
     <row r="309" spans="1:9" ht="19" customHeight="1">
       <c r="A309" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B309" s="20"/>
       <c r="C309" s="20" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D309" s="21" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E309" s="20"/>
       <c r="F309" s="20"/>
@@ -17851,14 +17957,14 @@
     </row>
     <row r="310" spans="1:9" ht="19" customHeight="1">
       <c r="A310" s="19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B310" s="20"/>
       <c r="C310" s="20" t="s">
-        <v>608</v>
-      </c>
-      <c r="D310" s="20" t="s">
-        <v>732</v>
+        <v>606</v>
+      </c>
+      <c r="D310" s="21" t="s">
+        <v>731</v>
       </c>
       <c r="E310" s="20"/>
       <c r="F310" s="20"/>
@@ -17868,14 +17974,14 @@
     </row>
     <row r="311" spans="1:9" ht="19" customHeight="1">
       <c r="A311" s="19" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B311" s="20"/>
       <c r="C311" s="20" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D311" s="20" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E311" s="20"/>
       <c r="F311" s="20"/>
@@ -17885,14 +17991,14 @@
     </row>
     <row r="312" spans="1:9" ht="19" customHeight="1">
       <c r="A312" s="19" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B312" s="20"/>
       <c r="C312" s="20" t="s">
-        <v>612</v>
-      </c>
-      <c r="D312" s="21" t="s">
-        <v>734</v>
+        <v>610</v>
+      </c>
+      <c r="D312" s="20" t="s">
+        <v>733</v>
       </c>
       <c r="E312" s="20"/>
       <c r="F312" s="20"/>
@@ -17902,14 +18008,14 @@
     </row>
     <row r="313" spans="1:9" ht="19" customHeight="1">
       <c r="A313" s="19" t="s">
-        <v>1070</v>
+        <v>611</v>
       </c>
       <c r="B313" s="20"/>
       <c r="C313" s="20" t="s">
-        <v>1071</v>
+        <v>612</v>
       </c>
       <c r="D313" s="21" t="s">
-        <v>1072</v>
+        <v>734</v>
       </c>
       <c r="E313" s="20"/>
       <c r="F313" s="20"/>
@@ -17919,14 +18025,14 @@
     </row>
     <row r="314" spans="1:9" ht="19" customHeight="1">
       <c r="A314" s="19" t="s">
-        <v>613</v>
+        <v>1070</v>
       </c>
       <c r="B314" s="20"/>
       <c r="C314" s="20" t="s">
-        <v>614</v>
-      </c>
-      <c r="D314" s="22" t="s">
-        <v>735</v>
+        <v>1071</v>
+      </c>
+      <c r="D314" s="21" t="s">
+        <v>1072</v>
       </c>
       <c r="E314" s="20"/>
       <c r="F314" s="20"/>
@@ -17936,14 +18042,14 @@
     </row>
     <row r="315" spans="1:9" ht="19" customHeight="1">
       <c r="A315" s="19" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B315" s="20"/>
       <c r="C315" s="20" t="s">
-        <v>616</v>
-      </c>
-      <c r="D315" s="21" t="s">
-        <v>930</v>
+        <v>614</v>
+      </c>
+      <c r="D315" s="22" t="s">
+        <v>735</v>
       </c>
       <c r="E315" s="20"/>
       <c r="F315" s="20"/>
@@ -17953,14 +18059,14 @@
     </row>
     <row r="316" spans="1:9" ht="19" customHeight="1">
       <c r="A316" s="19" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B316" s="20"/>
       <c r="C316" s="20" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D316" s="21" t="s">
-        <v>736</v>
+        <v>930</v>
       </c>
       <c r="E316" s="20"/>
       <c r="F316" s="20"/>
@@ -17970,14 +18076,14 @@
     </row>
     <row r="317" spans="1:9" ht="19" customHeight="1">
       <c r="A317" s="19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B317" s="20"/>
       <c r="C317" s="20" t="s">
-        <v>620</v>
-      </c>
-      <c r="D317" s="20" t="s">
-        <v>737</v>
+        <v>618</v>
+      </c>
+      <c r="D317" s="21" t="s">
+        <v>736</v>
       </c>
       <c r="E317" s="20"/>
       <c r="F317" s="20"/>
@@ -17987,14 +18093,14 @@
     </row>
     <row r="318" spans="1:9" ht="19" customHeight="1">
       <c r="A318" s="19" t="s">
-        <v>942</v>
+        <v>619</v>
       </c>
       <c r="B318" s="20"/>
       <c r="C318" s="20" t="s">
-        <v>943</v>
+        <v>620</v>
       </c>
       <c r="D318" s="20" t="s">
-        <v>944</v>
+        <v>737</v>
       </c>
       <c r="E318" s="20"/>
       <c r="F318" s="20"/>
@@ -18004,14 +18110,14 @@
     </row>
     <row r="319" spans="1:9" ht="19" customHeight="1">
       <c r="A319" s="19" t="s">
-        <v>621</v>
+        <v>942</v>
       </c>
       <c r="B319" s="20"/>
       <c r="C319" s="20" t="s">
-        <v>622</v>
-      </c>
-      <c r="D319" s="21" t="s">
-        <v>738</v>
+        <v>943</v>
+      </c>
+      <c r="D319" s="20" t="s">
+        <v>944</v>
       </c>
       <c r="E319" s="20"/>
       <c r="F319" s="20"/>
@@ -18021,14 +18127,14 @@
     </row>
     <row r="320" spans="1:9" ht="19" customHeight="1">
       <c r="A320" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B320" s="20"/>
       <c r="C320" s="20" t="s">
-        <v>945</v>
+        <v>622</v>
       </c>
       <c r="D320" s="21" t="s">
-        <v>946</v>
+        <v>738</v>
       </c>
       <c r="E320" s="20"/>
       <c r="F320" s="20"/>
@@ -18038,14 +18144,14 @@
     </row>
     <row r="321" spans="1:9" ht="19" customHeight="1">
       <c r="A321" s="19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B321" s="20"/>
       <c r="C321" s="20" t="s">
-        <v>625</v>
+        <v>945</v>
       </c>
       <c r="D321" s="21" t="s">
-        <v>739</v>
+        <v>946</v>
       </c>
       <c r="E321" s="20"/>
       <c r="F321" s="20"/>
@@ -18055,14 +18161,14 @@
     </row>
     <row r="322" spans="1:9" ht="19" customHeight="1">
       <c r="A322" s="19" t="s">
-        <v>947</v>
+        <v>624</v>
       </c>
       <c r="B322" s="20"/>
       <c r="C322" s="20" t="s">
-        <v>948</v>
-      </c>
-      <c r="D322" s="20" t="s">
-        <v>949</v>
+        <v>625</v>
+      </c>
+      <c r="D322" s="21" t="s">
+        <v>739</v>
       </c>
       <c r="E322" s="20"/>
       <c r="F322" s="20"/>
@@ -18072,14 +18178,14 @@
     </row>
     <row r="323" spans="1:9" ht="19" customHeight="1">
       <c r="A323" s="19" t="s">
-        <v>626</v>
+        <v>947</v>
       </c>
       <c r="B323" s="20"/>
       <c r="C323" s="20" t="s">
-        <v>627</v>
-      </c>
-      <c r="D323" s="21" t="s">
-        <v>740</v>
+        <v>948</v>
+      </c>
+      <c r="D323" s="20" t="s">
+        <v>949</v>
       </c>
       <c r="E323" s="20"/>
       <c r="F323" s="20"/>
@@ -18089,14 +18195,14 @@
     </row>
     <row r="324" spans="1:9" ht="19" customHeight="1">
       <c r="A324" s="19" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B324" s="20"/>
       <c r="C324" s="20" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D324" s="21" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E324" s="20"/>
       <c r="F324" s="20"/>
@@ -18106,14 +18212,14 @@
     </row>
     <row r="325" spans="1:9" ht="19" customHeight="1">
       <c r="A325" s="19" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B325" s="20"/>
       <c r="C325" s="20" t="s">
-        <v>631</v>
-      </c>
-      <c r="D325" s="20" t="s">
-        <v>742</v>
+        <v>629</v>
+      </c>
+      <c r="D325" s="21" t="s">
+        <v>741</v>
       </c>
       <c r="E325" s="20"/>
       <c r="F325" s="20"/>
@@ -18123,14 +18229,14 @@
     </row>
     <row r="326" spans="1:9" ht="19" customHeight="1">
       <c r="A326" s="19" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B326" s="20"/>
       <c r="C326" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="D326" s="21" t="s">
-        <v>743</v>
+        <v>631</v>
+      </c>
+      <c r="D326" s="20" t="s">
+        <v>742</v>
       </c>
       <c r="E326" s="20"/>
       <c r="F326" s="20"/>
@@ -18140,14 +18246,14 @@
     </row>
     <row r="327" spans="1:9" ht="19" customHeight="1">
       <c r="A327" s="19" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B327" s="20"/>
       <c r="C327" s="20" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D327" s="21" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E327" s="20"/>
       <c r="F327" s="20"/>
@@ -18157,14 +18263,14 @@
     </row>
     <row r="328" spans="1:9" ht="19" customHeight="1">
       <c r="A328" s="19" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B328" s="20"/>
       <c r="C328" s="20" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D328" s="21" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E328" s="20"/>
       <c r="F328" s="20"/>
@@ -18174,14 +18280,14 @@
     </row>
     <row r="329" spans="1:9" ht="19" customHeight="1">
       <c r="A329" s="19" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B329" s="20"/>
       <c r="C329" s="20" t="s">
-        <v>639</v>
-      </c>
-      <c r="D329" s="22" t="s">
-        <v>746</v>
+        <v>637</v>
+      </c>
+      <c r="D329" s="21" t="s">
+        <v>745</v>
       </c>
       <c r="E329" s="20"/>
       <c r="F329" s="20"/>
@@ -18191,14 +18297,14 @@
     </row>
     <row r="330" spans="1:9" ht="19" customHeight="1">
       <c r="A330" s="19" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B330" s="20"/>
       <c r="C330" s="20" t="s">
-        <v>641</v>
-      </c>
-      <c r="D330" s="21" t="s">
-        <v>747</v>
+        <v>639</v>
+      </c>
+      <c r="D330" s="22" t="s">
+        <v>746</v>
       </c>
       <c r="E330" s="20"/>
       <c r="F330" s="20"/>
@@ -18208,14 +18314,14 @@
     </row>
     <row r="331" spans="1:9" ht="19" customHeight="1">
       <c r="A331" s="19" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B331" s="20"/>
       <c r="C331" s="20" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D331" s="21" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E331" s="20"/>
       <c r="F331" s="20"/>
@@ -18225,14 +18331,14 @@
     </row>
     <row r="332" spans="1:9" ht="19" customHeight="1">
       <c r="A332" s="19" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B332" s="20"/>
       <c r="C332" s="20" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D332" s="21" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E332" s="20"/>
       <c r="F332" s="20"/>
@@ -18242,14 +18348,14 @@
     </row>
     <row r="333" spans="1:9" ht="19" customHeight="1">
       <c r="A333" s="19" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B333" s="20"/>
       <c r="C333" s="20" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D333" s="21" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E333" s="20"/>
       <c r="F333" s="20"/>
@@ -18259,14 +18365,14 @@
     </row>
     <row r="334" spans="1:9" ht="19" customHeight="1">
       <c r="A334" s="19" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B334" s="20"/>
       <c r="C334" s="20" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D334" s="21" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E334" s="20"/>
       <c r="F334" s="20"/>
@@ -18276,14 +18382,14 @@
     </row>
     <row r="335" spans="1:9" ht="19" customHeight="1">
       <c r="A335" s="19" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B335" s="20"/>
       <c r="C335" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="D335" s="20" t="s">
-        <v>752</v>
+        <v>649</v>
+      </c>
+      <c r="D335" s="21" t="s">
+        <v>751</v>
       </c>
       <c r="E335" s="20"/>
       <c r="F335" s="20"/>
@@ -18293,14 +18399,14 @@
     </row>
     <row r="336" spans="1:9" ht="19" customHeight="1">
       <c r="A336" s="19" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B336" s="20"/>
-      <c r="C336" s="27" t="s">
-        <v>653</v>
-      </c>
-      <c r="D336" s="27" t="s">
-        <v>753</v>
+      <c r="C336" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="D336" s="20" t="s">
+        <v>752</v>
       </c>
       <c r="E336" s="20"/>
       <c r="F336" s="20"/>
@@ -18310,14 +18416,14 @@
     </row>
     <row r="337" spans="1:9" ht="19" customHeight="1">
       <c r="A337" s="19" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B337" s="20"/>
-      <c r="C337" s="20" t="s">
-        <v>655</v>
-      </c>
-      <c r="D337" s="20" t="s">
-        <v>754</v>
+      <c r="C337" s="27" t="s">
+        <v>653</v>
+      </c>
+      <c r="D337" s="27" t="s">
+        <v>753</v>
       </c>
       <c r="E337" s="20"/>
       <c r="F337" s="20"/>
@@ -18327,14 +18433,14 @@
     </row>
     <row r="338" spans="1:9" ht="19" customHeight="1">
       <c r="A338" s="19" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B338" s="20"/>
       <c r="C338" s="20" t="s">
-        <v>657</v>
-      </c>
-      <c r="D338" s="21" t="s">
-        <v>755</v>
+        <v>655</v>
+      </c>
+      <c r="D338" s="20" t="s">
+        <v>754</v>
       </c>
       <c r="E338" s="20"/>
       <c r="F338" s="20"/>
@@ -18344,14 +18450,14 @@
     </row>
     <row r="339" spans="1:9" ht="19" customHeight="1">
       <c r="A339" s="19" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B339" s="20"/>
       <c r="C339" s="20" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D339" s="21" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E339" s="20"/>
       <c r="F339" s="20"/>
@@ -18361,14 +18467,14 @@
     </row>
     <row r="340" spans="1:9" ht="19" customHeight="1">
       <c r="A340" s="19" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B340" s="20"/>
       <c r="C340" s="20" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D340" s="21" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E340" s="20"/>
       <c r="F340" s="20"/>
@@ -18378,14 +18484,14 @@
     </row>
     <row r="341" spans="1:9" ht="19" customHeight="1">
       <c r="A341" s="19" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B341" s="20"/>
       <c r="C341" s="20" t="s">
-        <v>663</v>
-      </c>
-      <c r="D341" s="20" t="s">
-        <v>758</v>
+        <v>661</v>
+      </c>
+      <c r="D341" s="21" t="s">
+        <v>757</v>
       </c>
       <c r="E341" s="20"/>
       <c r="F341" s="20"/>
@@ -18395,14 +18501,14 @@
     </row>
     <row r="342" spans="1:9" ht="19" customHeight="1">
       <c r="A342" s="19" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B342" s="20"/>
       <c r="C342" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="D342" s="22" t="s">
-        <v>759</v>
+        <v>663</v>
+      </c>
+      <c r="D342" s="20" t="s">
+        <v>758</v>
       </c>
       <c r="E342" s="20"/>
       <c r="F342" s="20"/>
@@ -18412,14 +18518,14 @@
     </row>
     <row r="343" spans="1:9" ht="19" customHeight="1">
       <c r="A343" s="19" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B343" s="20"/>
       <c r="C343" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="D343" s="20" t="s">
-        <v>760</v>
+        <v>665</v>
+      </c>
+      <c r="D343" s="22" t="s">
+        <v>759</v>
       </c>
       <c r="E343" s="20"/>
       <c r="F343" s="20"/>
@@ -18429,14 +18535,14 @@
     </row>
     <row r="344" spans="1:9" ht="19" customHeight="1">
       <c r="A344" s="19" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B344" s="20"/>
       <c r="C344" s="20" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D344" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E344" s="20"/>
       <c r="F344" s="20"/>
@@ -18446,14 +18552,14 @@
     </row>
     <row r="345" spans="1:9" ht="19" customHeight="1">
       <c r="A345" s="19" t="s">
-        <v>939</v>
+        <v>668</v>
       </c>
       <c r="B345" s="20"/>
       <c r="C345" s="20" t="s">
-        <v>940</v>
+        <v>669</v>
       </c>
       <c r="D345" s="20" t="s">
-        <v>941</v>
+        <v>761</v>
       </c>
       <c r="E345" s="20"/>
       <c r="F345" s="20"/>
@@ -18463,14 +18569,14 @@
     </row>
     <row r="346" spans="1:9" ht="19" customHeight="1">
       <c r="A346" s="19" t="s">
-        <v>1062</v>
+        <v>939</v>
       </c>
       <c r="B346" s="20"/>
       <c r="C346" s="20" t="s">
-        <v>1063</v>
+        <v>940</v>
       </c>
       <c r="D346" s="20" t="s">
-        <v>1064</v>
+        <v>941</v>
       </c>
       <c r="E346" s="20"/>
       <c r="F346" s="20"/>
@@ -18480,14 +18586,14 @@
     </row>
     <row r="347" spans="1:9" ht="19" customHeight="1">
       <c r="A347" s="19" t="s">
-        <v>1130</v>
+        <v>1062</v>
       </c>
       <c r="B347" s="20"/>
       <c r="C347" s="20" t="s">
-        <v>1131</v>
+        <v>1063</v>
       </c>
       <c r="D347" s="20" t="s">
-        <v>1132</v>
+        <v>1064</v>
       </c>
       <c r="E347" s="20"/>
       <c r="F347" s="20"/>
@@ -18497,14 +18603,14 @@
     </row>
     <row r="348" spans="1:9" ht="19" customHeight="1">
       <c r="A348" s="19" t="s">
-        <v>1124</v>
+        <v>1130</v>
       </c>
       <c r="B348" s="20"/>
       <c r="C348" s="20" t="s">
-        <v>1125</v>
+        <v>1131</v>
       </c>
       <c r="D348" s="20" t="s">
-        <v>1126</v>
+        <v>1132</v>
       </c>
       <c r="E348" s="20"/>
       <c r="F348" s="20"/>
@@ -18514,14 +18620,14 @@
     </row>
     <row r="349" spans="1:9" ht="19" customHeight="1">
       <c r="A349" s="19" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="B349" s="20"/>
       <c r="C349" s="20" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="D349" s="20" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="E349" s="20"/>
       <c r="F349" s="20"/>
@@ -18531,14 +18637,14 @@
     </row>
     <row r="350" spans="1:9" ht="19" customHeight="1">
       <c r="A350" s="19" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="B350" s="20"/>
       <c r="C350" s="20" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="D350" s="20" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="E350" s="20"/>
       <c r="F350" s="20"/>
@@ -18548,14 +18654,14 @@
     </row>
     <row r="351" spans="1:9" ht="19" customHeight="1">
       <c r="A351" s="19" t="s">
-        <v>1145</v>
+        <v>1133</v>
       </c>
       <c r="B351" s="20"/>
       <c r="C351" s="20" t="s">
-        <v>1147</v>
+        <v>1134</v>
       </c>
       <c r="D351" s="20" t="s">
-        <v>1146</v>
+        <v>1135</v>
       </c>
       <c r="E351" s="20"/>
       <c r="F351" s="20"/>
@@ -18565,14 +18671,14 @@
     </row>
     <row r="352" spans="1:9" ht="19" customHeight="1">
       <c r="A352" s="19" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="B352" s="20"/>
       <c r="C352" s="20" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="D352" s="20" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="E352" s="20"/>
       <c r="F352" s="20"/>
@@ -18582,14 +18688,14 @@
     </row>
     <row r="353" spans="1:9" ht="19" customHeight="1">
       <c r="A353" s="19" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="B353" s="20"/>
       <c r="C353" s="20" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="D353" s="20" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="E353" s="20"/>
       <c r="F353" s="20"/>
@@ -18599,14 +18705,14 @@
     </row>
     <row r="354" spans="1:9" ht="19" customHeight="1">
       <c r="A354" s="19" t="s">
-        <v>1184</v>
+        <v>1151</v>
       </c>
       <c r="B354" s="20"/>
       <c r="C354" s="20" t="s">
-        <v>1186</v>
+        <v>1152</v>
       </c>
       <c r="D354" s="20" t="s">
-        <v>1185</v>
+        <v>1153</v>
       </c>
       <c r="E354" s="20"/>
       <c r="F354" s="20"/>
@@ -18616,14 +18722,14 @@
     </row>
     <row r="355" spans="1:9" ht="19" customHeight="1">
       <c r="A355" s="19" t="s">
-        <v>1181</v>
+        <v>1184</v>
       </c>
       <c r="B355" s="20"/>
       <c r="C355" s="20" t="s">
-        <v>1182</v>
+        <v>1186</v>
       </c>
       <c r="D355" s="20" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
       <c r="E355" s="20"/>
       <c r="F355" s="20"/>
@@ -18633,14 +18739,14 @@
     </row>
     <row r="356" spans="1:9" ht="19" customHeight="1">
       <c r="A356" s="19" t="s">
-        <v>1272</v>
+        <v>1181</v>
       </c>
       <c r="B356" s="20"/>
       <c r="C356" s="20" t="s">
-        <v>1273</v>
+        <v>1182</v>
       </c>
       <c r="D356" s="20" t="s">
-        <v>1274</v>
+        <v>1183</v>
       </c>
       <c r="E356" s="20"/>
       <c r="F356" s="20"/>
@@ -18650,14 +18756,14 @@
     </row>
     <row r="357" spans="1:9" ht="19" customHeight="1">
       <c r="A357" s="19" t="s">
-        <v>1406</v>
+        <v>1272</v>
       </c>
       <c r="B357" s="20"/>
       <c r="C357" s="20" t="s">
-        <v>1407</v>
+        <v>1273</v>
       </c>
       <c r="D357" s="20" t="s">
-        <v>1408</v>
+        <v>1274</v>
       </c>
       <c r="E357" s="20"/>
       <c r="F357" s="20"/>
@@ -18667,14 +18773,14 @@
     </row>
     <row r="358" spans="1:9" ht="19" customHeight="1">
       <c r="A358" s="19" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="B358" s="20"/>
       <c r="C358" s="20" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="D358" s="20" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="E358" s="20"/>
       <c r="F358" s="20"/>
@@ -18683,10 +18789,16 @@
       <c r="I358" s="18"/>
     </row>
     <row r="359" spans="1:9" ht="19" customHeight="1">
-      <c r="A359" s="19"/>
+      <c r="A359" s="19" t="s">
+        <v>1409</v>
+      </c>
       <c r="B359" s="20"/>
-      <c r="C359" s="20"/>
-      <c r="D359" s="20"/>
+      <c r="C359" s="20" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D359" s="20" t="s">
+        <v>1411</v>
+      </c>
       <c r="E359" s="20"/>
       <c r="F359" s="20"/>
       <c r="G359" s="18"/>
@@ -18738,45 +18850,39 @@
       <c r="I363" s="18"/>
     </row>
     <row r="364" spans="1:9" ht="19" customHeight="1">
-      <c r="A364" s="26" t="s">
+      <c r="A364" s="19"/>
+      <c r="B364" s="20"/>
+      <c r="C364" s="20"/>
+      <c r="D364" s="20"/>
+      <c r="E364" s="20"/>
+      <c r="F364" s="20"/>
+      <c r="G364" s="18"/>
+      <c r="H364" s="17"/>
+      <c r="I364" s="18"/>
+    </row>
+    <row r="365" spans="1:9" ht="19" customHeight="1">
+      <c r="A365" s="26" t="s">
         <v>1187</v>
       </c>
-      <c r="B364" s="23"/>
-      <c r="C364" s="23"/>
-      <c r="D364" s="23"/>
-      <c r="E364" s="23"/>
-      <c r="F364" s="23"/>
-      <c r="G364" s="24"/>
-      <c r="H364" s="25"/>
-      <c r="I364" s="24"/>
-    </row>
-    <row r="365" spans="1:9" ht="19" customHeight="1">
-      <c r="A365" s="19" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B365" s="20"/>
-      <c r="C365" s="20" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D365" s="20" t="s">
-        <v>1283</v>
-      </c>
-      <c r="E365" s="20"/>
-      <c r="F365" s="20"/>
-      <c r="G365" s="18"/>
-      <c r="H365" s="17"/>
-      <c r="I365" s="18"/>
+      <c r="B365" s="23"/>
+      <c r="C365" s="23"/>
+      <c r="D365" s="23"/>
+      <c r="E365" s="23"/>
+      <c r="F365" s="23"/>
+      <c r="G365" s="24"/>
+      <c r="H365" s="25"/>
+      <c r="I365" s="24"/>
     </row>
     <row r="366" spans="1:9" ht="19" customHeight="1">
       <c r="A366" s="19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B366" s="20"/>
       <c r="C366" s="20" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D366" s="20" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E366" s="20"/>
       <c r="F366" s="20"/>
@@ -18786,14 +18892,14 @@
     </row>
     <row r="367" spans="1:9" ht="19" customHeight="1">
       <c r="A367" s="19" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B367" s="20"/>
       <c r="C367" s="20" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D367" s="20" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="E367" s="20"/>
       <c r="F367" s="20"/>
@@ -18803,14 +18909,14 @@
     </row>
     <row r="368" spans="1:9" ht="19" customHeight="1">
       <c r="A368" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B368" s="20"/>
       <c r="C368" s="20" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D368" s="20" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E368" s="20"/>
       <c r="F368" s="20"/>
@@ -18820,14 +18926,14 @@
     </row>
     <row r="369" spans="1:9" ht="19" customHeight="1">
       <c r="A369" s="19" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B369" s="20"/>
       <c r="C369" s="20" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="D369" s="20" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E369" s="20"/>
       <c r="F369" s="20"/>
@@ -18837,14 +18943,14 @@
     </row>
     <row r="370" spans="1:9" ht="19" customHeight="1">
       <c r="A370" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B370" s="20"/>
       <c r="C370" s="20" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="D370" s="20" t="s">
-        <v>1285</v>
+        <v>1288</v>
       </c>
       <c r="E370" s="20"/>
       <c r="F370" s="20"/>
@@ -18854,14 +18960,14 @@
     </row>
     <row r="371" spans="1:9" ht="19" customHeight="1">
       <c r="A371" s="19" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B371" s="20"/>
       <c r="C371" s="20" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="D371" s="20" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="E371" s="20"/>
       <c r="F371" s="20"/>
@@ -18871,14 +18977,14 @@
     </row>
     <row r="372" spans="1:9" ht="19" customHeight="1">
       <c r="A372" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B372" s="20"/>
       <c r="C372" s="20" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D372" s="20" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="E372" s="20"/>
       <c r="F372" s="20"/>
@@ -18888,14 +18994,14 @@
     </row>
     <row r="373" spans="1:9" ht="19" customHeight="1">
       <c r="A373" s="19" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B373" s="20"/>
       <c r="C373" s="20" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D373" s="20" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="E373" s="20"/>
       <c r="F373" s="20"/>
@@ -18905,14 +19011,14 @@
     </row>
     <row r="374" spans="1:9" ht="19" customHeight="1">
       <c r="A374" s="19" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B374" s="20"/>
       <c r="C374" s="20" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D374" s="20" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E374" s="20"/>
       <c r="F374" s="20"/>
@@ -18922,14 +19028,14 @@
     </row>
     <row r="375" spans="1:9" ht="19" customHeight="1">
       <c r="A375" s="19" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B375" s="20"/>
       <c r="C375" s="20" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="D375" s="20" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="E375" s="20"/>
       <c r="F375" s="20"/>
@@ -18939,14 +19045,14 @@
     </row>
     <row r="376" spans="1:9" ht="19" customHeight="1">
       <c r="A376" s="19" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B376" s="20"/>
       <c r="C376" s="20" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D376" s="20" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="E376" s="20"/>
       <c r="F376" s="20"/>
@@ -18956,14 +19062,14 @@
     </row>
     <row r="377" spans="1:9" ht="19" customHeight="1">
       <c r="A377" s="19" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B377" s="20"/>
       <c r="C377" s="20" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="D377" s="20" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="E377" s="20"/>
       <c r="F377" s="20"/>
@@ -18973,14 +19079,14 @@
     </row>
     <row r="378" spans="1:9" ht="19" customHeight="1">
       <c r="A378" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B378" s="20"/>
       <c r="C378" s="20" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="D378" s="20" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E378" s="20"/>
       <c r="F378" s="20"/>
@@ -18990,14 +19096,14 @@
     </row>
     <row r="379" spans="1:9" ht="19" customHeight="1">
       <c r="A379" s="19" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B379" s="20"/>
       <c r="C379" s="20" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="D379" s="20" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="E379" s="20"/>
       <c r="F379" s="20"/>
@@ -19007,14 +19113,14 @@
     </row>
     <row r="380" spans="1:9" ht="19" customHeight="1">
       <c r="A380" s="19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B380" s="20"/>
       <c r="C380" s="20" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="D380" s="20" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E380" s="20"/>
       <c r="F380" s="20"/>
@@ -19024,14 +19130,14 @@
     </row>
     <row r="381" spans="1:9" ht="19" customHeight="1">
       <c r="A381" s="19" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B381" s="20"/>
       <c r="C381" s="20" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D381" s="20" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="E381" s="20"/>
       <c r="F381" s="20"/>
@@ -19041,14 +19147,14 @@
     </row>
     <row r="382" spans="1:9" ht="19" customHeight="1">
       <c r="A382" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B382" s="20"/>
       <c r="C382" s="20" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D382" s="20" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="E382" s="20"/>
       <c r="F382" s="20"/>
@@ -19058,14 +19164,14 @@
     </row>
     <row r="383" spans="1:9" ht="19" customHeight="1">
       <c r="A383" s="19" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B383" s="20"/>
       <c r="C383" s="20" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D383" s="20" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="E383" s="20"/>
       <c r="F383" s="20"/>
@@ -19075,14 +19181,14 @@
     </row>
     <row r="384" spans="1:9" ht="19" customHeight="1">
       <c r="A384" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B384" s="20"/>
       <c r="C384" s="20" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="D384" s="20" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E384" s="20"/>
       <c r="F384" s="20"/>
@@ -19092,14 +19198,14 @@
     </row>
     <row r="385" spans="1:9" ht="19" customHeight="1">
       <c r="A385" s="19" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B385" s="20"/>
       <c r="C385" s="20" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D385" s="20" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E385" s="20"/>
       <c r="F385" s="20"/>
@@ -19109,14 +19215,14 @@
     </row>
     <row r="386" spans="1:9" ht="19" customHeight="1">
       <c r="A386" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B386" s="20"/>
       <c r="C386" s="20" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D386" s="20" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="E386" s="20"/>
       <c r="F386" s="20"/>
@@ -19126,14 +19232,14 @@
     </row>
     <row r="387" spans="1:9" ht="19" customHeight="1">
       <c r="A387" s="19" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B387" s="20"/>
       <c r="C387" s="20" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D387" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="E387" s="20"/>
       <c r="F387" s="20"/>
@@ -19143,14 +19249,14 @@
     </row>
     <row r="388" spans="1:9" ht="19" customHeight="1">
       <c r="A388" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B388" s="20"/>
       <c r="C388" s="20" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="D388" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="E388" s="20"/>
       <c r="F388" s="20"/>
@@ -19160,14 +19266,14 @@
     </row>
     <row r="389" spans="1:9" ht="19" customHeight="1">
       <c r="A389" s="19" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B389" s="20"/>
-      <c r="C389" s="19" t="s">
-        <v>1356</v>
+      <c r="C389" s="20" t="s">
+        <v>1211</v>
       </c>
       <c r="D389" s="20" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="E389" s="20"/>
       <c r="F389" s="20"/>
@@ -19177,14 +19283,14 @@
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
       <c r="A390" s="19" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B390" s="20"/>
       <c r="C390" s="19" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D390" s="20" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="E390" s="20"/>
       <c r="F390" s="20"/>
@@ -19194,14 +19300,14 @@
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
       <c r="A391" s="19" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B391" s="20"/>
       <c r="C391" s="19" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="D391" s="20" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="E391" s="20"/>
       <c r="F391" s="20"/>
@@ -19211,14 +19317,14 @@
     </row>
     <row r="392" spans="1:9" ht="19" customHeight="1">
       <c r="A392" s="19" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B392" s="20"/>
       <c r="C392" s="19" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="D392" s="20" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
@@ -19228,14 +19334,14 @@
     </row>
     <row r="393" spans="1:9" ht="19" customHeight="1">
       <c r="A393" s="19" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B393" s="20"/>
       <c r="C393" s="19" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="D393" s="20" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
@@ -19245,14 +19351,14 @@
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
       <c r="A394" s="19" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B394" s="20"/>
       <c r="C394" s="19" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="D394" s="20" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="E394" s="20"/>
       <c r="F394" s="20"/>
@@ -19262,14 +19368,14 @@
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
       <c r="A395" s="19" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B395" s="20"/>
       <c r="C395" s="19" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="D395" s="20" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="E395" s="20"/>
       <c r="F395" s="20"/>
@@ -19279,14 +19385,14 @@
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
       <c r="A396" s="19" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B396" s="20"/>
       <c r="C396" s="19" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D396" s="20" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
@@ -19296,14 +19402,14 @@
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
       <c r="A397" s="19" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B397" s="20"/>
       <c r="C397" s="19" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="D397" s="20" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="E397" s="20"/>
       <c r="F397" s="20"/>
@@ -19313,14 +19419,14 @@
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="19" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -19330,14 +19436,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="19" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -19347,14 +19453,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="19" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -19364,14 +19470,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1260</v>
+        <v>1223</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="19" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -19381,11 +19487,11 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1224</v>
+        <v>1260</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="19" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="D402" s="20" t="s">
         <v>1319</v>
@@ -19398,14 +19504,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="19" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -19415,14 +19521,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="19" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -19432,14 +19538,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="19" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -19449,14 +19555,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="19" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -19466,14 +19572,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="19" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -19483,14 +19589,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1261</v>
+        <v>1229</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="19" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -19500,14 +19606,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1230</v>
+        <v>1261</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="19" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -19517,14 +19623,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="19" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -19534,14 +19640,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="19" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -19551,14 +19657,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="19" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -19568,14 +19674,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="19" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -19585,14 +19691,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="19" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -19602,14 +19708,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1254</v>
+        <v>1235</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="19" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -19619,14 +19725,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="19" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -19636,14 +19742,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="19" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -19653,14 +19759,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="19" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -19670,14 +19776,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="19" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -19687,14 +19793,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="19" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -19704,14 +19810,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1236</v>
+        <v>1259</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="19" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -19721,14 +19827,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="19" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -19738,14 +19844,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="19" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -19755,14 +19861,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="19" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -19772,14 +19878,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="19" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -19789,14 +19895,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="19" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -19806,14 +19912,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="19" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -19823,14 +19929,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="19" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -19840,14 +19946,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -19857,14 +19963,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -19874,14 +19980,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -19891,14 +19997,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -19908,14 +20014,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -19925,14 +20031,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>
@@ -19942,14 +20048,14 @@
     </row>
     <row r="435" spans="1:9" ht="19" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="19" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E435" s="20"/>
       <c r="F435" s="20"/>
@@ -19959,14 +20065,14 @@
     </row>
     <row r="436" spans="1:9" ht="19" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="19" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="D436" s="20" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="E436" s="20"/>
       <c r="F436" s="20"/>
@@ -19976,14 +20082,14 @@
     </row>
     <row r="437" spans="1:9" ht="19" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="19" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="D437" s="20" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="E437" s="20"/>
       <c r="F437" s="20"/>
@@ -19993,14 +20099,14 @@
     </row>
     <row r="438" spans="1:9" ht="19" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="19" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="D438" s="20" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="E438" s="20"/>
       <c r="F438" s="20"/>
@@ -20009,10 +20115,16 @@
       <c r="I438" s="18"/>
     </row>
     <row r="439" spans="1:9" ht="19" customHeight="1">
-      <c r="A439" s="19"/>
+      <c r="A439" s="19" t="s">
+        <v>1253</v>
+      </c>
       <c r="B439" s="20"/>
-      <c r="C439" s="20"/>
-      <c r="D439" s="20"/>
+      <c r="C439" s="19" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D439" s="20" t="s">
+        <v>1355</v>
+      </c>
       <c r="E439" s="20"/>
       <c r="F439" s="20"/>
       <c r="G439" s="18"/>
@@ -20657,80 +20769,91 @@
       <c r="H497" s="17"/>
       <c r="I497" s="18"/>
     </row>
+    <row r="498" spans="1:9" ht="19" customHeight="1">
+      <c r="A498" s="19"/>
+      <c r="B498" s="20"/>
+      <c r="C498" s="20"/>
+      <c r="D498" s="20"/>
+      <c r="E498" s="20"/>
+      <c r="F498" s="20"/>
+      <c r="G498" s="18"/>
+      <c r="H498" s="17"/>
+      <c r="I498" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J221" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A5:G235 I5:I497">
+  <conditionalFormatting sqref="A5:G236 I5:I498">
     <cfRule type="expression" dxfId="39" priority="37">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D236:D257 D260 D264:D266 D270:D274 D283 D291:D304 D308:D310 D314:D315 D317:D319 D323:D344">
+  <conditionalFormatting sqref="D237:D258 D261 D265:D267 D271:D275 D284 D292:D305 D309:D311 D315:D316 D318:D320 D324:D345">
     <cfRule type="expression" dxfId="38" priority="276">
-      <formula>$G238&lt;&gt;""</formula>
+      <formula>$G239&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D258">
+  <conditionalFormatting sqref="D259">
     <cfRule type="expression" dxfId="37" priority="315">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D259">
+  <conditionalFormatting sqref="D260">
     <cfRule type="expression" dxfId="36" priority="314">
-      <formula>$G260&lt;&gt;""</formula>
+      <formula>$G261&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D261:D263 D267:D269 D282 D305:D307 D311:D313 D320:D322">
+  <conditionalFormatting sqref="D262:D264 D268:D270 D283 D306:D308 D312:D314 D321:D323">
     <cfRule type="expression" dxfId="35" priority="279">
-      <formula>$G264&lt;&gt;""</formula>
+      <formula>$G265&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D275:D281">
+  <conditionalFormatting sqref="D276:D282">
     <cfRule type="expression" dxfId="34" priority="317">
-      <formula>$G283&lt;&gt;""</formula>
+      <formula>$G284&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D278">
+  <conditionalFormatting sqref="D279">
     <cfRule type="expression" dxfId="33" priority="351">
-      <formula>$G283&lt;&gt;""</formula>
+      <formula>$G284&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D279:D281">
+  <conditionalFormatting sqref="D280:D282">
     <cfRule type="expression" dxfId="32" priority="388">
-      <formula>$G283&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D284">
-    <cfRule type="expression" dxfId="31" priority="386">
-      <formula>$G291&lt;&gt;""</formula>
+      <formula>$G284&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D285">
-    <cfRule type="expression" dxfId="30" priority="283">
-      <formula>$G289&lt;&gt;""</formula>
+    <cfRule type="expression" dxfId="31" priority="386">
+      <formula>$G292&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D286:D288">
-    <cfRule type="expression" dxfId="29" priority="13">
-      <formula>$G286&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D286">
+    <cfRule type="expression" dxfId="30" priority="283">
+      <formula>$G290&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D289">
-    <cfRule type="expression" dxfId="28" priority="384">
-      <formula>$G294&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D287:D289">
+    <cfRule type="expression" dxfId="29" priority="13">
+      <formula>$G287&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D316">
+  <conditionalFormatting sqref="D290">
+    <cfRule type="expression" dxfId="28" priority="384">
+      <formula>$G295&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D317">
     <cfRule type="expression" dxfId="27" priority="383">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E236:G236 A236:C248 E237:E248 F237:G275 A249:E250 A251:C272 E251:E272 A273:E274 E275 A275:C307 E276:G288 E289:E307 F289:G347 D290 A308:E309 A310:C329 E310:E329 A330:E331 A332:C344 E332:E344 A345:E347 A348:G497">
+  <conditionalFormatting sqref="E237:G237 A237:C249 E238:E249 F238:G276 A250:E251 A252:C273 E252:E273 A274:E275 E276 A276:C308 E277:G289 E290:E308 F290:G348 D291 A309:E310 A311:C330 E311:E330 A331:E332 A333:C345 E333:E345 A346:E348 A349:G498">
     <cfRule type="expression" dxfId="26" priority="274">
-      <formula>$G236&lt;&gt;""</formula>
+      <formula>$G237&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H497">
+  <conditionalFormatting sqref="H5:H498">
     <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
@@ -20762,15 +20885,15 @@
       <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H364">
+  <conditionalFormatting sqref="H365">
     <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H364)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H365)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H364)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SKIP",H365)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H364)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ERROR",H365)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>

</xml_diff>

<commit_message>
Improve Spec-Report - branch functions
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75D5E1B-DA27-8241-8EBD-536818D3234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1E0753-2C8C-914F-A3CF-242C5AA6D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30220" yWindow="3120" windowWidth="37140" windowHeight="33260" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="1434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="1446">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11365,6 +11365,72 @@
   </si>
   <si>
     <t>if screen is not ${subject}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ifCanSelect</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if can select ${subject}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ifCanSelectNot</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if can not select ${subject}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ifTrue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ifFalse</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if true</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if false</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>trueの場合</t>
+    <rPh sb="5" eb="7">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>falseの場合</t>
+    <rPh sb="6" eb="8">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${subject}が存在する場合</t>
+    <rPh sb="11" eb="13">
+      <t>ソンザイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${subject}が存在しない場合</t>
+    <rPh sb="11" eb="13">
+      <t>ソンザイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>バアイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12306,11 +12372,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I498"/>
+  <dimension ref="A1:I502"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
+      <pane ySplit="4" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A227" sqref="A227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -16573,10 +16639,18 @@
       <c r="I226" s="18"/>
     </row>
     <row r="227" spans="1:9" ht="19" customHeight="1">
-      <c r="A227" s="19"/>
-      <c r="B227" s="20"/>
-      <c r="C227" s="20"/>
-      <c r="D227" s="20"/>
+      <c r="A227" s="19" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B227" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C227" s="20" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D227" s="20" t="s">
+        <v>1444</v>
+      </c>
       <c r="E227" s="20"/>
       <c r="F227" s="20"/>
       <c r="G227" s="18"/>
@@ -16584,10 +16658,18 @@
       <c r="I227" s="18"/>
     </row>
     <row r="228" spans="1:9" ht="19" customHeight="1">
-      <c r="A228" s="19"/>
-      <c r="B228" s="20"/>
-      <c r="C228" s="20"/>
-      <c r="D228" s="20"/>
+      <c r="A228" s="19" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B228" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C228" s="20" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D228" s="20" t="s">
+        <v>1445</v>
+      </c>
       <c r="E228" s="20"/>
       <c r="F228" s="20"/>
       <c r="G228" s="18"/>
@@ -16595,10 +16677,18 @@
       <c r="I228" s="18"/>
     </row>
     <row r="229" spans="1:9" ht="19" customHeight="1">
-      <c r="A229" s="19"/>
-      <c r="B229" s="20"/>
-      <c r="C229" s="20"/>
-      <c r="D229" s="20"/>
+      <c r="A229" s="19" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B229" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C229" s="20" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D229" s="20" t="s">
+        <v>1442</v>
+      </c>
       <c r="E229" s="20"/>
       <c r="F229" s="20"/>
       <c r="G229" s="18"/>
@@ -16606,10 +16696,18 @@
       <c r="I229" s="18"/>
     </row>
     <row r="230" spans="1:9" ht="19" customHeight="1">
-      <c r="A230" s="19"/>
-      <c r="B230" s="20"/>
-      <c r="C230" s="20"/>
-      <c r="D230" s="20"/>
+      <c r="A230" s="19" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B230" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="C230" s="20" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D230" s="20" t="s">
+        <v>1443</v>
+      </c>
       <c r="E230" s="20"/>
       <c r="F230" s="20"/>
       <c r="G230" s="18"/>
@@ -16617,29 +16715,21 @@
       <c r="I230" s="18"/>
     </row>
     <row r="231" spans="1:9" ht="19" customHeight="1">
-      <c r="A231" s="26" t="s">
-        <v>483</v>
-      </c>
-      <c r="B231" s="23"/>
-      <c r="C231" s="23"/>
-      <c r="D231" s="23"/>
-      <c r="E231" s="23"/>
-      <c r="F231" s="23"/>
-      <c r="G231" s="24"/>
-      <c r="H231" s="25"/>
-      <c r="I231" s="24"/>
+      <c r="A231" s="19"/>
+      <c r="B231" s="20"/>
+      <c r="C231" s="20"/>
+      <c r="D231" s="20"/>
+      <c r="E231" s="20"/>
+      <c r="F231" s="20"/>
+      <c r="G231" s="18"/>
+      <c r="H231" s="17"/>
+      <c r="I231" s="18"/>
     </row>
     <row r="232" spans="1:9" ht="19" customHeight="1">
-      <c r="A232" s="19" t="s">
-        <v>485</v>
-      </c>
+      <c r="A232" s="19"/>
       <c r="B232" s="20"/>
-      <c r="C232" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="D232" s="20" t="s">
-        <v>670</v>
-      </c>
+      <c r="C232" s="20"/>
+      <c r="D232" s="20"/>
       <c r="E232" s="20"/>
       <c r="F232" s="20"/>
       <c r="G232" s="18"/>
@@ -16647,16 +16737,10 @@
       <c r="I232" s="18"/>
     </row>
     <row r="233" spans="1:9" ht="19" customHeight="1">
-      <c r="A233" s="19" t="s">
-        <v>486</v>
-      </c>
+      <c r="A233" s="19"/>
       <c r="B233" s="20"/>
-      <c r="C233" s="20" t="s">
-        <v>486</v>
-      </c>
-      <c r="D233" s="22" t="s">
-        <v>671</v>
-      </c>
+      <c r="C233" s="20"/>
+      <c r="D233" s="20"/>
       <c r="E233" s="20"/>
       <c r="F233" s="20"/>
       <c r="G233" s="18"/>
@@ -16664,16 +16748,10 @@
       <c r="I233" s="18"/>
     </row>
     <row r="234" spans="1:9" ht="19" customHeight="1">
-      <c r="A234" s="19" t="s">
-        <v>487</v>
-      </c>
+      <c r="A234" s="19"/>
       <c r="B234" s="20"/>
-      <c r="C234" s="20" t="s">
-        <v>487</v>
-      </c>
-      <c r="D234" s="20" t="s">
-        <v>672</v>
-      </c>
+      <c r="C234" s="20"/>
+      <c r="D234" s="20"/>
       <c r="E234" s="20"/>
       <c r="F234" s="20"/>
       <c r="G234" s="18"/>
@@ -16681,32 +16759,28 @@
       <c r="I234" s="18"/>
     </row>
     <row r="235" spans="1:9" ht="19" customHeight="1">
-      <c r="A235" s="19" t="s">
-        <v>1422</v>
-      </c>
-      <c r="B235" s="20"/>
-      <c r="C235" s="20" t="s">
-        <v>1424</v>
-      </c>
-      <c r="D235" s="20" t="s">
-        <v>1423</v>
-      </c>
-      <c r="E235" s="20"/>
-      <c r="F235" s="20"/>
-      <c r="G235" s="18"/>
-      <c r="H235" s="17"/>
-      <c r="I235" s="18"/>
+      <c r="A235" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="B235" s="23"/>
+      <c r="C235" s="23"/>
+      <c r="D235" s="23"/>
+      <c r="E235" s="23"/>
+      <c r="F235" s="23"/>
+      <c r="G235" s="24"/>
+      <c r="H235" s="25"/>
+      <c r="I235" s="24"/>
     </row>
     <row r="236" spans="1:9" ht="19" customHeight="1">
       <c r="A236" s="19" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B236" s="20"/>
       <c r="C236" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="D236" s="22" t="s">
-        <v>673</v>
+        <v>485</v>
+      </c>
+      <c r="D236" s="20" t="s">
+        <v>670</v>
       </c>
       <c r="E236" s="20"/>
       <c r="F236" s="20"/>
@@ -16716,14 +16790,14 @@
     </row>
     <row r="237" spans="1:9" ht="19" customHeight="1">
       <c r="A237" s="19" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="B237" s="20"/>
       <c r="C237" s="20" t="s">
-        <v>493</v>
-      </c>
-      <c r="D237" s="21" t="s">
-        <v>674</v>
+        <v>486</v>
+      </c>
+      <c r="D237" s="22" t="s">
+        <v>671</v>
       </c>
       <c r="E237" s="20"/>
       <c r="F237" s="20"/>
@@ -16733,14 +16807,14 @@
     </row>
     <row r="238" spans="1:9" ht="19" customHeight="1">
       <c r="A238" s="19" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B238" s="20"/>
       <c r="C238" s="20" t="s">
-        <v>495</v>
-      </c>
-      <c r="D238" s="22" t="s">
-        <v>675</v>
+        <v>487</v>
+      </c>
+      <c r="D238" s="20" t="s">
+        <v>672</v>
       </c>
       <c r="E238" s="20"/>
       <c r="F238" s="20"/>
@@ -16750,14 +16824,14 @@
     </row>
     <row r="239" spans="1:9" ht="19" customHeight="1">
       <c r="A239" s="19" t="s">
-        <v>496</v>
+        <v>1422</v>
       </c>
       <c r="B239" s="20"/>
       <c r="C239" s="20" t="s">
-        <v>497</v>
-      </c>
-      <c r="D239" s="21" t="s">
-        <v>676</v>
+        <v>1424</v>
+      </c>
+      <c r="D239" s="20" t="s">
+        <v>1423</v>
       </c>
       <c r="E239" s="20"/>
       <c r="F239" s="20"/>
@@ -16767,14 +16841,14 @@
     </row>
     <row r="240" spans="1:9" ht="19" customHeight="1">
       <c r="A240" s="19" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="B240" s="20"/>
       <c r="C240" s="20" t="s">
-        <v>499</v>
-      </c>
-      <c r="D240" s="21" t="s">
-        <v>677</v>
+        <v>489</v>
+      </c>
+      <c r="D240" s="22" t="s">
+        <v>673</v>
       </c>
       <c r="E240" s="20"/>
       <c r="F240" s="20"/>
@@ -16784,14 +16858,14 @@
     </row>
     <row r="241" spans="1:9" ht="19" customHeight="1">
       <c r="A241" s="19" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B241" s="20"/>
       <c r="C241" s="20" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="D241" s="21" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="E241" s="20"/>
       <c r="F241" s="20"/>
@@ -16801,14 +16875,14 @@
     </row>
     <row r="242" spans="1:9" ht="19" customHeight="1">
       <c r="A242" s="19" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B242" s="20"/>
       <c r="C242" s="20" t="s">
-        <v>928</v>
-      </c>
-      <c r="D242" s="21" t="s">
-        <v>929</v>
+        <v>495</v>
+      </c>
+      <c r="D242" s="22" t="s">
+        <v>675</v>
       </c>
       <c r="E242" s="20"/>
       <c r="F242" s="20"/>
@@ -16818,14 +16892,14 @@
     </row>
     <row r="243" spans="1:9" ht="19" customHeight="1">
       <c r="A243" s="19" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="B243" s="20"/>
       <c r="C243" s="20" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="D243" s="21" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E243" s="20"/>
       <c r="F243" s="20"/>
@@ -16835,14 +16909,14 @@
     </row>
     <row r="244" spans="1:9" ht="19" customHeight="1">
       <c r="A244" s="19" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B244" s="20"/>
       <c r="C244" s="20" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="D244" s="21" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="E244" s="20"/>
       <c r="F244" s="20"/>
@@ -16852,14 +16926,14 @@
     </row>
     <row r="245" spans="1:9" ht="19" customHeight="1">
       <c r="A245" s="19" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="B245" s="20"/>
       <c r="C245" s="20" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D245" s="21" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E245" s="20"/>
       <c r="F245" s="20"/>
@@ -16869,14 +16943,14 @@
     </row>
     <row r="246" spans="1:9" ht="19" customHeight="1">
       <c r="A246" s="19" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="B246" s="20"/>
       <c r="C246" s="20" t="s">
-        <v>510</v>
+        <v>928</v>
       </c>
       <c r="D246" s="21" t="s">
-        <v>682</v>
+        <v>929</v>
       </c>
       <c r="E246" s="20"/>
       <c r="F246" s="20"/>
@@ -16886,14 +16960,14 @@
     </row>
     <row r="247" spans="1:9" ht="19" customHeight="1">
       <c r="A247" s="19" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="B247" s="20"/>
       <c r="C247" s="20" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="D247" s="21" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="E247" s="20"/>
       <c r="F247" s="20"/>
@@ -16903,14 +16977,14 @@
     </row>
     <row r="248" spans="1:9" ht="19" customHeight="1">
       <c r="A248" s="19" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B248" s="20"/>
       <c r="C248" s="20" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="D248" s="21" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="E248" s="20"/>
       <c r="F248" s="20"/>
@@ -16920,14 +16994,14 @@
     </row>
     <row r="249" spans="1:9" ht="19" customHeight="1">
       <c r="A249" s="19" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="B249" s="20"/>
       <c r="C249" s="20" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="D249" s="21" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="E249" s="20"/>
       <c r="F249" s="20"/>
@@ -16937,14 +17011,14 @@
     </row>
     <row r="250" spans="1:9" ht="19" customHeight="1">
       <c r="A250" s="19" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B250" s="20"/>
       <c r="C250" s="20" t="s">
-        <v>518</v>
-      </c>
-      <c r="D250" s="20" t="s">
-        <v>686</v>
+        <v>510</v>
+      </c>
+      <c r="D250" s="21" t="s">
+        <v>682</v>
       </c>
       <c r="E250" s="20"/>
       <c r="F250" s="20"/>
@@ -16954,14 +17028,14 @@
     </row>
     <row r="251" spans="1:9" ht="19" customHeight="1">
       <c r="A251" s="19" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="B251" s="20"/>
       <c r="C251" s="20" t="s">
-        <v>520</v>
-      </c>
-      <c r="D251" s="22" t="s">
-        <v>687</v>
+        <v>512</v>
+      </c>
+      <c r="D251" s="21" t="s">
+        <v>683</v>
       </c>
       <c r="E251" s="20"/>
       <c r="F251" s="20"/>
@@ -16971,14 +17045,14 @@
     </row>
     <row r="252" spans="1:9" ht="19" customHeight="1">
       <c r="A252" s="19" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B252" s="20"/>
       <c r="C252" s="20" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="D252" s="21" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="E252" s="20"/>
       <c r="F252" s="20"/>
@@ -16988,14 +17062,14 @@
     </row>
     <row r="253" spans="1:9" ht="19" customHeight="1">
       <c r="A253" s="19" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="B253" s="20"/>
       <c r="C253" s="20" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D253" s="20" t="s">
-        <v>1137</v>
+        <v>516</v>
+      </c>
+      <c r="D253" s="21" t="s">
+        <v>685</v>
       </c>
       <c r="E253" s="20"/>
       <c r="F253" s="20"/>
@@ -17005,14 +17079,14 @@
     </row>
     <row r="254" spans="1:9" ht="19" customHeight="1">
       <c r="A254" s="19" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B254" s="20"/>
       <c r="C254" s="20" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="D254" s="20" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E254" s="20"/>
       <c r="F254" s="20"/>
@@ -17022,14 +17096,14 @@
     </row>
     <row r="255" spans="1:9" ht="19" customHeight="1">
       <c r="A255" s="19" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="B255" s="20"/>
       <c r="C255" s="20" t="s">
-        <v>527</v>
-      </c>
-      <c r="D255" s="20" t="s">
-        <v>690</v>
+        <v>520</v>
+      </c>
+      <c r="D255" s="22" t="s">
+        <v>687</v>
       </c>
       <c r="E255" s="20"/>
       <c r="F255" s="20"/>
@@ -17039,14 +17113,14 @@
     </row>
     <row r="256" spans="1:9" ht="19" customHeight="1">
       <c r="A256" s="19" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="B256" s="20"/>
       <c r="C256" s="20" t="s">
-        <v>529</v>
-      </c>
-      <c r="D256" s="20" t="s">
-        <v>691</v>
+        <v>522</v>
+      </c>
+      <c r="D256" s="21" t="s">
+        <v>688</v>
       </c>
       <c r="E256" s="20"/>
       <c r="F256" s="20"/>
@@ -17056,14 +17130,14 @@
     </row>
     <row r="257" spans="1:9" ht="19" customHeight="1">
       <c r="A257" s="19" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="B257" s="20"/>
       <c r="C257" s="20" t="s">
-        <v>531</v>
+        <v>1136</v>
       </c>
       <c r="D257" s="20" t="s">
-        <v>692</v>
+        <v>1137</v>
       </c>
       <c r="E257" s="20"/>
       <c r="F257" s="20"/>
@@ -17073,14 +17147,14 @@
     </row>
     <row r="258" spans="1:9" ht="19" customHeight="1">
       <c r="A258" s="19" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="B258" s="20"/>
       <c r="C258" s="20" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="D258" s="20" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="E258" s="20"/>
       <c r="F258" s="20"/>
@@ -17090,14 +17164,14 @@
     </row>
     <row r="259" spans="1:9" ht="19" customHeight="1">
       <c r="A259" s="19" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="B259" s="20"/>
       <c r="C259" s="20" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="D259" s="20" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="E259" s="20"/>
       <c r="F259" s="20"/>
@@ -17107,14 +17181,14 @@
     </row>
     <row r="260" spans="1:9" ht="19" customHeight="1">
       <c r="A260" s="19" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="B260" s="20"/>
       <c r="C260" s="20" t="s">
-        <v>537</v>
-      </c>
-      <c r="D260" s="21" t="s">
-        <v>695</v>
+        <v>529</v>
+      </c>
+      <c r="D260" s="20" t="s">
+        <v>691</v>
       </c>
       <c r="E260" s="20"/>
       <c r="F260" s="20"/>
@@ -17124,14 +17198,14 @@
     </row>
     <row r="261" spans="1:9" ht="19" customHeight="1">
       <c r="A261" s="19" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="B261" s="20"/>
       <c r="C261" s="20" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="D261" s="20" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="E261" s="20"/>
       <c r="F261" s="20"/>
@@ -17141,14 +17215,14 @@
     </row>
     <row r="262" spans="1:9" ht="19" customHeight="1">
       <c r="A262" s="19" t="s">
-        <v>1017</v>
+        <v>532</v>
       </c>
       <c r="B262" s="20"/>
       <c r="C262" s="20" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="D262" s="20" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="E262" s="20"/>
       <c r="F262" s="20"/>
@@ -17158,14 +17232,14 @@
     </row>
     <row r="263" spans="1:9" ht="19" customHeight="1">
       <c r="A263" s="19" t="s">
-        <v>1018</v>
+        <v>534</v>
       </c>
       <c r="B263" s="20"/>
       <c r="C263" s="20" t="s">
-        <v>541</v>
-      </c>
-      <c r="D263" s="21" t="s">
-        <v>698</v>
+        <v>535</v>
+      </c>
+      <c r="D263" s="20" t="s">
+        <v>694</v>
       </c>
       <c r="E263" s="20"/>
       <c r="F263" s="20"/>
@@ -17175,14 +17249,14 @@
     </row>
     <row r="264" spans="1:9" ht="19" customHeight="1">
       <c r="A264" s="19" t="s">
-        <v>1019</v>
+        <v>536</v>
       </c>
       <c r="B264" s="20"/>
       <c r="C264" s="20" t="s">
-        <v>1020</v>
+        <v>537</v>
       </c>
       <c r="D264" s="21" t="s">
-        <v>1021</v>
+        <v>695</v>
       </c>
       <c r="E264" s="20"/>
       <c r="F264" s="20"/>
@@ -17192,14 +17266,14 @@
     </row>
     <row r="265" spans="1:9" ht="19" customHeight="1">
       <c r="A265" s="19" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B265" s="20"/>
       <c r="C265" s="20" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D265" s="20" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="E265" s="20"/>
       <c r="F265" s="20"/>
@@ -17209,14 +17283,14 @@
     </row>
     <row r="266" spans="1:9" ht="19" customHeight="1">
       <c r="A266" s="19" t="s">
-        <v>544</v>
+        <v>1017</v>
       </c>
       <c r="B266" s="20"/>
       <c r="C266" s="20" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="D266" s="20" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="E266" s="20"/>
       <c r="F266" s="20"/>
@@ -17226,14 +17300,14 @@
     </row>
     <row r="267" spans="1:9" ht="19" customHeight="1">
       <c r="A267" s="19" t="s">
-        <v>546</v>
+        <v>1018</v>
       </c>
       <c r="B267" s="20"/>
       <c r="C267" s="20" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D267" s="21" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="E267" s="20"/>
       <c r="F267" s="20"/>
@@ -17243,14 +17317,14 @@
     </row>
     <row r="268" spans="1:9" ht="19" customHeight="1">
       <c r="A268" s="19" t="s">
-        <v>548</v>
+        <v>1019</v>
       </c>
       <c r="B268" s="20"/>
       <c r="C268" s="20" t="s">
-        <v>549</v>
-      </c>
-      <c r="D268" s="20" t="s">
-        <v>702</v>
+        <v>1020</v>
+      </c>
+      <c r="D268" s="21" t="s">
+        <v>1021</v>
       </c>
       <c r="E268" s="20"/>
       <c r="F268" s="20"/>
@@ -17260,14 +17334,14 @@
     </row>
     <row r="269" spans="1:9" ht="19" customHeight="1">
       <c r="A269" s="19" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="B269" s="20"/>
       <c r="C269" s="20" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="D269" s="20" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="E269" s="20"/>
       <c r="F269" s="20"/>
@@ -17277,14 +17351,14 @@
     </row>
     <row r="270" spans="1:9" ht="19" customHeight="1">
       <c r="A270" s="19" t="s">
-        <v>1156</v>
+        <v>544</v>
       </c>
       <c r="B270" s="20"/>
       <c r="C270" s="20" t="s">
-        <v>1155</v>
+        <v>545</v>
       </c>
       <c r="D270" s="20" t="s">
-        <v>1154</v>
+        <v>700</v>
       </c>
       <c r="E270" s="20"/>
       <c r="F270" s="20"/>
@@ -17294,14 +17368,14 @@
     </row>
     <row r="271" spans="1:9" ht="19" customHeight="1">
       <c r="A271" s="19" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="B271" s="20"/>
       <c r="C271" s="20" t="s">
-        <v>553</v>
-      </c>
-      <c r="D271" s="20" t="s">
-        <v>704</v>
+        <v>547</v>
+      </c>
+      <c r="D271" s="21" t="s">
+        <v>701</v>
       </c>
       <c r="E271" s="20"/>
       <c r="F271" s="20"/>
@@ -17311,14 +17385,14 @@
     </row>
     <row r="272" spans="1:9" ht="19" customHeight="1">
       <c r="A272" s="19" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B272" s="20"/>
       <c r="C272" s="20" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="D272" s="20" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E272" s="20"/>
       <c r="F272" s="20"/>
@@ -17328,14 +17402,14 @@
     </row>
     <row r="273" spans="1:9" ht="19" customHeight="1">
       <c r="A273" s="19" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="B273" s="20"/>
       <c r="C273" s="20" t="s">
-        <v>557</v>
-      </c>
-      <c r="D273" s="21" t="s">
-        <v>706</v>
+        <v>551</v>
+      </c>
+      <c r="D273" s="20" t="s">
+        <v>703</v>
       </c>
       <c r="E273" s="20"/>
       <c r="F273" s="20"/>
@@ -17345,14 +17419,14 @@
     </row>
     <row r="274" spans="1:9" ht="19" customHeight="1">
       <c r="A274" s="19" t="s">
-        <v>558</v>
+        <v>1156</v>
       </c>
       <c r="B274" s="20"/>
       <c r="C274" s="20" t="s">
-        <v>559</v>
-      </c>
-      <c r="D274" s="21" t="s">
-        <v>707</v>
+        <v>1155</v>
+      </c>
+      <c r="D274" s="20" t="s">
+        <v>1154</v>
       </c>
       <c r="E274" s="20"/>
       <c r="F274" s="20"/>
@@ -17362,14 +17436,14 @@
     </row>
     <row r="275" spans="1:9" ht="19" customHeight="1">
       <c r="A275" s="19" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="B275" s="20"/>
       <c r="C275" s="20" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="D275" s="20" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="E275" s="20"/>
       <c r="F275" s="20"/>
@@ -17379,14 +17453,14 @@
     </row>
     <row r="276" spans="1:9" ht="19" customHeight="1">
       <c r="A276" s="19" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="B276" s="20"/>
       <c r="C276" s="20" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="D276" s="20" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="E276" s="20"/>
       <c r="F276" s="20"/>
@@ -17396,14 +17470,14 @@
     </row>
     <row r="277" spans="1:9" ht="19" customHeight="1">
       <c r="A277" s="19" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B277" s="20"/>
       <c r="C277" s="20" t="s">
-        <v>1163</v>
-      </c>
-      <c r="D277" s="20" t="s">
-        <v>710</v>
+        <v>557</v>
+      </c>
+      <c r="D277" s="21" t="s">
+        <v>706</v>
       </c>
       <c r="E277" s="20"/>
       <c r="F277" s="20"/>
@@ -17413,14 +17487,14 @@
     </row>
     <row r="278" spans="1:9" ht="19" customHeight="1">
       <c r="A278" s="19" t="s">
-        <v>1099</v>
+        <v>558</v>
       </c>
       <c r="B278" s="20"/>
       <c r="C278" s="20" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D278" s="20" t="s">
-        <v>1104</v>
+        <v>559</v>
+      </c>
+      <c r="D278" s="21" t="s">
+        <v>707</v>
       </c>
       <c r="E278" s="20"/>
       <c r="F278" s="20"/>
@@ -17430,14 +17504,14 @@
     </row>
     <row r="279" spans="1:9" ht="19" customHeight="1">
       <c r="A279" s="19" t="s">
-        <v>1112</v>
+        <v>560</v>
       </c>
       <c r="B279" s="20"/>
       <c r="C279" s="20" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D279" s="22" t="s">
-        <v>1121</v>
+        <v>561</v>
+      </c>
+      <c r="D279" s="20" t="s">
+        <v>708</v>
       </c>
       <c r="E279" s="20"/>
       <c r="F279" s="20"/>
@@ -17447,14 +17521,14 @@
     </row>
     <row r="280" spans="1:9" ht="19" customHeight="1">
       <c r="A280" s="19" t="s">
-        <v>1113</v>
+        <v>562</v>
       </c>
       <c r="B280" s="20"/>
       <c r="C280" s="20" t="s">
-        <v>1118</v>
-      </c>
-      <c r="D280" s="22" t="s">
-        <v>1119</v>
+        <v>563</v>
+      </c>
+      <c r="D280" s="20" t="s">
+        <v>709</v>
       </c>
       <c r="E280" s="20"/>
       <c r="F280" s="20"/>
@@ -17464,14 +17538,14 @@
     </row>
     <row r="281" spans="1:9" ht="19" customHeight="1">
       <c r="A281" s="19" t="s">
-        <v>1114</v>
+        <v>564</v>
       </c>
       <c r="B281" s="20"/>
       <c r="C281" s="20" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D281" s="22" t="s">
-        <v>1117</v>
+        <v>1163</v>
+      </c>
+      <c r="D281" s="20" t="s">
+        <v>710</v>
       </c>
       <c r="E281" s="20"/>
       <c r="F281" s="20"/>
@@ -17481,14 +17555,14 @@
     </row>
     <row r="282" spans="1:9" ht="19" customHeight="1">
       <c r="A282" s="19" t="s">
-        <v>1115</v>
+        <v>1099</v>
       </c>
       <c r="B282" s="20"/>
       <c r="C282" s="20" t="s">
-        <v>1161</v>
-      </c>
-      <c r="D282" s="22" t="s">
-        <v>1162</v>
+        <v>1103</v>
+      </c>
+      <c r="D282" s="20" t="s">
+        <v>1104</v>
       </c>
       <c r="E282" s="20"/>
       <c r="F282" s="20"/>
@@ -17498,14 +17572,14 @@
     </row>
     <row r="283" spans="1:9" ht="19" customHeight="1">
       <c r="A283" s="19" t="s">
-        <v>904</v>
+        <v>1112</v>
       </c>
       <c r="B283" s="20"/>
       <c r="C283" s="20" t="s">
-        <v>906</v>
-      </c>
-      <c r="D283" s="20" t="s">
-        <v>905</v>
+        <v>1120</v>
+      </c>
+      <c r="D283" s="22" t="s">
+        <v>1121</v>
       </c>
       <c r="E283" s="20"/>
       <c r="F283" s="20"/>
@@ -17515,14 +17589,14 @@
     </row>
     <row r="284" spans="1:9" ht="19" customHeight="1">
       <c r="A284" s="19" t="s">
-        <v>565</v>
+        <v>1113</v>
       </c>
       <c r="B284" s="20"/>
       <c r="C284" s="20" t="s">
-        <v>566</v>
-      </c>
-      <c r="D284" s="21" t="s">
-        <v>711</v>
+        <v>1118</v>
+      </c>
+      <c r="D284" s="22" t="s">
+        <v>1119</v>
       </c>
       <c r="E284" s="20"/>
       <c r="F284" s="20"/>
@@ -17532,14 +17606,14 @@
     </row>
     <row r="285" spans="1:9" ht="19" customHeight="1">
       <c r="A285" s="19" t="s">
-        <v>567</v>
+        <v>1114</v>
       </c>
       <c r="B285" s="20"/>
       <c r="C285" s="20" t="s">
-        <v>568</v>
-      </c>
-      <c r="D285" s="21" t="s">
-        <v>712</v>
+        <v>1116</v>
+      </c>
+      <c r="D285" s="22" t="s">
+        <v>1117</v>
       </c>
       <c r="E285" s="20"/>
       <c r="F285" s="20"/>
@@ -17549,14 +17623,14 @@
     </row>
     <row r="286" spans="1:9" ht="19" customHeight="1">
       <c r="A286" s="19" t="s">
-        <v>569</v>
+        <v>1115</v>
       </c>
       <c r="B286" s="20"/>
       <c r="C286" s="20" t="s">
-        <v>570</v>
-      </c>
-      <c r="D286" s="20" t="s">
-        <v>713</v>
+        <v>1161</v>
+      </c>
+      <c r="D286" s="22" t="s">
+        <v>1162</v>
       </c>
       <c r="E286" s="20"/>
       <c r="F286" s="20"/>
@@ -17566,14 +17640,14 @@
     </row>
     <row r="287" spans="1:9" ht="19" customHeight="1">
       <c r="A287" s="19" t="s">
-        <v>1100</v>
+        <v>904</v>
       </c>
       <c r="B287" s="20"/>
       <c r="C287" s="20" t="s">
-        <v>1122</v>
+        <v>906</v>
       </c>
       <c r="D287" s="20" t="s">
-        <v>1123</v>
+        <v>905</v>
       </c>
       <c r="E287" s="20"/>
       <c r="F287" s="20"/>
@@ -17583,14 +17657,14 @@
     </row>
     <row r="288" spans="1:9" ht="19" customHeight="1">
       <c r="A288" s="19" t="s">
-        <v>1101</v>
+        <v>565</v>
       </c>
       <c r="B288" s="20"/>
       <c r="C288" s="20" t="s">
-        <v>1102</v>
-      </c>
-      <c r="D288" s="20" t="s">
-        <v>1108</v>
+        <v>566</v>
+      </c>
+      <c r="D288" s="21" t="s">
+        <v>711</v>
       </c>
       <c r="E288" s="20"/>
       <c r="F288" s="20"/>
@@ -17600,14 +17674,14 @@
     </row>
     <row r="289" spans="1:9" ht="19" customHeight="1">
       <c r="A289" s="19" t="s">
-        <v>1109</v>
+        <v>567</v>
       </c>
       <c r="B289" s="20"/>
       <c r="C289" s="20" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D289" s="20" t="s">
-        <v>1111</v>
+        <v>568</v>
+      </c>
+      <c r="D289" s="21" t="s">
+        <v>712</v>
       </c>
       <c r="E289" s="20"/>
       <c r="F289" s="20"/>
@@ -17617,14 +17691,14 @@
     </row>
     <row r="290" spans="1:9" ht="19" customHeight="1">
       <c r="A290" s="19" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B290" s="20"/>
       <c r="C290" s="20" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D290" s="20" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="E290" s="20"/>
       <c r="F290" s="20"/>
@@ -17634,14 +17708,14 @@
     </row>
     <row r="291" spans="1:9" ht="19" customHeight="1">
       <c r="A291" s="19" t="s">
-        <v>1022</v>
+        <v>1100</v>
       </c>
       <c r="B291" s="20"/>
       <c r="C291" s="20" t="s">
-        <v>1023</v>
+        <v>1122</v>
       </c>
       <c r="D291" s="20" t="s">
-        <v>1164</v>
+        <v>1123</v>
       </c>
       <c r="E291" s="20"/>
       <c r="F291" s="20"/>
@@ -17651,14 +17725,14 @@
     </row>
     <row r="292" spans="1:9" ht="19" customHeight="1">
       <c r="A292" s="19" t="s">
-        <v>571</v>
+        <v>1101</v>
       </c>
       <c r="B292" s="20"/>
       <c r="C292" s="20" t="s">
-        <v>572</v>
+        <v>1102</v>
       </c>
       <c r="D292" s="20" t="s">
-        <v>714</v>
+        <v>1108</v>
       </c>
       <c r="E292" s="20"/>
       <c r="F292" s="20"/>
@@ -17668,14 +17742,14 @@
     </row>
     <row r="293" spans="1:9" ht="19" customHeight="1">
       <c r="A293" s="19" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="B293" s="20"/>
       <c r="C293" s="20" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="D293" s="20" t="s">
-        <v>1106</v>
+        <v>1111</v>
       </c>
       <c r="E293" s="20"/>
       <c r="F293" s="20"/>
@@ -17685,14 +17759,14 @@
     </row>
     <row r="294" spans="1:9" ht="19" customHeight="1">
       <c r="A294" s="19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B294" s="20"/>
       <c r="C294" s="20" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E294" s="20"/>
       <c r="F294" s="20"/>
@@ -17702,14 +17776,14 @@
     </row>
     <row r="295" spans="1:9" ht="19" customHeight="1">
       <c r="A295" s="19" t="s">
-        <v>577</v>
+        <v>1022</v>
       </c>
       <c r="B295" s="20"/>
       <c r="C295" s="20" t="s">
-        <v>578</v>
+        <v>1023</v>
       </c>
       <c r="D295" s="20" t="s">
-        <v>717</v>
+        <v>1164</v>
       </c>
       <c r="E295" s="20"/>
       <c r="F295" s="20"/>
@@ -17719,14 +17793,14 @@
     </row>
     <row r="296" spans="1:9" ht="19" customHeight="1">
       <c r="A296" s="19" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="B296" s="20"/>
       <c r="C296" s="20" t="s">
-        <v>580</v>
-      </c>
-      <c r="D296" s="21" t="s">
-        <v>718</v>
+        <v>572</v>
+      </c>
+      <c r="D296" s="20" t="s">
+        <v>714</v>
       </c>
       <c r="E296" s="20"/>
       <c r="F296" s="20"/>
@@ -17736,14 +17810,14 @@
     </row>
     <row r="297" spans="1:9" ht="19" customHeight="1">
       <c r="A297" s="19" t="s">
-        <v>581</v>
+        <v>1105</v>
       </c>
       <c r="B297" s="20"/>
       <c r="C297" s="20" t="s">
-        <v>582</v>
-      </c>
-      <c r="D297" s="21" t="s">
-        <v>719</v>
+        <v>1107</v>
+      </c>
+      <c r="D297" s="20" t="s">
+        <v>1106</v>
       </c>
       <c r="E297" s="20"/>
       <c r="F297" s="20"/>
@@ -17753,14 +17827,14 @@
     </row>
     <row r="298" spans="1:9" ht="19" customHeight="1">
       <c r="A298" s="19" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="B298" s="20"/>
       <c r="C298" s="20" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="D298" s="20" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="E298" s="20"/>
       <c r="F298" s="20"/>
@@ -17770,14 +17844,14 @@
     </row>
     <row r="299" spans="1:9" ht="19" customHeight="1">
       <c r="A299" s="19" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="B299" s="20"/>
       <c r="C299" s="20" t="s">
-        <v>586</v>
-      </c>
-      <c r="D299" s="21" t="s">
-        <v>721</v>
+        <v>578</v>
+      </c>
+      <c r="D299" s="20" t="s">
+        <v>717</v>
       </c>
       <c r="E299" s="20"/>
       <c r="F299" s="20"/>
@@ -17787,14 +17861,14 @@
     </row>
     <row r="300" spans="1:9" ht="19" customHeight="1">
       <c r="A300" s="19" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="B300" s="20"/>
       <c r="C300" s="20" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="D300" s="21" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="E300" s="20"/>
       <c r="F300" s="20"/>
@@ -17804,14 +17878,14 @@
     </row>
     <row r="301" spans="1:9" ht="19" customHeight="1">
       <c r="A301" s="19" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="B301" s="20"/>
       <c r="C301" s="20" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D301" s="21" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="E301" s="20"/>
       <c r="F301" s="20"/>
@@ -17821,14 +17895,14 @@
     </row>
     <row r="302" spans="1:9" ht="19" customHeight="1">
       <c r="A302" s="19" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="B302" s="20"/>
       <c r="C302" s="20" t="s">
-        <v>592</v>
-      </c>
-      <c r="D302" s="21" t="s">
-        <v>724</v>
+        <v>584</v>
+      </c>
+      <c r="D302" s="20" t="s">
+        <v>720</v>
       </c>
       <c r="E302" s="20"/>
       <c r="F302" s="20"/>
@@ -17838,14 +17912,14 @@
     </row>
     <row r="303" spans="1:9" ht="19" customHeight="1">
       <c r="A303" s="19" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="B303" s="20"/>
       <c r="C303" s="20" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="D303" s="21" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="E303" s="20"/>
       <c r="F303" s="20"/>
@@ -17855,14 +17929,14 @@
     </row>
     <row r="304" spans="1:9" ht="19" customHeight="1">
       <c r="A304" s="19" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="B304" s="20"/>
       <c r="C304" s="20" t="s">
-        <v>596</v>
-      </c>
-      <c r="D304" s="20" t="s">
-        <v>726</v>
+        <v>588</v>
+      </c>
+      <c r="D304" s="21" t="s">
+        <v>722</v>
       </c>
       <c r="E304" s="20"/>
       <c r="F304" s="20"/>
@@ -17872,14 +17946,14 @@
     </row>
     <row r="305" spans="1:9" ht="19" customHeight="1">
       <c r="A305" s="19" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="B305" s="20"/>
       <c r="C305" s="20" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="D305" s="21" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="E305" s="20"/>
       <c r="F305" s="20"/>
@@ -17889,14 +17963,14 @@
     </row>
     <row r="306" spans="1:9" ht="19" customHeight="1">
       <c r="A306" s="19" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="B306" s="20"/>
       <c r="C306" s="20" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="D306" s="21" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="E306" s="20"/>
       <c r="F306" s="20"/>
@@ -17906,14 +17980,14 @@
     </row>
     <row r="307" spans="1:9" ht="19" customHeight="1">
       <c r="A307" s="19" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="B307" s="20"/>
       <c r="C307" s="20" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="D307" s="21" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="E307" s="20"/>
       <c r="F307" s="20"/>
@@ -17923,14 +17997,14 @@
     </row>
     <row r="308" spans="1:9" ht="19" customHeight="1">
       <c r="A308" s="19" t="s">
-        <v>1014</v>
+        <v>595</v>
       </c>
       <c r="B308" s="20"/>
       <c r="C308" s="20" t="s">
-        <v>1015</v>
+        <v>596</v>
       </c>
       <c r="D308" s="20" t="s">
-        <v>1016</v>
+        <v>726</v>
       </c>
       <c r="E308" s="20"/>
       <c r="F308" s="20"/>
@@ -17940,14 +18014,14 @@
     </row>
     <row r="309" spans="1:9" ht="19" customHeight="1">
       <c r="A309" s="19" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B309" s="20"/>
       <c r="C309" s="20" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="D309" s="21" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="E309" s="20"/>
       <c r="F309" s="20"/>
@@ -17957,14 +18031,14 @@
     </row>
     <row r="310" spans="1:9" ht="19" customHeight="1">
       <c r="A310" s="19" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B310" s="20"/>
       <c r="C310" s="20" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="D310" s="21" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="E310" s="20"/>
       <c r="F310" s="20"/>
@@ -17974,14 +18048,14 @@
     </row>
     <row r="311" spans="1:9" ht="19" customHeight="1">
       <c r="A311" s="19" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B311" s="20"/>
       <c r="C311" s="20" t="s">
-        <v>608</v>
-      </c>
-      <c r="D311" s="20" t="s">
-        <v>732</v>
+        <v>602</v>
+      </c>
+      <c r="D311" s="21" t="s">
+        <v>729</v>
       </c>
       <c r="E311" s="20"/>
       <c r="F311" s="20"/>
@@ -17991,14 +18065,14 @@
     </row>
     <row r="312" spans="1:9" ht="19" customHeight="1">
       <c r="A312" s="19" t="s">
-        <v>609</v>
+        <v>1014</v>
       </c>
       <c r="B312" s="20"/>
       <c r="C312" s="20" t="s">
-        <v>610</v>
+        <v>1015</v>
       </c>
       <c r="D312" s="20" t="s">
-        <v>733</v>
+        <v>1016</v>
       </c>
       <c r="E312" s="20"/>
       <c r="F312" s="20"/>
@@ -18008,14 +18082,14 @@
     </row>
     <row r="313" spans="1:9" ht="19" customHeight="1">
       <c r="A313" s="19" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="B313" s="20"/>
       <c r="C313" s="20" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="D313" s="21" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="E313" s="20"/>
       <c r="F313" s="20"/>
@@ -18025,14 +18099,14 @@
     </row>
     <row r="314" spans="1:9" ht="19" customHeight="1">
       <c r="A314" s="19" t="s">
-        <v>1070</v>
+        <v>605</v>
       </c>
       <c r="B314" s="20"/>
       <c r="C314" s="20" t="s">
-        <v>1071</v>
+        <v>606</v>
       </c>
       <c r="D314" s="21" t="s">
-        <v>1072</v>
+        <v>731</v>
       </c>
       <c r="E314" s="20"/>
       <c r="F314" s="20"/>
@@ -18042,14 +18116,14 @@
     </row>
     <row r="315" spans="1:9" ht="19" customHeight="1">
       <c r="A315" s="19" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B315" s="20"/>
       <c r="C315" s="20" t="s">
-        <v>614</v>
-      </c>
-      <c r="D315" s="22" t="s">
-        <v>735</v>
+        <v>608</v>
+      </c>
+      <c r="D315" s="20" t="s">
+        <v>732</v>
       </c>
       <c r="E315" s="20"/>
       <c r="F315" s="20"/>
@@ -18059,14 +18133,14 @@
     </row>
     <row r="316" spans="1:9" ht="19" customHeight="1">
       <c r="A316" s="19" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="B316" s="20"/>
       <c r="C316" s="20" t="s">
-        <v>616</v>
-      </c>
-      <c r="D316" s="21" t="s">
-        <v>930</v>
+        <v>610</v>
+      </c>
+      <c r="D316" s="20" t="s">
+        <v>733</v>
       </c>
       <c r="E316" s="20"/>
       <c r="F316" s="20"/>
@@ -18076,14 +18150,14 @@
     </row>
     <row r="317" spans="1:9" ht="19" customHeight="1">
       <c r="A317" s="19" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B317" s="20"/>
       <c r="C317" s="20" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="D317" s="21" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E317" s="20"/>
       <c r="F317" s="20"/>
@@ -18093,14 +18167,14 @@
     </row>
     <row r="318" spans="1:9" ht="19" customHeight="1">
       <c r="A318" s="19" t="s">
-        <v>619</v>
+        <v>1070</v>
       </c>
       <c r="B318" s="20"/>
       <c r="C318" s="20" t="s">
-        <v>620</v>
-      </c>
-      <c r="D318" s="20" t="s">
-        <v>737</v>
+        <v>1071</v>
+      </c>
+      <c r="D318" s="21" t="s">
+        <v>1072</v>
       </c>
       <c r="E318" s="20"/>
       <c r="F318" s="20"/>
@@ -18110,14 +18184,14 @@
     </row>
     <row r="319" spans="1:9" ht="19" customHeight="1">
       <c r="A319" s="19" t="s">
-        <v>942</v>
+        <v>613</v>
       </c>
       <c r="B319" s="20"/>
       <c r="C319" s="20" t="s">
-        <v>943</v>
-      </c>
-      <c r="D319" s="20" t="s">
-        <v>944</v>
+        <v>614</v>
+      </c>
+      <c r="D319" s="22" t="s">
+        <v>735</v>
       </c>
       <c r="E319" s="20"/>
       <c r="F319" s="20"/>
@@ -18127,14 +18201,14 @@
     </row>
     <row r="320" spans="1:9" ht="19" customHeight="1">
       <c r="A320" s="19" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B320" s="20"/>
       <c r="C320" s="20" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="D320" s="21" t="s">
-        <v>738</v>
+        <v>930</v>
       </c>
       <c r="E320" s="20"/>
       <c r="F320" s="20"/>
@@ -18144,14 +18218,14 @@
     </row>
     <row r="321" spans="1:9" ht="19" customHeight="1">
       <c r="A321" s="19" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B321" s="20"/>
       <c r="C321" s="20" t="s">
-        <v>945</v>
+        <v>618</v>
       </c>
       <c r="D321" s="21" t="s">
-        <v>946</v>
+        <v>736</v>
       </c>
       <c r="E321" s="20"/>
       <c r="F321" s="20"/>
@@ -18161,14 +18235,14 @@
     </row>
     <row r="322" spans="1:9" ht="19" customHeight="1">
       <c r="A322" s="19" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="B322" s="20"/>
       <c r="C322" s="20" t="s">
-        <v>625</v>
-      </c>
-      <c r="D322" s="21" t="s">
-        <v>739</v>
+        <v>620</v>
+      </c>
+      <c r="D322" s="20" t="s">
+        <v>737</v>
       </c>
       <c r="E322" s="20"/>
       <c r="F322" s="20"/>
@@ -18178,14 +18252,14 @@
     </row>
     <row r="323" spans="1:9" ht="19" customHeight="1">
       <c r="A323" s="19" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="B323" s="20"/>
       <c r="C323" s="20" t="s">
-        <v>948</v>
+        <v>943</v>
       </c>
       <c r="D323" s="20" t="s">
-        <v>949</v>
+        <v>944</v>
       </c>
       <c r="E323" s="20"/>
       <c r="F323" s="20"/>
@@ -18195,14 +18269,14 @@
     </row>
     <row r="324" spans="1:9" ht="19" customHeight="1">
       <c r="A324" s="19" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="B324" s="20"/>
       <c r="C324" s="20" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="D324" s="21" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E324" s="20"/>
       <c r="F324" s="20"/>
@@ -18212,14 +18286,14 @@
     </row>
     <row r="325" spans="1:9" ht="19" customHeight="1">
       <c r="A325" s="19" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="B325" s="20"/>
       <c r="C325" s="20" t="s">
-        <v>629</v>
+        <v>945</v>
       </c>
       <c r="D325" s="21" t="s">
-        <v>741</v>
+        <v>946</v>
       </c>
       <c r="E325" s="20"/>
       <c r="F325" s="20"/>
@@ -18229,14 +18303,14 @@
     </row>
     <row r="326" spans="1:9" ht="19" customHeight="1">
       <c r="A326" s="19" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B326" s="20"/>
       <c r="C326" s="20" t="s">
-        <v>631</v>
-      </c>
-      <c r="D326" s="20" t="s">
-        <v>742</v>
+        <v>625</v>
+      </c>
+      <c r="D326" s="21" t="s">
+        <v>739</v>
       </c>
       <c r="E326" s="20"/>
       <c r="F326" s="20"/>
@@ -18246,14 +18320,14 @@
     </row>
     <row r="327" spans="1:9" ht="19" customHeight="1">
       <c r="A327" s="19" t="s">
-        <v>632</v>
+        <v>947</v>
       </c>
       <c r="B327" s="20"/>
       <c r="C327" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="D327" s="21" t="s">
-        <v>743</v>
+        <v>948</v>
+      </c>
+      <c r="D327" s="20" t="s">
+        <v>949</v>
       </c>
       <c r="E327" s="20"/>
       <c r="F327" s="20"/>
@@ -18263,14 +18337,14 @@
     </row>
     <row r="328" spans="1:9" ht="19" customHeight="1">
       <c r="A328" s="19" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="B328" s="20"/>
       <c r="C328" s="20" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="D328" s="21" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E328" s="20"/>
       <c r="F328" s="20"/>
@@ -18280,14 +18354,14 @@
     </row>
     <row r="329" spans="1:9" ht="19" customHeight="1">
       <c r="A329" s="19" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="B329" s="20"/>
       <c r="C329" s="20" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="D329" s="21" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E329" s="20"/>
       <c r="F329" s="20"/>
@@ -18297,14 +18371,14 @@
     </row>
     <row r="330" spans="1:9" ht="19" customHeight="1">
       <c r="A330" s="19" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="B330" s="20"/>
       <c r="C330" s="20" t="s">
-        <v>639</v>
-      </c>
-      <c r="D330" s="22" t="s">
-        <v>746</v>
+        <v>631</v>
+      </c>
+      <c r="D330" s="20" t="s">
+        <v>742</v>
       </c>
       <c r="E330" s="20"/>
       <c r="F330" s="20"/>
@@ -18314,14 +18388,14 @@
     </row>
     <row r="331" spans="1:9" ht="19" customHeight="1">
       <c r="A331" s="19" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="B331" s="20"/>
       <c r="C331" s="20" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="D331" s="21" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E331" s="20"/>
       <c r="F331" s="20"/>
@@ -18331,14 +18405,14 @@
     </row>
     <row r="332" spans="1:9" ht="19" customHeight="1">
       <c r="A332" s="19" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="B332" s="20"/>
       <c r="C332" s="20" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="D332" s="21" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="E332" s="20"/>
       <c r="F332" s="20"/>
@@ -18348,14 +18422,14 @@
     </row>
     <row r="333" spans="1:9" ht="19" customHeight="1">
       <c r="A333" s="19" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="B333" s="20"/>
       <c r="C333" s="20" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="D333" s="21" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E333" s="20"/>
       <c r="F333" s="20"/>
@@ -18365,14 +18439,14 @@
     </row>
     <row r="334" spans="1:9" ht="19" customHeight="1">
       <c r="A334" s="19" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="B334" s="20"/>
       <c r="C334" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="D334" s="21" t="s">
-        <v>750</v>
+        <v>639</v>
+      </c>
+      <c r="D334" s="22" t="s">
+        <v>746</v>
       </c>
       <c r="E334" s="20"/>
       <c r="F334" s="20"/>
@@ -18382,14 +18456,14 @@
     </row>
     <row r="335" spans="1:9" ht="19" customHeight="1">
       <c r="A335" s="19" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="B335" s="20"/>
       <c r="C335" s="20" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="D335" s="21" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="E335" s="20"/>
       <c r="F335" s="20"/>
@@ -18399,14 +18473,14 @@
     </row>
     <row r="336" spans="1:9" ht="19" customHeight="1">
       <c r="A336" s="19" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="B336" s="20"/>
       <c r="C336" s="20" t="s">
-        <v>651</v>
-      </c>
-      <c r="D336" s="20" t="s">
-        <v>752</v>
+        <v>642</v>
+      </c>
+      <c r="D336" s="21" t="s">
+        <v>748</v>
       </c>
       <c r="E336" s="20"/>
       <c r="F336" s="20"/>
@@ -18416,14 +18490,14 @@
     </row>
     <row r="337" spans="1:9" ht="19" customHeight="1">
       <c r="A337" s="19" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="B337" s="20"/>
-      <c r="C337" s="27" t="s">
-        <v>653</v>
-      </c>
-      <c r="D337" s="27" t="s">
-        <v>753</v>
+      <c r="C337" s="20" t="s">
+        <v>645</v>
+      </c>
+      <c r="D337" s="21" t="s">
+        <v>749</v>
       </c>
       <c r="E337" s="20"/>
       <c r="F337" s="20"/>
@@ -18433,14 +18507,14 @@
     </row>
     <row r="338" spans="1:9" ht="19" customHeight="1">
       <c r="A338" s="19" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="B338" s="20"/>
       <c r="C338" s="20" t="s">
-        <v>655</v>
-      </c>
-      <c r="D338" s="20" t="s">
-        <v>754</v>
+        <v>647</v>
+      </c>
+      <c r="D338" s="21" t="s">
+        <v>750</v>
       </c>
       <c r="E338" s="20"/>
       <c r="F338" s="20"/>
@@ -18450,14 +18524,14 @@
     </row>
     <row r="339" spans="1:9" ht="19" customHeight="1">
       <c r="A339" s="19" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="B339" s="20"/>
       <c r="C339" s="20" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="D339" s="21" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="E339" s="20"/>
       <c r="F339" s="20"/>
@@ -18467,14 +18541,14 @@
     </row>
     <row r="340" spans="1:9" ht="19" customHeight="1">
       <c r="A340" s="19" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="B340" s="20"/>
       <c r="C340" s="20" t="s">
-        <v>659</v>
-      </c>
-      <c r="D340" s="21" t="s">
-        <v>756</v>
+        <v>651</v>
+      </c>
+      <c r="D340" s="20" t="s">
+        <v>752</v>
       </c>
       <c r="E340" s="20"/>
       <c r="F340" s="20"/>
@@ -18484,14 +18558,14 @@
     </row>
     <row r="341" spans="1:9" ht="19" customHeight="1">
       <c r="A341" s="19" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="B341" s="20"/>
-      <c r="C341" s="20" t="s">
-        <v>661</v>
-      </c>
-      <c r="D341" s="21" t="s">
-        <v>757</v>
+      <c r="C341" s="27" t="s">
+        <v>653</v>
+      </c>
+      <c r="D341" s="27" t="s">
+        <v>753</v>
       </c>
       <c r="E341" s="20"/>
       <c r="F341" s="20"/>
@@ -18501,14 +18575,14 @@
     </row>
     <row r="342" spans="1:9" ht="19" customHeight="1">
       <c r="A342" s="19" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="B342" s="20"/>
       <c r="C342" s="20" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="D342" s="20" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="E342" s="20"/>
       <c r="F342" s="20"/>
@@ -18518,14 +18592,14 @@
     </row>
     <row r="343" spans="1:9" ht="19" customHeight="1">
       <c r="A343" s="19" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="B343" s="20"/>
       <c r="C343" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="D343" s="22" t="s">
-        <v>759</v>
+        <v>657</v>
+      </c>
+      <c r="D343" s="21" t="s">
+        <v>755</v>
       </c>
       <c r="E343" s="20"/>
       <c r="F343" s="20"/>
@@ -18535,14 +18609,14 @@
     </row>
     <row r="344" spans="1:9" ht="19" customHeight="1">
       <c r="A344" s="19" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="B344" s="20"/>
       <c r="C344" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="D344" s="20" t="s">
-        <v>760</v>
+        <v>659</v>
+      </c>
+      <c r="D344" s="21" t="s">
+        <v>756</v>
       </c>
       <c r="E344" s="20"/>
       <c r="F344" s="20"/>
@@ -18552,14 +18626,14 @@
     </row>
     <row r="345" spans="1:9" ht="19" customHeight="1">
       <c r="A345" s="19" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="B345" s="20"/>
       <c r="C345" s="20" t="s">
-        <v>669</v>
-      </c>
-      <c r="D345" s="20" t="s">
-        <v>761</v>
+        <v>661</v>
+      </c>
+      <c r="D345" s="21" t="s">
+        <v>757</v>
       </c>
       <c r="E345" s="20"/>
       <c r="F345" s="20"/>
@@ -18569,14 +18643,14 @@
     </row>
     <row r="346" spans="1:9" ht="19" customHeight="1">
       <c r="A346" s="19" t="s">
-        <v>939</v>
+        <v>662</v>
       </c>
       <c r="B346" s="20"/>
       <c r="C346" s="20" t="s">
-        <v>940</v>
+        <v>663</v>
       </c>
       <c r="D346" s="20" t="s">
-        <v>941</v>
+        <v>758</v>
       </c>
       <c r="E346" s="20"/>
       <c r="F346" s="20"/>
@@ -18586,14 +18660,14 @@
     </row>
     <row r="347" spans="1:9" ht="19" customHeight="1">
       <c r="A347" s="19" t="s">
-        <v>1062</v>
+        <v>664</v>
       </c>
       <c r="B347" s="20"/>
       <c r="C347" s="20" t="s">
-        <v>1063</v>
-      </c>
-      <c r="D347" s="20" t="s">
-        <v>1064</v>
+        <v>665</v>
+      </c>
+      <c r="D347" s="22" t="s">
+        <v>759</v>
       </c>
       <c r="E347" s="20"/>
       <c r="F347" s="20"/>
@@ -18603,14 +18677,14 @@
     </row>
     <row r="348" spans="1:9" ht="19" customHeight="1">
       <c r="A348" s="19" t="s">
-        <v>1130</v>
+        <v>666</v>
       </c>
       <c r="B348" s="20"/>
       <c r="C348" s="20" t="s">
-        <v>1131</v>
+        <v>667</v>
       </c>
       <c r="D348" s="20" t="s">
-        <v>1132</v>
+        <v>760</v>
       </c>
       <c r="E348" s="20"/>
       <c r="F348" s="20"/>
@@ -18620,14 +18694,14 @@
     </row>
     <row r="349" spans="1:9" ht="19" customHeight="1">
       <c r="A349" s="19" t="s">
-        <v>1124</v>
+        <v>668</v>
       </c>
       <c r="B349" s="20"/>
       <c r="C349" s="20" t="s">
-        <v>1125</v>
+        <v>669</v>
       </c>
       <c r="D349" s="20" t="s">
-        <v>1126</v>
+        <v>761</v>
       </c>
       <c r="E349" s="20"/>
       <c r="F349" s="20"/>
@@ -18637,14 +18711,14 @@
     </row>
     <row r="350" spans="1:9" ht="19" customHeight="1">
       <c r="A350" s="19" t="s">
-        <v>1127</v>
+        <v>939</v>
       </c>
       <c r="B350" s="20"/>
       <c r="C350" s="20" t="s">
-        <v>1128</v>
+        <v>940</v>
       </c>
       <c r="D350" s="20" t="s">
-        <v>1129</v>
+        <v>941</v>
       </c>
       <c r="E350" s="20"/>
       <c r="F350" s="20"/>
@@ -18654,14 +18728,14 @@
     </row>
     <row r="351" spans="1:9" ht="19" customHeight="1">
       <c r="A351" s="19" t="s">
-        <v>1133</v>
+        <v>1062</v>
       </c>
       <c r="B351" s="20"/>
       <c r="C351" s="20" t="s">
-        <v>1134</v>
+        <v>1063</v>
       </c>
       <c r="D351" s="20" t="s">
-        <v>1135</v>
+        <v>1064</v>
       </c>
       <c r="E351" s="20"/>
       <c r="F351" s="20"/>
@@ -18671,14 +18745,14 @@
     </row>
     <row r="352" spans="1:9" ht="19" customHeight="1">
       <c r="A352" s="19" t="s">
-        <v>1145</v>
+        <v>1130</v>
       </c>
       <c r="B352" s="20"/>
       <c r="C352" s="20" t="s">
-        <v>1147</v>
+        <v>1131</v>
       </c>
       <c r="D352" s="20" t="s">
-        <v>1146</v>
+        <v>1132</v>
       </c>
       <c r="E352" s="20"/>
       <c r="F352" s="20"/>
@@ -18688,14 +18762,14 @@
     </row>
     <row r="353" spans="1:9" ht="19" customHeight="1">
       <c r="A353" s="19" t="s">
-        <v>1148</v>
+        <v>1124</v>
       </c>
       <c r="B353" s="20"/>
       <c r="C353" s="20" t="s">
-        <v>1149</v>
+        <v>1125</v>
       </c>
       <c r="D353" s="20" t="s">
-        <v>1150</v>
+        <v>1126</v>
       </c>
       <c r="E353" s="20"/>
       <c r="F353" s="20"/>
@@ -18705,14 +18779,14 @@
     </row>
     <row r="354" spans="1:9" ht="19" customHeight="1">
       <c r="A354" s="19" t="s">
-        <v>1151</v>
+        <v>1127</v>
       </c>
       <c r="B354" s="20"/>
       <c r="C354" s="20" t="s">
-        <v>1152</v>
+        <v>1128</v>
       </c>
       <c r="D354" s="20" t="s">
-        <v>1153</v>
+        <v>1129</v>
       </c>
       <c r="E354" s="20"/>
       <c r="F354" s="20"/>
@@ -18722,14 +18796,14 @@
     </row>
     <row r="355" spans="1:9" ht="19" customHeight="1">
       <c r="A355" s="19" t="s">
-        <v>1184</v>
+        <v>1133</v>
       </c>
       <c r="B355" s="20"/>
       <c r="C355" s="20" t="s">
-        <v>1186</v>
+        <v>1134</v>
       </c>
       <c r="D355" s="20" t="s">
-        <v>1185</v>
+        <v>1135</v>
       </c>
       <c r="E355" s="20"/>
       <c r="F355" s="20"/>
@@ -18739,14 +18813,14 @@
     </row>
     <row r="356" spans="1:9" ht="19" customHeight="1">
       <c r="A356" s="19" t="s">
-        <v>1181</v>
+        <v>1145</v>
       </c>
       <c r="B356" s="20"/>
       <c r="C356" s="20" t="s">
-        <v>1182</v>
+        <v>1147</v>
       </c>
       <c r="D356" s="20" t="s">
-        <v>1183</v>
+        <v>1146</v>
       </c>
       <c r="E356" s="20"/>
       <c r="F356" s="20"/>
@@ -18756,14 +18830,14 @@
     </row>
     <row r="357" spans="1:9" ht="19" customHeight="1">
       <c r="A357" s="19" t="s">
-        <v>1272</v>
+        <v>1148</v>
       </c>
       <c r="B357" s="20"/>
       <c r="C357" s="20" t="s">
-        <v>1273</v>
+        <v>1149</v>
       </c>
       <c r="D357" s="20" t="s">
-        <v>1274</v>
+        <v>1150</v>
       </c>
       <c r="E357" s="20"/>
       <c r="F357" s="20"/>
@@ -18773,14 +18847,14 @@
     </row>
     <row r="358" spans="1:9" ht="19" customHeight="1">
       <c r="A358" s="19" t="s">
-        <v>1406</v>
+        <v>1151</v>
       </c>
       <c r="B358" s="20"/>
       <c r="C358" s="20" t="s">
-        <v>1407</v>
+        <v>1152</v>
       </c>
       <c r="D358" s="20" t="s">
-        <v>1408</v>
+        <v>1153</v>
       </c>
       <c r="E358" s="20"/>
       <c r="F358" s="20"/>
@@ -18790,14 +18864,14 @@
     </row>
     <row r="359" spans="1:9" ht="19" customHeight="1">
       <c r="A359" s="19" t="s">
-        <v>1409</v>
+        <v>1184</v>
       </c>
       <c r="B359" s="20"/>
       <c r="C359" s="20" t="s">
-        <v>1410</v>
+        <v>1186</v>
       </c>
       <c r="D359" s="20" t="s">
-        <v>1411</v>
+        <v>1185</v>
       </c>
       <c r="E359" s="20"/>
       <c r="F359" s="20"/>
@@ -18806,10 +18880,16 @@
       <c r="I359" s="18"/>
     </row>
     <row r="360" spans="1:9" ht="19" customHeight="1">
-      <c r="A360" s="19"/>
+      <c r="A360" s="19" t="s">
+        <v>1181</v>
+      </c>
       <c r="B360" s="20"/>
-      <c r="C360" s="20"/>
-      <c r="D360" s="20"/>
+      <c r="C360" s="20" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D360" s="20" t="s">
+        <v>1183</v>
+      </c>
       <c r="E360" s="20"/>
       <c r="F360" s="20"/>
       <c r="G360" s="18"/>
@@ -18817,10 +18897,16 @@
       <c r="I360" s="18"/>
     </row>
     <row r="361" spans="1:9" ht="19" customHeight="1">
-      <c r="A361" s="19"/>
+      <c r="A361" s="19" t="s">
+        <v>1272</v>
+      </c>
       <c r="B361" s="20"/>
-      <c r="C361" s="20"/>
-      <c r="D361" s="20"/>
+      <c r="C361" s="20" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D361" s="20" t="s">
+        <v>1274</v>
+      </c>
       <c r="E361" s="20"/>
       <c r="F361" s="20"/>
       <c r="G361" s="18"/>
@@ -18828,10 +18914,16 @@
       <c r="I361" s="18"/>
     </row>
     <row r="362" spans="1:9" ht="19" customHeight="1">
-      <c r="A362" s="19"/>
+      <c r="A362" s="19" t="s">
+        <v>1406</v>
+      </c>
       <c r="B362" s="20"/>
-      <c r="C362" s="20"/>
-      <c r="D362" s="20"/>
+      <c r="C362" s="20" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D362" s="20" t="s">
+        <v>1408</v>
+      </c>
       <c r="E362" s="20"/>
       <c r="F362" s="20"/>
       <c r="G362" s="18"/>
@@ -18839,10 +18931,16 @@
       <c r="I362" s="18"/>
     </row>
     <row r="363" spans="1:9" ht="19" customHeight="1">
-      <c r="A363" s="19"/>
+      <c r="A363" s="19" t="s">
+        <v>1409</v>
+      </c>
       <c r="B363" s="20"/>
-      <c r="C363" s="20"/>
-      <c r="D363" s="20"/>
+      <c r="C363" s="20" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D363" s="20" t="s">
+        <v>1411</v>
+      </c>
       <c r="E363" s="20"/>
       <c r="F363" s="20"/>
       <c r="G363" s="18"/>
@@ -18861,29 +18959,21 @@
       <c r="I364" s="18"/>
     </row>
     <row r="365" spans="1:9" ht="19" customHeight="1">
-      <c r="A365" s="26" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B365" s="23"/>
-      <c r="C365" s="23"/>
-      <c r="D365" s="23"/>
-      <c r="E365" s="23"/>
-      <c r="F365" s="23"/>
-      <c r="G365" s="24"/>
-      <c r="H365" s="25"/>
-      <c r="I365" s="24"/>
+      <c r="A365" s="19"/>
+      <c r="B365" s="20"/>
+      <c r="C365" s="20"/>
+      <c r="D365" s="20"/>
+      <c r="E365" s="20"/>
+      <c r="F365" s="20"/>
+      <c r="G365" s="18"/>
+      <c r="H365" s="17"/>
+      <c r="I365" s="18"/>
     </row>
     <row r="366" spans="1:9" ht="19" customHeight="1">
-      <c r="A366" s="19" t="s">
-        <v>1188</v>
-      </c>
+      <c r="A366" s="19"/>
       <c r="B366" s="20"/>
-      <c r="C366" s="20" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D366" s="20" t="s">
-        <v>1283</v>
-      </c>
+      <c r="C366" s="20"/>
+      <c r="D366" s="20"/>
       <c r="E366" s="20"/>
       <c r="F366" s="20"/>
       <c r="G366" s="18"/>
@@ -18891,16 +18981,10 @@
       <c r="I366" s="18"/>
     </row>
     <row r="367" spans="1:9" ht="19" customHeight="1">
-      <c r="A367" s="19" t="s">
-        <v>1189</v>
-      </c>
+      <c r="A367" s="19"/>
       <c r="B367" s="20"/>
-      <c r="C367" s="20" t="s">
-        <v>1189</v>
-      </c>
-      <c r="D367" s="20" t="s">
-        <v>1284</v>
-      </c>
+      <c r="C367" s="20"/>
+      <c r="D367" s="20"/>
       <c r="E367" s="20"/>
       <c r="F367" s="20"/>
       <c r="G367" s="18"/>
@@ -18908,16 +18992,10 @@
       <c r="I367" s="18"/>
     </row>
     <row r="368" spans="1:9" ht="19" customHeight="1">
-      <c r="A368" s="19" t="s">
-        <v>1190</v>
-      </c>
+      <c r="A368" s="19"/>
       <c r="B368" s="20"/>
-      <c r="C368" s="20" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D368" s="20" t="s">
-        <v>1286</v>
-      </c>
+      <c r="C368" s="20"/>
+      <c r="D368" s="20"/>
       <c r="E368" s="20"/>
       <c r="F368" s="20"/>
       <c r="G368" s="18"/>
@@ -18925,32 +19003,28 @@
       <c r="I368" s="18"/>
     </row>
     <row r="369" spans="1:9" ht="19" customHeight="1">
-      <c r="A369" s="19" t="s">
-        <v>1191</v>
-      </c>
-      <c r="B369" s="20"/>
-      <c r="C369" s="20" t="s">
-        <v>1191</v>
-      </c>
-      <c r="D369" s="20" t="s">
-        <v>1287</v>
-      </c>
-      <c r="E369" s="20"/>
-      <c r="F369" s="20"/>
-      <c r="G369" s="18"/>
-      <c r="H369" s="17"/>
-      <c r="I369" s="18"/>
+      <c r="A369" s="26" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B369" s="23"/>
+      <c r="C369" s="23"/>
+      <c r="D369" s="23"/>
+      <c r="E369" s="23"/>
+      <c r="F369" s="23"/>
+      <c r="G369" s="24"/>
+      <c r="H369" s="25"/>
+      <c r="I369" s="24"/>
     </row>
     <row r="370" spans="1:9" ht="19" customHeight="1">
       <c r="A370" s="19" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="B370" s="20"/>
       <c r="C370" s="20" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="D370" s="20" t="s">
-        <v>1288</v>
+        <v>1283</v>
       </c>
       <c r="E370" s="20"/>
       <c r="F370" s="20"/>
@@ -18960,14 +19034,14 @@
     </row>
     <row r="371" spans="1:9" ht="19" customHeight="1">
       <c r="A371" s="19" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="B371" s="20"/>
       <c r="C371" s="20" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="D371" s="20" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E371" s="20"/>
       <c r="F371" s="20"/>
@@ -18977,14 +19051,14 @@
     </row>
     <row r="372" spans="1:9" ht="19" customHeight="1">
       <c r="A372" s="19" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="B372" s="20"/>
       <c r="C372" s="20" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="D372" s="20" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="E372" s="20"/>
       <c r="F372" s="20"/>
@@ -18994,14 +19068,14 @@
     </row>
     <row r="373" spans="1:9" ht="19" customHeight="1">
       <c r="A373" s="19" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="B373" s="20"/>
       <c r="C373" s="20" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="D373" s="20" t="s">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="E373" s="20"/>
       <c r="F373" s="20"/>
@@ -19011,14 +19085,14 @@
     </row>
     <row r="374" spans="1:9" ht="19" customHeight="1">
       <c r="A374" s="19" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="B374" s="20"/>
       <c r="C374" s="20" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="D374" s="20" t="s">
-        <v>1291</v>
+        <v>1288</v>
       </c>
       <c r="E374" s="20"/>
       <c r="F374" s="20"/>
@@ -19028,14 +19102,14 @@
     </row>
     <row r="375" spans="1:9" ht="19" customHeight="1">
       <c r="A375" s="19" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="B375" s="20"/>
       <c r="C375" s="20" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="D375" s="20" t="s">
-        <v>1292</v>
+        <v>1285</v>
       </c>
       <c r="E375" s="20"/>
       <c r="F375" s="20"/>
@@ -19045,14 +19119,14 @@
     </row>
     <row r="376" spans="1:9" ht="19" customHeight="1">
       <c r="A376" s="19" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="B376" s="20"/>
       <c r="C376" s="20" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="D376" s="20" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="E376" s="20"/>
       <c r="F376" s="20"/>
@@ -19062,14 +19136,14 @@
     </row>
     <row r="377" spans="1:9" ht="19" customHeight="1">
       <c r="A377" s="19" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="B377" s="20"/>
       <c r="C377" s="20" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="D377" s="20" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="E377" s="20"/>
       <c r="F377" s="20"/>
@@ -19079,14 +19153,14 @@
     </row>
     <row r="378" spans="1:9" ht="19" customHeight="1">
       <c r="A378" s="19" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="B378" s="20"/>
       <c r="C378" s="20" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="D378" s="20" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="E378" s="20"/>
       <c r="F378" s="20"/>
@@ -19096,14 +19170,14 @@
     </row>
     <row r="379" spans="1:9" ht="19" customHeight="1">
       <c r="A379" s="19" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="B379" s="20"/>
       <c r="C379" s="20" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="D379" s="20" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="E379" s="20"/>
       <c r="F379" s="20"/>
@@ -19113,14 +19187,14 @@
     </row>
     <row r="380" spans="1:9" ht="19" customHeight="1">
       <c r="A380" s="19" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="B380" s="20"/>
       <c r="C380" s="20" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="D380" s="20" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="E380" s="20"/>
       <c r="F380" s="20"/>
@@ -19130,14 +19204,14 @@
     </row>
     <row r="381" spans="1:9" ht="19" customHeight="1">
       <c r="A381" s="19" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="B381" s="20"/>
       <c r="C381" s="20" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="D381" s="20" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="E381" s="20"/>
       <c r="F381" s="20"/>
@@ -19147,14 +19221,14 @@
     </row>
     <row r="382" spans="1:9" ht="19" customHeight="1">
       <c r="A382" s="19" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="B382" s="20"/>
       <c r="C382" s="20" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="D382" s="20" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="E382" s="20"/>
       <c r="F382" s="20"/>
@@ -19164,14 +19238,14 @@
     </row>
     <row r="383" spans="1:9" ht="19" customHeight="1">
       <c r="A383" s="19" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B383" s="20"/>
       <c r="C383" s="20" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="D383" s="20" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="E383" s="20"/>
       <c r="F383" s="20"/>
@@ -19181,14 +19255,14 @@
     </row>
     <row r="384" spans="1:9" ht="19" customHeight="1">
       <c r="A384" s="19" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="B384" s="20"/>
       <c r="C384" s="20" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="D384" s="20" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="E384" s="20"/>
       <c r="F384" s="20"/>
@@ -19198,14 +19272,14 @@
     </row>
     <row r="385" spans="1:9" ht="19" customHeight="1">
       <c r="A385" s="19" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="B385" s="20"/>
       <c r="C385" s="20" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="D385" s="20" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="E385" s="20"/>
       <c r="F385" s="20"/>
@@ -19215,14 +19289,14 @@
     </row>
     <row r="386" spans="1:9" ht="19" customHeight="1">
       <c r="A386" s="19" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="B386" s="20"/>
       <c r="C386" s="20" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="D386" s="20" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="E386" s="20"/>
       <c r="F386" s="20"/>
@@ -19232,14 +19306,14 @@
     </row>
     <row r="387" spans="1:9" ht="19" customHeight="1">
       <c r="A387" s="19" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="B387" s="20"/>
       <c r="C387" s="20" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="D387" s="20" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="E387" s="20"/>
       <c r="F387" s="20"/>
@@ -19249,14 +19323,14 @@
     </row>
     <row r="388" spans="1:9" ht="19" customHeight="1">
       <c r="A388" s="19" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="B388" s="20"/>
       <c r="C388" s="20" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="D388" s="20" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="E388" s="20"/>
       <c r="F388" s="20"/>
@@ -19266,14 +19340,14 @@
     </row>
     <row r="389" spans="1:9" ht="19" customHeight="1">
       <c r="A389" s="19" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="B389" s="20"/>
       <c r="C389" s="20" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="D389" s="20" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="E389" s="20"/>
       <c r="F389" s="20"/>
@@ -19283,14 +19357,14 @@
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
       <c r="A390" s="19" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="B390" s="20"/>
-      <c r="C390" s="19" t="s">
-        <v>1356</v>
+      <c r="C390" s="20" t="s">
+        <v>1208</v>
       </c>
       <c r="D390" s="20" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="E390" s="20"/>
       <c r="F390" s="20"/>
@@ -19300,14 +19374,14 @@
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
       <c r="A391" s="19" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="B391" s="20"/>
-      <c r="C391" s="19" t="s">
-        <v>1357</v>
+      <c r="C391" s="20" t="s">
+        <v>1209</v>
       </c>
       <c r="D391" s="20" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="E391" s="20"/>
       <c r="F391" s="20"/>
@@ -19317,14 +19391,14 @@
     </row>
     <row r="392" spans="1:9" ht="19" customHeight="1">
       <c r="A392" s="19" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="B392" s="20"/>
-      <c r="C392" s="19" t="s">
-        <v>1358</v>
+      <c r="C392" s="20" t="s">
+        <v>1210</v>
       </c>
       <c r="D392" s="20" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
@@ -19334,14 +19408,14 @@
     </row>
     <row r="393" spans="1:9" ht="19" customHeight="1">
       <c r="A393" s="19" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="B393" s="20"/>
-      <c r="C393" s="19" t="s">
-        <v>1359</v>
+      <c r="C393" s="20" t="s">
+        <v>1211</v>
       </c>
       <c r="D393" s="20" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
@@ -19351,14 +19425,14 @@
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
       <c r="A394" s="19" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="B394" s="20"/>
       <c r="C394" s="19" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="D394" s="20" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="E394" s="20"/>
       <c r="F394" s="20"/>
@@ -19368,14 +19442,14 @@
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
       <c r="A395" s="19" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="B395" s="20"/>
       <c r="C395" s="19" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="D395" s="20" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="E395" s="20"/>
       <c r="F395" s="20"/>
@@ -19385,14 +19459,14 @@
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
       <c r="A396" s="19" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="B396" s="20"/>
       <c r="C396" s="19" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="D396" s="20" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
@@ -19402,14 +19476,14 @@
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
       <c r="A397" s="19" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="B397" s="20"/>
       <c r="C397" s="19" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="D397" s="20" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="E397" s="20"/>
       <c r="F397" s="20"/>
@@ -19419,14 +19493,14 @@
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="19" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -19436,14 +19510,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="19" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -19453,14 +19527,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="19" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -19470,14 +19544,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="19" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -19487,14 +19561,14 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1260</v>
+        <v>1220</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="19" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="D402" s="20" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
@@ -19504,14 +19578,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="19" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -19521,14 +19595,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="19" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -19538,14 +19612,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="19" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -19555,14 +19629,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1227</v>
+        <v>1260</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="19" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -19572,14 +19646,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="19" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -19589,14 +19663,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="19" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -19606,14 +19680,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1261</v>
+        <v>1226</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="19" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -19623,14 +19697,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="19" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -19640,14 +19714,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="19" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -19657,14 +19731,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="19" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -19674,14 +19748,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1233</v>
+        <v>1261</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="19" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -19691,14 +19765,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="19" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -19708,14 +19782,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="19" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -19725,14 +19799,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1254</v>
+        <v>1232</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="19" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -19742,14 +19816,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1255</v>
+        <v>1233</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="19" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -19759,14 +19833,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1256</v>
+        <v>1234</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="19" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -19776,14 +19850,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1257</v>
+        <v>1235</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="19" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -19793,14 +19867,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="19" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -19810,14 +19884,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="19" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -19827,14 +19901,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1236</v>
+        <v>1256</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="19" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -19844,14 +19918,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1237</v>
+        <v>1257</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="19" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -19861,14 +19935,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1238</v>
+        <v>1258</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="19" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -19878,14 +19952,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1239</v>
+        <v>1259</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="19" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -19895,14 +19969,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="19" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -19912,14 +19986,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="19" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -19929,14 +20003,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="19" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -19946,14 +20020,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -19963,14 +20037,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -19980,14 +20054,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -19997,14 +20071,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -20014,14 +20088,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -20031,14 +20105,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>
@@ -20048,14 +20122,14 @@
     </row>
     <row r="435" spans="1:9" ht="19" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="19" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="E435" s="20"/>
       <c r="F435" s="20"/>
@@ -20065,14 +20139,14 @@
     </row>
     <row r="436" spans="1:9" ht="19" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="19" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="D436" s="20" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="E436" s="20"/>
       <c r="F436" s="20"/>
@@ -20082,14 +20156,14 @@
     </row>
     <row r="437" spans="1:9" ht="19" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="19" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
       <c r="D437" s="20" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="E437" s="20"/>
       <c r="F437" s="20"/>
@@ -20099,14 +20173,14 @@
     </row>
     <row r="438" spans="1:9" ht="19" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="19" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="D438" s="20" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="E438" s="20"/>
       <c r="F438" s="20"/>
@@ -20116,14 +20190,14 @@
     </row>
     <row r="439" spans="1:9" ht="19" customHeight="1">
       <c r="A439" s="19" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="B439" s="20"/>
       <c r="C439" s="19" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="D439" s="20" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="E439" s="20"/>
       <c r="F439" s="20"/>
@@ -20132,10 +20206,16 @@
       <c r="I439" s="18"/>
     </row>
     <row r="440" spans="1:9" ht="19" customHeight="1">
-      <c r="A440" s="19"/>
+      <c r="A440" s="19" t="s">
+        <v>1250</v>
+      </c>
       <c r="B440" s="20"/>
-      <c r="C440" s="20"/>
-      <c r="D440" s="20"/>
+      <c r="C440" s="19" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D440" s="20" t="s">
+        <v>1352</v>
+      </c>
       <c r="E440" s="20"/>
       <c r="F440" s="20"/>
       <c r="G440" s="18"/>
@@ -20143,10 +20223,16 @@
       <c r="I440" s="18"/>
     </row>
     <row r="441" spans="1:9" ht="19" customHeight="1">
-      <c r="A441" s="19"/>
+      <c r="A441" s="19" t="s">
+        <v>1251</v>
+      </c>
       <c r="B441" s="20"/>
-      <c r="C441" s="20"/>
-      <c r="D441" s="20"/>
+      <c r="C441" s="19" t="s">
+        <v>1403</v>
+      </c>
+      <c r="D441" s="20" t="s">
+        <v>1353</v>
+      </c>
       <c r="E441" s="20"/>
       <c r="F441" s="20"/>
       <c r="G441" s="18"/>
@@ -20154,10 +20240,16 @@
       <c r="I441" s="18"/>
     </row>
     <row r="442" spans="1:9" ht="19" customHeight="1">
-      <c r="A442" s="19"/>
+      <c r="A442" s="19" t="s">
+        <v>1252</v>
+      </c>
       <c r="B442" s="20"/>
-      <c r="C442" s="20"/>
-      <c r="D442" s="20"/>
+      <c r="C442" s="19" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D442" s="20" t="s">
+        <v>1354</v>
+      </c>
       <c r="E442" s="20"/>
       <c r="F442" s="20"/>
       <c r="G442" s="18"/>
@@ -20165,10 +20257,16 @@
       <c r="I442" s="18"/>
     </row>
     <row r="443" spans="1:9" ht="19" customHeight="1">
-      <c r="A443" s="19"/>
+      <c r="A443" s="19" t="s">
+        <v>1253</v>
+      </c>
       <c r="B443" s="20"/>
-      <c r="C443" s="20"/>
-      <c r="D443" s="20"/>
+      <c r="C443" s="19" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D443" s="20" t="s">
+        <v>1355</v>
+      </c>
       <c r="E443" s="20"/>
       <c r="F443" s="20"/>
       <c r="G443" s="18"/>
@@ -20780,80 +20878,124 @@
       <c r="H498" s="17"/>
       <c r="I498" s="18"/>
     </row>
+    <row r="499" spans="1:9" ht="19" customHeight="1">
+      <c r="A499" s="19"/>
+      <c r="B499" s="20"/>
+      <c r="C499" s="20"/>
+      <c r="D499" s="20"/>
+      <c r="E499" s="20"/>
+      <c r="F499" s="20"/>
+      <c r="G499" s="18"/>
+      <c r="H499" s="17"/>
+      <c r="I499" s="18"/>
+    </row>
+    <row r="500" spans="1:9" ht="19" customHeight="1">
+      <c r="A500" s="19"/>
+      <c r="B500" s="20"/>
+      <c r="C500" s="20"/>
+      <c r="D500" s="20"/>
+      <c r="E500" s="20"/>
+      <c r="F500" s="20"/>
+      <c r="G500" s="18"/>
+      <c r="H500" s="17"/>
+      <c r="I500" s="18"/>
+    </row>
+    <row r="501" spans="1:9" ht="19" customHeight="1">
+      <c r="A501" s="19"/>
+      <c r="B501" s="20"/>
+      <c r="C501" s="20"/>
+      <c r="D501" s="20"/>
+      <c r="E501" s="20"/>
+      <c r="F501" s="20"/>
+      <c r="G501" s="18"/>
+      <c r="H501" s="17"/>
+      <c r="I501" s="18"/>
+    </row>
+    <row r="502" spans="1:9" ht="19" customHeight="1">
+      <c r="A502" s="19"/>
+      <c r="B502" s="20"/>
+      <c r="C502" s="20"/>
+      <c r="D502" s="20"/>
+      <c r="E502" s="20"/>
+      <c r="F502" s="20"/>
+      <c r="G502" s="18"/>
+      <c r="H502" s="17"/>
+      <c r="I502" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J221" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A5:G236 I5:I498">
+  <conditionalFormatting sqref="A5:G240 I5:I502">
     <cfRule type="expression" dxfId="39" priority="37">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D237:D258 D261 D265:D267 D271:D275 D284 D292:D305 D309:D311 D315:D316 D318:D320 D324:D345">
+  <conditionalFormatting sqref="D241:D262 D265 D269:D271 D275:D279 D288 D296:D309 D313:D315 D319:D320 D322:D324 D328:D349">
     <cfRule type="expression" dxfId="38" priority="276">
-      <formula>$G239&lt;&gt;""</formula>
+      <formula>$G243&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D259">
+  <conditionalFormatting sqref="D263">
     <cfRule type="expression" dxfId="37" priority="315">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D260">
+  <conditionalFormatting sqref="D264">
     <cfRule type="expression" dxfId="36" priority="314">
-      <formula>$G261&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D262:D264 D268:D270 D283 D306:D308 D312:D314 D321:D323">
-    <cfRule type="expression" dxfId="35" priority="279">
       <formula>$G265&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D276:D282">
-    <cfRule type="expression" dxfId="34" priority="317">
-      <formula>$G284&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D266:D268 D272:D274 D287 D310:D312 D316:D318 D325:D327">
+    <cfRule type="expression" dxfId="35" priority="279">
+      <formula>$G269&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D279">
-    <cfRule type="expression" dxfId="33" priority="351">
-      <formula>$G284&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D280:D286">
+    <cfRule type="expression" dxfId="34" priority="317">
+      <formula>$G288&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D280:D282">
-    <cfRule type="expression" dxfId="32" priority="388">
-      <formula>$G284&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D283">
+    <cfRule type="expression" dxfId="33" priority="351">
+      <formula>$G288&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D285">
-    <cfRule type="expression" dxfId="31" priority="386">
-      <formula>$G292&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D284:D286">
+    <cfRule type="expression" dxfId="32" priority="388">
+      <formula>$G288&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D286">
-    <cfRule type="expression" dxfId="30" priority="283">
-      <formula>$G290&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D287:D289">
-    <cfRule type="expression" dxfId="29" priority="13">
-      <formula>$G287&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D289">
+    <cfRule type="expression" dxfId="31" priority="386">
+      <formula>$G296&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D290">
-    <cfRule type="expression" dxfId="28" priority="384">
-      <formula>$G295&lt;&gt;""</formula>
+    <cfRule type="expression" dxfId="30" priority="283">
+      <formula>$G294&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D317">
+  <conditionalFormatting sqref="D291:D293">
+    <cfRule type="expression" dxfId="29" priority="13">
+      <formula>$G291&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D294">
+    <cfRule type="expression" dxfId="28" priority="384">
+      <formula>$G299&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D321">
     <cfRule type="expression" dxfId="27" priority="383">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E237:G237 A237:C249 E238:E249 F238:G276 A250:E251 A252:C273 E252:E273 A274:E275 E276 A276:C308 E277:G289 E290:E308 F290:G348 D291 A309:E310 A311:C330 E311:E330 A331:E332 A333:C345 E333:E345 A346:E348 A349:G498">
+  <conditionalFormatting sqref="E241:G241 A241:C253 E242:E253 F242:G280 A254:E255 A256:C277 E256:E277 A278:E279 E280 A280:C312 E281:G293 E294:E312 F294:G352 D295 A313:E314 A315:C334 E315:E334 A335:E336 A337:C349 E337:E349 A350:E352 A353:G502">
     <cfRule type="expression" dxfId="26" priority="274">
-      <formula>$G237&lt;&gt;""</formula>
+      <formula>$G241&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H498">
+  <conditionalFormatting sqref="H5:H502">
     <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
@@ -20885,15 +21027,15 @@
       <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H365">
+  <conditionalFormatting sqref="H369">
     <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H365)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H369)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H365)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SKIP",H369)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H365)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ERROR",H369)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>

</xml_diff>

<commit_message>
Function renamed  suppressWithScroll -> withoutScroll
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA03BC95-E06E-C64F-93EC-1DF4EF93B685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DB8C5-3297-5243-B5F5-45F11E832EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17040" yWindow="6460" windowWidth="36000" windowHeight="20800" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -8725,25 +8725,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>suppressWithScroll</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>suppressWithScroll()</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Suppress withScroll</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>withScrollを抑制する</t>
-    <rPh sb="11" eb="13">
-      <t>ヨクセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>existWithScrollRight</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -11663,6 +11644,25 @@
   </si>
   <si>
     <t>cell</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>withoutScroll</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>withoutScroll()</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Without withScroll</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スクロールせずに実行する</t>
+    <rPh sb="8" eb="10">
+      <t>ジッコウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12053,6 +12053,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
@@ -12067,42 +12123,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12116,7 +12137,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12166,27 +12187,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12607,8 +12607,8 @@
   <dimension ref="A1:I519"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <pane ySplit="4" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -12676,13 +12676,13 @@
         <v>856</v>
       </c>
       <c r="B6" s="20" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>1390</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>1392</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>1394</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -12695,13 +12695,13 @@
         <v>857</v>
       </c>
       <c r="B7" s="20" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>1391</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>1393</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>1395</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -13053,16 +13053,16 @@
     </row>
     <row r="26" spans="1:9" ht="19" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>1492</v>
+        <v>1488</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
@@ -13072,16 +13072,16 @@
     </row>
     <row r="27" spans="1:9" ht="19" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
@@ -13230,10 +13230,10 @@
         <v>787</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
@@ -13243,16 +13243,16 @@
     </row>
     <row r="36" spans="1:9" ht="19" customHeight="1">
       <c r="A36" s="19" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>1075</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>1079</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
@@ -13262,16 +13262,16 @@
     </row>
     <row r="37" spans="1:9" ht="19" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
@@ -13338,16 +13338,16 @@
     </row>
     <row r="41" spans="1:9" ht="19" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="20"/>
@@ -13357,16 +13357,16 @@
     </row>
     <row r="42" spans="1:9" ht="19" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
@@ -13433,16 +13433,16 @@
     </row>
     <row r="46" spans="1:9" ht="19" customHeight="1">
       <c r="A46" s="19" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C46" s="20" t="s">
         <v>1040</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="D46" s="20" t="s">
         <v>1042</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>1046</v>
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="20"/>
@@ -13452,16 +13452,16 @@
     </row>
     <row r="47" spans="1:9" ht="19" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C47" s="20" t="s">
         <v>1041</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="D47" s="20" t="s">
         <v>1043</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>1047</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="20"/>
@@ -13547,16 +13547,16 @@
     </row>
     <row r="52" spans="1:9" ht="19" customHeight="1">
       <c r="A52" s="19" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
@@ -13604,16 +13604,16 @@
     </row>
     <row r="55" spans="1:9" ht="19" customHeight="1">
       <c r="A55" s="19" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C55" s="20" t="s">
         <v>1032</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="D55" s="20" t="s">
         <v>1034</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>1036</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>1038</v>
       </c>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -13623,16 +13623,16 @@
     </row>
     <row r="56" spans="1:9" ht="19" customHeight="1">
       <c r="A56" s="19" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C56" s="20" t="s">
         <v>1033</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="D56" s="20" t="s">
         <v>1035</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>1039</v>
       </c>
       <c r="E56" s="20"/>
       <c r="F56" s="20"/>
@@ -13642,13 +13642,13 @@
     </row>
     <row r="57" spans="1:9" ht="19" customHeight="1">
       <c r="A57" s="19" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>182</v>
@@ -13680,16 +13680,16 @@
     </row>
     <row r="59" spans="1:9" ht="19" customHeight="1">
       <c r="A59" s="19" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="20"/>
@@ -13927,7 +13927,7 @@
     </row>
     <row r="72" spans="1:9" ht="19" customHeight="1">
       <c r="A72" s="19" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="B72" s="20" t="s">
         <v>868</v>
@@ -14367,13 +14367,13 @@
         <v>96</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="E95" s="20"/>
       <c r="F95" s="20"/>
@@ -14383,16 +14383,16 @@
     </row>
     <row r="96" spans="1:9" ht="19" customHeight="1">
       <c r="A96" s="19" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="E96" s="20"/>
       <c r="F96" s="20"/>
@@ -14402,16 +14402,16 @@
     </row>
     <row r="97" spans="1:9" ht="19" customHeight="1">
       <c r="A97" s="19" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="D97" s="21" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="E97" s="20"/>
       <c r="F97" s="20"/>
@@ -14763,16 +14763,16 @@
     </row>
     <row r="116" spans="1:9" ht="19" customHeight="1">
       <c r="A116" s="19" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C116" s="20" t="s">
         <v>1161</v>
       </c>
-      <c r="B116" s="20" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C116" s="20" t="s">
-        <v>1165</v>
-      </c>
       <c r="D116" s="20" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="E116" s="20"/>
       <c r="F116" s="20"/>
@@ -14782,16 +14782,16 @@
     </row>
     <row r="117" spans="1:9" ht="19" customHeight="1">
       <c r="A117" s="19" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B117" s="20" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C117" s="20" t="s">
         <v>1162</v>
       </c>
-      <c r="B117" s="20" t="s">
-        <v>1164</v>
-      </c>
-      <c r="C117" s="20" t="s">
-        <v>1166</v>
-      </c>
       <c r="D117" s="20" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="E117" s="20"/>
       <c r="F117" s="20"/>
@@ -14801,16 +14801,16 @@
     </row>
     <row r="118" spans="1:9" ht="19" customHeight="1">
       <c r="A118" s="19" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B118" s="20" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C118" s="20" t="s">
         <v>1153</v>
       </c>
-      <c r="B118" s="20" t="s">
+      <c r="D118" s="20" t="s">
         <v>1155</v>
-      </c>
-      <c r="C118" s="20" t="s">
-        <v>1157</v>
-      </c>
-      <c r="D118" s="20" t="s">
-        <v>1159</v>
       </c>
       <c r="E118" s="20"/>
       <c r="F118" s="20"/>
@@ -14820,16 +14820,16 @@
     </row>
     <row r="119" spans="1:9" ht="19" customHeight="1">
       <c r="A119" s="19" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C119" s="20" t="s">
         <v>1154</v>
       </c>
-      <c r="B119" s="20" t="s">
+      <c r="D119" s="20" t="s">
         <v>1156</v>
-      </c>
-      <c r="C119" s="20" t="s">
-        <v>1158</v>
-      </c>
-      <c r="D119" s="20" t="s">
-        <v>1160</v>
       </c>
       <c r="E119" s="20"/>
       <c r="F119" s="20"/>
@@ -15057,7 +15057,7 @@
         <v>136</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
       <c r="E131" s="20"/>
       <c r="F131" s="20"/>
@@ -15076,7 +15076,7 @@
         <v>138</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
@@ -15095,7 +15095,7 @@
         <v>140</v>
       </c>
       <c r="D133" s="20" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="E133" s="20"/>
       <c r="F133" s="20"/>
@@ -15114,7 +15114,7 @@
         <v>142</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
       <c r="E134" s="20"/>
       <c r="F134" s="20"/>
@@ -15133,7 +15133,7 @@
         <v>17</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>1473</v>
+        <v>1469</v>
       </c>
       <c r="E135" s="20"/>
       <c r="F135" s="20"/>
@@ -15152,7 +15152,7 @@
         <v>145</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>1474</v>
+        <v>1470</v>
       </c>
       <c r="E136" s="20"/>
       <c r="F136" s="20"/>
@@ -15171,7 +15171,7 @@
         <v>19</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>1475</v>
+        <v>1471</v>
       </c>
       <c r="E137" s="20"/>
       <c r="F137" s="20"/>
@@ -15190,7 +15190,7 @@
         <v>148</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="E138" s="20"/>
       <c r="F138" s="20"/>
@@ -15209,7 +15209,7 @@
         <v>150</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
       <c r="E139" s="20"/>
       <c r="F139" s="20"/>
@@ -15228,7 +15228,7 @@
         <v>152</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>1478</v>
+        <v>1474</v>
       </c>
       <c r="E140" s="20"/>
       <c r="F140" s="20"/>
@@ -15247,7 +15247,7 @@
         <v>154</v>
       </c>
       <c r="D141" s="20" t="s">
-        <v>1479</v>
+        <v>1475</v>
       </c>
       <c r="E141" s="20"/>
       <c r="F141" s="20"/>
@@ -15266,7 +15266,7 @@
         <v>156</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>1480</v>
+        <v>1476</v>
       </c>
       <c r="E142" s="20"/>
       <c r="F142" s="20"/>
@@ -15833,7 +15833,7 @@
         <v>436</v>
       </c>
       <c r="C172" s="20" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="D172" s="22" t="s">
         <v>354</v>
@@ -15852,7 +15852,7 @@
         <v>443</v>
       </c>
       <c r="C173" s="20" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="D173" s="22" t="s">
         <v>361</v>
@@ -15871,7 +15871,7 @@
         <v>437</v>
       </c>
       <c r="C174" s="20" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="D174" s="22" t="s">
         <v>355</v>
@@ -15890,7 +15890,7 @@
         <v>438</v>
       </c>
       <c r="C175" s="20" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="D175" s="22" t="s">
         <v>356</v>
@@ -15909,7 +15909,7 @@
         <v>439</v>
       </c>
       <c r="C176" s="20" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="D176" s="22" t="s">
         <v>357</v>
@@ -15928,7 +15928,7 @@
         <v>440</v>
       </c>
       <c r="C177" s="20" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="D177" s="22" t="s">
         <v>358</v>
@@ -15947,7 +15947,7 @@
         <v>441</v>
       </c>
       <c r="C178" s="20" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="D178" s="22" t="s">
         <v>359</v>
@@ -15966,7 +15966,7 @@
         <v>442</v>
       </c>
       <c r="C179" s="20" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="D179" s="22" t="s">
         <v>360</v>
@@ -16055,16 +16055,16 @@
     </row>
     <row r="184" spans="1:9" ht="19" customHeight="1">
       <c r="A184" s="19" t="s">
-        <v>1028</v>
+        <v>1489</v>
       </c>
       <c r="B184" s="19" t="s">
-        <v>1029</v>
+        <v>1490</v>
       </c>
       <c r="C184" s="20" t="s">
-        <v>1030</v>
+        <v>1491</v>
       </c>
       <c r="D184" s="20" t="s">
-        <v>1031</v>
+        <v>1492</v>
       </c>
       <c r="E184" s="20"/>
       <c r="F184" s="20"/>
@@ -16080,7 +16080,7 @@
         <v>448</v>
       </c>
       <c r="C185" s="20" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="D185" s="22" t="s">
         <v>364</v>
@@ -16099,7 +16099,7 @@
         <v>449</v>
       </c>
       <c r="C186" s="20" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="D186" s="22" t="s">
         <v>865</v>
@@ -16118,7 +16118,7 @@
         <v>454</v>
       </c>
       <c r="C187" s="20" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="D187" s="22" t="s">
         <v>370</v>
@@ -16137,7 +16137,7 @@
         <v>455</v>
       </c>
       <c r="C188" s="20" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="D188" s="22" t="s">
         <v>371</v>
@@ -16156,7 +16156,7 @@
         <v>450</v>
       </c>
       <c r="C189" s="20" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="D189" s="22" t="s">
         <v>365</v>
@@ -16175,7 +16175,7 @@
         <v>451</v>
       </c>
       <c r="C190" s="20" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="D190" s="22" t="s">
         <v>366</v>
@@ -16194,7 +16194,7 @@
         <v>452</v>
       </c>
       <c r="C191" s="20" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="D191" s="22" t="s">
         <v>367</v>
@@ -16213,7 +16213,7 @@
         <v>453</v>
       </c>
       <c r="C192" s="20" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="D192" s="22" t="s">
         <v>368</v>
@@ -16802,10 +16802,10 @@
         <v>424</v>
       </c>
       <c r="C223" s="20" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="D223" s="20" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="E223" s="20"/>
       <c r="F223" s="20"/>
@@ -16821,10 +16821,10 @@
         <v>424</v>
       </c>
       <c r="C224" s="20" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="D224" s="20" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="E224" s="20"/>
       <c r="F224" s="20"/>
@@ -16834,16 +16834,16 @@
     </row>
     <row r="225" spans="1:9" ht="19" customHeight="1">
       <c r="A225" s="19" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="B225" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C225" s="20" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
       <c r="D225" s="20" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="E225" s="20"/>
       <c r="F225" s="20"/>
@@ -16853,16 +16853,16 @@
     </row>
     <row r="226" spans="1:9" ht="19" customHeight="1">
       <c r="A226" s="19" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="B226" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C226" s="20" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="D226" s="20" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="E226" s="20"/>
       <c r="F226" s="20"/>
@@ -16872,16 +16872,16 @@
     </row>
     <row r="227" spans="1:9" ht="19" customHeight="1">
       <c r="A227" s="19" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
       <c r="B227" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C227" s="20" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="D227" s="20" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="E227" s="20"/>
       <c r="F227" s="20"/>
@@ -16891,16 +16891,16 @@
     </row>
     <row r="228" spans="1:9" ht="19" customHeight="1">
       <c r="A228" s="19" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="B228" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="D228" s="20" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
       <c r="E228" s="20"/>
       <c r="F228" s="20"/>
@@ -16910,16 +16910,16 @@
     </row>
     <row r="229" spans="1:9" ht="19" customHeight="1">
       <c r="A229" s="19" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="B229" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C229" s="20" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="D229" s="20" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="E229" s="20"/>
       <c r="F229" s="20"/>
@@ -16929,16 +16929,16 @@
     </row>
     <row r="230" spans="1:9" ht="19" customHeight="1">
       <c r="A230" s="19" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="B230" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C230" s="20" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="D230" s="20" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
       <c r="E230" s="20"/>
       <c r="F230" s="20"/>
@@ -16948,16 +16948,16 @@
     </row>
     <row r="231" spans="1:9" ht="19" customHeight="1">
       <c r="A231" s="19" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="B231" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C231" s="20" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="D231" s="20" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="E231" s="20"/>
       <c r="F231" s="20"/>
@@ -16967,16 +16967,16 @@
     </row>
     <row r="232" spans="1:9" ht="19" customHeight="1">
       <c r="A232" s="19" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="B232" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C232" s="20" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="D232" s="20" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
       <c r="E232" s="20"/>
       <c r="F232" s="20"/>
@@ -16986,16 +16986,16 @@
     </row>
     <row r="233" spans="1:9" ht="19" customHeight="1">
       <c r="A233" s="19" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="B233" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C233" s="20" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="D233" s="20" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
       <c r="E233" s="20"/>
       <c r="F233" s="20"/>
@@ -17005,16 +17005,16 @@
     </row>
     <row r="234" spans="1:9" ht="19" customHeight="1">
       <c r="A234" s="19" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="B234" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C234" s="20" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="D234" s="20" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="E234" s="20"/>
       <c r="F234" s="20"/>
@@ -17024,16 +17024,16 @@
     </row>
     <row r="235" spans="1:9" ht="19" customHeight="1">
       <c r="A235" s="19" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="B235" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C235" s="20" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="D235" s="20" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="E235" s="20"/>
       <c r="F235" s="20"/>
@@ -17043,16 +17043,16 @@
     </row>
     <row r="236" spans="1:9" ht="19" customHeight="1">
       <c r="A236" s="19" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
       <c r="B236" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C236" s="20" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="D236" s="20" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
       <c r="E236" s="20"/>
       <c r="F236" s="20"/>
@@ -17062,16 +17062,16 @@
     </row>
     <row r="237" spans="1:9" ht="19" customHeight="1">
       <c r="A237" s="19" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="B237" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C237" s="20" t="s">
-        <v>1436</v>
+        <v>1432</v>
       </c>
       <c r="D237" s="20" t="s">
-        <v>1437</v>
+        <v>1433</v>
       </c>
       <c r="E237" s="20"/>
       <c r="F237" s="20"/>
@@ -17081,16 +17081,16 @@
     </row>
     <row r="238" spans="1:9" ht="19" customHeight="1">
       <c r="A238" s="19" t="s">
-        <v>1438</v>
+        <v>1434</v>
       </c>
       <c r="B238" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C238" s="20" t="s">
-        <v>1447</v>
+        <v>1443</v>
       </c>
       <c r="D238" s="20" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
       <c r="E238" s="20"/>
       <c r="F238" s="20"/>
@@ -17100,16 +17100,16 @@
     </row>
     <row r="239" spans="1:9" ht="19" customHeight="1">
       <c r="A239" s="19" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
       <c r="B239" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C239" s="20" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
       <c r="D239" s="20" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="E239" s="20"/>
       <c r="F239" s="20"/>
@@ -17119,16 +17119,16 @@
     </row>
     <row r="240" spans="1:9" ht="19" customHeight="1">
       <c r="A240" s="19" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
       <c r="B240" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C240" s="20" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="D240" s="20" t="s">
-        <v>1458</v>
+        <v>1454</v>
       </c>
       <c r="E240" s="20"/>
       <c r="F240" s="20"/>
@@ -17138,16 +17138,16 @@
     </row>
     <row r="241" spans="1:9" ht="19" customHeight="1">
       <c r="A241" s="19" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
       <c r="B241" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C241" s="20" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="D241" s="20" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
       <c r="E241" s="20"/>
       <c r="F241" s="20"/>
@@ -17157,16 +17157,16 @@
     </row>
     <row r="242" spans="1:9" ht="19" customHeight="1">
       <c r="A242" s="19" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
       <c r="B242" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C242" s="20" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="D242" s="20" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="E242" s="20"/>
       <c r="F242" s="20"/>
@@ -17176,16 +17176,16 @@
     </row>
     <row r="243" spans="1:9" ht="19" customHeight="1">
       <c r="A243" s="19" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
       <c r="B243" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C243" s="20" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
       <c r="D243" s="20" t="s">
-        <v>1461</v>
+        <v>1457</v>
       </c>
       <c r="E243" s="20"/>
       <c r="F243" s="20"/>
@@ -17195,16 +17195,16 @@
     </row>
     <row r="244" spans="1:9" ht="19" customHeight="1">
       <c r="A244" s="19" t="s">
-        <v>1444</v>
+        <v>1440</v>
       </c>
       <c r="B244" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C244" s="20" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="D244" s="20" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="E244" s="20"/>
       <c r="F244" s="20"/>
@@ -17214,16 +17214,16 @@
     </row>
     <row r="245" spans="1:9" ht="19" customHeight="1">
       <c r="A245" s="19" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="B245" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C245" s="20" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="D245" s="20" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
       <c r="E245" s="20"/>
       <c r="F245" s="20"/>
@@ -17233,16 +17233,16 @@
     </row>
     <row r="246" spans="1:9" ht="19" customHeight="1">
       <c r="A246" s="19" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="B246" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C246" s="20" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="D246" s="20" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="E246" s="20"/>
       <c r="F246" s="20"/>
@@ -17252,16 +17252,16 @@
     </row>
     <row r="247" spans="1:9" ht="19" customHeight="1">
       <c r="A247" s="19" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="B247" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C247" s="20" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
       <c r="D247" s="20" t="s">
-        <v>1469</v>
+        <v>1465</v>
       </c>
       <c r="E247" s="20"/>
       <c r="F247" s="20"/>
@@ -17271,16 +17271,16 @@
     </row>
     <row r="248" spans="1:9" ht="19" customHeight="1">
       <c r="A248" s="19" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
       <c r="B248" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C248" s="20" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="D248" s="20" t="s">
-        <v>1470</v>
+        <v>1466</v>
       </c>
       <c r="E248" s="20"/>
       <c r="F248" s="20"/>
@@ -17387,14 +17387,14 @@
     </row>
     <row r="256" spans="1:9" ht="19" customHeight="1">
       <c r="A256" s="19" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="B256" s="20"/>
       <c r="C256" s="20" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D256" s="20" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="E256" s="20"/>
       <c r="F256" s="20"/>
@@ -17697,10 +17697,10 @@
       </c>
       <c r="B274" s="20"/>
       <c r="C274" s="20" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="D274" s="20" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="E274" s="20"/>
       <c r="F274" s="20"/>
@@ -17982,14 +17982,14 @@
     </row>
     <row r="291" spans="1:9" ht="19" customHeight="1">
       <c r="A291" s="19" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="B291" s="20"/>
       <c r="C291" s="20" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="D291" s="20" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="E291" s="20"/>
       <c r="F291" s="20"/>
@@ -18105,7 +18105,7 @@
       </c>
       <c r="B298" s="20"/>
       <c r="C298" s="20" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="D298" s="20" t="s">
         <v>697</v>
@@ -18118,14 +18118,14 @@
     </row>
     <row r="299" spans="1:9" ht="19" customHeight="1">
       <c r="A299" s="19" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="B299" s="20"/>
       <c r="C299" s="20" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="D299" s="20" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="E299" s="20"/>
       <c r="F299" s="20"/>
@@ -18135,14 +18135,14 @@
     </row>
     <row r="300" spans="1:9" ht="19" customHeight="1">
       <c r="A300" s="19" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="B300" s="20"/>
       <c r="C300" s="20" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="D300" s="22" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="E300" s="20"/>
       <c r="F300" s="20"/>
@@ -18152,14 +18152,14 @@
     </row>
     <row r="301" spans="1:9" ht="19" customHeight="1">
       <c r="A301" s="19" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="B301" s="20"/>
       <c r="C301" s="20" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="D301" s="22" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="E301" s="20"/>
       <c r="F301" s="20"/>
@@ -18169,14 +18169,14 @@
     </row>
     <row r="302" spans="1:9" ht="19" customHeight="1">
       <c r="A302" s="19" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="B302" s="20"/>
       <c r="C302" s="20" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="D302" s="22" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="E302" s="20"/>
       <c r="F302" s="20"/>
@@ -18186,14 +18186,14 @@
     </row>
     <row r="303" spans="1:9" ht="19" customHeight="1">
       <c r="A303" s="19" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="B303" s="20"/>
       <c r="C303" s="20" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="D303" s="22" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="E303" s="20"/>
       <c r="F303" s="20"/>
@@ -18271,14 +18271,14 @@
     </row>
     <row r="308" spans="1:9" ht="19" customHeight="1">
       <c r="A308" s="19" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="B308" s="20"/>
       <c r="C308" s="20" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="D308" s="20" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="E308" s="20"/>
       <c r="F308" s="20"/>
@@ -18288,14 +18288,14 @@
     </row>
     <row r="309" spans="1:9" ht="19" customHeight="1">
       <c r="A309" s="19" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="B309" s="20"/>
       <c r="C309" s="20" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="D309" s="20" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="E309" s="20"/>
       <c r="F309" s="20"/>
@@ -18305,14 +18305,14 @@
     </row>
     <row r="310" spans="1:9" ht="19" customHeight="1">
       <c r="A310" s="19" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B310" s="20"/>
       <c r="C310" s="20" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="D310" s="20" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="E310" s="20"/>
       <c r="F310" s="20"/>
@@ -18346,7 +18346,7 @@
         <v>1009</v>
       </c>
       <c r="D312" s="20" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="E312" s="20"/>
       <c r="F312" s="20"/>
@@ -18373,14 +18373,14 @@
     </row>
     <row r="314" spans="1:9" ht="19" customHeight="1">
       <c r="A314" s="19" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="B314" s="20"/>
       <c r="C314" s="20" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="E314" s="20"/>
       <c r="F314" s="20"/>
@@ -18730,14 +18730,14 @@
     </row>
     <row r="335" spans="1:9" ht="19" customHeight="1">
       <c r="A335" s="19" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="B335" s="20"/>
       <c r="C335" s="20" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="D335" s="21" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="E335" s="20"/>
       <c r="F335" s="20"/>
@@ -19023,10 +19023,10 @@
       </c>
       <c r="B352" s="20"/>
       <c r="C352" s="20" t="s">
-        <v>1471</v>
+        <v>1467</v>
       </c>
       <c r="D352" s="21" t="s">
-        <v>1472</v>
+        <v>1468</v>
       </c>
       <c r="E352" s="20"/>
       <c r="F352" s="20"/>
@@ -19291,14 +19291,14 @@
     </row>
     <row r="368" spans="1:9" ht="19" customHeight="1">
       <c r="A368" s="19" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="B368" s="20"/>
       <c r="C368" s="20" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="D368" s="20" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="E368" s="20"/>
       <c r="F368" s="20"/>
@@ -19308,14 +19308,14 @@
     </row>
     <row r="369" spans="1:9" ht="19" customHeight="1">
       <c r="A369" s="19" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="B369" s="20"/>
       <c r="C369" s="20" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="D369" s="20" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="E369" s="20"/>
       <c r="F369" s="20"/>
@@ -19325,14 +19325,14 @@
     </row>
     <row r="370" spans="1:9" ht="19" customHeight="1">
       <c r="A370" s="19" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="B370" s="20"/>
       <c r="C370" s="20" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="D370" s="20" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="E370" s="20"/>
       <c r="F370" s="20"/>
@@ -19342,14 +19342,14 @@
     </row>
     <row r="371" spans="1:9" ht="19" customHeight="1">
       <c r="A371" s="19" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="B371" s="20"/>
       <c r="C371" s="20" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="D371" s="20" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="E371" s="20"/>
       <c r="F371" s="20"/>
@@ -19359,14 +19359,14 @@
     </row>
     <row r="372" spans="1:9" ht="19" customHeight="1">
       <c r="A372" s="19" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="B372" s="20"/>
       <c r="C372" s="20" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="D372" s="20" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="E372" s="20"/>
       <c r="F372" s="20"/>
@@ -19376,14 +19376,14 @@
     </row>
     <row r="373" spans="1:9" ht="19" customHeight="1">
       <c r="A373" s="19" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="B373" s="20"/>
       <c r="C373" s="20" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="D373" s="20" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="E373" s="20"/>
       <c r="F373" s="20"/>
@@ -19393,14 +19393,14 @@
     </row>
     <row r="374" spans="1:9" ht="19" customHeight="1">
       <c r="A374" s="19" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="B374" s="20"/>
       <c r="C374" s="20" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="D374" s="20" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="E374" s="20"/>
       <c r="F374" s="20"/>
@@ -19410,14 +19410,14 @@
     </row>
     <row r="375" spans="1:9" ht="19" customHeight="1">
       <c r="A375" s="19" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="B375" s="20"/>
       <c r="C375" s="20" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="D375" s="20" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="E375" s="20"/>
       <c r="F375" s="20"/>
@@ -19427,14 +19427,14 @@
     </row>
     <row r="376" spans="1:9" ht="19" customHeight="1">
       <c r="A376" s="19" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="B376" s="20"/>
       <c r="C376" s="20" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="D376" s="20" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="E376" s="20"/>
       <c r="F376" s="20"/>
@@ -19444,14 +19444,14 @@
     </row>
     <row r="377" spans="1:9" ht="19" customHeight="1">
       <c r="A377" s="19" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="B377" s="20"/>
       <c r="C377" s="20" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="D377" s="20" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="E377" s="20"/>
       <c r="F377" s="20"/>
@@ -19461,14 +19461,14 @@
     </row>
     <row r="378" spans="1:9" ht="19" customHeight="1">
       <c r="A378" s="19" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="B378" s="20"/>
       <c r="C378" s="20" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="D378" s="20" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="E378" s="20"/>
       <c r="F378" s="20"/>
@@ -19478,14 +19478,14 @@
     </row>
     <row r="379" spans="1:9" ht="19" customHeight="1">
       <c r="A379" s="19" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
       <c r="B379" s="20"/>
       <c r="C379" s="20" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="D379" s="20" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
       <c r="E379" s="20"/>
       <c r="F379" s="20"/>
@@ -19495,14 +19495,14 @@
     </row>
     <row r="380" spans="1:9" ht="19" customHeight="1">
       <c r="A380" s="19" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
       <c r="B380" s="20"/>
       <c r="C380" s="20" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
       <c r="D380" s="20" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="E380" s="20"/>
       <c r="F380" s="20"/>
@@ -19567,7 +19567,7 @@
     </row>
     <row r="386" spans="1:9" ht="19" customHeight="1">
       <c r="A386" s="26" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="B386" s="23"/>
       <c r="C386" s="23"/>
@@ -19580,14 +19580,14 @@
     </row>
     <row r="387" spans="1:9" ht="19" customHeight="1">
       <c r="A387" s="19" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="B387" s="20"/>
       <c r="C387" s="20" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="D387" s="20" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="E387" s="20"/>
       <c r="F387" s="20"/>
@@ -19597,14 +19597,14 @@
     </row>
     <row r="388" spans="1:9" ht="19" customHeight="1">
       <c r="A388" s="19" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="B388" s="20"/>
       <c r="C388" s="20" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="D388" s="20" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="E388" s="20"/>
       <c r="F388" s="20"/>
@@ -19614,14 +19614,14 @@
     </row>
     <row r="389" spans="1:9" ht="19" customHeight="1">
       <c r="A389" s="19" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="B389" s="20"/>
       <c r="C389" s="20" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="D389" s="20" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="E389" s="20"/>
       <c r="F389" s="20"/>
@@ -19631,14 +19631,14 @@
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
       <c r="A390" s="19" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="B390" s="20"/>
       <c r="C390" s="20" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="D390" s="20" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="E390" s="20"/>
       <c r="F390" s="20"/>
@@ -19648,14 +19648,14 @@
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
       <c r="A391" s="19" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="B391" s="20"/>
       <c r="C391" s="20" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="D391" s="20" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="E391" s="20"/>
       <c r="F391" s="20"/>
@@ -19665,14 +19665,14 @@
     </row>
     <row r="392" spans="1:9" ht="19" customHeight="1">
       <c r="A392" s="19" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="B392" s="20"/>
       <c r="C392" s="20" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="D392" s="20" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
@@ -19682,14 +19682,14 @@
     </row>
     <row r="393" spans="1:9" ht="19" customHeight="1">
       <c r="A393" s="19" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="B393" s="20"/>
       <c r="C393" s="20" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="D393" s="20" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
@@ -19699,14 +19699,14 @@
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
       <c r="A394" s="19" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="B394" s="20"/>
       <c r="C394" s="20" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="D394" s="20" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="E394" s="20"/>
       <c r="F394" s="20"/>
@@ -19716,14 +19716,14 @@
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
       <c r="A395" s="19" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="B395" s="20"/>
       <c r="C395" s="20" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="D395" s="20" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="E395" s="20"/>
       <c r="F395" s="20"/>
@@ -19733,14 +19733,14 @@
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
       <c r="A396" s="19" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="B396" s="20"/>
       <c r="C396" s="20" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="D396" s="20" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
@@ -19750,14 +19750,14 @@
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
       <c r="A397" s="19" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="B397" s="20"/>
       <c r="C397" s="20" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="D397" s="20" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="E397" s="20"/>
       <c r="F397" s="20"/>
@@ -19767,14 +19767,14 @@
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="20" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -19784,14 +19784,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="20" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -19801,14 +19801,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="20" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -19818,14 +19818,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="20" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -19835,14 +19835,14 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="20" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="D402" s="20" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
@@ -19852,14 +19852,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="20" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -19869,14 +19869,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="20" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -19886,14 +19886,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="20" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -19903,14 +19903,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="20" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -19920,14 +19920,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="20" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -19937,14 +19937,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="20" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -19954,14 +19954,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="20" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -19971,14 +19971,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="20" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -19988,14 +19988,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="19" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -20005,14 +20005,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="19" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -20022,14 +20022,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="19" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -20039,14 +20039,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="19" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -20056,14 +20056,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="19" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -20073,14 +20073,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="19" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -20090,14 +20090,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="19" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -20107,14 +20107,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="19" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -20124,14 +20124,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="19" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -20141,14 +20141,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="19" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -20158,14 +20158,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="19" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -20175,14 +20175,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="19" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -20192,14 +20192,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="19" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -20209,14 +20209,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="19" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -20226,14 +20226,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="19" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -20243,14 +20243,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="19" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -20260,14 +20260,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="19" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1488</v>
+        <v>1484</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -20277,14 +20277,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="19" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -20294,14 +20294,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -20311,14 +20311,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -20328,14 +20328,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -20345,14 +20345,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -20362,14 +20362,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -20379,14 +20379,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>
@@ -20396,14 +20396,14 @@
     </row>
     <row r="435" spans="1:9" ht="19" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="19" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="E435" s="20"/>
       <c r="F435" s="20"/>
@@ -20413,14 +20413,14 @@
     </row>
     <row r="436" spans="1:9" ht="19" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="19" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="D436" s="20" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="E436" s="20"/>
       <c r="F436" s="20"/>
@@ -20430,14 +20430,14 @@
     </row>
     <row r="437" spans="1:9" ht="19" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="19" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="D437" s="20" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="E437" s="20"/>
       <c r="F437" s="20"/>
@@ -20447,14 +20447,14 @@
     </row>
     <row r="438" spans="1:9" ht="19" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="19" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="D438" s="20" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="E438" s="20"/>
       <c r="F438" s="20"/>
@@ -20464,14 +20464,14 @@
     </row>
     <row r="439" spans="1:9" ht="19" customHeight="1">
       <c r="A439" s="19" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="B439" s="20"/>
       <c r="C439" s="19" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
       <c r="D439" s="20" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="E439" s="20"/>
       <c r="F439" s="20"/>
@@ -20481,14 +20481,14 @@
     </row>
     <row r="440" spans="1:9" ht="19" customHeight="1">
       <c r="A440" s="19" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="B440" s="20"/>
       <c r="C440" s="19" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
       <c r="D440" s="20" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="E440" s="20"/>
       <c r="F440" s="20"/>
@@ -20498,14 +20498,14 @@
     </row>
     <row r="441" spans="1:9" ht="19" customHeight="1">
       <c r="A441" s="19" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="B441" s="20"/>
       <c r="C441" s="19" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="D441" s="20" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="E441" s="20"/>
       <c r="F441" s="20"/>
@@ -20515,14 +20515,14 @@
     </row>
     <row r="442" spans="1:9" ht="19" customHeight="1">
       <c r="A442" s="19" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="B442" s="20"/>
       <c r="C442" s="19" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="D442" s="20" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="E442" s="20"/>
       <c r="F442" s="20"/>
@@ -20532,14 +20532,14 @@
     </row>
     <row r="443" spans="1:9" ht="19" customHeight="1">
       <c r="A443" s="19" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="B443" s="20"/>
       <c r="C443" s="19" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="D443" s="20" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="E443" s="20"/>
       <c r="F443" s="20"/>
@@ -20549,14 +20549,14 @@
     </row>
     <row r="444" spans="1:9" ht="19" customHeight="1">
       <c r="A444" s="19" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="B444" s="20"/>
       <c r="C444" s="19" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="D444" s="20" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="E444" s="20"/>
       <c r="F444" s="20"/>
@@ -20566,14 +20566,14 @@
     </row>
     <row r="445" spans="1:9" ht="19" customHeight="1">
       <c r="A445" s="19" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="B445" s="20"/>
       <c r="C445" s="19" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="D445" s="20" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="E445" s="20"/>
       <c r="F445" s="20"/>
@@ -20583,14 +20583,14 @@
     </row>
     <row r="446" spans="1:9" ht="19" customHeight="1">
       <c r="A446" s="19" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="B446" s="20"/>
       <c r="C446" s="19" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="D446" s="20" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="E446" s="20"/>
       <c r="F446" s="20"/>
@@ -20600,14 +20600,14 @@
     </row>
     <row r="447" spans="1:9" ht="19" customHeight="1">
       <c r="A447" s="19" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="B447" s="20"/>
       <c r="C447" s="19" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="D447" s="20" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="E447" s="20"/>
       <c r="F447" s="20"/>
@@ -20617,14 +20617,14 @@
     </row>
     <row r="448" spans="1:9" ht="19" customHeight="1">
       <c r="A448" s="19" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="B448" s="20"/>
       <c r="C448" s="19" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="D448" s="20" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
       <c r="E448" s="20"/>
       <c r="F448" s="20"/>
@@ -20634,14 +20634,14 @@
     </row>
     <row r="449" spans="1:9" ht="19" customHeight="1">
       <c r="A449" s="19" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="B449" s="20"/>
       <c r="C449" s="19" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="D449" s="20" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="E449" s="20"/>
       <c r="F449" s="20"/>
@@ -20651,14 +20651,14 @@
     </row>
     <row r="450" spans="1:9" ht="19" customHeight="1">
       <c r="A450" s="19" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="B450" s="20"/>
       <c r="C450" s="19" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="D450" s="20" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="E450" s="20"/>
       <c r="F450" s="20"/>
@@ -20668,14 +20668,14 @@
     </row>
     <row r="451" spans="1:9" ht="19" customHeight="1">
       <c r="A451" s="19" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="B451" s="20"/>
       <c r="C451" s="19" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="D451" s="20" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="E451" s="20"/>
       <c r="F451" s="20"/>
@@ -20685,14 +20685,14 @@
     </row>
     <row r="452" spans="1:9" ht="19" customHeight="1">
       <c r="A452" s="19" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="B452" s="20"/>
       <c r="C452" s="19" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="D452" s="20" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
       <c r="E452" s="20"/>
       <c r="F452" s="20"/>
@@ -20702,14 +20702,14 @@
     </row>
     <row r="453" spans="1:9" ht="19" customHeight="1">
       <c r="A453" s="19" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="B453" s="20"/>
       <c r="C453" s="19" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D453" s="20" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="E453" s="20"/>
       <c r="F453" s="20"/>
@@ -20719,14 +20719,14 @@
     </row>
     <row r="454" spans="1:9" ht="19" customHeight="1">
       <c r="A454" s="19" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="B454" s="20"/>
       <c r="C454" s="19" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
       <c r="D454" s="20" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="E454" s="20"/>
       <c r="F454" s="20"/>
@@ -20736,14 +20736,14 @@
     </row>
     <row r="455" spans="1:9" ht="19" customHeight="1">
       <c r="A455" s="19" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="B455" s="20"/>
       <c r="C455" s="19" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="D455" s="20" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="E455" s="20"/>
       <c r="F455" s="20"/>
@@ -20753,14 +20753,14 @@
     </row>
     <row r="456" spans="1:9" ht="19" customHeight="1">
       <c r="A456" s="19" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="B456" s="20"/>
       <c r="C456" s="19" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="D456" s="20" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="E456" s="20"/>
       <c r="F456" s="20"/>
@@ -20770,14 +20770,14 @@
     </row>
     <row r="457" spans="1:9" ht="19" customHeight="1">
       <c r="A457" s="19" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="B457" s="20"/>
       <c r="C457" s="19" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
       <c r="D457" s="20" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="E457" s="20"/>
       <c r="F457" s="20"/>
@@ -20787,14 +20787,14 @@
     </row>
     <row r="458" spans="1:9" ht="19" customHeight="1">
       <c r="A458" s="19" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="B458" s="20"/>
       <c r="C458" s="19" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
       <c r="D458" s="20" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="E458" s="20"/>
       <c r="F458" s="20"/>
@@ -20804,14 +20804,14 @@
     </row>
     <row r="459" spans="1:9" ht="19" customHeight="1">
       <c r="A459" s="19" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="B459" s="20"/>
       <c r="C459" s="19" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
       <c r="D459" s="20" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="E459" s="20"/>
       <c r="F459" s="20"/>
@@ -20821,14 +20821,14 @@
     </row>
     <row r="460" spans="1:9" ht="19" customHeight="1">
       <c r="A460" s="19" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="B460" s="20"/>
       <c r="C460" s="19" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
       <c r="D460" s="20" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="E460" s="20"/>
       <c r="F460" s="20"/>
@@ -21488,7 +21488,7 @@
   </sheetData>
   <autoFilter ref="A4:J222" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="I5:I519 A5:G257">
+  <conditionalFormatting sqref="A5:G257 I5:I519">
     <cfRule type="expression" dxfId="39" priority="37">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
@@ -21559,67 +21559,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H519">
-    <cfRule type="cellIs" dxfId="25" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H386">
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H386)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H386)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H386)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H386)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H386)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H386)))</formula>
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve - select in cell - Spec-Report indent
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DB8C5-3297-5243-B5F5-45F11E832EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F254D6C-0A45-AA47-89E4-AEB0E0FE641D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17040" yWindow="6460" windowWidth="36000" windowHeight="20800" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="1493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="1496">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11663,6 +11663,18 @@
     <rPh sb="8" eb="10">
       <t>ジッコウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cell("${subject}")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cell ${subject}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>セル ${subject}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12607,8 +12619,8 @@
   <dimension ref="A1:I519"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A184" sqref="A184"/>
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -13056,13 +13068,13 @@
         <v>1488</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>1252</v>
+        <v>1493</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>1249</v>
+        <v>1494</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>1250</v>
+        <v>1495</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>

</xml_diff>

<commit_message>
New Parameters enableIsInViewLog enableIsSafeLog
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B76466-3D91-4A4D-AA23-2E3F5F002DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C60C8-A5CF-214A-B67B-5E2FE911339F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="6460" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
+    <workbookView xWindow="25280" yWindow="7620" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
   <sheets>
     <sheet name="message" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="1511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="1514">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11814,6 +11814,66 @@
     <rPh sb="17" eb="19">
       <t>ジッコウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tappingUnsafeElementNotAllowed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unsafeな要素のタップは許可されていません。要素が非表示・領域内に収まっていない・オーバレイと重なっている、などの場合に要素はunsafeと判定されます。要素を強制的にタップする場合はtap関数の引数で"safeElementOnly = false"を指定してください。 (${subject})</t>
+    <rPh sb="7" eb="9">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="27" eb="30">
+      <t>ヒヒョウ</t>
+    </rPh>
+    <rPh sb="31" eb="34">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>オサマッテ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>カサナッテ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ハンテイ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="82" eb="85">
+      <t>キョウセイ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tapping unsafe element is not allowed. An element is considered unsafe if it is hidden, does not fit within an area, or overlaps an overlay. To force a tap on an element, specify "safeElementOnly = false" as an argument to the tap function. (${subject})</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12204,6 +12264,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
@@ -12218,42 +12334,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12267,7 +12348,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12317,27 +12398,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12758,8 +12818,8 @@
   <dimension ref="A1:I523"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A215" sqref="A215"/>
+      <pane ySplit="4" topLeftCell="A374" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A386" sqref="A386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19738,10 +19798,16 @@
       <c r="I384" s="18"/>
     </row>
     <row r="385" spans="1:9" ht="19" customHeight="1">
-      <c r="A385" s="19"/>
+      <c r="A385" s="19" t="s">
+        <v>1511</v>
+      </c>
       <c r="B385" s="20"/>
-      <c r="C385" s="20"/>
-      <c r="D385" s="20"/>
+      <c r="C385" s="20" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D385" s="20" t="s">
+        <v>1512</v>
+      </c>
       <c r="E385" s="20"/>
       <c r="F385" s="20"/>
       <c r="G385" s="18"/>
@@ -21715,7 +21781,7 @@
   </sheetData>
   <autoFilter ref="A4:J226" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="I5:I523 A5:G261">
+  <conditionalFormatting sqref="A5:G261 I5:I523">
     <cfRule type="expression" dxfId="39" priority="37">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
@@ -21786,67 +21852,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H523">
-    <cfRule type="cellIs" dxfId="25" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H390">
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H390)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H390)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H390)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H390)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H390)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H390)))</formula>
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug Fix Retry once on an unexpectedly long processing times occured
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C60C8-A5CF-214A-B67B-5E2FE911339F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05450CD0-2A95-B049-ACAA-CA6AA64D36DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="7620" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="1514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="1517">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11874,6 +11874,24 @@
   </si>
   <si>
     <t>Tapping unsafe element is not allowed. An element is considered unsafe if it is hidden, does not fit within an area, or overlaps an overlay. To force a tap on an element, specify "safeElementOnly = false" as an argument to the tap function. (${subject})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>timeoutOnScreenIs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenIs関数でタイムアウトが発生しました。 (submessage=${submessage})</t>
+    <rPh sb="8" eb="10">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Timeout on screenIs function. (${submessage})</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12518,9 +12536,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -12558,7 +12576,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -12664,7 +12682,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -12806,7 +12824,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12819,7 +12837,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A374" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A386" sqref="A386"/>
+      <selection pane="bottomLeft" activeCell="A387" sqref="A387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19815,10 +19833,16 @@
       <c r="I385" s="18"/>
     </row>
     <row r="386" spans="1:9" ht="19" customHeight="1">
-      <c r="A386" s="19"/>
+      <c r="A386" s="19" t="s">
+        <v>1514</v>
+      </c>
       <c r="B386" s="20"/>
-      <c r="C386" s="20"/>
-      <c r="D386" s="20"/>
+      <c r="C386" s="20" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D386" s="20" t="s">
+        <v>1515</v>
+      </c>
       <c r="E386" s="20"/>
       <c r="F386" s="20"/>
       <c r="G386" s="18"/>

</xml_diff>

<commit_message>
New Parameter - enableWarnOnSelectTimeout - enableRerunScenario
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3875777B-FDA2-6448-AA27-D73E56F3F051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545147EF-67C9-7A41-AF49-FF120EE90EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="7620" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="1520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="1526">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11906,6 +11906,39 @@
     <t>selectにおいてタイムアウトが発生しました。 (selector=${arg1}, ${submessage})</t>
     <rPh sb="46" eb="48">
       <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>couldNotGetContentOfWebView</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>WebViewのコンテンツを取得できませんでした。</t>
+    <rPh sb="14" eb="16">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not get context of the WebView.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rerunningScenarioRequested</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rerunning scenario requested.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストシナリオの再実行が要求されました。</t>
+    <rPh sb="8" eb="11">
+      <t>サイジッコウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ヨウキュウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -12297,62 +12330,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
@@ -12367,7 +12344,42 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12381,7 +12393,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12431,6 +12443,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12848,11 +12881,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I523"/>
+  <dimension ref="A1:I527"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A374" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A388" sqref="A388"/>
+      <selection pane="bottomLeft" activeCell="A390" sqref="A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19882,10 +19915,16 @@
       <c r="I387" s="18"/>
     </row>
     <row r="388" spans="1:9" ht="19" customHeight="1">
-      <c r="A388" s="19"/>
+      <c r="A388" s="19" t="s">
+        <v>1520</v>
+      </c>
       <c r="B388" s="20"/>
-      <c r="C388" s="20"/>
-      <c r="D388" s="20"/>
+      <c r="C388" s="20" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D388" s="20" t="s">
+        <v>1521</v>
+      </c>
       <c r="E388" s="20"/>
       <c r="F388" s="20"/>
       <c r="G388" s="18"/>
@@ -19893,10 +19932,16 @@
       <c r="I388" s="18"/>
     </row>
     <row r="389" spans="1:9" ht="19" customHeight="1">
-      <c r="A389" s="19"/>
+      <c r="A389" s="19" t="s">
+        <v>1523</v>
+      </c>
       <c r="B389" s="20"/>
-      <c r="C389" s="20"/>
-      <c r="D389" s="20"/>
+      <c r="C389" s="20" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D389" s="20" t="s">
+        <v>1525</v>
+      </c>
       <c r="E389" s="20"/>
       <c r="F389" s="20"/>
       <c r="G389" s="18"/>
@@ -19904,29 +19949,21 @@
       <c r="I389" s="18"/>
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
-      <c r="A390" s="26" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B390" s="23"/>
-      <c r="C390" s="23"/>
-      <c r="D390" s="23"/>
-      <c r="E390" s="23"/>
-      <c r="F390" s="23"/>
-      <c r="G390" s="24"/>
-      <c r="H390" s="25"/>
-      <c r="I390" s="24"/>
+      <c r="A390" s="19"/>
+      <c r="B390" s="20"/>
+      <c r="C390" s="20"/>
+      <c r="D390" s="20"/>
+      <c r="E390" s="20"/>
+      <c r="F390" s="20"/>
+      <c r="G390" s="18"/>
+      <c r="H390" s="17"/>
+      <c r="I390" s="18"/>
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
-      <c r="A391" s="19" t="s">
-        <v>1170</v>
-      </c>
+      <c r="A391" s="19"/>
       <c r="B391" s="20"/>
-      <c r="C391" s="20" t="s">
-        <v>1170</v>
-      </c>
-      <c r="D391" s="20" t="s">
-        <v>1264</v>
-      </c>
+      <c r="C391" s="20"/>
+      <c r="D391" s="20"/>
       <c r="E391" s="20"/>
       <c r="F391" s="20"/>
       <c r="G391" s="18"/>
@@ -19934,16 +19971,10 @@
       <c r="I391" s="18"/>
     </row>
     <row r="392" spans="1:9" ht="19" customHeight="1">
-      <c r="A392" s="19" t="s">
-        <v>1171</v>
-      </c>
+      <c r="A392" s="19"/>
       <c r="B392" s="20"/>
-      <c r="C392" s="20" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D392" s="20" t="s">
-        <v>1265</v>
-      </c>
+      <c r="C392" s="20"/>
+      <c r="D392" s="20"/>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
       <c r="G392" s="18"/>
@@ -19951,16 +19982,10 @@
       <c r="I392" s="18"/>
     </row>
     <row r="393" spans="1:9" ht="19" customHeight="1">
-      <c r="A393" s="19" t="s">
-        <v>1172</v>
-      </c>
+      <c r="A393" s="19"/>
       <c r="B393" s="20"/>
-      <c r="C393" s="20" t="s">
-        <v>1172</v>
-      </c>
-      <c r="D393" s="20" t="s">
-        <v>1267</v>
-      </c>
+      <c r="C393" s="20"/>
+      <c r="D393" s="20"/>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
       <c r="G393" s="18"/>
@@ -19968,32 +19993,28 @@
       <c r="I393" s="18"/>
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
-      <c r="A394" s="19" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B394" s="20"/>
-      <c r="C394" s="20" t="s">
-        <v>1173</v>
-      </c>
-      <c r="D394" s="20" t="s">
-        <v>1268</v>
-      </c>
-      <c r="E394" s="20"/>
-      <c r="F394" s="20"/>
-      <c r="G394" s="18"/>
-      <c r="H394" s="17"/>
-      <c r="I394" s="18"/>
+      <c r="A394" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B394" s="23"/>
+      <c r="C394" s="23"/>
+      <c r="D394" s="23"/>
+      <c r="E394" s="23"/>
+      <c r="F394" s="23"/>
+      <c r="G394" s="24"/>
+      <c r="H394" s="25"/>
+      <c r="I394" s="24"/>
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
       <c r="A395" s="19" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="B395" s="20"/>
       <c r="C395" s="20" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="D395" s="20" t="s">
-        <v>1269</v>
+        <v>1264</v>
       </c>
       <c r="E395" s="20"/>
       <c r="F395" s="20"/>
@@ -20003,14 +20024,14 @@
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
       <c r="A396" s="19" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="B396" s="20"/>
       <c r="C396" s="20" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="D396" s="20" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
@@ -20020,14 +20041,14 @@
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
       <c r="A397" s="19" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="B397" s="20"/>
       <c r="C397" s="20" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="D397" s="20" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="E397" s="20"/>
       <c r="F397" s="20"/>
@@ -20037,14 +20058,14 @@
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="20" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -20054,14 +20075,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="20" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -20071,14 +20092,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="20" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1273</v>
+        <v>1266</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -20088,14 +20109,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="20" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -20105,14 +20126,14 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="20" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="D402" s="20" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
@@ -20122,14 +20143,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="20" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -20139,14 +20160,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="20" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -20156,14 +20177,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="20" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -20173,14 +20194,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="20" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -20190,14 +20211,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="20" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -20207,14 +20228,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="20" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -20224,14 +20245,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="20" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -20241,14 +20262,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="20" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -20258,14 +20279,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="20" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -20275,14 +20296,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="20" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -20292,14 +20313,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="20" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -20309,14 +20330,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="20" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -20326,14 +20347,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="B415" s="20"/>
-      <c r="C415" s="19" t="s">
-        <v>1331</v>
+      <c r="C415" s="20" t="s">
+        <v>1190</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -20343,14 +20364,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="B416" s="20"/>
-      <c r="C416" s="19" t="s">
-        <v>1332</v>
+      <c r="C416" s="20" t="s">
+        <v>1191</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -20360,14 +20381,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="B417" s="20"/>
-      <c r="C417" s="19" t="s">
-        <v>1333</v>
+      <c r="C417" s="20" t="s">
+        <v>1192</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -20377,14 +20398,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="B418" s="20"/>
-      <c r="C418" s="19" t="s">
-        <v>1334</v>
+      <c r="C418" s="20" t="s">
+        <v>1193</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -20394,14 +20415,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="19" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -20411,14 +20432,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="19" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -20428,14 +20449,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="19" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -20445,14 +20466,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="19" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -20462,14 +20483,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="19" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -20479,14 +20500,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="19" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -20496,14 +20517,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="19" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -20513,14 +20534,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="19" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -20530,14 +20551,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1242</v>
+        <v>1202</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="19" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1487</v>
+        <v>1296</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -20547,14 +20568,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="19" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1481</v>
+        <v>1297</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -20564,14 +20585,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1207</v>
+        <v>1341</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1482</v>
+        <v>1298</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -20581,14 +20602,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1208</v>
+        <v>1342</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1483</v>
+        <v>1299</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -20598,14 +20619,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1209</v>
+        <v>1242</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1209</v>
+        <v>1343</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1484</v>
+        <v>1487</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -20615,14 +20636,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1210</v>
+        <v>1344</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -20632,14 +20653,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -20649,14 +20670,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1243</v>
+        <v>1208</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1345</v>
+        <v>1208</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1300</v>
+        <v>1483</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>
@@ -20666,14 +20687,14 @@
     </row>
     <row r="435" spans="1:9" ht="19" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="19" t="s">
-        <v>1346</v>
+        <v>1209</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>1301</v>
+        <v>1484</v>
       </c>
       <c r="E435" s="20"/>
       <c r="F435" s="20"/>
@@ -20683,14 +20704,14 @@
     </row>
     <row r="436" spans="1:9" ht="19" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="19" t="s">
-        <v>1347</v>
+        <v>1210</v>
       </c>
       <c r="D436" s="20" t="s">
-        <v>1302</v>
+        <v>1485</v>
       </c>
       <c r="E436" s="20"/>
       <c r="F436" s="20"/>
@@ -20700,14 +20721,14 @@
     </row>
     <row r="437" spans="1:9" ht="19" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="19" t="s">
-        <v>1348</v>
+        <v>1211</v>
       </c>
       <c r="D437" s="20" t="s">
-        <v>1303</v>
+        <v>1486</v>
       </c>
       <c r="E437" s="20"/>
       <c r="F437" s="20"/>
@@ -20717,14 +20738,14 @@
     </row>
     <row r="438" spans="1:9" ht="19" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>1215</v>
+        <v>1243</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="19" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="D438" s="20" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="E438" s="20"/>
       <c r="F438" s="20"/>
@@ -20734,14 +20755,14 @@
     </row>
     <row r="439" spans="1:9" ht="19" customHeight="1">
       <c r="A439" s="19" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="B439" s="20"/>
       <c r="C439" s="19" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="D439" s="20" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="E439" s="20"/>
       <c r="F439" s="20"/>
@@ -20751,14 +20772,14 @@
     </row>
     <row r="440" spans="1:9" ht="19" customHeight="1">
       <c r="A440" s="19" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="B440" s="20"/>
       <c r="C440" s="19" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="D440" s="20" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="E440" s="20"/>
       <c r="F440" s="20"/>
@@ -20768,14 +20789,14 @@
     </row>
     <row r="441" spans="1:9" ht="19" customHeight="1">
       <c r="A441" s="19" t="s">
-        <v>1236</v>
+        <v>1214</v>
       </c>
       <c r="B441" s="20"/>
       <c r="C441" s="19" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="D441" s="20" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="E441" s="20"/>
       <c r="F441" s="20"/>
@@ -20785,14 +20806,14 @@
     </row>
     <row r="442" spans="1:9" ht="19" customHeight="1">
       <c r="A442" s="19" t="s">
-        <v>1237</v>
+        <v>1215</v>
       </c>
       <c r="B442" s="20"/>
       <c r="C442" s="19" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="D442" s="20" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="E442" s="20"/>
       <c r="F442" s="20"/>
@@ -20802,14 +20823,14 @@
     </row>
     <row r="443" spans="1:9" ht="19" customHeight="1">
       <c r="A443" s="19" t="s">
-        <v>1238</v>
+        <v>1216</v>
       </c>
       <c r="B443" s="20"/>
       <c r="C443" s="19" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="D443" s="20" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="E443" s="20"/>
       <c r="F443" s="20"/>
@@ -20819,14 +20840,14 @@
     </row>
     <row r="444" spans="1:9" ht="19" customHeight="1">
       <c r="A444" s="19" t="s">
-        <v>1239</v>
+        <v>1217</v>
       </c>
       <c r="B444" s="20"/>
       <c r="C444" s="19" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="D444" s="20" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="E444" s="20"/>
       <c r="F444" s="20"/>
@@ -20836,14 +20857,14 @@
     </row>
     <row r="445" spans="1:9" ht="19" customHeight="1">
       <c r="A445" s="19" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="B445" s="20"/>
       <c r="C445" s="19" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="D445" s="20" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="E445" s="20"/>
       <c r="F445" s="20"/>
@@ -20853,14 +20874,14 @@
     </row>
     <row r="446" spans="1:9" ht="19" customHeight="1">
       <c r="A446" s="19" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B446" s="20"/>
       <c r="C446" s="19" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="D446" s="20" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="E446" s="20"/>
       <c r="F446" s="20"/>
@@ -20870,14 +20891,14 @@
     </row>
     <row r="447" spans="1:9" ht="19" customHeight="1">
       <c r="A447" s="19" t="s">
-        <v>1218</v>
+        <v>1238</v>
       </c>
       <c r="B447" s="20"/>
       <c r="C447" s="19" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
       <c r="D447" s="20" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="E447" s="20"/>
       <c r="F447" s="20"/>
@@ -20887,14 +20908,14 @@
     </row>
     <row r="448" spans="1:9" ht="19" customHeight="1">
       <c r="A448" s="19" t="s">
-        <v>1219</v>
+        <v>1239</v>
       </c>
       <c r="B448" s="20"/>
       <c r="C448" s="19" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
       <c r="D448" s="20" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="E448" s="20"/>
       <c r="F448" s="20"/>
@@ -20904,14 +20925,14 @@
     </row>
     <row r="449" spans="1:9" ht="19" customHeight="1">
       <c r="A449" s="19" t="s">
-        <v>1220</v>
+        <v>1240</v>
       </c>
       <c r="B449" s="20"/>
       <c r="C449" s="19" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="D449" s="20" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="E449" s="20"/>
       <c r="F449" s="20"/>
@@ -20921,14 +20942,14 @@
     </row>
     <row r="450" spans="1:9" ht="19" customHeight="1">
       <c r="A450" s="19" t="s">
-        <v>1221</v>
+        <v>1241</v>
       </c>
       <c r="B450" s="20"/>
       <c r="C450" s="19" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="D450" s="20" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="E450" s="20"/>
       <c r="F450" s="20"/>
@@ -20938,14 +20959,14 @@
     </row>
     <row r="451" spans="1:9" ht="19" customHeight="1">
       <c r="A451" s="19" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="B451" s="20"/>
       <c r="C451" s="19" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="D451" s="20" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="E451" s="20"/>
       <c r="F451" s="20"/>
@@ -20955,14 +20976,14 @@
     </row>
     <row r="452" spans="1:9" ht="19" customHeight="1">
       <c r="A452" s="19" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="B452" s="20"/>
       <c r="C452" s="19" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="D452" s="20" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="E452" s="20"/>
       <c r="F452" s="20"/>
@@ -20972,14 +20993,14 @@
     </row>
     <row r="453" spans="1:9" ht="19" customHeight="1">
       <c r="A453" s="19" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="B453" s="20"/>
       <c r="C453" s="19" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="D453" s="20" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="E453" s="20"/>
       <c r="F453" s="20"/>
@@ -20989,14 +21010,14 @@
     </row>
     <row r="454" spans="1:9" ht="19" customHeight="1">
       <c r="A454" s="19" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="B454" s="20"/>
       <c r="C454" s="19" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="D454" s="20" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="E454" s="20"/>
       <c r="F454" s="20"/>
@@ -21006,14 +21027,14 @@
     </row>
     <row r="455" spans="1:9" ht="19" customHeight="1">
       <c r="A455" s="19" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="B455" s="20"/>
       <c r="C455" s="19" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="D455" s="20" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="E455" s="20"/>
       <c r="F455" s="20"/>
@@ -21023,14 +21044,14 @@
     </row>
     <row r="456" spans="1:9" ht="19" customHeight="1">
       <c r="A456" s="19" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="B456" s="20"/>
       <c r="C456" s="19" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="D456" s="20" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
       <c r="E456" s="20"/>
       <c r="F456" s="20"/>
@@ -21040,14 +21061,14 @@
     </row>
     <row r="457" spans="1:9" ht="19" customHeight="1">
       <c r="A457" s="19" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="B457" s="20"/>
       <c r="C457" s="19" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="D457" s="20" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="E457" s="20"/>
       <c r="F457" s="20"/>
@@ -21057,14 +21078,14 @@
     </row>
     <row r="458" spans="1:9" ht="19" customHeight="1">
       <c r="A458" s="19" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="B458" s="20"/>
       <c r="C458" s="19" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="D458" s="20" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="E458" s="20"/>
       <c r="F458" s="20"/>
@@ -21074,14 +21095,14 @@
     </row>
     <row r="459" spans="1:9" ht="19" customHeight="1">
       <c r="A459" s="19" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="B459" s="20"/>
       <c r="C459" s="19" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="D459" s="20" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="E459" s="20"/>
       <c r="F459" s="20"/>
@@ -21091,14 +21112,14 @@
     </row>
     <row r="460" spans="1:9" ht="19" customHeight="1">
       <c r="A460" s="19" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="B460" s="20"/>
       <c r="C460" s="19" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="D460" s="20" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
       <c r="E460" s="20"/>
       <c r="F460" s="20"/>
@@ -21108,14 +21129,14 @@
     </row>
     <row r="461" spans="1:9" ht="19" customHeight="1">
       <c r="A461" s="19" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="B461" s="20"/>
       <c r="C461" s="19" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D461" s="20" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="E461" s="20"/>
       <c r="F461" s="20"/>
@@ -21125,14 +21146,14 @@
     </row>
     <row r="462" spans="1:9" ht="19" customHeight="1">
       <c r="A462" s="19" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="B462" s="20"/>
       <c r="C462" s="19" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
       <c r="D462" s="20" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="E462" s="20"/>
       <c r="F462" s="20"/>
@@ -21142,14 +21163,14 @@
     </row>
     <row r="463" spans="1:9" ht="19" customHeight="1">
       <c r="A463" s="19" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="B463" s="20"/>
       <c r="C463" s="19" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="D463" s="20" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="E463" s="20"/>
       <c r="F463" s="20"/>
@@ -21159,14 +21180,14 @@
     </row>
     <row r="464" spans="1:9" ht="19" customHeight="1">
       <c r="A464" s="19" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="B464" s="20"/>
       <c r="C464" s="19" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="E464" s="20"/>
       <c r="F464" s="20"/>
@@ -21175,10 +21196,16 @@
       <c r="I464" s="18"/>
     </row>
     <row r="465" spans="1:9" ht="19" customHeight="1">
-      <c r="A465" s="19"/>
+      <c r="A465" s="19" t="s">
+        <v>1232</v>
+      </c>
       <c r="B465" s="20"/>
-      <c r="C465" s="20"/>
-      <c r="D465" s="20"/>
+      <c r="C465" s="19" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D465" s="20" t="s">
+        <v>1327</v>
+      </c>
       <c r="E465" s="20"/>
       <c r="F465" s="20"/>
       <c r="G465" s="18"/>
@@ -21186,10 +21213,16 @@
       <c r="I465" s="18"/>
     </row>
     <row r="466" spans="1:9" ht="19" customHeight="1">
-      <c r="A466" s="19"/>
+      <c r="A466" s="19" t="s">
+        <v>1233</v>
+      </c>
       <c r="B466" s="20"/>
-      <c r="C466" s="20"/>
-      <c r="D466" s="20"/>
+      <c r="C466" s="19" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D466" s="20" t="s">
+        <v>1328</v>
+      </c>
       <c r="E466" s="20"/>
       <c r="F466" s="20"/>
       <c r="G466" s="18"/>
@@ -21197,10 +21230,16 @@
       <c r="I466" s="18"/>
     </row>
     <row r="467" spans="1:9" ht="19" customHeight="1">
-      <c r="A467" s="19"/>
+      <c r="A467" s="19" t="s">
+        <v>1234</v>
+      </c>
       <c r="B467" s="20"/>
-      <c r="C467" s="20"/>
-      <c r="D467" s="20"/>
+      <c r="C467" s="19" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D467" s="20" t="s">
+        <v>1329</v>
+      </c>
       <c r="E467" s="20"/>
       <c r="F467" s="20"/>
       <c r="G467" s="18"/>
@@ -21208,10 +21247,16 @@
       <c r="I467" s="18"/>
     </row>
     <row r="468" spans="1:9" ht="19" customHeight="1">
-      <c r="A468" s="19"/>
+      <c r="A468" s="19" t="s">
+        <v>1235</v>
+      </c>
       <c r="B468" s="20"/>
-      <c r="C468" s="20"/>
-      <c r="D468" s="20"/>
+      <c r="C468" s="19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D468" s="20" t="s">
+        <v>1330</v>
+      </c>
       <c r="E468" s="20"/>
       <c r="F468" s="20"/>
       <c r="G468" s="18"/>
@@ -21823,10 +21868,54 @@
       <c r="H523" s="17"/>
       <c r="I523" s="18"/>
     </row>
+    <row r="524" spans="1:9" ht="19" customHeight="1">
+      <c r="A524" s="19"/>
+      <c r="B524" s="20"/>
+      <c r="C524" s="20"/>
+      <c r="D524" s="20"/>
+      <c r="E524" s="20"/>
+      <c r="F524" s="20"/>
+      <c r="G524" s="18"/>
+      <c r="H524" s="17"/>
+      <c r="I524" s="18"/>
+    </row>
+    <row r="525" spans="1:9" ht="19" customHeight="1">
+      <c r="A525" s="19"/>
+      <c r="B525" s="20"/>
+      <c r="C525" s="20"/>
+      <c r="D525" s="20"/>
+      <c r="E525" s="20"/>
+      <c r="F525" s="20"/>
+      <c r="G525" s="18"/>
+      <c r="H525" s="17"/>
+      <c r="I525" s="18"/>
+    </row>
+    <row r="526" spans="1:9" ht="19" customHeight="1">
+      <c r="A526" s="19"/>
+      <c r="B526" s="20"/>
+      <c r="C526" s="20"/>
+      <c r="D526" s="20"/>
+      <c r="E526" s="20"/>
+      <c r="F526" s="20"/>
+      <c r="G526" s="18"/>
+      <c r="H526" s="17"/>
+      <c r="I526" s="18"/>
+    </row>
+    <row r="527" spans="1:9" ht="19" customHeight="1">
+      <c r="A527" s="19"/>
+      <c r="B527" s="20"/>
+      <c r="C527" s="20"/>
+      <c r="D527" s="20"/>
+      <c r="E527" s="20"/>
+      <c r="F527" s="20"/>
+      <c r="G527" s="18"/>
+      <c r="H527" s="17"/>
+      <c r="I527" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J226" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A5:G261 I5:I523">
+  <conditionalFormatting sqref="A5:G261 I5:I527">
     <cfRule type="expression" dxfId="39" priority="37">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
@@ -21891,73 +21980,73 @@
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G373 D316 A334:E335 A336:C355 E336:E355 A356:E357 A358:C370 E358:E370 A371:E373 A374:G523">
+  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G373 D316 A334:E335 A336:C355 E336:E355 A356:E357 A358:C370 E358:E370 A371:E373 A374:G527">
     <cfRule type="expression" dxfId="26" priority="274">
       <formula>$G262&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H523">
-    <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H5:H527">
+    <cfRule type="cellIs" dxfId="25" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="19" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="20" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="22" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="18" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="17" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="16" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H394">
+    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
+    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H390">
-    <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H390)))</formula>
+    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H390)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H390)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
+    <cfRule type="containsText" dxfId="8" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H394)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
+    <cfRule type="containsText" dxfId="7" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H394)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="containsText" dxfId="6" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H394)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Parameter - enableAlwaysRerunOnErrorAndroid - enableAlwaysRerunOnErrorIos
New Callback
- testContext.isRerunRequested
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545147EF-67C9-7A41-AF49-FF120EE90EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93CC97-8D80-8D49-9EF0-C3E88121E553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="7620" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="1526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="1529">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11910,10 +11910,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>couldNotGetContentOfWebView</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>WebViewのコンテンツを取得できませんでした。</t>
     <rPh sb="14" eb="16">
       <t>シュトク</t>
@@ -11921,10 +11917,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Could not get context of the WebView.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>rerunningScenarioRequested</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -11940,6 +11932,32 @@
     <rPh sb="12" eb="14">
       <t>ヨウキュウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not get contents of the WebView.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>couldNotGetContentsOfWebView</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>couldNotGetContentsOfScreen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画面のコンテンツを取得できませんでした。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ガメン </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not get contexts of the screen.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12330,6 +12348,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
@@ -12344,42 +12418,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12393,7 +12432,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12443,27 +12482,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12881,11 +12899,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I527"/>
+  <dimension ref="A1:I528"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A374" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A390" sqref="A390"/>
+      <pane ySplit="4" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A391" sqref="A391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19916,14 +19934,14 @@
     </row>
     <row r="388" spans="1:9" ht="19" customHeight="1">
       <c r="A388" s="19" t="s">
-        <v>1520</v>
+        <v>1526</v>
       </c>
       <c r="B388" s="20"/>
       <c r="C388" s="20" t="s">
-        <v>1522</v>
+        <v>1528</v>
       </c>
       <c r="D388" s="20" t="s">
-        <v>1521</v>
+        <v>1527</v>
       </c>
       <c r="E388" s="20"/>
       <c r="F388" s="20"/>
@@ -19933,14 +19951,14 @@
     </row>
     <row r="389" spans="1:9" ht="19" customHeight="1">
       <c r="A389" s="19" t="s">
-        <v>1523</v>
+        <v>1525</v>
       </c>
       <c r="B389" s="20"/>
       <c r="C389" s="20" t="s">
         <v>1524</v>
       </c>
       <c r="D389" s="20" t="s">
-        <v>1525</v>
+        <v>1520</v>
       </c>
       <c r="E389" s="20"/>
       <c r="F389" s="20"/>
@@ -19949,10 +19967,16 @@
       <c r="I389" s="18"/>
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
-      <c r="A390" s="19"/>
+      <c r="A390" s="19" t="s">
+        <v>1521</v>
+      </c>
       <c r="B390" s="20"/>
-      <c r="C390" s="20"/>
-      <c r="D390" s="20"/>
+      <c r="C390" s="20" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D390" s="20" t="s">
+        <v>1523</v>
+      </c>
       <c r="E390" s="20"/>
       <c r="F390" s="20"/>
       <c r="G390" s="18"/>
@@ -19993,45 +20017,39 @@
       <c r="I393" s="18"/>
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
-      <c r="A394" s="26" t="s">
+      <c r="A394" s="19"/>
+      <c r="B394" s="20"/>
+      <c r="C394" s="20"/>
+      <c r="D394" s="20"/>
+      <c r="E394" s="20"/>
+      <c r="F394" s="20"/>
+      <c r="G394" s="18"/>
+      <c r="H394" s="17"/>
+      <c r="I394" s="18"/>
+    </row>
+    <row r="395" spans="1:9" ht="19" customHeight="1">
+      <c r="A395" s="26" t="s">
         <v>1169</v>
       </c>
-      <c r="B394" s="23"/>
-      <c r="C394" s="23"/>
-      <c r="D394" s="23"/>
-      <c r="E394" s="23"/>
-      <c r="F394" s="23"/>
-      <c r="G394" s="24"/>
-      <c r="H394" s="25"/>
-      <c r="I394" s="24"/>
-    </row>
-    <row r="395" spans="1:9" ht="19" customHeight="1">
-      <c r="A395" s="19" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B395" s="20"/>
-      <c r="C395" s="20" t="s">
-        <v>1170</v>
-      </c>
-      <c r="D395" s="20" t="s">
-        <v>1264</v>
-      </c>
-      <c r="E395" s="20"/>
-      <c r="F395" s="20"/>
-      <c r="G395" s="18"/>
-      <c r="H395" s="17"/>
-      <c r="I395" s="18"/>
+      <c r="B395" s="23"/>
+      <c r="C395" s="23"/>
+      <c r="D395" s="23"/>
+      <c r="E395" s="23"/>
+      <c r="F395" s="23"/>
+      <c r="G395" s="24"/>
+      <c r="H395" s="25"/>
+      <c r="I395" s="24"/>
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
       <c r="A396" s="19" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B396" s="20"/>
       <c r="C396" s="20" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="D396" s="20" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
@@ -20041,14 +20059,14 @@
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
       <c r="A397" s="19" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B397" s="20"/>
       <c r="C397" s="20" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="D397" s="20" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E397" s="20"/>
       <c r="F397" s="20"/>
@@ -20058,14 +20076,14 @@
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="20" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -20075,14 +20093,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="20" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -20092,14 +20110,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="20" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1266</v>
+        <v>1269</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -20109,14 +20127,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="20" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -20126,14 +20144,14 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="20" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D402" s="20" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
@@ -20143,14 +20161,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="20" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -20160,14 +20178,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="20" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -20177,14 +20195,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="20" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -20194,14 +20212,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="20" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -20211,14 +20229,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="20" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -20228,14 +20246,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="20" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -20245,14 +20263,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="20" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -20262,14 +20280,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="20" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -20279,14 +20297,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="20" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -20296,14 +20314,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="20" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -20313,14 +20331,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="20" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -20330,14 +20348,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="20" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -20347,14 +20365,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="20" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -20364,14 +20382,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="20" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -20381,14 +20399,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="20" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -20398,14 +20416,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="20" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -20415,14 +20433,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B419" s="20"/>
-      <c r="C419" s="19" t="s">
-        <v>1331</v>
+      <c r="C419" s="20" t="s">
+        <v>1193</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -20432,14 +20450,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="19" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -20449,14 +20467,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="19" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -20466,14 +20484,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="19" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -20483,14 +20501,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="19" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -20500,14 +20518,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="19" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -20517,14 +20535,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="19" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -20534,14 +20552,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="19" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -20551,14 +20569,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="19" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -20568,14 +20586,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="19" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -20585,14 +20603,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -20602,14 +20620,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -20619,14 +20637,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1242</v>
+        <v>1205</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1487</v>
+        <v>1299</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -20636,14 +20654,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1206</v>
+        <v>1242</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1481</v>
+        <v>1487</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -20653,14 +20671,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1207</v>
+        <v>1344</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -20670,14 +20688,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>
@@ -20687,14 +20705,14 @@
     </row>
     <row r="435" spans="1:9" ht="19" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="E435" s="20"/>
       <c r="F435" s="20"/>
@@ -20704,14 +20722,14 @@
     </row>
     <row r="436" spans="1:9" ht="19" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="19" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D436" s="20" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="E436" s="20"/>
       <c r="F436" s="20"/>
@@ -20721,14 +20739,14 @@
     </row>
     <row r="437" spans="1:9" ht="19" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="D437" s="20" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="E437" s="20"/>
       <c r="F437" s="20"/>
@@ -20738,14 +20756,14 @@
     </row>
     <row r="438" spans="1:9" ht="19" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>1243</v>
+        <v>1211</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="19" t="s">
-        <v>1345</v>
+        <v>1211</v>
       </c>
       <c r="D438" s="20" t="s">
-        <v>1300</v>
+        <v>1486</v>
       </c>
       <c r="E438" s="20"/>
       <c r="F438" s="20"/>
@@ -20755,14 +20773,14 @@
     </row>
     <row r="439" spans="1:9" ht="19" customHeight="1">
       <c r="A439" s="19" t="s">
-        <v>1212</v>
+        <v>1243</v>
       </c>
       <c r="B439" s="20"/>
       <c r="C439" s="19" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="D439" s="20" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="E439" s="20"/>
       <c r="F439" s="20"/>
@@ -20772,14 +20790,14 @@
     </row>
     <row r="440" spans="1:9" ht="19" customHeight="1">
       <c r="A440" s="19" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B440" s="20"/>
       <c r="C440" s="19" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="D440" s="20" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E440" s="20"/>
       <c r="F440" s="20"/>
@@ -20789,14 +20807,14 @@
     </row>
     <row r="441" spans="1:9" ht="19" customHeight="1">
       <c r="A441" s="19" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B441" s="20"/>
       <c r="C441" s="19" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="D441" s="20" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E441" s="20"/>
       <c r="F441" s="20"/>
@@ -20806,14 +20824,14 @@
     </row>
     <row r="442" spans="1:9" ht="19" customHeight="1">
       <c r="A442" s="19" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B442" s="20"/>
       <c r="C442" s="19" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="D442" s="20" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="E442" s="20"/>
       <c r="F442" s="20"/>
@@ -20823,14 +20841,14 @@
     </row>
     <row r="443" spans="1:9" ht="19" customHeight="1">
       <c r="A443" s="19" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B443" s="20"/>
       <c r="C443" s="19" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="D443" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="E443" s="20"/>
       <c r="F443" s="20"/>
@@ -20840,14 +20858,14 @@
     </row>
     <row r="444" spans="1:9" ht="19" customHeight="1">
       <c r="A444" s="19" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B444" s="20"/>
       <c r="C444" s="19" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="D444" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="E444" s="20"/>
       <c r="F444" s="20"/>
@@ -20857,14 +20875,14 @@
     </row>
     <row r="445" spans="1:9" ht="19" customHeight="1">
       <c r="A445" s="19" t="s">
-        <v>1236</v>
+        <v>1217</v>
       </c>
       <c r="B445" s="20"/>
       <c r="C445" s="19" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D445" s="20" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="E445" s="20"/>
       <c r="F445" s="20"/>
@@ -20874,14 +20892,14 @@
     </row>
     <row r="446" spans="1:9" ht="19" customHeight="1">
       <c r="A446" s="19" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B446" s="20"/>
       <c r="C446" s="19" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D446" s="20" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="E446" s="20"/>
       <c r="F446" s="20"/>
@@ -20891,14 +20909,14 @@
     </row>
     <row r="447" spans="1:9" ht="19" customHeight="1">
       <c r="A447" s="19" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B447" s="20"/>
       <c r="C447" s="19" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="D447" s="20" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="E447" s="20"/>
       <c r="F447" s="20"/>
@@ -20908,14 +20926,14 @@
     </row>
     <row r="448" spans="1:9" ht="19" customHeight="1">
       <c r="A448" s="19" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B448" s="20"/>
       <c r="C448" s="19" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="D448" s="20" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="E448" s="20"/>
       <c r="F448" s="20"/>
@@ -20925,14 +20943,14 @@
     </row>
     <row r="449" spans="1:9" ht="19" customHeight="1">
       <c r="A449" s="19" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B449" s="20"/>
       <c r="C449" s="19" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="D449" s="20" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="E449" s="20"/>
       <c r="F449" s="20"/>
@@ -20942,14 +20960,14 @@
     </row>
     <row r="450" spans="1:9" ht="19" customHeight="1">
       <c r="A450" s="19" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B450" s="20"/>
       <c r="C450" s="19" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D450" s="20" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="E450" s="20"/>
       <c r="F450" s="20"/>
@@ -20959,14 +20977,14 @@
     </row>
     <row r="451" spans="1:9" ht="19" customHeight="1">
       <c r="A451" s="19" t="s">
-        <v>1218</v>
+        <v>1241</v>
       </c>
       <c r="B451" s="20"/>
       <c r="C451" s="19" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="D451" s="20" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="E451" s="20"/>
       <c r="F451" s="20"/>
@@ -20976,14 +20994,14 @@
     </row>
     <row r="452" spans="1:9" ht="19" customHeight="1">
       <c r="A452" s="19" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B452" s="20"/>
       <c r="C452" s="19" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="D452" s="20" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="E452" s="20"/>
       <c r="F452" s="20"/>
@@ -20993,14 +21011,14 @@
     </row>
     <row r="453" spans="1:9" ht="19" customHeight="1">
       <c r="A453" s="19" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B453" s="20"/>
       <c r="C453" s="19" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="D453" s="20" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="E453" s="20"/>
       <c r="F453" s="20"/>
@@ -21010,14 +21028,14 @@
     </row>
     <row r="454" spans="1:9" ht="19" customHeight="1">
       <c r="A454" s="19" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B454" s="20"/>
       <c r="C454" s="19" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="D454" s="20" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="E454" s="20"/>
       <c r="F454" s="20"/>
@@ -21027,14 +21045,14 @@
     </row>
     <row r="455" spans="1:9" ht="19" customHeight="1">
       <c r="A455" s="19" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B455" s="20"/>
       <c r="C455" s="19" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="D455" s="20" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="E455" s="20"/>
       <c r="F455" s="20"/>
@@ -21044,14 +21062,14 @@
     </row>
     <row r="456" spans="1:9" ht="19" customHeight="1">
       <c r="A456" s="19" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B456" s="20"/>
       <c r="C456" s="19" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D456" s="20" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="E456" s="20"/>
       <c r="F456" s="20"/>
@@ -21061,14 +21079,14 @@
     </row>
     <row r="457" spans="1:9" ht="19" customHeight="1">
       <c r="A457" s="19" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B457" s="20"/>
       <c r="C457" s="19" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="D457" s="20" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="E457" s="20"/>
       <c r="F457" s="20"/>
@@ -21078,14 +21096,14 @@
     </row>
     <row r="458" spans="1:9" ht="19" customHeight="1">
       <c r="A458" s="19" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B458" s="20"/>
       <c r="C458" s="19" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="D458" s="20" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="E458" s="20"/>
       <c r="F458" s="20"/>
@@ -21095,14 +21113,14 @@
     </row>
     <row r="459" spans="1:9" ht="19" customHeight="1">
       <c r="A459" s="19" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B459" s="20"/>
       <c r="C459" s="19" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="D459" s="20" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="E459" s="20"/>
       <c r="F459" s="20"/>
@@ -21112,14 +21130,14 @@
     </row>
     <row r="460" spans="1:9" ht="19" customHeight="1">
       <c r="A460" s="19" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B460" s="20"/>
       <c r="C460" s="19" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="D460" s="20" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E460" s="20"/>
       <c r="F460" s="20"/>
@@ -21129,14 +21147,14 @@
     </row>
     <row r="461" spans="1:9" ht="19" customHeight="1">
       <c r="A461" s="19" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B461" s="20"/>
       <c r="C461" s="19" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="D461" s="20" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E461" s="20"/>
       <c r="F461" s="20"/>
@@ -21146,14 +21164,14 @@
     </row>
     <row r="462" spans="1:9" ht="19" customHeight="1">
       <c r="A462" s="19" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B462" s="20"/>
       <c r="C462" s="19" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="D462" s="20" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="E462" s="20"/>
       <c r="F462" s="20"/>
@@ -21163,14 +21181,14 @@
     </row>
     <row r="463" spans="1:9" ht="19" customHeight="1">
       <c r="A463" s="19" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B463" s="20"/>
       <c r="C463" s="19" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="D463" s="20" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="E463" s="20"/>
       <c r="F463" s="20"/>
@@ -21180,14 +21198,14 @@
     </row>
     <row r="464" spans="1:9" ht="19" customHeight="1">
       <c r="A464" s="19" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B464" s="20"/>
       <c r="C464" s="19" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="E464" s="20"/>
       <c r="F464" s="20"/>
@@ -21197,14 +21215,14 @@
     </row>
     <row r="465" spans="1:9" ht="19" customHeight="1">
       <c r="A465" s="19" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B465" s="20"/>
       <c r="C465" s="19" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="E465" s="20"/>
       <c r="F465" s="20"/>
@@ -21214,14 +21232,14 @@
     </row>
     <row r="466" spans="1:9" ht="19" customHeight="1">
       <c r="A466" s="19" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B466" s="20"/>
       <c r="C466" s="19" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D466" s="20" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="E466" s="20"/>
       <c r="F466" s="20"/>
@@ -21231,14 +21249,14 @@
     </row>
     <row r="467" spans="1:9" ht="19" customHeight="1">
       <c r="A467" s="19" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B467" s="20"/>
       <c r="C467" s="19" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="E467" s="20"/>
       <c r="F467" s="20"/>
@@ -21248,14 +21266,14 @@
     </row>
     <row r="468" spans="1:9" ht="19" customHeight="1">
       <c r="A468" s="19" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B468" s="20"/>
       <c r="C468" s="19" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D468" s="20" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="E468" s="20"/>
       <c r="F468" s="20"/>
@@ -21264,10 +21282,16 @@
       <c r="I468" s="18"/>
     </row>
     <row r="469" spans="1:9" ht="19" customHeight="1">
-      <c r="A469" s="19"/>
+      <c r="A469" s="19" t="s">
+        <v>1235</v>
+      </c>
       <c r="B469" s="20"/>
-      <c r="C469" s="20"/>
-      <c r="D469" s="20"/>
+      <c r="C469" s="19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D469" s="20" t="s">
+        <v>1330</v>
+      </c>
       <c r="E469" s="20"/>
       <c r="F469" s="20"/>
       <c r="G469" s="18"/>
@@ -21912,10 +21936,21 @@
       <c r="H527" s="17"/>
       <c r="I527" s="18"/>
     </row>
+    <row r="528" spans="1:9" ht="19" customHeight="1">
+      <c r="A528" s="19"/>
+      <c r="B528" s="20"/>
+      <c r="C528" s="20"/>
+      <c r="D528" s="20"/>
+      <c r="E528" s="20"/>
+      <c r="F528" s="20"/>
+      <c r="G528" s="18"/>
+      <c r="H528" s="17"/>
+      <c r="I528" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J226" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A5:G261 I5:I527">
+  <conditionalFormatting sqref="A5:G261 I5:I528">
     <cfRule type="expression" dxfId="39" priority="37">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
@@ -21980,73 +22015,73 @@
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G373 D316 A334:E335 A336:C355 E336:E355 A356:E357 A358:C370 E358:E370 A371:E373 A374:G527">
+  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G373 D316 A334:E335 A336:C355 E336:E355 A356:E357 A358:C370 E358:E370 A371:E373 A374:G528">
     <cfRule type="expression" dxfId="26" priority="274">
       <formula>$G262&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H527">
-    <cfRule type="cellIs" dxfId="25" priority="16" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H5:H528">
+    <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="17" stopIfTrue="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H395">
+    <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H395)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H395)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H395)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H394">
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H394)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H394)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H394)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Parameter - rerunScenarioWords
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93CC97-8D80-8D49-9EF0-C3E88121E553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0467B9E2-12D5-4847-B6F6-8B2555FE3D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="7620" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="1529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="1532">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11957,7 +11957,25 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Could not get contexts of the screen.</t>
+    <t>rerunFailed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rerun failed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストシナリオの再実行が失敗しました。</t>
+    <rPh sb="8" eb="11">
+      <t>サイジッコウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>シッパイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Could not get contents of the screen.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12602,9 +12620,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -12642,7 +12660,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -12748,7 +12766,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -12890,7 +12908,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12903,7 +12921,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A391" sqref="A391"/>
+      <selection pane="bottomLeft" activeCell="A392" sqref="A392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19938,7 +19956,7 @@
       </c>
       <c r="B388" s="20"/>
       <c r="C388" s="20" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
       <c r="D388" s="20" t="s">
         <v>1527</v>
@@ -19984,10 +20002,16 @@
       <c r="I390" s="18"/>
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
-      <c r="A391" s="19"/>
+      <c r="A391" s="19" t="s">
+        <v>1528</v>
+      </c>
       <c r="B391" s="20"/>
-      <c r="C391" s="20"/>
-      <c r="D391" s="20"/>
+      <c r="C391" s="20" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D391" s="20" t="s">
+        <v>1530</v>
+      </c>
       <c r="E391" s="20"/>
       <c r="F391" s="20"/>
       <c r="G391" s="18"/>

</xml_diff>

<commit_message>
New Parameter - enableRerunOnScreenshotBlackout - screenshotBlackoutThreshold
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0467B9E2-12D5-4847-B6F6-8B2555FE3D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8A00BD-41B1-264F-B40E-3FBF8A5D171F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="7620" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="1532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="1538">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11976,6 +11976,66 @@
   </si>
   <si>
     <t>Could not get contents of the screen.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenIsBlackout</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenshotBlackoutThreshold</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenshotBlackoutThreshold is allowed from 0.9 to 1.0. (${value})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>screenshotBlackoutThreshold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>は</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.9-1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>で設定してください。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(value=${value})</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The screenshot is blacked out. (threshold=${value})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スクリーンショットがブラックアウトしました。(threshold=${value})</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12917,11 +12977,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I528"/>
+  <dimension ref="A1:I530"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A392" sqref="A392"/>
+      <pane ySplit="4" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A345" sqref="A345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19204,14 +19264,14 @@
     </row>
     <row r="344" spans="1:9" ht="19" customHeight="1">
       <c r="A344" s="19" t="s">
-        <v>928</v>
+        <v>1533</v>
       </c>
       <c r="B344" s="20"/>
       <c r="C344" s="20" t="s">
-        <v>929</v>
+        <v>1534</v>
       </c>
       <c r="D344" s="20" t="s">
-        <v>930</v>
+        <v>1535</v>
       </c>
       <c r="E344" s="20"/>
       <c r="F344" s="20"/>
@@ -19221,14 +19281,14 @@
     </row>
     <row r="345" spans="1:9" ht="19" customHeight="1">
       <c r="A345" s="19" t="s">
-        <v>609</v>
+        <v>1532</v>
       </c>
       <c r="B345" s="20"/>
       <c r="C345" s="20" t="s">
-        <v>610</v>
-      </c>
-      <c r="D345" s="21" t="s">
-        <v>725</v>
+        <v>1536</v>
+      </c>
+      <c r="D345" s="20" t="s">
+        <v>1537</v>
       </c>
       <c r="E345" s="20"/>
       <c r="F345" s="20"/>
@@ -19238,14 +19298,14 @@
     </row>
     <row r="346" spans="1:9" ht="19" customHeight="1">
       <c r="A346" s="19" t="s">
-        <v>611</v>
+        <v>928</v>
       </c>
       <c r="B346" s="20"/>
       <c r="C346" s="20" t="s">
-        <v>931</v>
-      </c>
-      <c r="D346" s="21" t="s">
-        <v>932</v>
+        <v>929</v>
+      </c>
+      <c r="D346" s="20" t="s">
+        <v>930</v>
       </c>
       <c r="E346" s="20"/>
       <c r="F346" s="20"/>
@@ -19255,14 +19315,14 @@
     </row>
     <row r="347" spans="1:9" ht="19" customHeight="1">
       <c r="A347" s="19" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B347" s="20"/>
       <c r="C347" s="20" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D347" s="21" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E347" s="20"/>
       <c r="F347" s="20"/>
@@ -19272,14 +19332,14 @@
     </row>
     <row r="348" spans="1:9" ht="19" customHeight="1">
       <c r="A348" s="19" t="s">
-        <v>933</v>
+        <v>611</v>
       </c>
       <c r="B348" s="20"/>
       <c r="C348" s="20" t="s">
-        <v>934</v>
-      </c>
-      <c r="D348" s="20" t="s">
-        <v>935</v>
+        <v>931</v>
+      </c>
+      <c r="D348" s="21" t="s">
+        <v>932</v>
       </c>
       <c r="E348" s="20"/>
       <c r="F348" s="20"/>
@@ -19289,14 +19349,14 @@
     </row>
     <row r="349" spans="1:9" ht="19" customHeight="1">
       <c r="A349" s="19" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B349" s="20"/>
       <c r="C349" s="20" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D349" s="21" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E349" s="20"/>
       <c r="F349" s="20"/>
@@ -19306,14 +19366,14 @@
     </row>
     <row r="350" spans="1:9" ht="19" customHeight="1">
       <c r="A350" s="19" t="s">
-        <v>616</v>
+        <v>933</v>
       </c>
       <c r="B350" s="20"/>
       <c r="C350" s="20" t="s">
-        <v>617</v>
-      </c>
-      <c r="D350" s="21" t="s">
-        <v>728</v>
+        <v>934</v>
+      </c>
+      <c r="D350" s="20" t="s">
+        <v>935</v>
       </c>
       <c r="E350" s="20"/>
       <c r="F350" s="20"/>
@@ -19323,14 +19383,14 @@
     </row>
     <row r="351" spans="1:9" ht="19" customHeight="1">
       <c r="A351" s="19" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B351" s="20"/>
       <c r="C351" s="20" t="s">
-        <v>619</v>
-      </c>
-      <c r="D351" s="20" t="s">
-        <v>729</v>
+        <v>615</v>
+      </c>
+      <c r="D351" s="21" t="s">
+        <v>727</v>
       </c>
       <c r="E351" s="20"/>
       <c r="F351" s="20"/>
@@ -19340,14 +19400,14 @@
     </row>
     <row r="352" spans="1:9" ht="19" customHeight="1">
       <c r="A352" s="19" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B352" s="20"/>
       <c r="C352" s="20" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D352" s="21" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E352" s="20"/>
       <c r="F352" s="20"/>
@@ -19357,14 +19417,14 @@
     </row>
     <row r="353" spans="1:9" ht="19" customHeight="1">
       <c r="A353" s="19" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B353" s="20"/>
       <c r="C353" s="20" t="s">
-        <v>623</v>
-      </c>
-      <c r="D353" s="21" t="s">
-        <v>731</v>
+        <v>619</v>
+      </c>
+      <c r="D353" s="20" t="s">
+        <v>729</v>
       </c>
       <c r="E353" s="20"/>
       <c r="F353" s="20"/>
@@ -19374,14 +19434,14 @@
     </row>
     <row r="354" spans="1:9" ht="19" customHeight="1">
       <c r="A354" s="19" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="B354" s="20"/>
       <c r="C354" s="20" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D354" s="21" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E354" s="20"/>
       <c r="F354" s="20"/>
@@ -19391,14 +19451,14 @@
     </row>
     <row r="355" spans="1:9" ht="19" customHeight="1">
       <c r="A355" s="19" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B355" s="20"/>
       <c r="C355" s="20" t="s">
-        <v>627</v>
-      </c>
-      <c r="D355" s="22" t="s">
-        <v>733</v>
+        <v>623</v>
+      </c>
+      <c r="D355" s="21" t="s">
+        <v>731</v>
       </c>
       <c r="E355" s="20"/>
       <c r="F355" s="20"/>
@@ -19408,14 +19468,14 @@
     </row>
     <row r="356" spans="1:9" ht="19" customHeight="1">
       <c r="A356" s="19" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="B356" s="20"/>
       <c r="C356" s="20" t="s">
-        <v>1467</v>
+        <v>625</v>
       </c>
       <c r="D356" s="21" t="s">
-        <v>1468</v>
+        <v>732</v>
       </c>
       <c r="E356" s="20"/>
       <c r="F356" s="20"/>
@@ -19425,14 +19485,14 @@
     </row>
     <row r="357" spans="1:9" ht="19" customHeight="1">
       <c r="A357" s="19" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B357" s="20"/>
       <c r="C357" s="20" t="s">
-        <v>629</v>
-      </c>
-      <c r="D357" s="21" t="s">
-        <v>734</v>
+        <v>627</v>
+      </c>
+      <c r="D357" s="22" t="s">
+        <v>733</v>
       </c>
       <c r="E357" s="20"/>
       <c r="F357" s="20"/>
@@ -19442,14 +19502,14 @@
     </row>
     <row r="358" spans="1:9" ht="19" customHeight="1">
       <c r="A358" s="19" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B358" s="20"/>
       <c r="C358" s="20" t="s">
-        <v>632</v>
+        <v>1467</v>
       </c>
       <c r="D358" s="21" t="s">
-        <v>735</v>
+        <v>1468</v>
       </c>
       <c r="E358" s="20"/>
       <c r="F358" s="20"/>
@@ -19459,14 +19519,14 @@
     </row>
     <row r="359" spans="1:9" ht="19" customHeight="1">
       <c r="A359" s="19" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="B359" s="20"/>
       <c r="C359" s="20" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="D359" s="21" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E359" s="20"/>
       <c r="F359" s="20"/>
@@ -19476,14 +19536,14 @@
     </row>
     <row r="360" spans="1:9" ht="19" customHeight="1">
       <c r="A360" s="19" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B360" s="20"/>
       <c r="C360" s="20" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D360" s="21" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E360" s="20"/>
       <c r="F360" s="20"/>
@@ -19493,14 +19553,14 @@
     </row>
     <row r="361" spans="1:9" ht="19" customHeight="1">
       <c r="A361" s="19" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B361" s="20"/>
       <c r="C361" s="20" t="s">
-        <v>638</v>
-      </c>
-      <c r="D361" s="20" t="s">
-        <v>738</v>
+        <v>634</v>
+      </c>
+      <c r="D361" s="21" t="s">
+        <v>736</v>
       </c>
       <c r="E361" s="20"/>
       <c r="F361" s="20"/>
@@ -19510,14 +19570,14 @@
     </row>
     <row r="362" spans="1:9" ht="19" customHeight="1">
       <c r="A362" s="19" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B362" s="20"/>
-      <c r="C362" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="D362" s="27" t="s">
-        <v>739</v>
+      <c r="C362" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="D362" s="21" t="s">
+        <v>737</v>
       </c>
       <c r="E362" s="20"/>
       <c r="F362" s="20"/>
@@ -19527,14 +19587,14 @@
     </row>
     <row r="363" spans="1:9" ht="19" customHeight="1">
       <c r="A363" s="19" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B363" s="20"/>
       <c r="C363" s="20" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="D363" s="20" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E363" s="20"/>
       <c r="F363" s="20"/>
@@ -19544,14 +19604,14 @@
     </row>
     <row r="364" spans="1:9" ht="19" customHeight="1">
       <c r="A364" s="19" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B364" s="20"/>
-      <c r="C364" s="20" t="s">
-        <v>644</v>
-      </c>
-      <c r="D364" s="21" t="s">
-        <v>741</v>
+      <c r="C364" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="D364" s="27" t="s">
+        <v>739</v>
       </c>
       <c r="E364" s="20"/>
       <c r="F364" s="20"/>
@@ -19561,14 +19621,14 @@
     </row>
     <row r="365" spans="1:9" ht="19" customHeight="1">
       <c r="A365" s="19" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B365" s="20"/>
       <c r="C365" s="20" t="s">
-        <v>646</v>
-      </c>
-      <c r="D365" s="21" t="s">
-        <v>742</v>
+        <v>642</v>
+      </c>
+      <c r="D365" s="20" t="s">
+        <v>740</v>
       </c>
       <c r="E365" s="20"/>
       <c r="F365" s="20"/>
@@ -19578,14 +19638,14 @@
     </row>
     <row r="366" spans="1:9" ht="19" customHeight="1">
       <c r="A366" s="19" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B366" s="20"/>
       <c r="C366" s="20" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D366" s="21" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E366" s="20"/>
       <c r="F366" s="20"/>
@@ -19595,14 +19655,14 @@
     </row>
     <row r="367" spans="1:9" ht="19" customHeight="1">
       <c r="A367" s="19" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B367" s="20"/>
       <c r="C367" s="20" t="s">
-        <v>650</v>
-      </c>
-      <c r="D367" s="20" t="s">
-        <v>744</v>
+        <v>646</v>
+      </c>
+      <c r="D367" s="21" t="s">
+        <v>742</v>
       </c>
       <c r="E367" s="20"/>
       <c r="F367" s="20"/>
@@ -19612,14 +19672,14 @@
     </row>
     <row r="368" spans="1:9" ht="19" customHeight="1">
       <c r="A368" s="19" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B368" s="20"/>
       <c r="C368" s="20" t="s">
-        <v>652</v>
-      </c>
-      <c r="D368" s="22" t="s">
-        <v>745</v>
+        <v>648</v>
+      </c>
+      <c r="D368" s="21" t="s">
+        <v>743</v>
       </c>
       <c r="E368" s="20"/>
       <c r="F368" s="20"/>
@@ -19629,14 +19689,14 @@
     </row>
     <row r="369" spans="1:9" ht="19" customHeight="1">
       <c r="A369" s="19" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B369" s="20"/>
       <c r="C369" s="20" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="D369" s="20" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E369" s="20"/>
       <c r="F369" s="20"/>
@@ -19646,14 +19706,14 @@
     </row>
     <row r="370" spans="1:9" ht="19" customHeight="1">
       <c r="A370" s="19" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="B370" s="20"/>
       <c r="C370" s="20" t="s">
-        <v>656</v>
-      </c>
-      <c r="D370" s="20" t="s">
-        <v>747</v>
+        <v>652</v>
+      </c>
+      <c r="D370" s="22" t="s">
+        <v>745</v>
       </c>
       <c r="E370" s="20"/>
       <c r="F370" s="20"/>
@@ -19663,14 +19723,14 @@
     </row>
     <row r="371" spans="1:9" ht="19" customHeight="1">
       <c r="A371" s="19" t="s">
-        <v>925</v>
+        <v>653</v>
       </c>
       <c r="B371" s="20"/>
       <c r="C371" s="20" t="s">
-        <v>926</v>
+        <v>654</v>
       </c>
       <c r="D371" s="20" t="s">
-        <v>927</v>
+        <v>746</v>
       </c>
       <c r="E371" s="20"/>
       <c r="F371" s="20"/>
@@ -19680,14 +19740,14 @@
     </row>
     <row r="372" spans="1:9" ht="19" customHeight="1">
       <c r="A372" s="19" t="s">
-        <v>1044</v>
+        <v>655</v>
       </c>
       <c r="B372" s="20"/>
       <c r="C372" s="20" t="s">
-        <v>1045</v>
+        <v>656</v>
       </c>
       <c r="D372" s="20" t="s">
-        <v>1046</v>
+        <v>747</v>
       </c>
       <c r="E372" s="20"/>
       <c r="F372" s="20"/>
@@ -19697,14 +19757,14 @@
     </row>
     <row r="373" spans="1:9" ht="19" customHeight="1">
       <c r="A373" s="19" t="s">
-        <v>1112</v>
+        <v>925</v>
       </c>
       <c r="B373" s="20"/>
       <c r="C373" s="20" t="s">
-        <v>1113</v>
+        <v>926</v>
       </c>
       <c r="D373" s="20" t="s">
-        <v>1114</v>
+        <v>927</v>
       </c>
       <c r="E373" s="20"/>
       <c r="F373" s="20"/>
@@ -19714,14 +19774,14 @@
     </row>
     <row r="374" spans="1:9" ht="19" customHeight="1">
       <c r="A374" s="19" t="s">
-        <v>1106</v>
+        <v>1044</v>
       </c>
       <c r="B374" s="20"/>
       <c r="C374" s="20" t="s">
-        <v>1107</v>
+        <v>1045</v>
       </c>
       <c r="D374" s="20" t="s">
-        <v>1108</v>
+        <v>1046</v>
       </c>
       <c r="E374" s="20"/>
       <c r="F374" s="20"/>
@@ -19731,14 +19791,14 @@
     </row>
     <row r="375" spans="1:9" ht="19" customHeight="1">
       <c r="A375" s="19" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="B375" s="20"/>
       <c r="C375" s="20" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="D375" s="20" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="E375" s="20"/>
       <c r="F375" s="20"/>
@@ -19748,14 +19808,14 @@
     </row>
     <row r="376" spans="1:9" ht="19" customHeight="1">
       <c r="A376" s="19" t="s">
-        <v>1115</v>
+        <v>1106</v>
       </c>
       <c r="B376" s="20"/>
       <c r="C376" s="20" t="s">
-        <v>1116</v>
+        <v>1107</v>
       </c>
       <c r="D376" s="20" t="s">
-        <v>1117</v>
+        <v>1108</v>
       </c>
       <c r="E376" s="20"/>
       <c r="F376" s="20"/>
@@ -19765,14 +19825,14 @@
     </row>
     <row r="377" spans="1:9" ht="19" customHeight="1">
       <c r="A377" s="19" t="s">
-        <v>1127</v>
+        <v>1109</v>
       </c>
       <c r="B377" s="20"/>
       <c r="C377" s="20" t="s">
-        <v>1129</v>
+        <v>1110</v>
       </c>
       <c r="D377" s="20" t="s">
-        <v>1128</v>
+        <v>1111</v>
       </c>
       <c r="E377" s="20"/>
       <c r="F377" s="20"/>
@@ -19782,14 +19842,14 @@
     </row>
     <row r="378" spans="1:9" ht="19" customHeight="1">
       <c r="A378" s="19" t="s">
-        <v>1130</v>
+        <v>1115</v>
       </c>
       <c r="B378" s="20"/>
       <c r="C378" s="20" t="s">
-        <v>1131</v>
+        <v>1116</v>
       </c>
       <c r="D378" s="20" t="s">
-        <v>1132</v>
+        <v>1117</v>
       </c>
       <c r="E378" s="20"/>
       <c r="F378" s="20"/>
@@ -19799,14 +19859,14 @@
     </row>
     <row r="379" spans="1:9" ht="19" customHeight="1">
       <c r="A379" s="19" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="B379" s="20"/>
       <c r="C379" s="20" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="D379" s="20" t="s">
-        <v>1135</v>
+        <v>1128</v>
       </c>
       <c r="E379" s="20"/>
       <c r="F379" s="20"/>
@@ -19816,14 +19876,14 @@
     </row>
     <row r="380" spans="1:9" ht="19" customHeight="1">
       <c r="A380" s="19" t="s">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="B380" s="20"/>
       <c r="C380" s="20" t="s">
-        <v>1168</v>
+        <v>1131</v>
       </c>
       <c r="D380" s="20" t="s">
-        <v>1167</v>
+        <v>1132</v>
       </c>
       <c r="E380" s="20"/>
       <c r="F380" s="20"/>
@@ -19833,14 +19893,14 @@
     </row>
     <row r="381" spans="1:9" ht="19" customHeight="1">
       <c r="A381" s="19" t="s">
-        <v>1163</v>
+        <v>1133</v>
       </c>
       <c r="B381" s="20"/>
       <c r="C381" s="20" t="s">
-        <v>1164</v>
+        <v>1134</v>
       </c>
       <c r="D381" s="20" t="s">
-        <v>1165</v>
+        <v>1135</v>
       </c>
       <c r="E381" s="20"/>
       <c r="F381" s="20"/>
@@ -19850,14 +19910,14 @@
     </row>
     <row r="382" spans="1:9" ht="19" customHeight="1">
       <c r="A382" s="19" t="s">
-        <v>1253</v>
+        <v>1166</v>
       </c>
       <c r="B382" s="20"/>
       <c r="C382" s="20" t="s">
-        <v>1254</v>
+        <v>1168</v>
       </c>
       <c r="D382" s="20" t="s">
-        <v>1255</v>
+        <v>1167</v>
       </c>
       <c r="E382" s="20"/>
       <c r="F382" s="20"/>
@@ -19867,14 +19927,14 @@
     </row>
     <row r="383" spans="1:9" ht="19" customHeight="1">
       <c r="A383" s="19" t="s">
-        <v>1376</v>
+        <v>1163</v>
       </c>
       <c r="B383" s="20"/>
       <c r="C383" s="20" t="s">
-        <v>1377</v>
+        <v>1164</v>
       </c>
       <c r="D383" s="20" t="s">
-        <v>1378</v>
+        <v>1165</v>
       </c>
       <c r="E383" s="20"/>
       <c r="F383" s="20"/>
@@ -19884,14 +19944,14 @@
     </row>
     <row r="384" spans="1:9" ht="19" customHeight="1">
       <c r="A384" s="19" t="s">
-        <v>1379</v>
+        <v>1253</v>
       </c>
       <c r="B384" s="20"/>
       <c r="C384" s="20" t="s">
-        <v>1380</v>
+        <v>1254</v>
       </c>
       <c r="D384" s="20" t="s">
-        <v>1381</v>
+        <v>1255</v>
       </c>
       <c r="E384" s="20"/>
       <c r="F384" s="20"/>
@@ -19901,14 +19961,14 @@
     </row>
     <row r="385" spans="1:9" ht="19" customHeight="1">
       <c r="A385" s="19" t="s">
-        <v>1511</v>
+        <v>1376</v>
       </c>
       <c r="B385" s="20"/>
       <c r="C385" s="20" t="s">
-        <v>1513</v>
+        <v>1377</v>
       </c>
       <c r="D385" s="20" t="s">
-        <v>1512</v>
+        <v>1378</v>
       </c>
       <c r="E385" s="20"/>
       <c r="F385" s="20"/>
@@ -19918,14 +19978,14 @@
     </row>
     <row r="386" spans="1:9" ht="19" customHeight="1">
       <c r="A386" s="19" t="s">
-        <v>1514</v>
+        <v>1379</v>
       </c>
       <c r="B386" s="20"/>
       <c r="C386" s="20" t="s">
-        <v>1515</v>
+        <v>1380</v>
       </c>
       <c r="D386" s="20" t="s">
-        <v>1516</v>
+        <v>1381</v>
       </c>
       <c r="E386" s="20"/>
       <c r="F386" s="20"/>
@@ -19935,14 +19995,14 @@
     </row>
     <row r="387" spans="1:9" ht="19" customHeight="1">
       <c r="A387" s="19" t="s">
-        <v>1517</v>
+        <v>1511</v>
       </c>
       <c r="B387" s="20"/>
       <c r="C387" s="20" t="s">
-        <v>1518</v>
+        <v>1513</v>
       </c>
       <c r="D387" s="20" t="s">
-        <v>1519</v>
+        <v>1512</v>
       </c>
       <c r="E387" s="20"/>
       <c r="F387" s="20"/>
@@ -19952,14 +20012,14 @@
     </row>
     <row r="388" spans="1:9" ht="19" customHeight="1">
       <c r="A388" s="19" t="s">
-        <v>1526</v>
+        <v>1514</v>
       </c>
       <c r="B388" s="20"/>
       <c r="C388" s="20" t="s">
-        <v>1531</v>
+        <v>1515</v>
       </c>
       <c r="D388" s="20" t="s">
-        <v>1527</v>
+        <v>1516</v>
       </c>
       <c r="E388" s="20"/>
       <c r="F388" s="20"/>
@@ -19969,14 +20029,14 @@
     </row>
     <row r="389" spans="1:9" ht="19" customHeight="1">
       <c r="A389" s="19" t="s">
-        <v>1525</v>
+        <v>1517</v>
       </c>
       <c r="B389" s="20"/>
       <c r="C389" s="20" t="s">
-        <v>1524</v>
+        <v>1518</v>
       </c>
       <c r="D389" s="20" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="E389" s="20"/>
       <c r="F389" s="20"/>
@@ -19986,14 +20046,14 @@
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
       <c r="A390" s="19" t="s">
-        <v>1521</v>
+        <v>1526</v>
       </c>
       <c r="B390" s="20"/>
       <c r="C390" s="20" t="s">
-        <v>1522</v>
+        <v>1531</v>
       </c>
       <c r="D390" s="20" t="s">
-        <v>1523</v>
+        <v>1527</v>
       </c>
       <c r="E390" s="20"/>
       <c r="F390" s="20"/>
@@ -20003,14 +20063,14 @@
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
       <c r="A391" s="19" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="B391" s="20"/>
       <c r="C391" s="20" t="s">
-        <v>1529</v>
+        <v>1524</v>
       </c>
       <c r="D391" s="20" t="s">
-        <v>1530</v>
+        <v>1520</v>
       </c>
       <c r="E391" s="20"/>
       <c r="F391" s="20"/>
@@ -20019,10 +20079,16 @@
       <c r="I391" s="18"/>
     </row>
     <row r="392" spans="1:9" ht="19" customHeight="1">
-      <c r="A392" s="19"/>
+      <c r="A392" s="19" t="s">
+        <v>1521</v>
+      </c>
       <c r="B392" s="20"/>
-      <c r="C392" s="20"/>
-      <c r="D392" s="20"/>
+      <c r="C392" s="20" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D392" s="20" t="s">
+        <v>1523</v>
+      </c>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
       <c r="G392" s="18"/>
@@ -20030,10 +20096,16 @@
       <c r="I392" s="18"/>
     </row>
     <row r="393" spans="1:9" ht="19" customHeight="1">
-      <c r="A393" s="19"/>
+      <c r="A393" s="19" t="s">
+        <v>1528</v>
+      </c>
       <c r="B393" s="20"/>
-      <c r="C393" s="20"/>
-      <c r="D393" s="20"/>
+      <c r="C393" s="20" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D393" s="20" t="s">
+        <v>1530</v>
+      </c>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
       <c r="G393" s="18"/>
@@ -20052,29 +20124,21 @@
       <c r="I394" s="18"/>
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
-      <c r="A395" s="26" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B395" s="23"/>
-      <c r="C395" s="23"/>
-      <c r="D395" s="23"/>
-      <c r="E395" s="23"/>
-      <c r="F395" s="23"/>
-      <c r="G395" s="24"/>
-      <c r="H395" s="25"/>
-      <c r="I395" s="24"/>
+      <c r="A395" s="19"/>
+      <c r="B395" s="20"/>
+      <c r="C395" s="20"/>
+      <c r="D395" s="20"/>
+      <c r="E395" s="20"/>
+      <c r="F395" s="20"/>
+      <c r="G395" s="18"/>
+      <c r="H395" s="17"/>
+      <c r="I395" s="18"/>
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
-      <c r="A396" s="19" t="s">
-        <v>1170</v>
-      </c>
+      <c r="A396" s="19"/>
       <c r="B396" s="20"/>
-      <c r="C396" s="20" t="s">
-        <v>1170</v>
-      </c>
-      <c r="D396" s="20" t="s">
-        <v>1264</v>
-      </c>
+      <c r="C396" s="20"/>
+      <c r="D396" s="20"/>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
       <c r="G396" s="18"/>
@@ -20082,32 +20146,28 @@
       <c r="I396" s="18"/>
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
-      <c r="A397" s="19" t="s">
-        <v>1171</v>
-      </c>
-      <c r="B397" s="20"/>
-      <c r="C397" s="20" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D397" s="20" t="s">
-        <v>1265</v>
-      </c>
-      <c r="E397" s="20"/>
-      <c r="F397" s="20"/>
-      <c r="G397" s="18"/>
-      <c r="H397" s="17"/>
-      <c r="I397" s="18"/>
+      <c r="A397" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B397" s="23"/>
+      <c r="C397" s="23"/>
+      <c r="D397" s="23"/>
+      <c r="E397" s="23"/>
+      <c r="F397" s="23"/>
+      <c r="G397" s="24"/>
+      <c r="H397" s="25"/>
+      <c r="I397" s="24"/>
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="20" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -20117,14 +20177,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="20" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -20134,14 +20194,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="20" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -20151,14 +20211,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="20" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -20168,14 +20228,14 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="20" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="D402" s="20" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
@@ -20185,14 +20245,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="20" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1271</v>
+        <v>1266</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -20202,14 +20262,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="20" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -20219,14 +20279,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="20" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -20236,14 +20296,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="20" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -20253,14 +20313,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="20" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -20270,14 +20330,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="20" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -20287,14 +20347,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="20" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -20304,14 +20364,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="20" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -20321,14 +20381,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="20" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -20338,14 +20398,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="20" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -20355,14 +20415,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="20" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -20372,14 +20432,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="20" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -20389,14 +20449,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="20" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -20406,14 +20466,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="20" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -20423,14 +20483,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="20" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -20440,14 +20500,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="20" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -20457,14 +20517,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="20" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -20474,14 +20534,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="B420" s="20"/>
-      <c r="C420" s="19" t="s">
-        <v>1331</v>
+      <c r="C420" s="20" t="s">
+        <v>1192</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -20491,14 +20551,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="B421" s="20"/>
-      <c r="C421" s="19" t="s">
-        <v>1332</v>
+      <c r="C421" s="20" t="s">
+        <v>1193</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -20508,14 +20568,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="B422" s="20"/>
       <c r="C422" s="19" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -20525,14 +20585,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="B423" s="20"/>
       <c r="C423" s="19" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -20542,14 +20602,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="B424" s="20"/>
       <c r="C424" s="19" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -20559,14 +20619,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="B425" s="20"/>
       <c r="C425" s="19" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -20576,14 +20636,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="B426" s="20"/>
       <c r="C426" s="19" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -20593,14 +20653,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="B427" s="20"/>
       <c r="C427" s="19" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -20610,14 +20670,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="B428" s="20"/>
       <c r="C428" s="19" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -20627,14 +20687,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -20644,14 +20704,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -20661,14 +20721,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -20678,14 +20738,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1242</v>
+        <v>1204</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1487</v>
+        <v>1298</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -20695,14 +20755,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1481</v>
+        <v>1299</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -20712,14 +20772,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1207</v>
+        <v>1242</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1207</v>
+        <v>1343</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1482</v>
+        <v>1487</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>
@@ -20729,14 +20789,14 @@
     </row>
     <row r="435" spans="1:9" ht="19" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="19" t="s">
-        <v>1208</v>
+        <v>1344</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="E435" s="20"/>
       <c r="F435" s="20"/>
@@ -20746,14 +20806,14 @@
     </row>
     <row r="436" spans="1:9" ht="19" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="19" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="D436" s="20" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="E436" s="20"/>
       <c r="F436" s="20"/>
@@ -20763,14 +20823,14 @@
     </row>
     <row r="437" spans="1:9" ht="19" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="19" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="D437" s="20" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="E437" s="20"/>
       <c r="F437" s="20"/>
@@ -20780,14 +20840,14 @@
     </row>
     <row r="438" spans="1:9" ht="19" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="19" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="D438" s="20" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="E438" s="20"/>
       <c r="F438" s="20"/>
@@ -20797,14 +20857,14 @@
     </row>
     <row r="439" spans="1:9" ht="19" customHeight="1">
       <c r="A439" s="19" t="s">
-        <v>1243</v>
+        <v>1210</v>
       </c>
       <c r="B439" s="20"/>
       <c r="C439" s="19" t="s">
-        <v>1345</v>
+        <v>1210</v>
       </c>
       <c r="D439" s="20" t="s">
-        <v>1300</v>
+        <v>1485</v>
       </c>
       <c r="E439" s="20"/>
       <c r="F439" s="20"/>
@@ -20814,14 +20874,14 @@
     </row>
     <row r="440" spans="1:9" ht="19" customHeight="1">
       <c r="A440" s="19" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B440" s="20"/>
       <c r="C440" s="19" t="s">
-        <v>1346</v>
+        <v>1211</v>
       </c>
       <c r="D440" s="20" t="s">
-        <v>1301</v>
+        <v>1486</v>
       </c>
       <c r="E440" s="20"/>
       <c r="F440" s="20"/>
@@ -20831,14 +20891,14 @@
     </row>
     <row r="441" spans="1:9" ht="19" customHeight="1">
       <c r="A441" s="19" t="s">
-        <v>1213</v>
+        <v>1243</v>
       </c>
       <c r="B441" s="20"/>
       <c r="C441" s="19" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D441" s="20" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="E441" s="20"/>
       <c r="F441" s="20"/>
@@ -20848,14 +20908,14 @@
     </row>
     <row r="442" spans="1:9" ht="19" customHeight="1">
       <c r="A442" s="19" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="B442" s="20"/>
       <c r="C442" s="19" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D442" s="20" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="E442" s="20"/>
       <c r="F442" s="20"/>
@@ -20865,14 +20925,14 @@
     </row>
     <row r="443" spans="1:9" ht="19" customHeight="1">
       <c r="A443" s="19" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="B443" s="20"/>
       <c r="C443" s="19" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D443" s="20" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="E443" s="20"/>
       <c r="F443" s="20"/>
@@ -20882,14 +20942,14 @@
     </row>
     <row r="444" spans="1:9" ht="19" customHeight="1">
       <c r="A444" s="19" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="B444" s="20"/>
       <c r="C444" s="19" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D444" s="20" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="E444" s="20"/>
       <c r="F444" s="20"/>
@@ -20899,14 +20959,14 @@
     </row>
     <row r="445" spans="1:9" ht="19" customHeight="1">
       <c r="A445" s="19" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="B445" s="20"/>
       <c r="C445" s="19" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D445" s="20" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="E445" s="20"/>
       <c r="F445" s="20"/>
@@ -20916,14 +20976,14 @@
     </row>
     <row r="446" spans="1:9" ht="19" customHeight="1">
       <c r="A446" s="19" t="s">
-        <v>1236</v>
+        <v>1216</v>
       </c>
       <c r="B446" s="20"/>
       <c r="C446" s="19" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D446" s="20" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="E446" s="20"/>
       <c r="F446" s="20"/>
@@ -20933,14 +20993,14 @@
     </row>
     <row r="447" spans="1:9" ht="19" customHeight="1">
       <c r="A447" s="19" t="s">
-        <v>1237</v>
+        <v>1217</v>
       </c>
       <c r="B447" s="20"/>
       <c r="C447" s="19" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D447" s="20" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="E447" s="20"/>
       <c r="F447" s="20"/>
@@ -20950,14 +21010,14 @@
     </row>
     <row r="448" spans="1:9" ht="19" customHeight="1">
       <c r="A448" s="19" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B448" s="20"/>
       <c r="C448" s="19" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="D448" s="20" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="E448" s="20"/>
       <c r="F448" s="20"/>
@@ -20967,14 +21027,14 @@
     </row>
     <row r="449" spans="1:9" ht="19" customHeight="1">
       <c r="A449" s="19" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B449" s="20"/>
       <c r="C449" s="19" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="D449" s="20" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="E449" s="20"/>
       <c r="F449" s="20"/>
@@ -20984,14 +21044,14 @@
     </row>
     <row r="450" spans="1:9" ht="19" customHeight="1">
       <c r="A450" s="19" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B450" s="20"/>
       <c r="C450" s="19" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="D450" s="20" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="E450" s="20"/>
       <c r="F450" s="20"/>
@@ -21001,14 +21061,14 @@
     </row>
     <row r="451" spans="1:9" ht="19" customHeight="1">
       <c r="A451" s="19" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="B451" s="20"/>
       <c r="C451" s="19" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D451" s="20" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="E451" s="20"/>
       <c r="F451" s="20"/>
@@ -21018,14 +21078,14 @@
     </row>
     <row r="452" spans="1:9" ht="19" customHeight="1">
       <c r="A452" s="19" t="s">
-        <v>1218</v>
+        <v>1240</v>
       </c>
       <c r="B452" s="20"/>
       <c r="C452" s="19" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="D452" s="20" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="E452" s="20"/>
       <c r="F452" s="20"/>
@@ -21035,14 +21095,14 @@
     </row>
     <row r="453" spans="1:9" ht="19" customHeight="1">
       <c r="A453" s="19" t="s">
-        <v>1219</v>
+        <v>1241</v>
       </c>
       <c r="B453" s="20"/>
       <c r="C453" s="19" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="D453" s="20" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="E453" s="20"/>
       <c r="F453" s="20"/>
@@ -21052,14 +21112,14 @@
     </row>
     <row r="454" spans="1:9" ht="19" customHeight="1">
       <c r="A454" s="19" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="B454" s="20"/>
       <c r="C454" s="19" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="D454" s="20" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="E454" s="20"/>
       <c r="F454" s="20"/>
@@ -21069,14 +21129,14 @@
     </row>
     <row r="455" spans="1:9" ht="19" customHeight="1">
       <c r="A455" s="19" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="B455" s="20"/>
       <c r="C455" s="19" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="D455" s="20" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E455" s="20"/>
       <c r="F455" s="20"/>
@@ -21086,14 +21146,14 @@
     </row>
     <row r="456" spans="1:9" ht="19" customHeight="1">
       <c r="A456" s="19" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="B456" s="20"/>
       <c r="C456" s="19" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="D456" s="20" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="E456" s="20"/>
       <c r="F456" s="20"/>
@@ -21103,14 +21163,14 @@
     </row>
     <row r="457" spans="1:9" ht="19" customHeight="1">
       <c r="A457" s="19" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="B457" s="20"/>
       <c r="C457" s="19" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="D457" s="20" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="E457" s="20"/>
       <c r="F457" s="20"/>
@@ -21120,14 +21180,14 @@
     </row>
     <row r="458" spans="1:9" ht="19" customHeight="1">
       <c r="A458" s="19" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="B458" s="20"/>
       <c r="C458" s="19" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="D458" s="20" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="E458" s="20"/>
       <c r="F458" s="20"/>
@@ -21137,14 +21197,14 @@
     </row>
     <row r="459" spans="1:9" ht="19" customHeight="1">
       <c r="A459" s="19" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="B459" s="20"/>
       <c r="C459" s="19" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="D459" s="20" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="E459" s="20"/>
       <c r="F459" s="20"/>
@@ -21154,14 +21214,14 @@
     </row>
     <row r="460" spans="1:9" ht="19" customHeight="1">
       <c r="A460" s="19" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="B460" s="20"/>
       <c r="C460" s="19" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D460" s="20" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="E460" s="20"/>
       <c r="F460" s="20"/>
@@ -21171,14 +21231,14 @@
     </row>
     <row r="461" spans="1:9" ht="19" customHeight="1">
       <c r="A461" s="19" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="B461" s="20"/>
       <c r="C461" s="19" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="D461" s="20" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="E461" s="20"/>
       <c r="F461" s="20"/>
@@ -21188,14 +21248,14 @@
     </row>
     <row r="462" spans="1:9" ht="19" customHeight="1">
       <c r="A462" s="19" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="B462" s="20"/>
       <c r="C462" s="19" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="D462" s="20" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="E462" s="20"/>
       <c r="F462" s="20"/>
@@ -21205,14 +21265,14 @@
     </row>
     <row r="463" spans="1:9" ht="19" customHeight="1">
       <c r="A463" s="19" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="B463" s="20"/>
       <c r="C463" s="19" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="D463" s="20" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="E463" s="20"/>
       <c r="F463" s="20"/>
@@ -21222,14 +21282,14 @@
     </row>
     <row r="464" spans="1:9" ht="19" customHeight="1">
       <c r="A464" s="19" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="B464" s="20"/>
       <c r="C464" s="19" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="E464" s="20"/>
       <c r="F464" s="20"/>
@@ -21239,14 +21299,14 @@
     </row>
     <row r="465" spans="1:9" ht="19" customHeight="1">
       <c r="A465" s="19" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="B465" s="20"/>
       <c r="C465" s="19" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="E465" s="20"/>
       <c r="F465" s="20"/>
@@ -21256,14 +21316,14 @@
     </row>
     <row r="466" spans="1:9" ht="19" customHeight="1">
       <c r="A466" s="19" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="B466" s="20"/>
       <c r="C466" s="19" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="D466" s="20" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="E466" s="20"/>
       <c r="F466" s="20"/>
@@ -21273,14 +21333,14 @@
     </row>
     <row r="467" spans="1:9" ht="19" customHeight="1">
       <c r="A467" s="19" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="B467" s="20"/>
       <c r="C467" s="19" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="E467" s="20"/>
       <c r="F467" s="20"/>
@@ -21290,14 +21350,14 @@
     </row>
     <row r="468" spans="1:9" ht="19" customHeight="1">
       <c r="A468" s="19" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="B468" s="20"/>
       <c r="C468" s="19" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="D468" s="20" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="E468" s="20"/>
       <c r="F468" s="20"/>
@@ -21307,14 +21367,14 @@
     </row>
     <row r="469" spans="1:9" ht="19" customHeight="1">
       <c r="A469" s="19" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="B469" s="20"/>
       <c r="C469" s="19" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="D469" s="20" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="E469" s="20"/>
       <c r="F469" s="20"/>
@@ -21323,10 +21383,16 @@
       <c r="I469" s="18"/>
     </row>
     <row r="470" spans="1:9" ht="19" customHeight="1">
-      <c r="A470" s="19"/>
+      <c r="A470" s="19" t="s">
+        <v>1234</v>
+      </c>
       <c r="B470" s="20"/>
-      <c r="C470" s="20"/>
-      <c r="D470" s="20"/>
+      <c r="C470" s="19" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D470" s="20" t="s">
+        <v>1329</v>
+      </c>
       <c r="E470" s="20"/>
       <c r="F470" s="20"/>
       <c r="G470" s="18"/>
@@ -21334,10 +21400,16 @@
       <c r="I470" s="18"/>
     </row>
     <row r="471" spans="1:9" ht="19" customHeight="1">
-      <c r="A471" s="19"/>
+      <c r="A471" s="19" t="s">
+        <v>1235</v>
+      </c>
       <c r="B471" s="20"/>
-      <c r="C471" s="20"/>
-      <c r="D471" s="20"/>
+      <c r="C471" s="19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D471" s="20" t="s">
+        <v>1330</v>
+      </c>
       <c r="E471" s="20"/>
       <c r="F471" s="20"/>
       <c r="G471" s="18"/>
@@ -21971,15 +22043,37 @@
       <c r="H528" s="17"/>
       <c r="I528" s="18"/>
     </row>
+    <row r="529" spans="1:9" ht="19" customHeight="1">
+      <c r="A529" s="19"/>
+      <c r="B529" s="20"/>
+      <c r="C529" s="20"/>
+      <c r="D529" s="20"/>
+      <c r="E529" s="20"/>
+      <c r="F529" s="20"/>
+      <c r="G529" s="18"/>
+      <c r="H529" s="17"/>
+      <c r="I529" s="18"/>
+    </row>
+    <row r="530" spans="1:9" ht="19" customHeight="1">
+      <c r="A530" s="19"/>
+      <c r="B530" s="20"/>
+      <c r="C530" s="20"/>
+      <c r="D530" s="20"/>
+      <c r="E530" s="20"/>
+      <c r="F530" s="20"/>
+      <c r="G530" s="18"/>
+      <c r="H530" s="17"/>
+      <c r="I530" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J226" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A5:G261 I5:I528">
+  <conditionalFormatting sqref="A5:G261 I5:I530">
     <cfRule type="expression" dxfId="39" priority="37">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D262:D283 D286 D290:D292 D296:D300 D309 D317:D330 D334:D336 D340:D341 D343:D345 D349:D370">
+  <conditionalFormatting sqref="D262:D283 D286 D290:D292 D296:D300 D309 D317:D330 D334:D336 D340:D341 D346:D347 D351:D372">
     <cfRule type="expression" dxfId="38" priority="276">
       <formula>$G264&lt;&gt;""</formula>
     </cfRule>
@@ -21994,7 +22088,7 @@
       <formula>$G286&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D287:D289 D293:D295 D308 D331:D333 D337:D339 D346:D348">
+  <conditionalFormatting sqref="D287:D289 D293:D295 D308 D331:D333 D337:D339 D348:D350">
     <cfRule type="expression" dxfId="35" priority="279">
       <formula>$G290&lt;&gt;""</formula>
     </cfRule>
@@ -22009,7 +22103,7 @@
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D305:D307">
+  <conditionalFormatting sqref="D305:D307 D343:D345">
     <cfRule type="expression" dxfId="32" priority="388">
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
@@ -22039,12 +22133,12 @@
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G373 D316 A334:E335 A336:C355 E336:E355 A356:E357 A358:C370 E358:E370 A371:E373 A374:G528">
+  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G375 D316 A334:E335 A336:C357 E336:E357 A358:E359 A360:C372 E360:E372 A373:E375 A376:G530">
     <cfRule type="expression" dxfId="26" priority="274">
       <formula>$G262&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H528">
+  <conditionalFormatting sqref="H5:H530">
     <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
@@ -22076,15 +22170,15 @@
       <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H395">
+  <conditionalFormatting sqref="H397">
     <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H395)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H397)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H395)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SKIP",H397)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H395)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ERROR",H397)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>

</xml_diff>

<commit_message>
New Parameter - scenarioTimeoutSeconds - scenarioMaxCount
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8A00BD-41B1-264F-B40E-3FBF8A5D171F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F6DD02-456C-0947-91F2-932567EBA827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25280" yWindow="7620" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
+    <workbookView xWindow="41320" yWindow="3060" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
   <sheets>
     <sheet name="message" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="1538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="1544">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -11921,20 +11921,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Rerunning scenario requested.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テストシナリオの再実行が要求されました。</t>
-    <rPh sb="8" eb="11">
-      <t>サイジッコウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ヨウキュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Could not get contents of the WebView.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -11961,11 +11947,75 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Rerun failed.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テストシナリオの再実行が失敗しました。</t>
+    <t>Could not get contents of the screen.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenIsBlackout</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenshotBlackoutThreshold</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenshotBlackoutThreshold is allowed from 0.9 to 1.0. (${value})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>screenshotBlackoutThreshold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>は</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0.9-1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>で設定してください。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(value=${value})</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The screenshot is blacked out. (threshold=${value})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スクリーンショットがブラックアウトしました。(threshold=${value})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rerun failed. ${submessage}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストシナリオの再実行が失敗しました。${submessage}</t>
     <rPh sb="8" eb="11">
       <t>サイジッコウ</t>
     </rPh>
@@ -11975,24 +12025,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Could not get contents of the screen.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>screenIsBlackout</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>screenshotBlackoutThreshold</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>screenshotBlackoutThreshold is allowed from 0.9 to 1.0. (${value})</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>screenshotBlackoutThreshold</t>
+    <t>scenarioTimeoutSeconds</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>scenarioTimeoutSeconds</t>
     </r>
     <r>
       <rPr>
@@ -12009,16 +12047,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>0.9-1.0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tsukushi A Round Gothic Bold"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>で設定してください。</t>
+      <t>0以上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>の値を設定してください。</t>
     </r>
     <r>
       <rPr>
@@ -12028,14 +12066,51 @@
       </rPr>
       <t>(value=${value})</t>
     </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The screenshot is blacked out. (threshold=${value})</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スクリーンショットがブラックアウトしました。(threshold=${value})</t>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">イジョウ </t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>scenarioTimeoutSeconds should be set to 0 or higher. (${value})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rerunning scenario requested. (${submessage})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストシナリオの再実行が要求されました。(${submessage})</t>
+    <rPh sb="8" eb="11">
+      <t>サイジッコウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ヨウキュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>scenarioMaxCount</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>scenarioMaxCount should be set to 1 or higher. (${value})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>scenarioMaxCountは1以上の値を設定してください。 (${value})</t>
+    <rPh sb="15" eb="17">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>セッテイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12380,7 +12455,7 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{C40AA10B-FA57-1748-8D8E-3E12991DC054}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="42">
     <dxf>
       <fill>
         <patternFill>
@@ -12420,6 +12495,13 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12489,7 +12571,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFA0D8EF"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12497,20 +12586,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12545,7 +12620,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12560,6 +12635,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12977,11 +13066,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I530"/>
+  <dimension ref="A1:I537"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A345" sqref="A345"/>
+      <pane ySplit="4" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A396" sqref="A396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19264,14 +19353,14 @@
     </row>
     <row r="344" spans="1:9" ht="19" customHeight="1">
       <c r="A344" s="19" t="s">
-        <v>1533</v>
+        <v>1529</v>
       </c>
       <c r="B344" s="20"/>
       <c r="C344" s="20" t="s">
-        <v>1534</v>
+        <v>1530</v>
       </c>
       <c r="D344" s="20" t="s">
-        <v>1535</v>
+        <v>1531</v>
       </c>
       <c r="E344" s="20"/>
       <c r="F344" s="20"/>
@@ -19281,14 +19370,14 @@
     </row>
     <row r="345" spans="1:9" ht="19" customHeight="1">
       <c r="A345" s="19" t="s">
-        <v>1532</v>
+        <v>1528</v>
       </c>
       <c r="B345" s="20"/>
       <c r="C345" s="20" t="s">
-        <v>1536</v>
+        <v>1532</v>
       </c>
       <c r="D345" s="20" t="s">
-        <v>1537</v>
+        <v>1533</v>
       </c>
       <c r="E345" s="20"/>
       <c r="F345" s="20"/>
@@ -20046,14 +20135,14 @@
     </row>
     <row r="390" spans="1:9" ht="19" customHeight="1">
       <c r="A390" s="19" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="B390" s="20"/>
       <c r="C390" s="20" t="s">
-        <v>1531</v>
+        <v>1527</v>
       </c>
       <c r="D390" s="20" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="E390" s="20"/>
       <c r="F390" s="20"/>
@@ -20063,11 +20152,11 @@
     </row>
     <row r="391" spans="1:9" ht="19" customHeight="1">
       <c r="A391" s="19" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="B391" s="20"/>
       <c r="C391" s="20" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="D391" s="20" t="s">
         <v>1520</v>
@@ -20084,10 +20173,10 @@
       </c>
       <c r="B392" s="20"/>
       <c r="C392" s="20" t="s">
-        <v>1522</v>
+        <v>1539</v>
       </c>
       <c r="D392" s="20" t="s">
-        <v>1523</v>
+        <v>1540</v>
       </c>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
@@ -20097,14 +20186,14 @@
     </row>
     <row r="393" spans="1:9" ht="19" customHeight="1">
       <c r="A393" s="19" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="B393" s="20"/>
       <c r="C393" s="20" t="s">
-        <v>1529</v>
+        <v>1534</v>
       </c>
       <c r="D393" s="20" t="s">
-        <v>1530</v>
+        <v>1535</v>
       </c>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
@@ -20113,10 +20202,16 @@
       <c r="I393" s="18"/>
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
-      <c r="A394" s="19"/>
+      <c r="A394" s="19" t="s">
+        <v>1536</v>
+      </c>
       <c r="B394" s="20"/>
-      <c r="C394" s="20"/>
-      <c r="D394" s="20"/>
+      <c r="C394" s="20" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D394" s="20" t="s">
+        <v>1537</v>
+      </c>
       <c r="E394" s="20"/>
       <c r="F394" s="20"/>
       <c r="G394" s="18"/>
@@ -20124,10 +20219,16 @@
       <c r="I394" s="18"/>
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
-      <c r="A395" s="19"/>
+      <c r="A395" s="19" t="s">
+        <v>1541</v>
+      </c>
       <c r="B395" s="20"/>
-      <c r="C395" s="20"/>
-      <c r="D395" s="20"/>
+      <c r="C395" s="20" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D395" s="20" t="s">
+        <v>1543</v>
+      </c>
       <c r="E395" s="20"/>
       <c r="F395" s="20"/>
       <c r="G395" s="18"/>
@@ -20146,29 +20247,21 @@
       <c r="I396" s="18"/>
     </row>
     <row r="397" spans="1:9" ht="19" customHeight="1">
-      <c r="A397" s="26" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B397" s="23"/>
-      <c r="C397" s="23"/>
-      <c r="D397" s="23"/>
-      <c r="E397" s="23"/>
-      <c r="F397" s="23"/>
-      <c r="G397" s="24"/>
-      <c r="H397" s="25"/>
-      <c r="I397" s="24"/>
+      <c r="A397" s="19"/>
+      <c r="B397" s="20"/>
+      <c r="C397" s="20"/>
+      <c r="D397" s="20"/>
+      <c r="E397" s="20"/>
+      <c r="F397" s="20"/>
+      <c r="G397" s="18"/>
+      <c r="H397" s="17"/>
+      <c r="I397" s="18"/>
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
-      <c r="A398" s="19" t="s">
-        <v>1170</v>
-      </c>
+      <c r="A398" s="19"/>
       <c r="B398" s="20"/>
-      <c r="C398" s="20" t="s">
-        <v>1170</v>
-      </c>
-      <c r="D398" s="20" t="s">
-        <v>1264</v>
-      </c>
+      <c r="C398" s="20"/>
+      <c r="D398" s="20"/>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
       <c r="G398" s="18"/>
@@ -20176,16 +20269,10 @@
       <c r="I398" s="18"/>
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
-      <c r="A399" s="19" t="s">
-        <v>1171</v>
-      </c>
+      <c r="A399" s="19"/>
       <c r="B399" s="20"/>
-      <c r="C399" s="20" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D399" s="20" t="s">
-        <v>1265</v>
-      </c>
+      <c r="C399" s="20"/>
+      <c r="D399" s="20"/>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
       <c r="G399" s="18"/>
@@ -20193,16 +20280,10 @@
       <c r="I399" s="18"/>
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
-      <c r="A400" s="19" t="s">
-        <v>1172</v>
-      </c>
+      <c r="A400" s="19"/>
       <c r="B400" s="20"/>
-      <c r="C400" s="20" t="s">
-        <v>1172</v>
-      </c>
-      <c r="D400" s="20" t="s">
-        <v>1267</v>
-      </c>
+      <c r="C400" s="20"/>
+      <c r="D400" s="20"/>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
       <c r="G400" s="18"/>
@@ -20210,16 +20291,10 @@
       <c r="I400" s="18"/>
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
-      <c r="A401" s="19" t="s">
-        <v>1173</v>
-      </c>
+      <c r="A401" s="19"/>
       <c r="B401" s="20"/>
-      <c r="C401" s="20" t="s">
-        <v>1173</v>
-      </c>
-      <c r="D401" s="20" t="s">
-        <v>1268</v>
-      </c>
+      <c r="C401" s="20"/>
+      <c r="D401" s="20"/>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
       <c r="G401" s="18"/>
@@ -20227,16 +20302,10 @@
       <c r="I401" s="18"/>
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
-      <c r="A402" s="19" t="s">
-        <v>1174</v>
-      </c>
+      <c r="A402" s="19"/>
       <c r="B402" s="20"/>
-      <c r="C402" s="20" t="s">
-        <v>1174</v>
-      </c>
-      <c r="D402" s="20" t="s">
-        <v>1269</v>
-      </c>
+      <c r="C402" s="20"/>
+      <c r="D402" s="20"/>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
       <c r="G402" s="18"/>
@@ -20244,16 +20313,10 @@
       <c r="I402" s="18"/>
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
-      <c r="A403" s="19" t="s">
-        <v>1175</v>
-      </c>
+      <c r="A403" s="19"/>
       <c r="B403" s="20"/>
-      <c r="C403" s="20" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D403" s="20" t="s">
-        <v>1266</v>
-      </c>
+      <c r="C403" s="20"/>
+      <c r="D403" s="20"/>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
       <c r="G403" s="18"/>
@@ -20261,32 +20324,28 @@
       <c r="I403" s="18"/>
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
-      <c r="A404" s="19" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B404" s="20"/>
-      <c r="C404" s="20" t="s">
-        <v>1176</v>
-      </c>
-      <c r="D404" s="20" t="s">
-        <v>1270</v>
-      </c>
-      <c r="E404" s="20"/>
-      <c r="F404" s="20"/>
-      <c r="G404" s="18"/>
-      <c r="H404" s="17"/>
-      <c r="I404" s="18"/>
+      <c r="A404" s="26" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B404" s="23"/>
+      <c r="C404" s="23"/>
+      <c r="D404" s="23"/>
+      <c r="E404" s="23"/>
+      <c r="F404" s="23"/>
+      <c r="G404" s="24"/>
+      <c r="H404" s="25"/>
+      <c r="I404" s="24"/>
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1177</v>
+        <v>1170</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="20" t="s">
-        <v>1177</v>
+        <v>1170</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1271</v>
+        <v>1264</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -20296,14 +20355,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1178</v>
+        <v>1171</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="20" t="s">
-        <v>1178</v>
+        <v>1171</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1272</v>
+        <v>1265</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -20313,14 +20372,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1179</v>
+        <v>1172</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="20" t="s">
-        <v>1179</v>
+        <v>1172</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -20330,14 +20389,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1180</v>
+        <v>1173</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="20" t="s">
-        <v>1180</v>
+        <v>1173</v>
       </c>
       <c r="D408" s="20" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -20347,14 +20406,14 @@
     </row>
     <row r="409" spans="1:9" ht="19" customHeight="1">
       <c r="A409" s="19" t="s">
-        <v>1181</v>
+        <v>1174</v>
       </c>
       <c r="B409" s="20"/>
       <c r="C409" s="20" t="s">
-        <v>1181</v>
+        <v>1174</v>
       </c>
       <c r="D409" s="20" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
       <c r="E409" s="20"/>
       <c r="F409" s="20"/>
@@ -20364,14 +20423,14 @@
     </row>
     <row r="410" spans="1:9" ht="19" customHeight="1">
       <c r="A410" s="19" t="s">
-        <v>1182</v>
+        <v>1175</v>
       </c>
       <c r="B410" s="20"/>
       <c r="C410" s="20" t="s">
-        <v>1182</v>
+        <v>1175</v>
       </c>
       <c r="D410" s="20" t="s">
-        <v>1276</v>
+        <v>1266</v>
       </c>
       <c r="E410" s="20"/>
       <c r="F410" s="20"/>
@@ -20381,14 +20440,14 @@
     </row>
     <row r="411" spans="1:9" ht="19" customHeight="1">
       <c r="A411" s="19" t="s">
-        <v>1183</v>
+        <v>1176</v>
       </c>
       <c r="B411" s="20"/>
       <c r="C411" s="20" t="s">
-        <v>1183</v>
+        <v>1176</v>
       </c>
       <c r="D411" s="20" t="s">
-        <v>1277</v>
+        <v>1270</v>
       </c>
       <c r="E411" s="20"/>
       <c r="F411" s="20"/>
@@ -20398,14 +20457,14 @@
     </row>
     <row r="412" spans="1:9" ht="19" customHeight="1">
       <c r="A412" s="19" t="s">
-        <v>1184</v>
+        <v>1177</v>
       </c>
       <c r="B412" s="20"/>
       <c r="C412" s="20" t="s">
-        <v>1184</v>
+        <v>1177</v>
       </c>
       <c r="D412" s="20" t="s">
-        <v>1278</v>
+        <v>1271</v>
       </c>
       <c r="E412" s="20"/>
       <c r="F412" s="20"/>
@@ -20415,14 +20474,14 @@
     </row>
     <row r="413" spans="1:9" ht="19" customHeight="1">
       <c r="A413" s="19" t="s">
-        <v>1185</v>
+        <v>1178</v>
       </c>
       <c r="B413" s="20"/>
       <c r="C413" s="20" t="s">
-        <v>1185</v>
+        <v>1178</v>
       </c>
       <c r="D413" s="20" t="s">
-        <v>1279</v>
+        <v>1272</v>
       </c>
       <c r="E413" s="20"/>
       <c r="F413" s="20"/>
@@ -20432,14 +20491,14 @@
     </row>
     <row r="414" spans="1:9" ht="19" customHeight="1">
       <c r="A414" s="19" t="s">
-        <v>1186</v>
+        <v>1179</v>
       </c>
       <c r="B414" s="20"/>
       <c r="C414" s="20" t="s">
-        <v>1186</v>
+        <v>1179</v>
       </c>
       <c r="D414" s="20" t="s">
-        <v>1280</v>
+        <v>1273</v>
       </c>
       <c r="E414" s="20"/>
       <c r="F414" s="20"/>
@@ -20449,14 +20508,14 @@
     </row>
     <row r="415" spans="1:9" ht="19" customHeight="1">
       <c r="A415" s="19" t="s">
-        <v>1187</v>
+        <v>1180</v>
       </c>
       <c r="B415" s="20"/>
       <c r="C415" s="20" t="s">
-        <v>1187</v>
+        <v>1180</v>
       </c>
       <c r="D415" s="20" t="s">
-        <v>1281</v>
+        <v>1274</v>
       </c>
       <c r="E415" s="20"/>
       <c r="F415" s="20"/>
@@ -20466,14 +20525,14 @@
     </row>
     <row r="416" spans="1:9" ht="19" customHeight="1">
       <c r="A416" s="19" t="s">
-        <v>1188</v>
+        <v>1181</v>
       </c>
       <c r="B416" s="20"/>
       <c r="C416" s="20" t="s">
-        <v>1188</v>
+        <v>1181</v>
       </c>
       <c r="D416" s="20" t="s">
-        <v>1282</v>
+        <v>1275</v>
       </c>
       <c r="E416" s="20"/>
       <c r="F416" s="20"/>
@@ -20483,14 +20542,14 @@
     </row>
     <row r="417" spans="1:9" ht="19" customHeight="1">
       <c r="A417" s="19" t="s">
-        <v>1189</v>
+        <v>1182</v>
       </c>
       <c r="B417" s="20"/>
       <c r="C417" s="20" t="s">
-        <v>1189</v>
+        <v>1182</v>
       </c>
       <c r="D417" s="20" t="s">
-        <v>1283</v>
+        <v>1276</v>
       </c>
       <c r="E417" s="20"/>
       <c r="F417" s="20"/>
@@ -20500,14 +20559,14 @@
     </row>
     <row r="418" spans="1:9" ht="19" customHeight="1">
       <c r="A418" s="19" t="s">
-        <v>1190</v>
+        <v>1183</v>
       </c>
       <c r="B418" s="20"/>
       <c r="C418" s="20" t="s">
-        <v>1190</v>
+        <v>1183</v>
       </c>
       <c r="D418" s="20" t="s">
-        <v>1284</v>
+        <v>1277</v>
       </c>
       <c r="E418" s="20"/>
       <c r="F418" s="20"/>
@@ -20517,14 +20576,14 @@
     </row>
     <row r="419" spans="1:9" ht="19" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>1191</v>
+        <v>1184</v>
       </c>
       <c r="B419" s="20"/>
       <c r="C419" s="20" t="s">
-        <v>1191</v>
+        <v>1184</v>
       </c>
       <c r="D419" s="20" t="s">
-        <v>1285</v>
+        <v>1278</v>
       </c>
       <c r="E419" s="20"/>
       <c r="F419" s="20"/>
@@ -20534,14 +20593,14 @@
     </row>
     <row r="420" spans="1:9" ht="19" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>1192</v>
+        <v>1185</v>
       </c>
       <c r="B420" s="20"/>
       <c r="C420" s="20" t="s">
-        <v>1192</v>
+        <v>1185</v>
       </c>
       <c r="D420" s="20" t="s">
-        <v>1286</v>
+        <v>1279</v>
       </c>
       <c r="E420" s="20"/>
       <c r="F420" s="20"/>
@@ -20551,14 +20610,14 @@
     </row>
     <row r="421" spans="1:9" ht="19" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>1193</v>
+        <v>1186</v>
       </c>
       <c r="B421" s="20"/>
       <c r="C421" s="20" t="s">
-        <v>1193</v>
+        <v>1186</v>
       </c>
       <c r="D421" s="20" t="s">
-        <v>1287</v>
+        <v>1280</v>
       </c>
       <c r="E421" s="20"/>
       <c r="F421" s="20"/>
@@ -20568,14 +20627,14 @@
     </row>
     <row r="422" spans="1:9" ht="19" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>1194</v>
+        <v>1187</v>
       </c>
       <c r="B422" s="20"/>
-      <c r="C422" s="19" t="s">
-        <v>1331</v>
+      <c r="C422" s="20" t="s">
+        <v>1187</v>
       </c>
       <c r="D422" s="20" t="s">
-        <v>1288</v>
+        <v>1281</v>
       </c>
       <c r="E422" s="20"/>
       <c r="F422" s="20"/>
@@ -20585,14 +20644,14 @@
     </row>
     <row r="423" spans="1:9" ht="19" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>1195</v>
+        <v>1188</v>
       </c>
       <c r="B423" s="20"/>
-      <c r="C423" s="19" t="s">
-        <v>1332</v>
+      <c r="C423" s="20" t="s">
+        <v>1188</v>
       </c>
       <c r="D423" s="20" t="s">
-        <v>1289</v>
+        <v>1282</v>
       </c>
       <c r="E423" s="20"/>
       <c r="F423" s="20"/>
@@ -20602,14 +20661,14 @@
     </row>
     <row r="424" spans="1:9" ht="19" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>1196</v>
+        <v>1189</v>
       </c>
       <c r="B424" s="20"/>
-      <c r="C424" s="19" t="s">
-        <v>1333</v>
+      <c r="C424" s="20" t="s">
+        <v>1189</v>
       </c>
       <c r="D424" s="20" t="s">
-        <v>1290</v>
+        <v>1283</v>
       </c>
       <c r="E424" s="20"/>
       <c r="F424" s="20"/>
@@ -20619,14 +20678,14 @@
     </row>
     <row r="425" spans="1:9" ht="19" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>1197</v>
+        <v>1190</v>
       </c>
       <c r="B425" s="20"/>
-      <c r="C425" s="19" t="s">
-        <v>1334</v>
+      <c r="C425" s="20" t="s">
+        <v>1190</v>
       </c>
       <c r="D425" s="20" t="s">
-        <v>1291</v>
+        <v>1284</v>
       </c>
       <c r="E425" s="20"/>
       <c r="F425" s="20"/>
@@ -20636,14 +20695,14 @@
     </row>
     <row r="426" spans="1:9" ht="19" customHeight="1">
       <c r="A426" s="19" t="s">
-        <v>1198</v>
+        <v>1191</v>
       </c>
       <c r="B426" s="20"/>
-      <c r="C426" s="19" t="s">
-        <v>1335</v>
+      <c r="C426" s="20" t="s">
+        <v>1191</v>
       </c>
       <c r="D426" s="20" t="s">
-        <v>1292</v>
+        <v>1285</v>
       </c>
       <c r="E426" s="20"/>
       <c r="F426" s="20"/>
@@ -20653,14 +20712,14 @@
     </row>
     <row r="427" spans="1:9" ht="19" customHeight="1">
       <c r="A427" s="19" t="s">
-        <v>1199</v>
+        <v>1192</v>
       </c>
       <c r="B427" s="20"/>
-      <c r="C427" s="19" t="s">
-        <v>1336</v>
+      <c r="C427" s="20" t="s">
+        <v>1192</v>
       </c>
       <c r="D427" s="20" t="s">
-        <v>1293</v>
+        <v>1286</v>
       </c>
       <c r="E427" s="20"/>
       <c r="F427" s="20"/>
@@ -20670,14 +20729,14 @@
     </row>
     <row r="428" spans="1:9" ht="19" customHeight="1">
       <c r="A428" s="19" t="s">
-        <v>1200</v>
+        <v>1193</v>
       </c>
       <c r="B428" s="20"/>
-      <c r="C428" s="19" t="s">
-        <v>1337</v>
+      <c r="C428" s="20" t="s">
+        <v>1193</v>
       </c>
       <c r="D428" s="20" t="s">
-        <v>1294</v>
+        <v>1287</v>
       </c>
       <c r="E428" s="20"/>
       <c r="F428" s="20"/>
@@ -20687,14 +20746,14 @@
     </row>
     <row r="429" spans="1:9" ht="19" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>1201</v>
+        <v>1194</v>
       </c>
       <c r="B429" s="20"/>
       <c r="C429" s="19" t="s">
-        <v>1338</v>
+        <v>1331</v>
       </c>
       <c r="D429" s="20" t="s">
-        <v>1295</v>
+        <v>1288</v>
       </c>
       <c r="E429" s="20"/>
       <c r="F429" s="20"/>
@@ -20704,14 +20763,14 @@
     </row>
     <row r="430" spans="1:9" ht="19" customHeight="1">
       <c r="A430" s="19" t="s">
-        <v>1202</v>
+        <v>1195</v>
       </c>
       <c r="B430" s="20"/>
       <c r="C430" s="19" t="s">
-        <v>1339</v>
+        <v>1332</v>
       </c>
       <c r="D430" s="20" t="s">
-        <v>1296</v>
+        <v>1289</v>
       </c>
       <c r="E430" s="20"/>
       <c r="F430" s="20"/>
@@ -20721,14 +20780,14 @@
     </row>
     <row r="431" spans="1:9" ht="19" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>1203</v>
+        <v>1196</v>
       </c>
       <c r="B431" s="20"/>
       <c r="C431" s="19" t="s">
-        <v>1340</v>
+        <v>1333</v>
       </c>
       <c r="D431" s="20" t="s">
-        <v>1297</v>
+        <v>1290</v>
       </c>
       <c r="E431" s="20"/>
       <c r="F431" s="20"/>
@@ -20738,14 +20797,14 @@
     </row>
     <row r="432" spans="1:9" ht="19" customHeight="1">
       <c r="A432" s="19" t="s">
-        <v>1204</v>
+        <v>1197</v>
       </c>
       <c r="B432" s="20"/>
       <c r="C432" s="19" t="s">
-        <v>1341</v>
+        <v>1334</v>
       </c>
       <c r="D432" s="20" t="s">
-        <v>1298</v>
+        <v>1291</v>
       </c>
       <c r="E432" s="20"/>
       <c r="F432" s="20"/>
@@ -20755,14 +20814,14 @@
     </row>
     <row r="433" spans="1:9" ht="19" customHeight="1">
       <c r="A433" s="19" t="s">
-        <v>1205</v>
+        <v>1198</v>
       </c>
       <c r="B433" s="20"/>
       <c r="C433" s="19" t="s">
-        <v>1342</v>
+        <v>1335</v>
       </c>
       <c r="D433" s="20" t="s">
-        <v>1299</v>
+        <v>1292</v>
       </c>
       <c r="E433" s="20"/>
       <c r="F433" s="20"/>
@@ -20772,14 +20831,14 @@
     </row>
     <row r="434" spans="1:9" ht="19" customHeight="1">
       <c r="A434" s="19" t="s">
-        <v>1242</v>
+        <v>1199</v>
       </c>
       <c r="B434" s="20"/>
       <c r="C434" s="19" t="s">
-        <v>1343</v>
+        <v>1336</v>
       </c>
       <c r="D434" s="20" t="s">
-        <v>1487</v>
+        <v>1293</v>
       </c>
       <c r="E434" s="20"/>
       <c r="F434" s="20"/>
@@ -20789,14 +20848,14 @@
     </row>
     <row r="435" spans="1:9" ht="19" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>1206</v>
+        <v>1200</v>
       </c>
       <c r="B435" s="20"/>
       <c r="C435" s="19" t="s">
-        <v>1344</v>
+        <v>1337</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>1481</v>
+        <v>1294</v>
       </c>
       <c r="E435" s="20"/>
       <c r="F435" s="20"/>
@@ -20806,14 +20865,14 @@
     </row>
     <row r="436" spans="1:9" ht="19" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>1207</v>
+        <v>1201</v>
       </c>
       <c r="B436" s="20"/>
       <c r="C436" s="19" t="s">
-        <v>1207</v>
+        <v>1338</v>
       </c>
       <c r="D436" s="20" t="s">
-        <v>1482</v>
+        <v>1295</v>
       </c>
       <c r="E436" s="20"/>
       <c r="F436" s="20"/>
@@ -20823,14 +20882,14 @@
     </row>
     <row r="437" spans="1:9" ht="19" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>1208</v>
+        <v>1202</v>
       </c>
       <c r="B437" s="20"/>
       <c r="C437" s="19" t="s">
-        <v>1208</v>
+        <v>1339</v>
       </c>
       <c r="D437" s="20" t="s">
-        <v>1483</v>
+        <v>1296</v>
       </c>
       <c r="E437" s="20"/>
       <c r="F437" s="20"/>
@@ -20840,14 +20899,14 @@
     </row>
     <row r="438" spans="1:9" ht="19" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>1209</v>
+        <v>1203</v>
       </c>
       <c r="B438" s="20"/>
       <c r="C438" s="19" t="s">
-        <v>1209</v>
+        <v>1340</v>
       </c>
       <c r="D438" s="20" t="s">
-        <v>1484</v>
+        <v>1297</v>
       </c>
       <c r="E438" s="20"/>
       <c r="F438" s="20"/>
@@ -20857,14 +20916,14 @@
     </row>
     <row r="439" spans="1:9" ht="19" customHeight="1">
       <c r="A439" s="19" t="s">
-        <v>1210</v>
+        <v>1204</v>
       </c>
       <c r="B439" s="20"/>
       <c r="C439" s="19" t="s">
-        <v>1210</v>
+        <v>1341</v>
       </c>
       <c r="D439" s="20" t="s">
-        <v>1485</v>
+        <v>1298</v>
       </c>
       <c r="E439" s="20"/>
       <c r="F439" s="20"/>
@@ -20874,14 +20933,14 @@
     </row>
     <row r="440" spans="1:9" ht="19" customHeight="1">
       <c r="A440" s="19" t="s">
-        <v>1211</v>
+        <v>1205</v>
       </c>
       <c r="B440" s="20"/>
       <c r="C440" s="19" t="s">
-        <v>1211</v>
+        <v>1342</v>
       </c>
       <c r="D440" s="20" t="s">
-        <v>1486</v>
+        <v>1299</v>
       </c>
       <c r="E440" s="20"/>
       <c r="F440" s="20"/>
@@ -20891,14 +20950,14 @@
     </row>
     <row r="441" spans="1:9" ht="19" customHeight="1">
       <c r="A441" s="19" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B441" s="20"/>
       <c r="C441" s="19" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D441" s="20" t="s">
-        <v>1300</v>
+        <v>1487</v>
       </c>
       <c r="E441" s="20"/>
       <c r="F441" s="20"/>
@@ -20908,14 +20967,14 @@
     </row>
     <row r="442" spans="1:9" ht="19" customHeight="1">
       <c r="A442" s="19" t="s">
-        <v>1212</v>
+        <v>1206</v>
       </c>
       <c r="B442" s="20"/>
       <c r="C442" s="19" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D442" s="20" t="s">
-        <v>1301</v>
+        <v>1481</v>
       </c>
       <c r="E442" s="20"/>
       <c r="F442" s="20"/>
@@ -20925,14 +20984,14 @@
     </row>
     <row r="443" spans="1:9" ht="19" customHeight="1">
       <c r="A443" s="19" t="s">
-        <v>1213</v>
+        <v>1207</v>
       </c>
       <c r="B443" s="20"/>
       <c r="C443" s="19" t="s">
-        <v>1347</v>
+        <v>1207</v>
       </c>
       <c r="D443" s="20" t="s">
-        <v>1302</v>
+        <v>1482</v>
       </c>
       <c r="E443" s="20"/>
       <c r="F443" s="20"/>
@@ -20942,14 +21001,14 @@
     </row>
     <row r="444" spans="1:9" ht="19" customHeight="1">
       <c r="A444" s="19" t="s">
-        <v>1214</v>
+        <v>1208</v>
       </c>
       <c r="B444" s="20"/>
       <c r="C444" s="19" t="s">
-        <v>1348</v>
+        <v>1208</v>
       </c>
       <c r="D444" s="20" t="s">
-        <v>1303</v>
+        <v>1483</v>
       </c>
       <c r="E444" s="20"/>
       <c r="F444" s="20"/>
@@ -20959,14 +21018,14 @@
     </row>
     <row r="445" spans="1:9" ht="19" customHeight="1">
       <c r="A445" s="19" t="s">
-        <v>1215</v>
+        <v>1209</v>
       </c>
       <c r="B445" s="20"/>
       <c r="C445" s="19" t="s">
-        <v>1349</v>
+        <v>1209</v>
       </c>
       <c r="D445" s="20" t="s">
-        <v>1304</v>
+        <v>1484</v>
       </c>
       <c r="E445" s="20"/>
       <c r="F445" s="20"/>
@@ -20976,14 +21035,14 @@
     </row>
     <row r="446" spans="1:9" ht="19" customHeight="1">
       <c r="A446" s="19" t="s">
-        <v>1216</v>
+        <v>1210</v>
       </c>
       <c r="B446" s="20"/>
       <c r="C446" s="19" t="s">
-        <v>1350</v>
+        <v>1210</v>
       </c>
       <c r="D446" s="20" t="s">
-        <v>1305</v>
+        <v>1485</v>
       </c>
       <c r="E446" s="20"/>
       <c r="F446" s="20"/>
@@ -20993,14 +21052,14 @@
     </row>
     <row r="447" spans="1:9" ht="19" customHeight="1">
       <c r="A447" s="19" t="s">
-        <v>1217</v>
+        <v>1211</v>
       </c>
       <c r="B447" s="20"/>
       <c r="C447" s="19" t="s">
-        <v>1351</v>
+        <v>1211</v>
       </c>
       <c r="D447" s="20" t="s">
-        <v>1306</v>
+        <v>1486</v>
       </c>
       <c r="E447" s="20"/>
       <c r="F447" s="20"/>
@@ -21010,14 +21069,14 @@
     </row>
     <row r="448" spans="1:9" ht="19" customHeight="1">
       <c r="A448" s="19" t="s">
-        <v>1236</v>
+        <v>1243</v>
       </c>
       <c r="B448" s="20"/>
       <c r="C448" s="19" t="s">
-        <v>1352</v>
+        <v>1345</v>
       </c>
       <c r="D448" s="20" t="s">
-        <v>1307</v>
+        <v>1300</v>
       </c>
       <c r="E448" s="20"/>
       <c r="F448" s="20"/>
@@ -21027,14 +21086,14 @@
     </row>
     <row r="449" spans="1:9" ht="19" customHeight="1">
       <c r="A449" s="19" t="s">
-        <v>1237</v>
+        <v>1212</v>
       </c>
       <c r="B449" s="20"/>
       <c r="C449" s="19" t="s">
-        <v>1353</v>
+        <v>1346</v>
       </c>
       <c r="D449" s="20" t="s">
-        <v>1308</v>
+        <v>1301</v>
       </c>
       <c r="E449" s="20"/>
       <c r="F449" s="20"/>
@@ -21044,14 +21103,14 @@
     </row>
     <row r="450" spans="1:9" ht="19" customHeight="1">
       <c r="A450" s="19" t="s">
-        <v>1238</v>
+        <v>1213</v>
       </c>
       <c r="B450" s="20"/>
       <c r="C450" s="19" t="s">
-        <v>1354</v>
+        <v>1347</v>
       </c>
       <c r="D450" s="20" t="s">
-        <v>1309</v>
+        <v>1302</v>
       </c>
       <c r="E450" s="20"/>
       <c r="F450" s="20"/>
@@ -21061,14 +21120,14 @@
     </row>
     <row r="451" spans="1:9" ht="19" customHeight="1">
       <c r="A451" s="19" t="s">
-        <v>1239</v>
+        <v>1214</v>
       </c>
       <c r="B451" s="20"/>
       <c r="C451" s="19" t="s">
-        <v>1355</v>
+        <v>1348</v>
       </c>
       <c r="D451" s="20" t="s">
-        <v>1310</v>
+        <v>1303</v>
       </c>
       <c r="E451" s="20"/>
       <c r="F451" s="20"/>
@@ -21078,14 +21137,14 @@
     </row>
     <row r="452" spans="1:9" ht="19" customHeight="1">
       <c r="A452" s="19" t="s">
-        <v>1240</v>
+        <v>1215</v>
       </c>
       <c r="B452" s="20"/>
       <c r="C452" s="19" t="s">
-        <v>1356</v>
+        <v>1349</v>
       </c>
       <c r="D452" s="20" t="s">
-        <v>1311</v>
+        <v>1304</v>
       </c>
       <c r="E452" s="20"/>
       <c r="F452" s="20"/>
@@ -21095,14 +21154,14 @@
     </row>
     <row r="453" spans="1:9" ht="19" customHeight="1">
       <c r="A453" s="19" t="s">
-        <v>1241</v>
+        <v>1216</v>
       </c>
       <c r="B453" s="20"/>
       <c r="C453" s="19" t="s">
-        <v>1357</v>
+        <v>1350</v>
       </c>
       <c r="D453" s="20" t="s">
-        <v>1312</v>
+        <v>1305</v>
       </c>
       <c r="E453" s="20"/>
       <c r="F453" s="20"/>
@@ -21112,14 +21171,14 @@
     </row>
     <row r="454" spans="1:9" ht="19" customHeight="1">
       <c r="A454" s="19" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B454" s="20"/>
       <c r="C454" s="19" t="s">
-        <v>1358</v>
+        <v>1351</v>
       </c>
       <c r="D454" s="20" t="s">
-        <v>1313</v>
+        <v>1306</v>
       </c>
       <c r="E454" s="20"/>
       <c r="F454" s="20"/>
@@ -21129,14 +21188,14 @@
     </row>
     <row r="455" spans="1:9" ht="19" customHeight="1">
       <c r="A455" s="19" t="s">
-        <v>1219</v>
+        <v>1236</v>
       </c>
       <c r="B455" s="20"/>
       <c r="C455" s="19" t="s">
-        <v>1359</v>
+        <v>1352</v>
       </c>
       <c r="D455" s="20" t="s">
-        <v>1314</v>
+        <v>1307</v>
       </c>
       <c r="E455" s="20"/>
       <c r="F455" s="20"/>
@@ -21146,14 +21205,14 @@
     </row>
     <row r="456" spans="1:9" ht="19" customHeight="1">
       <c r="A456" s="19" t="s">
-        <v>1220</v>
+        <v>1237</v>
       </c>
       <c r="B456" s="20"/>
       <c r="C456" s="19" t="s">
-        <v>1360</v>
+        <v>1353</v>
       </c>
       <c r="D456" s="20" t="s">
-        <v>1315</v>
+        <v>1308</v>
       </c>
       <c r="E456" s="20"/>
       <c r="F456" s="20"/>
@@ -21163,14 +21222,14 @@
     </row>
     <row r="457" spans="1:9" ht="19" customHeight="1">
       <c r="A457" s="19" t="s">
-        <v>1221</v>
+        <v>1238</v>
       </c>
       <c r="B457" s="20"/>
       <c r="C457" s="19" t="s">
-        <v>1361</v>
+        <v>1354</v>
       </c>
       <c r="D457" s="20" t="s">
-        <v>1316</v>
+        <v>1309</v>
       </c>
       <c r="E457" s="20"/>
       <c r="F457" s="20"/>
@@ -21180,14 +21239,14 @@
     </row>
     <row r="458" spans="1:9" ht="19" customHeight="1">
       <c r="A458" s="19" t="s">
-        <v>1222</v>
+        <v>1239</v>
       </c>
       <c r="B458" s="20"/>
       <c r="C458" s="19" t="s">
-        <v>1362</v>
+        <v>1355</v>
       </c>
       <c r="D458" s="20" t="s">
-        <v>1317</v>
+        <v>1310</v>
       </c>
       <c r="E458" s="20"/>
       <c r="F458" s="20"/>
@@ -21197,14 +21256,14 @@
     </row>
     <row r="459" spans="1:9" ht="19" customHeight="1">
       <c r="A459" s="19" t="s">
-        <v>1223</v>
+        <v>1240</v>
       </c>
       <c r="B459" s="20"/>
       <c r="C459" s="19" t="s">
-        <v>1363</v>
+        <v>1356</v>
       </c>
       <c r="D459" s="20" t="s">
-        <v>1318</v>
+        <v>1311</v>
       </c>
       <c r="E459" s="20"/>
       <c r="F459" s="20"/>
@@ -21214,14 +21273,14 @@
     </row>
     <row r="460" spans="1:9" ht="19" customHeight="1">
       <c r="A460" s="19" t="s">
-        <v>1224</v>
+        <v>1241</v>
       </c>
       <c r="B460" s="20"/>
       <c r="C460" s="19" t="s">
-        <v>1364</v>
+        <v>1357</v>
       </c>
       <c r="D460" s="20" t="s">
-        <v>1319</v>
+        <v>1312</v>
       </c>
       <c r="E460" s="20"/>
       <c r="F460" s="20"/>
@@ -21231,14 +21290,14 @@
     </row>
     <row r="461" spans="1:9" ht="19" customHeight="1">
       <c r="A461" s="19" t="s">
-        <v>1225</v>
+        <v>1218</v>
       </c>
       <c r="B461" s="20"/>
       <c r="C461" s="19" t="s">
-        <v>1365</v>
+        <v>1358</v>
       </c>
       <c r="D461" s="20" t="s">
-        <v>1320</v>
+        <v>1313</v>
       </c>
       <c r="E461" s="20"/>
       <c r="F461" s="20"/>
@@ -21248,14 +21307,14 @@
     </row>
     <row r="462" spans="1:9" ht="19" customHeight="1">
       <c r="A462" s="19" t="s">
-        <v>1226</v>
+        <v>1219</v>
       </c>
       <c r="B462" s="20"/>
       <c r="C462" s="19" t="s">
-        <v>1366</v>
+        <v>1359</v>
       </c>
       <c r="D462" s="20" t="s">
-        <v>1321</v>
+        <v>1314</v>
       </c>
       <c r="E462" s="20"/>
       <c r="F462" s="20"/>
@@ -21265,14 +21324,14 @@
     </row>
     <row r="463" spans="1:9" ht="19" customHeight="1">
       <c r="A463" s="19" t="s">
-        <v>1227</v>
+        <v>1220</v>
       </c>
       <c r="B463" s="20"/>
       <c r="C463" s="19" t="s">
-        <v>1367</v>
+        <v>1360</v>
       </c>
       <c r="D463" s="20" t="s">
-        <v>1322</v>
+        <v>1315</v>
       </c>
       <c r="E463" s="20"/>
       <c r="F463" s="20"/>
@@ -21282,14 +21341,14 @@
     </row>
     <row r="464" spans="1:9" ht="19" customHeight="1">
       <c r="A464" s="19" t="s">
-        <v>1228</v>
+        <v>1221</v>
       </c>
       <c r="B464" s="20"/>
       <c r="C464" s="19" t="s">
-        <v>1368</v>
+        <v>1361</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>1323</v>
+        <v>1316</v>
       </c>
       <c r="E464" s="20"/>
       <c r="F464" s="20"/>
@@ -21299,14 +21358,14 @@
     </row>
     <row r="465" spans="1:9" ht="19" customHeight="1">
       <c r="A465" s="19" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
       <c r="B465" s="20"/>
       <c r="C465" s="19" t="s">
-        <v>1369</v>
+        <v>1362</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>1324</v>
+        <v>1317</v>
       </c>
       <c r="E465" s="20"/>
       <c r="F465" s="20"/>
@@ -21316,14 +21375,14 @@
     </row>
     <row r="466" spans="1:9" ht="19" customHeight="1">
       <c r="A466" s="19" t="s">
-        <v>1230</v>
+        <v>1223</v>
       </c>
       <c r="B466" s="20"/>
       <c r="C466" s="19" t="s">
-        <v>1370</v>
+        <v>1363</v>
       </c>
       <c r="D466" s="20" t="s">
-        <v>1325</v>
+        <v>1318</v>
       </c>
       <c r="E466" s="20"/>
       <c r="F466" s="20"/>
@@ -21333,14 +21392,14 @@
     </row>
     <row r="467" spans="1:9" ht="19" customHeight="1">
       <c r="A467" s="19" t="s">
-        <v>1231</v>
+        <v>1224</v>
       </c>
       <c r="B467" s="20"/>
       <c r="C467" s="19" t="s">
-        <v>1371</v>
+        <v>1364</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>1326</v>
+        <v>1319</v>
       </c>
       <c r="E467" s="20"/>
       <c r="F467" s="20"/>
@@ -21350,14 +21409,14 @@
     </row>
     <row r="468" spans="1:9" ht="19" customHeight="1">
       <c r="A468" s="19" t="s">
-        <v>1232</v>
+        <v>1225</v>
       </c>
       <c r="B468" s="20"/>
       <c r="C468" s="19" t="s">
-        <v>1372</v>
+        <v>1365</v>
       </c>
       <c r="D468" s="20" t="s">
-        <v>1327</v>
+        <v>1320</v>
       </c>
       <c r="E468" s="20"/>
       <c r="F468" s="20"/>
@@ -21367,14 +21426,14 @@
     </row>
     <row r="469" spans="1:9" ht="19" customHeight="1">
       <c r="A469" s="19" t="s">
-        <v>1233</v>
+        <v>1226</v>
       </c>
       <c r="B469" s="20"/>
       <c r="C469" s="19" t="s">
-        <v>1373</v>
+        <v>1366</v>
       </c>
       <c r="D469" s="20" t="s">
-        <v>1328</v>
+        <v>1321</v>
       </c>
       <c r="E469" s="20"/>
       <c r="F469" s="20"/>
@@ -21384,14 +21443,14 @@
     </row>
     <row r="470" spans="1:9" ht="19" customHeight="1">
       <c r="A470" s="19" t="s">
-        <v>1234</v>
+        <v>1227</v>
       </c>
       <c r="B470" s="20"/>
       <c r="C470" s="19" t="s">
-        <v>1374</v>
+        <v>1367</v>
       </c>
       <c r="D470" s="20" t="s">
-        <v>1329</v>
+        <v>1322</v>
       </c>
       <c r="E470" s="20"/>
       <c r="F470" s="20"/>
@@ -21401,14 +21460,14 @@
     </row>
     <row r="471" spans="1:9" ht="19" customHeight="1">
       <c r="A471" s="19" t="s">
-        <v>1235</v>
+        <v>1228</v>
       </c>
       <c r="B471" s="20"/>
       <c r="C471" s="19" t="s">
-        <v>1375</v>
+        <v>1368</v>
       </c>
       <c r="D471" s="20" t="s">
-        <v>1330</v>
+        <v>1323</v>
       </c>
       <c r="E471" s="20"/>
       <c r="F471" s="20"/>
@@ -21417,10 +21476,16 @@
       <c r="I471" s="18"/>
     </row>
     <row r="472" spans="1:9" ht="19" customHeight="1">
-      <c r="A472" s="19"/>
+      <c r="A472" s="19" t="s">
+        <v>1229</v>
+      </c>
       <c r="B472" s="20"/>
-      <c r="C472" s="20"/>
-      <c r="D472" s="20"/>
+      <c r="C472" s="19" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D472" s="20" t="s">
+        <v>1324</v>
+      </c>
       <c r="E472" s="20"/>
       <c r="F472" s="20"/>
       <c r="G472" s="18"/>
@@ -21428,10 +21493,16 @@
       <c r="I472" s="18"/>
     </row>
     <row r="473" spans="1:9" ht="19" customHeight="1">
-      <c r="A473" s="19"/>
+      <c r="A473" s="19" t="s">
+        <v>1230</v>
+      </c>
       <c r="B473" s="20"/>
-      <c r="C473" s="20"/>
-      <c r="D473" s="20"/>
+      <c r="C473" s="19" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D473" s="20" t="s">
+        <v>1325</v>
+      </c>
       <c r="E473" s="20"/>
       <c r="F473" s="20"/>
       <c r="G473" s="18"/>
@@ -21439,10 +21510,16 @@
       <c r="I473" s="18"/>
     </row>
     <row r="474" spans="1:9" ht="19" customHeight="1">
-      <c r="A474" s="19"/>
+      <c r="A474" s="19" t="s">
+        <v>1231</v>
+      </c>
       <c r="B474" s="20"/>
-      <c r="C474" s="20"/>
-      <c r="D474" s="20"/>
+      <c r="C474" s="19" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D474" s="20" t="s">
+        <v>1326</v>
+      </c>
       <c r="E474" s="20"/>
       <c r="F474" s="20"/>
       <c r="G474" s="18"/>
@@ -21450,10 +21527,16 @@
       <c r="I474" s="18"/>
     </row>
     <row r="475" spans="1:9" ht="19" customHeight="1">
-      <c r="A475" s="19"/>
+      <c r="A475" s="19" t="s">
+        <v>1232</v>
+      </c>
       <c r="B475" s="20"/>
-      <c r="C475" s="20"/>
-      <c r="D475" s="20"/>
+      <c r="C475" s="19" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D475" s="20" t="s">
+        <v>1327</v>
+      </c>
       <c r="E475" s="20"/>
       <c r="F475" s="20"/>
       <c r="G475" s="18"/>
@@ -21461,10 +21544,16 @@
       <c r="I475" s="18"/>
     </row>
     <row r="476" spans="1:9" ht="19" customHeight="1">
-      <c r="A476" s="19"/>
+      <c r="A476" s="19" t="s">
+        <v>1233</v>
+      </c>
       <c r="B476" s="20"/>
-      <c r="C476" s="20"/>
-      <c r="D476" s="20"/>
+      <c r="C476" s="19" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D476" s="20" t="s">
+        <v>1328</v>
+      </c>
       <c r="E476" s="20"/>
       <c r="F476" s="20"/>
       <c r="G476" s="18"/>
@@ -21472,10 +21561,16 @@
       <c r="I476" s="18"/>
     </row>
     <row r="477" spans="1:9" ht="19" customHeight="1">
-      <c r="A477" s="19"/>
+      <c r="A477" s="19" t="s">
+        <v>1234</v>
+      </c>
       <c r="B477" s="20"/>
-      <c r="C477" s="20"/>
-      <c r="D477" s="20"/>
+      <c r="C477" s="19" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D477" s="20" t="s">
+        <v>1329</v>
+      </c>
       <c r="E477" s="20"/>
       <c r="F477" s="20"/>
       <c r="G477" s="18"/>
@@ -21483,10 +21578,16 @@
       <c r="I477" s="18"/>
     </row>
     <row r="478" spans="1:9" ht="19" customHeight="1">
-      <c r="A478" s="19"/>
+      <c r="A478" s="19" t="s">
+        <v>1235</v>
+      </c>
       <c r="B478" s="20"/>
-      <c r="C478" s="20"/>
-      <c r="D478" s="20"/>
+      <c r="C478" s="19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D478" s="20" t="s">
+        <v>1330</v>
+      </c>
       <c r="E478" s="20"/>
       <c r="F478" s="20"/>
       <c r="G478" s="18"/>
@@ -22065,141 +22166,228 @@
       <c r="H530" s="17"/>
       <c r="I530" s="18"/>
     </row>
+    <row r="531" spans="1:9" ht="19" customHeight="1">
+      <c r="A531" s="19"/>
+      <c r="B531" s="20"/>
+      <c r="C531" s="20"/>
+      <c r="D531" s="20"/>
+      <c r="E531" s="20"/>
+      <c r="F531" s="20"/>
+      <c r="G531" s="18"/>
+      <c r="H531" s="17"/>
+      <c r="I531" s="18"/>
+    </row>
+    <row r="532" spans="1:9" ht="19" customHeight="1">
+      <c r="A532" s="19"/>
+      <c r="B532" s="20"/>
+      <c r="C532" s="20"/>
+      <c r="D532" s="20"/>
+      <c r="E532" s="20"/>
+      <c r="F532" s="20"/>
+      <c r="G532" s="18"/>
+      <c r="H532" s="17"/>
+      <c r="I532" s="18"/>
+    </row>
+    <row r="533" spans="1:9" ht="19" customHeight="1">
+      <c r="A533" s="19"/>
+      <c r="B533" s="20"/>
+      <c r="C533" s="20"/>
+      <c r="D533" s="20"/>
+      <c r="E533" s="20"/>
+      <c r="F533" s="20"/>
+      <c r="G533" s="18"/>
+      <c r="H533" s="17"/>
+      <c r="I533" s="18"/>
+    </row>
+    <row r="534" spans="1:9" ht="19" customHeight="1">
+      <c r="A534" s="19"/>
+      <c r="B534" s="20"/>
+      <c r="C534" s="20"/>
+      <c r="D534" s="20"/>
+      <c r="E534" s="20"/>
+      <c r="F534" s="20"/>
+      <c r="G534" s="18"/>
+      <c r="H534" s="17"/>
+      <c r="I534" s="18"/>
+    </row>
+    <row r="535" spans="1:9" ht="19" customHeight="1">
+      <c r="A535" s="19"/>
+      <c r="B535" s="20"/>
+      <c r="C535" s="20"/>
+      <c r="D535" s="20"/>
+      <c r="E535" s="20"/>
+      <c r="F535" s="20"/>
+      <c r="G535" s="18"/>
+      <c r="H535" s="17"/>
+      <c r="I535" s="18"/>
+    </row>
+    <row r="536" spans="1:9" ht="19" customHeight="1">
+      <c r="A536" s="19"/>
+      <c r="B536" s="20"/>
+      <c r="C536" s="20"/>
+      <c r="D536" s="20"/>
+      <c r="E536" s="20"/>
+      <c r="F536" s="20"/>
+      <c r="G536" s="18"/>
+      <c r="H536" s="17"/>
+      <c r="I536" s="18"/>
+    </row>
+    <row r="537" spans="1:9" ht="19" customHeight="1">
+      <c r="A537" s="19"/>
+      <c r="B537" s="20"/>
+      <c r="C537" s="20"/>
+      <c r="D537" s="20"/>
+      <c r="E537" s="20"/>
+      <c r="F537" s="20"/>
+      <c r="G537" s="18"/>
+      <c r="H537" s="17"/>
+      <c r="I537" s="18"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:J226" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A5:G261 I5:I530">
-    <cfRule type="expression" dxfId="39" priority="37">
+  <conditionalFormatting sqref="A5:G261 I5:I537">
+    <cfRule type="expression" dxfId="41" priority="39">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D262:D283 D286 D290:D292 D296:D300 D309 D317:D330 D334:D336 D340:D341 D346:D347 D351:D372">
-    <cfRule type="expression" dxfId="38" priority="276">
+    <cfRule type="expression" dxfId="40" priority="278">
       <formula>$G264&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D284">
-    <cfRule type="expression" dxfId="37" priority="315">
+    <cfRule type="expression" dxfId="39" priority="317">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D285">
-    <cfRule type="expression" dxfId="36" priority="314">
+    <cfRule type="expression" dxfId="38" priority="316">
       <formula>$G286&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D287:D289 D293:D295 D308 D331:D333 D337:D339 D348:D350">
-    <cfRule type="expression" dxfId="35" priority="279">
+    <cfRule type="expression" dxfId="37" priority="281">
       <formula>$G290&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D301:D307">
-    <cfRule type="expression" dxfId="34" priority="317">
+    <cfRule type="expression" dxfId="36" priority="319">
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D304">
-    <cfRule type="expression" dxfId="33" priority="351">
+    <cfRule type="expression" dxfId="35" priority="353">
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D305:D307 D343:D345">
-    <cfRule type="expression" dxfId="32" priority="388">
+    <cfRule type="expression" dxfId="34" priority="390">
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D310">
-    <cfRule type="expression" dxfId="31" priority="386">
+    <cfRule type="expression" dxfId="33" priority="388">
       <formula>$G317&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D311">
-    <cfRule type="expression" dxfId="30" priority="283">
+    <cfRule type="expression" dxfId="32" priority="285">
       <formula>$G315&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D312:D314">
-    <cfRule type="expression" dxfId="29" priority="13">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>$G312&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D315">
-    <cfRule type="expression" dxfId="28" priority="384">
+    <cfRule type="expression" dxfId="30" priority="386">
       <formula>$G320&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D342">
-    <cfRule type="expression" dxfId="27" priority="383">
+    <cfRule type="expression" dxfId="29" priority="385">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G375 D316 A334:E335 A336:C357 E336:E357 A358:E359 A360:C372 E360:E372 A373:E375 A376:G530">
-    <cfRule type="expression" dxfId="26" priority="274">
+  <conditionalFormatting sqref="D394 D396:D401">
+    <cfRule type="expression" dxfId="28" priority="2">
+      <formula>$G405&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D395">
+    <cfRule type="expression" dxfId="27" priority="1">
+      <formula>$G395&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G375 D316 A334:E335 A336:C357 E336:E357 A358:E359 A360:C372 E360:E372 A373:E375 A376:G393 A394:C401 E394:G401 A402:G537">
+    <cfRule type="expression" dxfId="26" priority="276">
       <formula>$G262&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H530">
-    <cfRule type="cellIs" dxfId="25" priority="19" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H5:H537">
+    <cfRule type="cellIs" dxfId="25" priority="21" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
+    <cfRule type="cellIs" dxfId="23" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="23" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="21" priority="25" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="24" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="20" priority="26" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="25" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="19" priority="27" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" stopIfTrue="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H404">
+    <cfRule type="containsText" dxfId="15" priority="12" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H404)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="11" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H404)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H397">
-    <cfRule type="containsText" dxfId="15" priority="11" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H397)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H397)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="9" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H397)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="containsText" dxfId="6" priority="13" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H404)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Parameter - emulatorPort - enableRestartDeviceOnResettingAppiumSession
Deprecated Parameter
- rerunScenarioWords
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F6DD02-456C-0947-91F2-932567EBA827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA19F0D7-8A92-9048-8366-C8516984D286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41320" yWindow="3060" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
+    <workbookView xWindow="40900" yWindow="3060" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
   <sheets>
     <sheet name="message" sheetId="2" r:id="rId1"/>
@@ -11951,10 +11951,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>screenIsBlackout</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>screenshotBlackoutThreshold</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -12000,14 +11996,6 @@
       </rPr>
       <t>(value=${value})</t>
     </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The screenshot is blacked out. (threshold=${value})</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スクリーンショットがブラックアウトしました。(threshold=${value})</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -12111,6 +12099,18 @@
     <rPh sb="20" eb="22">
       <t>セッテイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The screenshot is blacked out. (value:${arg1} &gt; threshold:${arg2})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スクリーンショットがブラックアウトしました。(value:${arg1} &gt; threshold:${arg2})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>screenshotIsBlackout</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -13069,8 +13069,8 @@
   <dimension ref="A1:I537"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A396" sqref="A396"/>
+      <pane ySplit="4" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A345" sqref="A345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -19353,14 +19353,14 @@
     </row>
     <row r="344" spans="1:9" ht="19" customHeight="1">
       <c r="A344" s="19" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B344" s="20"/>
       <c r="C344" s="20" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D344" s="20" t="s">
         <v>1530</v>
-      </c>
-      <c r="D344" s="20" t="s">
-        <v>1531</v>
       </c>
       <c r="E344" s="20"/>
       <c r="F344" s="20"/>
@@ -19370,14 +19370,14 @@
     </row>
     <row r="345" spans="1:9" ht="19" customHeight="1">
       <c r="A345" s="19" t="s">
-        <v>1528</v>
+        <v>1543</v>
       </c>
       <c r="B345" s="20"/>
       <c r="C345" s="20" t="s">
-        <v>1532</v>
+        <v>1541</v>
       </c>
       <c r="D345" s="20" t="s">
-        <v>1533</v>
+        <v>1542</v>
       </c>
       <c r="E345" s="20"/>
       <c r="F345" s="20"/>
@@ -20173,10 +20173,10 @@
       </c>
       <c r="B392" s="20"/>
       <c r="C392" s="20" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
       <c r="D392" s="20" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
       <c r="E392" s="20"/>
       <c r="F392" s="20"/>
@@ -20190,10 +20190,10 @@
       </c>
       <c r="B393" s="20"/>
       <c r="C393" s="20" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="D393" s="20" t="s">
-        <v>1535</v>
+        <v>1532</v>
       </c>
       <c r="E393" s="20"/>
       <c r="F393" s="20"/>
@@ -20203,14 +20203,14 @@
     </row>
     <row r="394" spans="1:9" ht="19" customHeight="1">
       <c r="A394" s="19" t="s">
-        <v>1536</v>
+        <v>1533</v>
       </c>
       <c r="B394" s="20"/>
       <c r="C394" s="20" t="s">
-        <v>1538</v>
+        <v>1535</v>
       </c>
       <c r="D394" s="20" t="s">
-        <v>1537</v>
+        <v>1534</v>
       </c>
       <c r="E394" s="20"/>
       <c r="F394" s="20"/>
@@ -20220,14 +20220,14 @@
     </row>
     <row r="395" spans="1:9" ht="19" customHeight="1">
       <c r="A395" s="19" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="B395" s="20"/>
       <c r="C395" s="20" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="D395" s="20" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="E395" s="20"/>
       <c r="F395" s="20"/>

</xml_diff>

<commit_message>
Improve Retrying and message
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA19F0D7-8A92-9048-8366-C8516984D286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC1F22B-5455-E840-94F3-A440AD76AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40900" yWindow="3060" windowWidth="35900" windowHeight="29280" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="1544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="1547">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -12111,6 +12111,24 @@
   </si>
   <si>
     <t>screenshotIsBlackout</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>packageOrBundleIdNotFound</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>package or bundleId not found. Confirm the app is installed. (${arg1}) ${submessage}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>package または bundleIdが見つかりません。アプリがインストールされているか確認してください。 (${arg1}) ${submessage}</t>
+    <rPh sb="21" eb="22">
+      <t>ミツカリ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>カクニn</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12455,7 +12473,14 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{C40AA10B-FA57-1748-8D8E-3E12991DC054}"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="43">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -12508,14 +12533,42 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12529,56 +12582,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA0D8EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12620,7 +12624,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12635,6 +12639,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13069,8 +13094,8 @@
   <dimension ref="A1:I537"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A345" sqref="A345"/>
+      <pane ySplit="4" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A397" sqref="A397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -20236,10 +20261,16 @@
       <c r="I395" s="18"/>
     </row>
     <row r="396" spans="1:9" ht="19" customHeight="1">
-      <c r="A396" s="19"/>
+      <c r="A396" s="19" t="s">
+        <v>1544</v>
+      </c>
       <c r="B396" s="20"/>
-      <c r="C396" s="20"/>
-      <c r="D396" s="20"/>
+      <c r="C396" s="20" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D396" s="20" t="s">
+        <v>1546</v>
+      </c>
       <c r="E396" s="20"/>
       <c r="F396" s="20"/>
       <c r="G396" s="18"/>
@@ -22244,150 +22275,154 @@
       <c r="I537" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J226" xr:uid="{C4FA0F16-CA74-7F4E-89C7-E1A2B23ACF88}"/>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A5:G261 I5:I537">
-    <cfRule type="expression" dxfId="41" priority="39">
+  <conditionalFormatting sqref="A5:G261 I5:I537 F263:G301 A299:E300">
+    <cfRule type="expression" dxfId="42" priority="40">
       <formula>$G5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D262:D283 D286 D290:D292 D296:D300 D309 D317:D330 D334:D336 D340:D341 D346:D347 D351:D372">
-    <cfRule type="expression" dxfId="40" priority="278">
+  <conditionalFormatting sqref="D262:D283 D286 D290:D292 D309 D317:D330 D334:D336 D340:D341 D346:D347 D351:D372 D296:D300">
+    <cfRule type="expression" dxfId="41" priority="279">
       <formula>$G264&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D284">
-    <cfRule type="expression" dxfId="39" priority="317">
+    <cfRule type="expression" dxfId="40" priority="318">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D285">
-    <cfRule type="expression" dxfId="38" priority="316">
+    <cfRule type="expression" dxfId="39" priority="317">
       <formula>$G286&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D287:D289 D293:D295 D308 D331:D333 D337:D339 D348:D350">
-    <cfRule type="expression" dxfId="37" priority="281">
+    <cfRule type="expression" dxfId="38" priority="282">
       <formula>$G290&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D301:D307">
-    <cfRule type="expression" dxfId="36" priority="319">
+    <cfRule type="expression" dxfId="37" priority="320">
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D304">
-    <cfRule type="expression" dxfId="35" priority="353">
+    <cfRule type="expression" dxfId="36" priority="354">
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D305:D307 D343:D345">
-    <cfRule type="expression" dxfId="34" priority="390">
+    <cfRule type="expression" dxfId="35" priority="391">
       <formula>$G309&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D310">
-    <cfRule type="expression" dxfId="33" priority="388">
+    <cfRule type="expression" dxfId="34" priority="389">
       <formula>$G317&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D311">
-    <cfRule type="expression" dxfId="32" priority="285">
+    <cfRule type="expression" dxfId="33" priority="286">
       <formula>$G315&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D312:D314">
-    <cfRule type="expression" dxfId="31" priority="15">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>$G312&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D315">
-    <cfRule type="expression" dxfId="30" priority="386">
+    <cfRule type="expression" dxfId="31" priority="387">
       <formula>$G320&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D342">
-    <cfRule type="expression" dxfId="29" priority="385">
+    <cfRule type="expression" dxfId="30" priority="386">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D394 D396:D401">
-    <cfRule type="expression" dxfId="28" priority="2">
+  <conditionalFormatting sqref="D394 D397:D401">
+    <cfRule type="expression" dxfId="29" priority="3">
       <formula>$G405&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D395">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>$G395&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 F263:G301 A275:E276 A277:C298 E277:E298 A299:E300 E301 A301:C333 E302:G314 E315:E333 F315:G375 D316 A334:E335 A336:C357 E336:E357 A358:E359 A360:C372 E360:E372 A373:E375 A376:G393 A394:C401 E394:G401 A402:G537">
-    <cfRule type="expression" dxfId="26" priority="276">
+  <conditionalFormatting sqref="E262:G262 A262:C274 E263:E274 A275:E276 A277:C298 E277:E298 E301 A301:C333 E302:G314 E315:E333 F315:G375 D316 A334:E335 A336:C357 E336:E357 A358:E359 A360:C372 E360:E372 A373:E375 A376:G393 A394:C401 E394:G401 A402:G537">
+    <cfRule type="expression" dxfId="27" priority="277">
       <formula>$G262&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H537">
-    <cfRule type="cellIs" dxfId="25" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="22" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="24" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="25" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="25" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="19" priority="26" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="26" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="18" priority="27" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="27" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="17" priority="28" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H404">
-    <cfRule type="containsText" dxfId="15" priority="12" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H404)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="13" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H404)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H404)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="14" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H404)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="13" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H404)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D396">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G396&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22500,22 +22535,22 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="A3:A12">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Bug Fix swipeBack -> goBack
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EA67E2-5BB4-2943-8BF3-3F22DCD7A3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CB1589-ABBA-5346-BE8E-961C04B91EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7820" yWindow="5360" windowWidth="43360" windowHeight="31740" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -12616,19 +12616,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>swipeBack</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>swipeBack()</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Swipe back</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スワイプバックする</t>
+    <t>goBack</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>goBack()</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Go back with swipe</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スワイプして戻る</t>
+    <rPh sb="6" eb="7">
+      <t>モドル</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -13045,6 +13048,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
@@ -13059,13 +13118,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -13073,28 +13125,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13102,13 +13133,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13136,7 +13160,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13158,27 +13182,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -23076,67 +23079,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H547">
-    <cfRule type="cellIs" dxfId="25" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="24" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="25" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="27" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="28" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="29" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="25" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="26" stopIfTrue="1" operator="equal">
       <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="27" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="28" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="29" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H413">
-    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="containsText" dxfId="15" priority="15" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H413)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="containsText" dxfId="14" priority="14" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H413)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="13" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H413)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="13" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H413)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="14" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H413)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="15" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H413)))</formula>
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Function - goPreviousTask
Deleted Function
- goBack

Deleted Property
- pressBackSelector
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CB1589-ABBA-5346-BE8E-961C04B91EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52F3214-5ADB-A14A-A069-919F3493609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="5360" windowWidth="43360" windowHeight="31740" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
+    <workbookView xWindow="25280" yWindow="9600" windowWidth="43360" windowHeight="31740" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
   <sheets>
     <sheet name="message" sheetId="2" r:id="rId1"/>
@@ -12616,22 +12616,25 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>goBack</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>goBack()</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Go back with swipe</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スワイプして戻る</t>
+    <t>前のタスクに戻る</t>
+    <rPh sb="0" eb="1">
+      <t>マエノ</t>
+    </rPh>
     <rPh sb="6" eb="7">
       <t>モドル</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>goPreviousTask</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>goPreviousTask()</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Go previous task</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -13616,8 +13619,8 @@
   <dimension ref="A1:I547"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
+      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.42578125" defaultRowHeight="19" customHeight="1" outlineLevelCol="1"/>
@@ -14803,16 +14806,16 @@
     </row>
     <row r="65" spans="1:9" ht="19" customHeight="1">
       <c r="A65" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B65" s="20" t="s">
-        <v>800</v>
+        <v>1584</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>1585</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>281</v>
+        <v>1586</v>
+      </c>
+      <c r="D65" s="30" t="s">
+        <v>1583</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
@@ -14822,16 +14825,16 @@
     </row>
     <row r="66" spans="1:9" ht="19" customHeight="1">
       <c r="A66" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>282</v>
+        <v>62</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>281</v>
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
@@ -14841,16 +14844,16 @@
     </row>
     <row r="67" spans="1:9" ht="19" customHeight="1">
       <c r="A67" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>283</v>
+        <v>64</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>282</v>
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
@@ -14860,16 +14863,16 @@
     </row>
     <row r="68" spans="1:9" ht="19" customHeight="1">
       <c r="A68" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="20"/>
@@ -14879,16 +14882,16 @@
     </row>
     <row r="69" spans="1:9" ht="19" customHeight="1">
       <c r="A69" s="19" t="s">
-        <v>899</v>
+        <v>67</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>900</v>
+        <v>402</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>901</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>901</v>
+        <v>68</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>284</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="20"/>
@@ -14898,16 +14901,16 @@
     </row>
     <row r="70" spans="1:9" ht="19" customHeight="1">
       <c r="A70" s="19" t="s">
-        <v>804</v>
+        <v>899</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>806</v>
+        <v>900</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>807</v>
+        <v>901</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>808</v>
+        <v>901</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
@@ -14917,16 +14920,16 @@
     </row>
     <row r="71" spans="1:9" ht="19" customHeight="1">
       <c r="A71" s="19" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
@@ -14936,16 +14939,16 @@
     </row>
     <row r="72" spans="1:9" ht="19" customHeight="1">
       <c r="A72" s="19" t="s">
-        <v>1051</v>
+        <v>805</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>868</v>
+        <v>810</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>867</v>
+        <v>811</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="20"/>
@@ -14955,16 +14958,16 @@
     </row>
     <row r="73" spans="1:9" ht="19" customHeight="1">
       <c r="A73" s="19" t="s">
-        <v>802</v>
+        <v>1051</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>803</v>
+        <v>868</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>866</v>
+        <v>809</v>
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="20"/>
@@ -14974,16 +14977,16 @@
     </row>
     <row r="74" spans="1:9" ht="19" customHeight="1">
       <c r="A74" s="19" t="s">
-        <v>817</v>
+        <v>802</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>820</v>
+        <v>803</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>821</v>
+        <v>869</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>822</v>
+        <v>866</v>
       </c>
       <c r="E74" s="20"/>
       <c r="F74" s="20"/>
@@ -14993,16 +14996,16 @@
     </row>
     <row r="75" spans="1:9" ht="19" customHeight="1">
       <c r="A75" s="19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>859</v>
+        <v>821</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>861</v>
+        <v>822</v>
       </c>
       <c r="E75" s="20"/>
       <c r="F75" s="20"/>
@@ -15012,16 +15015,16 @@
     </row>
     <row r="76" spans="1:9" ht="19" customHeight="1">
       <c r="A76" s="19" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D76" s="20" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E76" s="20"/>
       <c r="F76" s="20"/>
@@ -15031,16 +15034,16 @@
     </row>
     <row r="77" spans="1:9" ht="19" customHeight="1">
       <c r="A77" s="19" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="B77" s="20" t="s">
-        <v>816</v>
+        <v>824</v>
       </c>
       <c r="C77" s="20" t="s">
-        <v>863</v>
-      </c>
-      <c r="D77" s="21" t="s">
-        <v>864</v>
+        <v>860</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>862</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="20"/>
@@ -15050,16 +15053,16 @@
     </row>
     <row r="78" spans="1:9" ht="19" customHeight="1">
       <c r="A78" s="19" t="s">
-        <v>69</v>
+        <v>815</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>403</v>
+        <v>816</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>881</v>
+        <v>863</v>
+      </c>
+      <c r="D78" s="21" t="s">
+        <v>864</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="20"/>
@@ -15069,16 +15072,16 @@
     </row>
     <row r="79" spans="1:9" ht="19" customHeight="1">
       <c r="A79" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B79" s="20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>285</v>
+        <v>881</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="20"/>
@@ -15088,16 +15091,16 @@
     </row>
     <row r="80" spans="1:9" ht="19" customHeight="1">
       <c r="A80" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>882</v>
+        <v>285</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="20"/>
@@ -15107,16 +15110,16 @@
     </row>
     <row r="81" spans="1:9" ht="19" customHeight="1">
       <c r="A81" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D81" s="20" t="s">
-        <v>286</v>
+        <v>882</v>
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="20"/>
@@ -15126,16 +15129,16 @@
     </row>
     <row r="82" spans="1:9" ht="19" customHeight="1">
       <c r="A82" s="19" t="s">
-        <v>910</v>
+        <v>75</v>
       </c>
       <c r="B82" s="20" t="s">
-        <v>911</v>
+        <v>406</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>912</v>
+        <v>76</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>913</v>
+        <v>286</v>
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="20"/>
@@ -15145,16 +15148,16 @@
     </row>
     <row r="83" spans="1:9" ht="19" customHeight="1">
       <c r="A83" s="19" t="s">
-        <v>77</v>
+        <v>910</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>407</v>
+        <v>911</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D83" s="22" t="s">
-        <v>287</v>
+        <v>912</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>913</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="20"/>
@@ -15164,16 +15167,16 @@
     </row>
     <row r="84" spans="1:9" ht="19" customHeight="1">
       <c r="A84" s="19" t="s">
-        <v>878</v>
+        <v>77</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>879</v>
+        <v>407</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>880</v>
+        <v>78</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>883</v>
+        <v>287</v>
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="20"/>
@@ -15183,16 +15186,16 @@
     </row>
     <row r="85" spans="1:9" ht="19" customHeight="1">
       <c r="A85" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>408</v>
+        <v>878</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>879</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D85" s="21" t="s">
-        <v>288</v>
+        <v>880</v>
+      </c>
+      <c r="D85" s="22" t="s">
+        <v>883</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="20"/>
@@ -15202,16 +15205,16 @@
     </row>
     <row r="86" spans="1:9" ht="19" customHeight="1">
       <c r="A86" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B86" s="20" t="s">
-        <v>409</v>
+        <v>79</v>
+      </c>
+      <c r="B86" s="19" t="s">
+        <v>408</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>289</v>
+        <v>80</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>288</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="20"/>
@@ -15221,16 +15224,16 @@
     </row>
     <row r="87" spans="1:9" ht="19" customHeight="1">
       <c r="A87" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B87" s="19" t="s">
-        <v>411</v>
+        <v>81</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>409</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>410</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>290</v>
+        <v>82</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>289</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="20"/>
@@ -15240,16 +15243,16 @@
     </row>
     <row r="88" spans="1:9" ht="19" customHeight="1">
       <c r="A88" s="19" t="s">
-        <v>1583</v>
+        <v>83</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>1584</v>
+        <v>411</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>1585</v>
-      </c>
-      <c r="D88" s="30" t="s">
-        <v>1586</v>
+        <v>410</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>290</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="20"/>

</xml_diff>

<commit_message>
Rename Function goPreviousTask -> goPreviousApp
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52F3214-5ADB-A14A-A069-919F3493609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32BD2F2-306E-D34D-80BD-15CD1496A6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="9600" windowWidth="43360" windowHeight="31740" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -12616,25 +12616,25 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>前のタスクに戻る</t>
+    <t>goPreviousApp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>goPreviousApp()</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Go previous app</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>前のアプリに戻る</t>
     <rPh sb="0" eb="1">
       <t>マエノ</t>
     </rPh>
     <rPh sb="6" eb="7">
       <t>モドル</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>goPreviousTask</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>goPreviousTask()</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Go previous task</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -14806,16 +14806,16 @@
     </row>
     <row r="65" spans="1:9" ht="19" customHeight="1">
       <c r="A65" s="19" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B65" s="19" t="s">
         <v>1584</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="C65" s="20" t="s">
         <v>1585</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="D65" s="30" t="s">
         <v>1586</v>
-      </c>
-      <c r="D65" s="30" t="s">
-        <v>1583</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>

</xml_diff>

<commit_message>
New Function - goPreviousApp
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32BD2F2-306E-D34D-80BD-15CD1496A6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C091A7-DAAA-B34B-A284-1AD8A6180D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="9600" windowWidth="43360" windowHeight="31740" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -12624,10 +12624,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Go previous app</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>前のアプリに戻る</t>
     <rPh sb="0" eb="1">
       <t>マエノ</t>
@@ -12635,6 +12631,10 @@
     <rPh sb="6" eb="7">
       <t>モドル</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Go to previous app</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -14812,10 +14812,10 @@
         <v>1584</v>
       </c>
       <c r="C65" s="20" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D65" s="30" t="s">
         <v>1585</v>
-      </c>
-      <c r="D65" s="30" t="s">
-        <v>1586</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>

</xml_diff>

<commit_message>
Bug Fix - dataPattern
</commit_message>
<xml_diff>
--- a/src/main/resources/message.xlsx
+++ b/src/main/resources/message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C159B6-8BBD-AA46-98F0-65AFF72E5D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367E23F3-3B45-7242-A14B-55437B0EE224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25280" yWindow="9600" windowWidth="43360" windowHeight="31740" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -11241,30 +11241,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Data pattern. (${subject}=${arg1})</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tsukushi A Round Gothic Bold"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>データパターン</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (${subject}=${arg1})</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <r>
       <t>${subject}</t>
     </r>
@@ -12666,6 +12642,30 @@
     <rPh sb="6" eb="8">
       <t>シュトク</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data pattern. (${subject} -&gt; ${arg1})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tsukushi A Round Gothic Bold"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>データパターン</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (${subject} -&gt; ${arg1})</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -13040,13 +13040,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -13089,6 +13082,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
@@ -13103,13 +13152,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -13117,28 +13159,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13152,7 +13173,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13180,7 +13201,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFBDD7EE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13195,27 +13216,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13657,7 +13657,7 @@
   <dimension ref="A1:I548"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -14103,16 +14103,16 @@
     </row>
     <row r="26" spans="1:9" ht="19" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="B26" s="20" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>1486</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>1487</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>1488</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
@@ -14844,16 +14844,16 @@
     </row>
     <row r="65" spans="1:9" ht="19" customHeight="1">
       <c r="A65" s="19" t="s">
+        <v>1581</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D65" s="30" t="s">
         <v>1583</v>
-      </c>
-      <c r="B65" s="19" t="s">
-        <v>1584</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>1586</v>
-      </c>
-      <c r="D65" s="30" t="s">
-        <v>1585</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
@@ -15680,16 +15680,16 @@
     </row>
     <row r="109" spans="1:9" ht="19" customHeight="1">
       <c r="A109" s="19" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B109" s="19" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C109" s="20" t="s">
         <v>1489</v>
       </c>
-      <c r="B109" s="19" t="s">
+      <c r="D109" s="20" t="s">
         <v>1490</v>
-      </c>
-      <c r="C109" s="20" t="s">
-        <v>1491</v>
-      </c>
-      <c r="D109" s="20" t="s">
-        <v>1492</v>
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="20"/>
@@ -16145,7 +16145,7 @@
         <v>136</v>
       </c>
       <c r="D133" s="20" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="E133" s="20"/>
       <c r="F133" s="20"/>
@@ -16164,7 +16164,7 @@
         <v>138</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="E134" s="20"/>
       <c r="F134" s="20"/>
@@ -16183,7 +16183,7 @@
         <v>140</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="E135" s="20"/>
       <c r="F135" s="20"/>
@@ -16202,7 +16202,7 @@
         <v>142</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="E136" s="20"/>
       <c r="F136" s="20"/>
@@ -16221,7 +16221,7 @@
         <v>17</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="E137" s="20"/>
       <c r="F137" s="20"/>
@@ -16240,7 +16240,7 @@
         <v>145</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="E138" s="20"/>
       <c r="F138" s="20"/>
@@ -16259,7 +16259,7 @@
         <v>19</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="E139" s="20"/>
       <c r="F139" s="20"/>
@@ -16278,7 +16278,7 @@
         <v>148</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="E140" s="20"/>
       <c r="F140" s="20"/>
@@ -16297,7 +16297,7 @@
         <v>150</v>
       </c>
       <c r="D141" s="20" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="E141" s="20"/>
       <c r="F141" s="20"/>
@@ -16316,7 +16316,7 @@
         <v>152</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="E142" s="20"/>
       <c r="F142" s="20"/>
@@ -16326,16 +16326,16 @@
     </row>
     <row r="143" spans="1:9" ht="19" customHeight="1">
       <c r="A143" s="19" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B143" s="19" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C143" s="20" t="s">
         <v>1493</v>
       </c>
-      <c r="B143" s="19" t="s">
+      <c r="D143" s="20" t="s">
         <v>1494</v>
-      </c>
-      <c r="C143" s="20" t="s">
-        <v>1495</v>
-      </c>
-      <c r="D143" s="20" t="s">
-        <v>1496</v>
       </c>
       <c r="E143" s="20"/>
       <c r="F143" s="20"/>
@@ -16354,7 +16354,7 @@
         <v>154</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="E144" s="20"/>
       <c r="F144" s="20"/>
@@ -16373,7 +16373,7 @@
         <v>156</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="E145" s="20"/>
       <c r="F145" s="20"/>
@@ -16573,16 +16573,16 @@
     </row>
     <row r="156" spans="1:9" ht="19" customHeight="1">
       <c r="A156" s="19" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B156" s="19" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C156" s="20" t="s">
         <v>1497</v>
       </c>
-      <c r="B156" s="19" t="s">
+      <c r="D156" s="20" t="s">
         <v>1498</v>
-      </c>
-      <c r="C156" s="20" t="s">
-        <v>1499</v>
-      </c>
-      <c r="D156" s="20" t="s">
-        <v>1500</v>
       </c>
       <c r="E156" s="20"/>
       <c r="F156" s="20"/>
@@ -16668,7 +16668,7 @@
     </row>
     <row r="161" spans="1:9" ht="19" customHeight="1">
       <c r="A161" s="19" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="B161" s="20" t="s">
         <v>424</v>
@@ -17200,16 +17200,16 @@
     </row>
     <row r="189" spans="1:9" ht="19" customHeight="1">
       <c r="A189" s="19" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B189" s="19" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C189" s="20" t="s">
         <v>1482</v>
       </c>
-      <c r="B189" s="19" t="s">
+      <c r="D189" s="20" t="s">
         <v>1483</v>
-      </c>
-      <c r="C189" s="20" t="s">
-        <v>1484</v>
-      </c>
-      <c r="D189" s="20" t="s">
-        <v>1485</v>
       </c>
       <c r="E189" s="20"/>
       <c r="F189" s="20"/>
@@ -17599,16 +17599,16 @@
     </row>
     <row r="210" spans="1:9" ht="19" customHeight="1">
       <c r="A210" s="19" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="B210" s="19" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="C210" s="20" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="D210" s="20" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="E210" s="20"/>
       <c r="F210" s="20"/>
@@ -17618,16 +17618,16 @@
     </row>
     <row r="211" spans="1:9" ht="19" customHeight="1">
       <c r="A211" s="19" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="B211" s="19" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="C211" s="20" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="D211" s="20" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="E211" s="20"/>
       <c r="F211" s="20"/>
@@ -17637,16 +17637,16 @@
     </row>
     <row r="212" spans="1:9" ht="19" customHeight="1">
       <c r="A212" s="19" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="B212" s="19" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="C212" s="20" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="D212" s="20" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="E212" s="20"/>
       <c r="F212" s="20"/>
@@ -17656,16 +17656,16 @@
     </row>
     <row r="213" spans="1:9" ht="19" customHeight="1">
       <c r="A213" s="19" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="B213" s="19" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="C213" s="20" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="D213" s="20" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="E213" s="20"/>
       <c r="F213" s="20"/>
@@ -17808,16 +17808,16 @@
     </row>
     <row r="221" spans="1:9" ht="19" customHeight="1">
       <c r="A221" s="19" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="B221" s="19" t="s">
         <v>424</v>
       </c>
       <c r="C221" s="20" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="D221" s="20" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="E221" s="20"/>
       <c r="F221" s="20"/>
@@ -18074,14 +18074,14 @@
     </row>
     <row r="235" spans="1:9" ht="19" customHeight="1">
       <c r="A235" s="19" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="B235" s="20"/>
       <c r="C235" s="20" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="D235" s="20" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="E235" s="20"/>
       <c r="F235" s="20"/>
@@ -18091,14 +18091,14 @@
     </row>
     <row r="236" spans="1:9" ht="19" customHeight="1">
       <c r="A236" s="19" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="B236" s="20"/>
       <c r="C236" s="20" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="D236" s="20" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="E236" s="20"/>
       <c r="F236" s="20"/>
@@ -19494,14 +19494,14 @@
     </row>
     <row r="317" spans="1:9" ht="19" customHeight="1">
       <c r="A317" s="19" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="B317" s="20"/>
       <c r="C317" s="20" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="D317" s="29" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="E317" s="20"/>
       <c r="F317" s="20"/>
@@ -19613,14 +19613,14 @@
     </row>
     <row r="324" spans="1:9" ht="19" customHeight="1">
       <c r="A324" s="19" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="B324" s="20"/>
       <c r="C324" s="20" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="D324" s="20" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="E324" s="20"/>
       <c r="F324" s="20"/>
@@ -20123,14 +20123,14 @@
     </row>
     <row r="354" spans="1:9" ht="19" customHeight="1">
       <c r="A354" s="19" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="B354" s="20"/>
       <c r="C354" s="20" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="D354" s="20" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="E354" s="20"/>
       <c r="F354" s="20"/>
@@ -20140,14 +20140,14 @@
     </row>
     <row r="355" spans="1:9" ht="19" customHeight="1">
       <c r="A355" s="19" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="B355" s="20"/>
       <c r="C355" s="20" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="D355" s="20" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="E355" s="20"/>
       <c r="F355" s="20"/>
@@ -20327,14 +20327,14 @@
     </row>
     <row r="366" spans="1:9" ht="19" customHeight="1">
       <c r="A366" s="19" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="B366" s="20"/>
       <c r="C366" s="20" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="D366" s="21" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="E366" s="20"/>
       <c r="F366" s="20"/>
@@ -20382,10 +20382,10 @@
       </c>
       <c r="B369" s="20"/>
       <c r="C369" s="20" t="s">
-        <v>1467</v>
+        <v>1588</v>
       </c>
       <c r="D369" s="21" t="s">
-        <v>1468</v>
+        <v>1589</v>
       </c>
       <c r="E369" s="20"/>
       <c r="F369" s="20"/>
@@ -20871,14 +20871,14 @@
     </row>
     <row r="398" spans="1:9" ht="19" customHeight="1">
       <c r="A398" s="19" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="B398" s="20"/>
       <c r="C398" s="20" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="D398" s="20" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="E398" s="20"/>
       <c r="F398" s="20"/>
@@ -20888,14 +20888,14 @@
     </row>
     <row r="399" spans="1:9" ht="19" customHeight="1">
       <c r="A399" s="19" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="B399" s="20"/>
       <c r="C399" s="20" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="D399" s="20" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="E399" s="20"/>
       <c r="F399" s="20"/>
@@ -20905,14 +20905,14 @@
     </row>
     <row r="400" spans="1:9" ht="19" customHeight="1">
       <c r="A400" s="19" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="B400" s="20"/>
       <c r="C400" s="20" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="D400" s="20" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="E400" s="20"/>
       <c r="F400" s="20"/>
@@ -20922,14 +20922,14 @@
     </row>
     <row r="401" spans="1:9" ht="19" customHeight="1">
       <c r="A401" s="19" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="B401" s="20"/>
       <c r="C401" s="20" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="D401" s="20" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="E401" s="20"/>
       <c r="F401" s="20"/>
@@ -20939,14 +20939,14 @@
     </row>
     <row r="402" spans="1:9" ht="19" customHeight="1">
       <c r="A402" s="19" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="B402" s="20"/>
       <c r="C402" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="D402" s="20" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="E402" s="20"/>
       <c r="F402" s="20"/>
@@ -20956,14 +20956,14 @@
     </row>
     <row r="403" spans="1:9" ht="19" customHeight="1">
       <c r="A403" s="19" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="B403" s="20"/>
       <c r="C403" s="20" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="D403" s="20" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="E403" s="20"/>
       <c r="F403" s="20"/>
@@ -20973,14 +20973,14 @@
     </row>
     <row r="404" spans="1:9" ht="19" customHeight="1">
       <c r="A404" s="19" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="B404" s="20"/>
       <c r="C404" s="20" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="D404" s="20" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="E404" s="20"/>
       <c r="F404" s="20"/>
@@ -20990,14 +20990,14 @@
     </row>
     <row r="405" spans="1:9" ht="19" customHeight="1">
       <c r="A405" s="19" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="B405" s="20"/>
       <c r="C405" s="20" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="D405" s="20" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
@@ -21007,14 +21007,14 @@
     </row>
     <row r="406" spans="1:9" ht="19" customHeight="1">
       <c r="A406" s="19" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="B406" s="20"/>
       <c r="C406" s="20" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="D406" s="20" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="E406" s="20"/>
       <c r="F406" s="20"/>
@@ -21024,14 +21024,14 @@
     </row>
     <row r="407" spans="1:9" ht="19" customHeight="1">
       <c r="A407" s="19" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="B407" s="20"/>
       <c r="C407" s="20" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="D407" s="20" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="E407" s="20"/>
       <c r="F407" s="20"/>
@@ -21041,14 +21041,14 @@
     </row>
     <row r="408" spans="1:9" ht="19" customHeight="1">
       <c r="A408" s="19" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="B408" s="20"/>
       <c r="C408" s="20" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="D408" s="29" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="E408" s="20"/>
       <c r="F408" s="20"/>
@@ -21738,14 +21738,14 @@
     </row>
     <row r="451" spans="1:9" ht="19" customHeight="1">
       <c r="A451" s="19" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="B451" s="20"/>
       <c r="C451" s="19" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="D451" s="20" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="E451" s="20"/>
       <c r="F451" s="20"/>
@@ -21755,14 +21755,14 @@
     </row>
     <row r="452" spans="1:9" ht="19" customHeight="1">
       <c r="A452" s="19" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="B452" s="20"/>
       <c r="C452" s="19" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="D452" s="20" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="E452" s="20"/>
       <c r="F452" s="20"/>
@@ -21779,7 +21779,7 @@
         <v>1343</v>
       </c>
       <c r="D453" s="20" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="E453" s="20"/>
       <c r="F453" s="20"/>
@@ -21796,7 +21796,7 @@
         <v>1344</v>
       </c>
       <c r="D454" s="20" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="E454" s="20"/>
       <c r="F454" s="20"/>
@@ -21813,7 +21813,7 @@
         <v>1207</v>
       </c>
       <c r="D455" s="20" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="E455" s="20"/>
       <c r="F455" s="20"/>
@@ -21830,7 +21830,7 @@
         <v>1208</v>
       </c>
       <c r="D456" s="20" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="E456" s="20"/>
       <c r="F456" s="20"/>
@@ -21847,7 +21847,7 @@
         <v>1209</v>
       </c>
       <c r="D457" s="20" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="E457" s="20"/>
       <c r="F457" s="20"/>
@@ -21864,7 +21864,7 @@
         <v>1210</v>
       </c>
       <c r="D458" s="20" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="E458" s="20"/>
       <c r="F458" s="20"/>
@@ -21881,7 +21881,7 @@
         <v>1211</v>
       </c>
       <c r="D459" s="20" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="E459" s="20"/>
       <c r="F459" s="20"/>
@@ -23086,14 +23086,14 @@
       <formula>$G318&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D325 D313:D315">
-    <cfRule type="expression" dxfId="36" priority="355">
+  <conditionalFormatting sqref="D312">
+    <cfRule type="expression" dxfId="36" priority="397">
       <formula>$G318&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D324 D353:D355 D316:D317">
-    <cfRule type="expression" dxfId="35" priority="392">
-      <formula>$G320&lt;&gt;""</formula>
+  <conditionalFormatting sqref="D313:D315 D325">
+    <cfRule type="expression" dxfId="35" priority="355">
+      <formula>$G318&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D315">
@@ -23101,108 +23101,108 @@
       <formula>$G325&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D316:D317 D324 D353:D355">
+    <cfRule type="expression" dxfId="33" priority="392">
+      <formula>$G320&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D319">
-    <cfRule type="expression" dxfId="33" priority="390">
+    <cfRule type="expression" dxfId="32" priority="390">
       <formula>$G327&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D320">
-    <cfRule type="expression" dxfId="32" priority="287">
+    <cfRule type="expression" dxfId="31" priority="287">
       <formula>$G325&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D321:D323">
-    <cfRule type="expression" dxfId="31" priority="17">
+    <cfRule type="expression" dxfId="30" priority="17">
       <formula>$G321&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D352">
-    <cfRule type="expression" dxfId="30" priority="387">
+    <cfRule type="expression" dxfId="29" priority="387">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D405">
-    <cfRule type="expression" dxfId="29" priority="395">
+    <cfRule type="expression" dxfId="28" priority="395">
       <formula>$G415&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D408:D411">
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="27" priority="4">
       <formula>$G419&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E270:G270 A270:C282 E271:E282 A283:E284 A285:C306 E285:E306 E309 E325:E343 F325:G386 D326 A344:E345 A346:C368 E346:E368 A369:E370 A371:C383 E371:E383 A384:E386 A387:G404">
-    <cfRule type="expression" dxfId="27" priority="278">
+    <cfRule type="expression" dxfId="26" priority="278">
       <formula>$G270&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H548">
-    <cfRule type="cellIs" dxfId="26" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="cellIs" dxfId="25" priority="24" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
+    <cfRule type="cellIs" dxfId="24" priority="25" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="23" priority="23" stopIfTrue="1" operator="equal">
       <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="27" stopIfTrue="1" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="22" priority="27" stopIfTrue="1" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="28" stopIfTrue="1" operator="containsText" text="SKIP">
+    <cfRule type="containsText" dxfId="21" priority="28" stopIfTrue="1" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="29" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="containsText" dxfId="20" priority="29" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",H5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H414">
-    <cfRule type="cellIs" dxfId="16" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
+    <cfRule type="containsText" dxfId="15" priority="15" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H414)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
+    <cfRule type="containsText" dxfId="14" priority="14" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",H414)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
+    <cfRule type="containsText" dxfId="13" priority="13" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",H414)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="13" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",H414)))</formula>
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="14" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",H414)))</formula>
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="15" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",H414)))</formula>
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D312">
-    <cfRule type="expression" dxfId="0" priority="397">
-      <formula>$G318&lt;&gt;""</formula>
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23315,22 +23315,22 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="A3:A12">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"実施対象外"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>